<commit_message>
Added CV for CSIRO, NUIM, and IITM
</commit_message>
<xml_diff>
--- a/CORDEX_ESGF_coordination_issues.xlsx
+++ b/CORDEX_ESGF_coordination_issues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="768" windowWidth="16608" windowHeight="8676" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="768" windowWidth="16608" windowHeight="8676" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralRemarks" sheetId="7" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="DataAvail" sheetId="11" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DataAvail!$B$3:$F$49</definedName>
     <definedName name="AFR_22" localSheetId="3">ControlledVocabulary!#REF!</definedName>
     <definedName name="AFR_22" localSheetId="2">DatVol!$B$34</definedName>
     <definedName name="AFR_22" localSheetId="0">GeneralRemarks!#REF!</definedName>
@@ -34,8 +35,8 @@
     <definedName name="ANT44tier1">DatVol!$C$36</definedName>
     <definedName name="ARC_44">DatVol!$B$37</definedName>
     <definedName name="ARC44tier1">DatVol!$C$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$AV$13</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AW$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$AW$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AX$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">DatVol!$A$1:$BA$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$4</definedName>
     <definedName name="EUR_11" localSheetId="3">ControlledVocabulary!#REF!</definedName>
@@ -54,8 +55,8 @@
     <definedName name="MED44tier1" localSheetId="2">DatVol!$C$32</definedName>
     <definedName name="MED44tier1" localSheetId="0">GeneralRemarks!#REF!</definedName>
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
-    <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AV$9</definedName>
-    <definedName name="Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AT$5</definedName>
+    <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AW$9</definedName>
+    <definedName name="Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AU$5</definedName>
     <definedName name="Print_Area" localSheetId="2">DatVol!$A$1:$AZ$39</definedName>
     <definedName name="Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$2</definedName>
   </definedNames>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="230">
   <si>
     <t>Domain</t>
   </si>
@@ -1014,9 +1015,6 @@
     <t>IPSL/INERIS</t>
   </si>
   <si>
-    <t>robert.vautard@lsce.ipsl.fr</t>
-  </si>
-  <si>
     <t>confirmed by
 Robert V.</t>
   </si>
@@ -1035,9 +1033,6 @@
   </si>
   <si>
     <t>University of Castilla-La Mancha, Toledo, Spain</t>
-  </si>
-  <si>
-    <t>marta.dominguez@uclm.es; miguel.gaertner@uclm.es</t>
   </si>
   <si>
     <t>Helmholtz-Zentrum Geesthacht, Climate Service Center, Max Planck Institute for Meteorology</t>
@@ -1205,6 +1200,55 @@
   </si>
   <si>
     <t>EUR-11 EUR-11i</t>
+  </si>
+  <si>
+    <t>National University of Ireland Maynooth</t>
+  </si>
+  <si>
+    <t>Rowan Fealy : rowan.fealy
+@nuim.ie</t>
+  </si>
+  <si>
+    <t>robert.vautard
+@lsce.ipsl.fr</t>
+  </si>
+  <si>
+    <t>marta.dominguez@uclm.es; miguel.gaertner
+@uclm.es</t>
+  </si>
+  <si>
+    <t>Indian Institute of Tropical Meteorology</t>
+  </si>
+  <si>
+    <t>IITM</t>
+  </si>
+  <si>
+    <t>RegCM4-1</t>
+  </si>
+  <si>
+    <t>J. Sanjay sanjay
+@tropmet.res.in</t>
+  </si>
+  <si>
+    <t>confirmed by 
+Rowan Fealy</t>
+  </si>
+  <si>
+    <t>confirmed by
+J. Sanjay</t>
+  </si>
+  <si>
+    <t>CSIRO</t>
+  </si>
+  <si>
+    <t>Commonwealth Scientific and Industrial Research Organisation</t>
+  </si>
+  <si>
+    <t>Jack.Katzfey@csiro.au</t>
+  </si>
+  <si>
+    <t>confirmed by 
+Jack Katzfey</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1541,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="74">
+  <borders count="76">
     <border>
       <left/>
       <right/>
@@ -2462,6 +2506,32 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -2472,7 +2542,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2919,6 +2989,9 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2987,6 +3060,30 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2996,227 +3093,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <color auto="1"/>
@@ -3733,7 +3610,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3743,27 +3620,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="191" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="190"/>
-      <c r="K1" s="190"/>
-      <c r="L1" s="190"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="191"/>
       <c r="M1" s="21"/>
       <c r="N1" s="20"/>
       <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="54">
-        <v>41731</v>
+        <v>41901</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -3781,12 +3658,12 @@
       <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" s="148" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="191" t="s">
-        <v>185</v>
-      </c>
-      <c r="B3" s="191"/>
-      <c r="C3" s="191"/>
-      <c r="D3" s="191"/>
+      <c r="A3" s="192" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="192"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
       <c r="E3" s="147"/>
       <c r="F3" s="147"/>
       <c r="G3" s="147"/>
@@ -3822,10 +3699,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BQ38"/>
+  <dimension ref="A1:BZ38"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AN7" sqref="AN7:AN11"/>
+    <sheetView topLeftCell="U2" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3853,33 +3730,34 @@
     <col min="27" max="27" width="20" customWidth="1"/>
     <col min="28" max="28" width="13.88671875" customWidth="1"/>
     <col min="29" max="29" width="13.109375" customWidth="1"/>
-    <col min="30" max="30" width="12.5546875" customWidth="1"/>
-    <col min="31" max="31" width="13.109375" customWidth="1"/>
-    <col min="32" max="32" width="12" customWidth="1"/>
-    <col min="33" max="35" width="16.6640625" customWidth="1"/>
-    <col min="36" max="47" width="13.77734375" customWidth="1"/>
-    <col min="48" max="48" width="22.44140625" customWidth="1"/>
+    <col min="30" max="30" width="13.77734375" customWidth="1"/>
+    <col min="31" max="31" width="12.5546875" customWidth="1"/>
+    <col min="32" max="32" width="13.109375" customWidth="1"/>
+    <col min="33" max="33" width="12" customWidth="1"/>
+    <col min="34" max="36" width="16.6640625" customWidth="1"/>
+    <col min="37" max="48" width="13.77734375" customWidth="1"/>
+    <col min="49" max="49" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="192" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="190"/>
-      <c r="K1" s="190"/>
-      <c r="L1" s="190"/>
-      <c r="M1" s="190"/>
-      <c r="N1" s="190"/>
-      <c r="O1" s="190"/>
-      <c r="P1" s="190"/>
+    <row r="1" spans="1:78" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="193" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="191"/>
+      <c r="M1" s="191"/>
+      <c r="N1" s="191"/>
+      <c r="O1" s="191"/>
+      <c r="P1" s="191"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="20"/>
       <c r="S1" s="20"/>
@@ -3911,19 +3789,29 @@
       <c r="AS1" s="20"/>
       <c r="AT1" s="20"/>
       <c r="AU1" s="20"/>
+      <c r="AV1" s="20"/>
+      <c r="BR1" s="26"/>
+      <c r="BS1" s="26"/>
+      <c r="BT1" s="26"/>
+      <c r="BU1" s="26"/>
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="26"/>
+      <c r="BX1" s="26"/>
+      <c r="BY1" s="26"/>
+      <c r="BZ1" s="26"/>
     </row>
-    <row r="2" spans="1:69" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:78" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="53">
         <f>GeneralRemarks!A2</f>
-        <v>41731</v>
-      </c>
-      <c r="B2" s="194"/>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
-      <c r="E2" s="194"/>
-      <c r="F2" s="194"/>
-      <c r="G2" s="194"/>
-      <c r="H2" s="194"/>
+        <v>41901</v>
+      </c>
+      <c r="B2" s="195"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
       <c r="I2" s="51"/>
       <c r="J2" s="51"/>
       <c r="K2" s="51"/>
@@ -3940,7 +3828,7 @@
       <c r="V2" s="20"/>
       <c r="W2" s="54">
         <f>A2</f>
-        <v>41731</v>
+        <v>41901</v>
       </c>
       <c r="X2" s="20"/>
       <c r="Y2" s="20"/>
@@ -3966,12 +3854,22 @@
       <c r="AS2" s="20"/>
       <c r="AT2" s="20"/>
       <c r="AU2" s="20"/>
-      <c r="AV2" s="73">
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="73">
         <f>A2</f>
-        <v>41731</v>
-      </c>
+        <v>41901</v>
+      </c>
+      <c r="BR2" s="26"/>
+      <c r="BS2" s="26"/>
+      <c r="BT2" s="26"/>
+      <c r="BU2" s="26"/>
+      <c r="BV2" s="26"/>
+      <c r="BW2" s="26"/>
+      <c r="BX2" s="26"/>
+      <c r="BY2" s="26"/>
+      <c r="BZ2" s="26"/>
     </row>
-    <row r="3" spans="1:69" s="1" customFormat="1" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:78" s="1" customFormat="1" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="168" t="s">
         <v>57</v>
       </c>
@@ -4003,7 +3901,7 @@
         <v>100</v>
       </c>
       <c r="K3" s="112" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L3" s="112" t="s">
         <v>101</v>
@@ -4042,51 +3940,57 @@
         <v>117</v>
       </c>
       <c r="X3" s="112" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Y3" s="112" t="s">
-        <v>173</v>
+        <v>219</v>
       </c>
       <c r="Z3" s="112" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA3" s="112" t="s">
         <v>205</v>
-      </c>
-      <c r="AA3" s="112" t="s">
-        <v>207</v>
       </c>
       <c r="AB3" s="112"/>
       <c r="AC3" s="112" t="s">
         <v>135</v>
       </c>
-      <c r="AD3" s="112"/>
-      <c r="AE3" s="167" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF3" s="112"/>
-      <c r="AG3" s="112"/>
-      <c r="AH3" s="113" t="s">
-        <v>98</v>
-      </c>
+      <c r="AD3" s="214" t="s">
+        <v>223</v>
+      </c>
+      <c r="AE3" s="112"/>
+      <c r="AF3" s="167" t="s">
+        <v>178</v>
+      </c>
+      <c r="AG3" s="112" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH3" s="112"/>
       <c r="AI3" s="113" t="s">
         <v>98</v>
       </c>
-      <c r="AJ3" s="112"/>
+      <c r="AJ3" s="113" t="s">
+        <v>98</v>
+      </c>
       <c r="AK3" s="112"/>
       <c r="AL3" s="112"/>
       <c r="AM3" s="112"/>
-      <c r="AN3" s="112" t="s">
-        <v>166</v>
-      </c>
-      <c r="AO3" s="112"/>
+      <c r="AN3" s="112"/>
+      <c r="AO3" s="112" t="s">
+        <v>218</v>
+      </c>
       <c r="AP3" s="112"/>
       <c r="AQ3" s="112"/>
-      <c r="AR3" s="112"/>
+      <c r="AR3" s="214" t="s">
+        <v>217</v>
+      </c>
       <c r="AS3" s="112"/>
       <c r="AT3" s="112"/>
       <c r="AU3" s="112"/>
-      <c r="AV3" s="168" t="s">
+      <c r="AV3" s="112"/>
+      <c r="AW3" s="168" t="s">
         <v>57</v>
       </c>
-      <c r="AW3" s="2"/>
       <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
@@ -4107,8 +4011,17 @@
       <c r="BO3" s="2"/>
       <c r="BP3" s="2"/>
       <c r="BQ3" s="2"/>
+      <c r="BR3" s="2"/>
+      <c r="BS3" s="2"/>
+      <c r="BT3" s="2"/>
+      <c r="BU3" s="2"/>
+      <c r="BV3" s="2"/>
+      <c r="BW3" s="2"/>
+      <c r="BX3" s="2"/>
+      <c r="BY3" s="2"/>
+      <c r="BZ3" s="2"/>
     </row>
-    <row r="4" spans="1:69" s="1" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:78" s="1" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="170" t="s">
         <v>41</v>
       </c>
@@ -4187,7 +4100,7 @@
         <v>KNMI</v>
       </c>
       <c r="X4" s="115" t="str">
-        <f t="shared" ref="X4:AH4" si="2">X7</f>
+        <f t="shared" ref="X4:AI4" si="2">X7</f>
         <v>UQAM</v>
       </c>
       <c r="Y4" s="115" t="str">
@@ -4207,81 +4120,81 @@
         <f t="shared" si="2"/>
         <v>DHMZ</v>
       </c>
-      <c r="AD4" s="115" t="str">
+      <c r="AD4" s="215"/>
+      <c r="AE4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>GISS</v>
       </c>
-      <c r="AE4" s="115" t="str">
+      <c r="AF4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>CCCma</v>
       </c>
-      <c r="AF4" s="115" t="str">
-        <f t="shared" si="2"/>
-        <v>CSIR</v>
-      </c>
       <c r="AG4" s="115" t="str">
+        <f>AG7</f>
+        <v>CSIRO</v>
+      </c>
+      <c r="AH4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>KAUST</v>
       </c>
-      <c r="AH4" s="116" t="str">
+      <c r="AI4" s="116" t="str">
         <f t="shared" si="2"/>
         <v>MOHC</v>
       </c>
-      <c r="AI4" s="116" t="str">
-        <f t="shared" ref="AI4" si="3">AI7</f>
+      <c r="AJ4" s="116" t="str">
+        <f t="shared" ref="AJ4" si="3">AJ7</f>
         <v>MOHC</v>
       </c>
-      <c r="AJ4" s="115" t="str">
-        <f>AJ7</f>
+      <c r="AK4" s="115" t="str">
+        <f>AK7</f>
         <v>MIUB</v>
       </c>
-      <c r="AK4" s="115" t="str">
-        <f t="shared" ref="AK4:AU4" si="4">AK7</f>
+      <c r="AL4" s="115" t="str">
+        <f t="shared" ref="AL4:AV4" si="4">AL7</f>
         <v>BCCR</v>
       </c>
-      <c r="AL4" s="115" t="str">
+      <c r="AM4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>CRP-GL</v>
       </c>
-      <c r="AM4" s="115" t="str">
+      <c r="AN4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>IDL</v>
       </c>
-      <c r="AN4" s="115" t="s">
+      <c r="AO4" s="115" t="s">
         <v>165</v>
       </c>
-      <c r="AO4" s="115" t="str">
+      <c r="AP4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>AUTH-Met</v>
       </c>
-      <c r="AP4" s="115" t="str">
+      <c r="AQ4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>AUTH-LHTEE</v>
       </c>
-      <c r="AQ4" s="115" t="str">
+      <c r="AR4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>NUIM</v>
       </c>
-      <c r="AR4" s="115" t="str">
+      <c r="AS4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>UHOH</v>
       </c>
-      <c r="AS4" s="115" t="str">
+      <c r="AT4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>UM</v>
-      </c>
-      <c r="AT4" s="115" t="str">
-        <f t="shared" si="4"/>
-        <v>UCAN</v>
       </c>
       <c r="AU4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>UCAN</v>
       </c>
-      <c r="AV4" s="170" t="s">
+      <c r="AV4" s="115" t="str">
+        <f t="shared" si="4"/>
+        <v>UCAN</v>
+      </c>
+      <c r="AW4" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="AW4" s="2"/>
       <c r="AX4" s="2"/>
       <c r="AY4" s="2"/>
       <c r="AZ4" s="2"/>
@@ -4302,8 +4215,17 @@
       <c r="BO4" s="2"/>
       <c r="BP4" s="2"/>
       <c r="BQ4" s="2"/>
+      <c r="BR4" s="2"/>
+      <c r="BS4" s="2"/>
+      <c r="BT4" s="2"/>
+      <c r="BU4" s="2"/>
+      <c r="BV4" s="2"/>
+      <c r="BW4" s="2"/>
+      <c r="BX4" s="2"/>
+      <c r="BY4" s="2"/>
+      <c r="BZ4" s="2"/>
     </row>
-    <row r="5" spans="1:69" s="136" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:78" s="136" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="171" t="s">
         <v>126</v>
       </c>
@@ -4341,28 +4263,28 @@
       <c r="AA5" s="131"/>
       <c r="AB5" s="131"/>
       <c r="AC5" s="131"/>
-      <c r="AD5" s="131"/>
+      <c r="AD5" s="216"/>
       <c r="AE5" s="131"/>
       <c r="AF5" s="131"/>
       <c r="AG5" s="131"/>
-      <c r="AH5" s="132"/>
+      <c r="AH5" s="131"/>
       <c r="AI5" s="132"/>
-      <c r="AJ5" s="133"/>
+      <c r="AJ5" s="132"/>
       <c r="AK5" s="133"/>
-      <c r="AL5" s="134"/>
+      <c r="AL5" s="133"/>
       <c r="AM5" s="134"/>
       <c r="AN5" s="134"/>
-      <c r="AO5" s="131"/>
+      <c r="AO5" s="134"/>
       <c r="AP5" s="131"/>
       <c r="AQ5" s="131"/>
       <c r="AR5" s="131"/>
       <c r="AS5" s="131"/>
       <c r="AT5" s="131"/>
       <c r="AU5" s="131"/>
-      <c r="AV5" s="171" t="s">
+      <c r="AV5" s="131"/>
+      <c r="AW5" s="171" t="s">
         <v>126</v>
       </c>
-      <c r="AW5" s="135"/>
       <c r="AX5" s="135"/>
       <c r="AY5" s="135"/>
       <c r="AZ5" s="135"/>
@@ -4383,8 +4305,17 @@
       <c r="BO5" s="135"/>
       <c r="BP5" s="135"/>
       <c r="BQ5" s="135"/>
+      <c r="BR5" s="135"/>
+      <c r="BS5" s="135"/>
+      <c r="BT5" s="135"/>
+      <c r="BU5" s="135"/>
+      <c r="BV5" s="135"/>
+      <c r="BW5" s="135"/>
+      <c r="BX5" s="135"/>
+      <c r="BY5" s="135"/>
+      <c r="BZ5" s="135"/>
     </row>
-    <row r="6" spans="1:69" s="1" customFormat="1" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:78" s="1" customFormat="1" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="170" t="s">
         <v>64</v>
       </c>
@@ -4416,13 +4347,13 @@
       <c r="AA6" s="115"/>
       <c r="AB6" s="115"/>
       <c r="AC6" s="115"/>
-      <c r="AD6" s="115"/>
+      <c r="AD6" s="215"/>
       <c r="AE6" s="115"/>
       <c r="AF6" s="115"/>
       <c r="AG6" s="115"/>
-      <c r="AH6" s="116"/>
+      <c r="AH6" s="115"/>
       <c r="AI6" s="116"/>
-      <c r="AJ6" s="115"/>
+      <c r="AJ6" s="116"/>
       <c r="AK6" s="115"/>
       <c r="AL6" s="115"/>
       <c r="AM6" s="115"/>
@@ -4434,10 +4365,10 @@
       <c r="AS6" s="115"/>
       <c r="AT6" s="115"/>
       <c r="AU6" s="115"/>
-      <c r="AV6" s="170" t="s">
+      <c r="AV6" s="115"/>
+      <c r="AW6" s="170" t="s">
         <v>64</v>
       </c>
-      <c r="AW6" s="2"/>
       <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
       <c r="AZ6" s="2"/>
@@ -4458,10 +4389,19 @@
       <c r="BO6" s="2"/>
       <c r="BP6" s="2"/>
       <c r="BQ6" s="2"/>
+      <c r="BR6" s="2"/>
+      <c r="BS6" s="2"/>
+      <c r="BT6" s="2"/>
+      <c r="BU6" s="2"/>
+      <c r="BV6" s="2"/>
+      <c r="BW6" s="2"/>
+      <c r="BX6" s="2"/>
+      <c r="BY6" s="2"/>
+      <c r="BZ6" s="2"/>
     </row>
-    <row r="7" spans="1:69" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:78" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="171" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B7" s="177" t="s">
         <v>22</v>
@@ -4539,7 +4479,7 @@
         <v>38</v>
       </c>
       <c r="AA7" s="178" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AB7" s="178" t="s">
         <v>51</v>
@@ -4547,64 +4487,66 @@
       <c r="AC7" s="178" t="s">
         <v>48</v>
       </c>
-      <c r="AD7" s="178" t="s">
+      <c r="AD7" s="217" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE7" s="178" t="s">
         <v>37</v>
       </c>
-      <c r="AE7" s="178" t="s">
+      <c r="AF7" s="178" t="s">
         <v>120</v>
       </c>
-      <c r="AF7" s="178" t="s">
-        <v>54</v>
-      </c>
       <c r="AG7" s="178" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH7" s="178" t="s">
         <v>55</v>
-      </c>
-      <c r="AH7" s="178" t="s">
-        <v>53</v>
       </c>
       <c r="AI7" s="178" t="s">
         <v>53</v>
       </c>
-      <c r="AJ7" s="183" t="s">
+      <c r="AJ7" s="178" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK7" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="AK7" s="183" t="s">
+      <c r="AL7" s="183" t="s">
         <v>45</v>
       </c>
-      <c r="AL7" s="186" t="s">
+      <c r="AM7" s="186" t="s">
         <v>36</v>
       </c>
-      <c r="AM7" s="186" t="s">
+      <c r="AN7" s="186" t="s">
         <v>46</v>
       </c>
-      <c r="AN7" s="186" t="s">
+      <c r="AO7" s="186" t="s">
         <v>164</v>
       </c>
-      <c r="AO7" s="178" t="s">
+      <c r="AP7" s="178" t="s">
         <v>144</v>
       </c>
-      <c r="AP7" s="178" t="s">
+      <c r="AQ7" s="178" t="s">
         <v>145</v>
       </c>
-      <c r="AQ7" s="178" t="s">
+      <c r="AR7" s="178" t="s">
         <v>56</v>
       </c>
-      <c r="AR7" s="178" t="s">
+      <c r="AS7" s="178" t="s">
         <v>33</v>
       </c>
-      <c r="AS7" s="178" t="s">
+      <c r="AT7" s="178" t="s">
         <v>32</v>
-      </c>
-      <c r="AT7" s="178" t="s">
-        <v>140</v>
       </c>
       <c r="AU7" s="178" t="s">
         <v>140</v>
       </c>
-      <c r="AV7" s="171" t="s">
-        <v>187</v>
-      </c>
-      <c r="AW7" s="2"/>
+      <c r="AV7" s="178" t="s">
+        <v>140</v>
+      </c>
+      <c r="AW7" s="171" t="s">
+        <v>185</v>
+      </c>
       <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
@@ -4625,8 +4567,17 @@
       <c r="BO7" s="2"/>
       <c r="BP7" s="2"/>
       <c r="BQ7" s="2"/>
+      <c r="BR7" s="2"/>
+      <c r="BS7" s="2"/>
+      <c r="BT7" s="2"/>
+      <c r="BU7" s="2"/>
+      <c r="BV7" s="2"/>
+      <c r="BW7" s="2"/>
+      <c r="BX7" s="2"/>
+      <c r="BY7" s="2"/>
+      <c r="BZ7" s="2"/>
     </row>
-    <row r="8" spans="1:69" s="121" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:78" s="121" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="171" t="s">
         <v>86</v>
       </c>
@@ -4714,64 +4665,66 @@
       <c r="AC8" s="180" t="s">
         <v>134</v>
       </c>
-      <c r="AD8" s="182" t="s">
+      <c r="AD8" s="218" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE8" s="182" t="s">
         <v>27</v>
       </c>
-      <c r="AE8" s="180" t="s">
+      <c r="AF8" s="180" t="s">
         <v>28</v>
       </c>
-      <c r="AF8" s="180" t="s">
+      <c r="AG8" s="180" t="s">
         <v>29</v>
       </c>
-      <c r="AG8" s="180" t="s">
+      <c r="AH8" s="180" t="s">
         <v>30</v>
       </c>
-      <c r="AH8" s="179" t="s">
+      <c r="AI8" s="179" t="s">
         <v>114</v>
       </c>
-      <c r="AI8" s="179" t="s">
+      <c r="AJ8" s="179" t="s">
         <v>128</v>
       </c>
-      <c r="AJ8" s="184" t="s">
+      <c r="AK8" s="184" t="s">
         <v>137</v>
       </c>
-      <c r="AK8" s="184" t="s">
+      <c r="AL8" s="184" t="s">
         <v>136</v>
       </c>
-      <c r="AL8" s="187" t="s">
+      <c r="AM8" s="187" t="s">
         <v>137</v>
       </c>
-      <c r="AM8" s="187" t="s">
+      <c r="AN8" s="187" t="s">
         <v>138</v>
       </c>
-      <c r="AN8" s="187" t="s">
+      <c r="AO8" s="187" t="s">
         <v>139</v>
       </c>
-      <c r="AO8" s="182" t="s">
+      <c r="AP8" s="182" t="s">
         <v>137</v>
       </c>
-      <c r="AP8" s="180" t="s">
+      <c r="AQ8" s="180" t="s">
         <v>146</v>
       </c>
-      <c r="AQ8" s="182" t="s">
-        <v>177</v>
-      </c>
       <c r="AR8" s="182" t="s">
+        <v>175</v>
+      </c>
+      <c r="AS8" s="182" t="s">
         <v>142</v>
       </c>
-      <c r="AS8" s="182" t="s">
+      <c r="AT8" s="182" t="s">
         <v>24</v>
       </c>
-      <c r="AT8" s="188" t="s">
+      <c r="AU8" s="188" t="s">
         <v>141</v>
       </c>
-      <c r="AU8" s="182" t="s">
+      <c r="AV8" s="182" t="s">
         <v>147</v>
       </c>
-      <c r="AV8" s="171" t="s">
+      <c r="AW8" s="171" t="s">
         <v>86</v>
       </c>
-      <c r="AW8" s="120"/>
       <c r="AX8" s="120"/>
       <c r="AY8" s="120"/>
       <c r="AZ8" s="120"/>
@@ -4792,119 +4745,134 @@
       <c r="BO8" s="120"/>
       <c r="BP8" s="120"/>
       <c r="BQ8" s="120"/>
+      <c r="BR8" s="120"/>
+      <c r="BS8" s="120"/>
+      <c r="BT8" s="120"/>
+      <c r="BU8" s="120"/>
+      <c r="BV8" s="120"/>
+      <c r="BW8" s="120"/>
+      <c r="BX8" s="120"/>
+      <c r="BY8" s="120"/>
+      <c r="BZ8" s="120"/>
     </row>
-    <row r="9" spans="1:69" s="35" customFormat="1" ht="72" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:78" s="35" customFormat="1" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="170" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="116"/>
       <c r="C9" s="116" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D9" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E9" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F9" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G9" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H9" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I9" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J9" s="116" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K9" s="116" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L9" s="116" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M9" s="116" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N9" s="116" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O9" s="116" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P9" s="116" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q9" s="116"/>
       <c r="R9" s="116" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="S9" s="116" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="T9" s="185" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="U9" s="185" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="V9" s="185" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="W9" s="185" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X9" s="116" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Y9" s="116" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Z9" s="116" t="s">
+        <v>202</v>
+      </c>
+      <c r="AA9" s="116" t="s">
         <v>204</v>
-      </c>
-      <c r="AA9" s="116" t="s">
-        <v>206</v>
       </c>
       <c r="AB9" s="116"/>
       <c r="AC9" s="116" t="s">
-        <v>190</v>
-      </c>
-      <c r="AD9" s="116"/>
-      <c r="AE9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="AF9" s="116"/>
-      <c r="AG9" s="116"/>
-      <c r="AH9" s="116" t="s">
+        <v>188</v>
+      </c>
+      <c r="AD9" s="219" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE9" s="116"/>
+      <c r="AF9" s="116" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG9" s="116" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH9" s="116"/>
+      <c r="AI9" s="116" t="s">
+        <v>189</v>
+      </c>
+      <c r="AJ9" s="116" t="s">
+        <v>189</v>
+      </c>
+      <c r="AK9" s="185"/>
+      <c r="AL9" s="185" t="s">
         <v>191</v>
       </c>
-      <c r="AI9" s="116" t="s">
-        <v>191</v>
-      </c>
-      <c r="AJ9" s="185"/>
-      <c r="AK9" s="185" t="s">
-        <v>193</v>
-      </c>
-      <c r="AL9" s="185"/>
       <c r="AM9" s="185"/>
       <c r="AN9" s="185"/>
-      <c r="AO9" s="116"/>
+      <c r="AO9" s="185"/>
       <c r="AP9" s="116"/>
       <c r="AQ9" s="116"/>
-      <c r="AR9" s="116"/>
+      <c r="AR9" s="219" t="s">
+        <v>216</v>
+      </c>
       <c r="AS9" s="116"/>
       <c r="AT9" s="116"/>
       <c r="AU9" s="116"/>
-      <c r="AV9" s="170" t="s">
-        <v>168</v>
-      </c>
-      <c r="AW9" s="72"/>
+      <c r="AV9" s="116"/>
+      <c r="AW9" s="170" t="s">
+        <v>167</v>
+      </c>
       <c r="AX9" s="72"/>
       <c r="AY9" s="72"/>
       <c r="AZ9" s="72"/>
@@ -4925,17 +4893,26 @@
       <c r="BO9" s="72"/>
       <c r="BP9" s="72"/>
       <c r="BQ9" s="72"/>
+      <c r="BR9" s="72"/>
+      <c r="BS9" s="72"/>
+      <c r="BT9" s="72"/>
+      <c r="BU9" s="72"/>
+      <c r="BV9" s="72"/>
+      <c r="BW9" s="72"/>
+      <c r="BX9" s="72"/>
+      <c r="BY9" s="72"/>
+      <c r="BZ9" s="72"/>
     </row>
-    <row r="10" spans="1:69" s="1" customFormat="1" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:78" s="1" customFormat="1" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="170" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B10" s="181" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C10" s="181"/>
       <c r="D10" s="181" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E10" s="181"/>
       <c r="F10" s="181"/>
@@ -4944,31 +4921,31 @@
       <c r="I10" s="181"/>
       <c r="J10" s="189"/>
       <c r="K10" s="189" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L10" s="189"/>
       <c r="M10" s="189"/>
       <c r="N10" s="189" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O10" s="189"/>
       <c r="P10" s="181" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="Q10" s="181"/>
       <c r="R10" s="116" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="S10" s="181"/>
       <c r="T10" s="181"/>
       <c r="U10" s="181" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="V10" s="181" t="s">
+        <v>210</v>
+      </c>
+      <c r="W10" s="181" t="s">
         <v>212</v>
-      </c>
-      <c r="W10" s="181" t="s">
-        <v>214</v>
       </c>
       <c r="X10" s="116"/>
       <c r="Y10" s="116"/>
@@ -4976,34 +4953,34 @@
       <c r="AA10" s="116"/>
       <c r="AB10" s="116"/>
       <c r="AC10" s="116"/>
-      <c r="AD10" s="116"/>
+      <c r="AD10" s="219"/>
       <c r="AE10" s="116"/>
       <c r="AF10" s="116"/>
       <c r="AG10" s="116"/>
       <c r="AH10" s="116"/>
-      <c r="AI10" s="116" t="s">
-        <v>211</v>
-      </c>
-      <c r="AJ10" s="116"/>
+      <c r="AI10" s="116"/>
+      <c r="AJ10" s="116" t="s">
+        <v>209</v>
+      </c>
       <c r="AK10" s="116"/>
       <c r="AL10" s="116"/>
       <c r="AM10" s="116"/>
-      <c r="AN10" s="116" t="s">
-        <v>200</v>
-      </c>
-      <c r="AO10" s="116"/>
+      <c r="AN10" s="116"/>
+      <c r="AO10" s="116" t="s">
+        <v>198</v>
+      </c>
       <c r="AP10" s="116"/>
       <c r="AQ10" s="116"/>
       <c r="AR10" s="116"/>
       <c r="AS10" s="116"/>
-      <c r="AT10" s="116" t="s">
-        <v>202</v>
-      </c>
-      <c r="AU10" s="116"/>
-      <c r="AV10" s="170" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW10" s="2"/>
+      <c r="AT10" s="116"/>
+      <c r="AU10" s="116" t="s">
+        <v>200</v>
+      </c>
+      <c r="AV10" s="116"/>
+      <c r="AW10" s="170" t="s">
+        <v>197</v>
+      </c>
       <c r="AX10" s="2"/>
       <c r="AY10" s="2"/>
       <c r="AZ10" s="2"/>
@@ -5024,121 +5001,134 @@
       <c r="BO10" s="2"/>
       <c r="BP10" s="2"/>
       <c r="BQ10" s="2"/>
+      <c r="BR10" s="2"/>
+      <c r="BS10" s="2"/>
+      <c r="BT10" s="2"/>
+      <c r="BU10" s="2"/>
+      <c r="BV10" s="2"/>
+      <c r="BW10" s="2"/>
+      <c r="BX10" s="2"/>
+      <c r="BY10" s="2"/>
+      <c r="BZ10" s="2"/>
     </row>
-    <row r="11" spans="1:69" s="136" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:78" s="136" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="172" t="s">
         <v>153</v>
       </c>
       <c r="B11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C11" s="116"/>
       <c r="D11" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E11" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F11" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G11" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H11" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I11" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="N11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="O11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="P11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Q11" s="116"/>
       <c r="R11" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="S11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="T11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="U11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="V11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="W11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="X11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y11" s="116"/>
       <c r="Z11" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AA11" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AB11" s="116"/>
       <c r="AC11" s="116" t="s">
-        <v>183</v>
-      </c>
-      <c r="AD11" s="116"/>
-      <c r="AE11" s="116" t="s">
-        <v>178</v>
-      </c>
-      <c r="AF11" s="116"/>
+        <v>181</v>
+      </c>
+      <c r="AD11" s="116" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE11" s="116"/>
+      <c r="AF11" s="116" t="s">
+        <v>176</v>
+      </c>
       <c r="AG11" s="116"/>
-      <c r="AH11" s="116" t="s">
-        <v>178</v>
-      </c>
+      <c r="AH11" s="116"/>
       <c r="AI11" s="116" t="s">
-        <v>178</v>
-      </c>
-      <c r="AJ11" s="116"/>
-      <c r="AK11" s="116" t="s">
-        <v>178</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="AJ11" s="116" t="s">
+        <v>176</v>
+      </c>
+      <c r="AK11" s="116"/>
       <c r="AL11" s="116" t="s">
-        <v>178</v>
-      </c>
-      <c r="AM11" s="116"/>
+        <v>176</v>
+      </c>
+      <c r="AM11" s="116" t="s">
+        <v>176</v>
+      </c>
       <c r="AN11" s="116"/>
       <c r="AO11" s="116"/>
       <c r="AP11" s="116"/>
       <c r="AQ11" s="116"/>
-      <c r="AR11" s="116"/>
+      <c r="AR11" s="116" t="s">
+        <v>181</v>
+      </c>
       <c r="AS11" s="116"/>
-      <c r="AT11" s="116" t="s">
-        <v>183</v>
-      </c>
-      <c r="AU11" s="116"/>
-      <c r="AV11" s="172" t="s">
+      <c r="AT11" s="116"/>
+      <c r="AU11" s="116" t="s">
+        <v>181</v>
+      </c>
+      <c r="AV11" s="116"/>
+      <c r="AW11" s="220" t="s">
         <v>153</v>
       </c>
-      <c r="AW11" s="135"/>
       <c r="AX11" s="135"/>
       <c r="AY11" s="135"/>
       <c r="AZ11" s="135"/>
@@ -5159,18 +5149,27 @@
       <c r="BO11" s="135"/>
       <c r="BP11" s="135"/>
       <c r="BQ11" s="135"/>
+      <c r="BR11" s="135"/>
+      <c r="BS11" s="135"/>
+      <c r="BT11" s="135"/>
+      <c r="BU11" s="135"/>
+      <c r="BV11" s="135"/>
+      <c r="BW11" s="135"/>
+      <c r="BX11" s="135"/>
+      <c r="BY11" s="135"/>
+      <c r="BZ11" s="135"/>
     </row>
-    <row r="12" spans="1:69" s="26" customFormat="1" ht="21.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="193" t="s">
+    <row r="12" spans="1:78" s="26" customFormat="1" ht="21.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="194" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="193"/>
-      <c r="C12" s="193"/>
-      <c r="D12" s="193"/>
-      <c r="E12" s="193"/>
-      <c r="F12" s="193"/>
-      <c r="G12" s="193"/>
-      <c r="H12" s="193"/>
+      <c r="B12" s="194"/>
+      <c r="C12" s="194"/>
+      <c r="D12" s="194"/>
+      <c r="E12" s="194"/>
+      <c r="F12" s="194"/>
+      <c r="G12" s="194"/>
+      <c r="H12" s="194"/>
       <c r="I12" s="127"/>
       <c r="J12" s="127"/>
       <c r="K12" s="127"/>
@@ -5192,7 +5191,7 @@
       <c r="AA12" s="151"/>
       <c r="AB12" s="127"/>
       <c r="AC12" s="127"/>
-      <c r="AD12" s="127"/>
+      <c r="AD12" s="190"/>
       <c r="AE12" s="127"/>
       <c r="AF12" s="127"/>
       <c r="AG12" s="127"/>
@@ -5210,16 +5209,17 @@
       <c r="AS12" s="127"/>
       <c r="AT12" s="127"/>
       <c r="AU12" s="127"/>
+      <c r="AV12" s="127"/>
     </row>
-    <row r="13" spans="1:69" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="193" t="s">
+    <row r="13" spans="1:78" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="194" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="193"/>
-      <c r="C13" s="193"/>
-      <c r="D13" s="193"/>
-      <c r="E13" s="193"/>
-      <c r="F13" s="193"/>
+      <c r="B13" s="194"/>
+      <c r="C13" s="194"/>
+      <c r="D13" s="194"/>
+      <c r="E13" s="194"/>
+      <c r="F13" s="194"/>
       <c r="G13" s="141"/>
       <c r="H13" s="141"/>
       <c r="I13" s="141"/>
@@ -5261,9 +5261,10 @@
       <c r="AS13" s="141"/>
       <c r="AT13" s="141"/>
       <c r="AU13" s="141"/>
+      <c r="AV13" s="141"/>
     </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.3">
-      <c r="AV14" s="72"/>
+    <row r="14" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="AW14" s="72"/>
     </row>
     <row r="22" spans="4:14" x14ac:dyDescent="0.3">
       <c r="N22" s="122"/>
@@ -5283,18 +5284,23 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A13:F13"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:AU11">
-    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="B7:AC11 AE11:AV11 AD7:AV10">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AD11">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",AD11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="AE3" r:id="rId1" display="mailto:John.Scinocca@ec.gc.ca"/>
+    <hyperlink ref="AF3" r:id="rId1" display="mailto:John.Scinocca@ec.gc.ca"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="47" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="33" max="8" man="1"/>
+    <brk id="34" max="8" man="1"/>
   </colBreaks>
 </worksheet>
 </file>
@@ -5351,25 +5357,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:144" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="191" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="190"/>
-      <c r="K1" s="190"/>
-      <c r="L1" s="190"/>
-      <c r="M1" s="190"/>
-      <c r="N1" s="190"/>
-      <c r="O1" s="190"/>
-      <c r="P1" s="190"/>
-      <c r="Q1" s="190"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="191"/>
+      <c r="M1" s="191"/>
+      <c r="N1" s="191"/>
+      <c r="O1" s="191"/>
+      <c r="P1" s="191"/>
+      <c r="Q1" s="191"/>
       <c r="R1" s="21"/>
       <c r="S1" s="20"/>
       <c r="T1" s="20"/>
@@ -5407,7 +5413,7 @@
     <row r="2" spans="1:144" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="53">
         <f>GeneralRemarks!A2</f>
-        <v>41731</v>
+        <v>41901</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -5433,7 +5439,7 @@
       <c r="W2" s="20"/>
       <c r="X2" s="54">
         <f>GeneralRemarks!A2</f>
-        <v>41731</v>
+        <v>41901</v>
       </c>
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
@@ -5463,7 +5469,7 @@
       <c r="AX2" s="20"/>
       <c r="AZ2" s="73">
         <f>A2</f>
-        <v>41731</v>
+        <v>41901</v>
       </c>
     </row>
     <row r="3" spans="1:144" s="1" customFormat="1" ht="36.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5598,7 +5604,8 @@
       </c>
       <c r="AA3" s="29" t="str">
         <f>AllEntries!Y3</f>
-        <v>marta.dominguez@uclm.es; miguel.gaertner@uclm.es</v>
+        <v>marta.dominguez@uclm.es; miguel.gaertner
+@uclm.es</v>
       </c>
       <c r="AB3" s="29" t="str">
         <f>AllEntries!Z3</f>
@@ -5619,11 +5626,11 @@
 Cedo Brankovic</v>
       </c>
       <c r="AF3" s="29">
-        <f>AllEntries!AD3</f>
+        <f>AllEntries!AE3</f>
         <v>0</v>
       </c>
       <c r="AG3" s="27" t="str">
-        <f>AllEntries!AE3</f>
+        <f>AllEntries!AF3</f>
         <v>John.Scinocca
 @ec.gc.ca</v>
       </c>
@@ -5631,62 +5638,64 @@
         <f>AllEntries!A3</f>
         <v>Contact</v>
       </c>
-      <c r="AI3" s="27">
-        <f>AllEntries!AF3</f>
-        <v>0</v>
+      <c r="AI3" s="27" t="str">
+        <f>AllEntries!AG3</f>
+        <v>Jack.Katzfey@csiro.au</v>
       </c>
       <c r="AJ3" s="29">
-        <f>AllEntries!AG3</f>
+        <f>AllEntries!AH3</f>
         <v>0</v>
       </c>
       <c r="AK3" s="55" t="str">
-        <f>AllEntries!AH3</f>
-        <v>carlo.buontempo
-@metoffice.gov.uk</v>
-      </c>
-      <c r="AL3" s="55" t="str">
         <f>AllEntries!AI3</f>
         <v>carlo.buontempo
 @metoffice.gov.uk</v>
       </c>
+      <c r="AL3" s="55" t="str">
+        <f>AllEntries!AJ3</f>
+        <v>carlo.buontempo
+@metoffice.gov.uk</v>
+      </c>
       <c r="AM3" s="29">
-        <f>AllEntries!AJ3</f>
+        <f>AllEntries!AK3</f>
         <v>0</v>
       </c>
       <c r="AN3" s="29">
-        <f>AllEntries!AK3</f>
+        <f>AllEntries!AL3</f>
         <v>0</v>
       </c>
       <c r="AO3" s="29">
-        <f>AllEntries!AL3</f>
+        <f>AllEntries!AM3</f>
         <v>0</v>
       </c>
       <c r="AP3" s="29">
-        <f>AllEntries!AM3</f>
+        <f>AllEntries!AN3</f>
         <v>0</v>
       </c>
       <c r="AQ3" s="29" t="str">
-        <f>AllEntries!AN3</f>
-        <v>robert.vautard@lsce.ipsl.fr</v>
+        <f>AllEntries!AO3</f>
+        <v>robert.vautard
+@lsce.ipsl.fr</v>
       </c>
       <c r="AR3" s="29">
-        <f>AllEntries!AO3</f>
+        <f>AllEntries!AP3</f>
         <v>0</v>
       </c>
       <c r="AS3" s="29">
-        <f>AllEntries!AP3</f>
-        <v>0</v>
-      </c>
-      <c r="AT3" s="29">
         <f>AllEntries!AQ3</f>
         <v>0</v>
       </c>
+      <c r="AT3" s="29" t="str">
+        <f>AllEntries!AR3</f>
+        <v>Rowan Fealy : rowan.fealy
+@nuim.ie</v>
+      </c>
       <c r="AU3" s="29">
-        <f>AllEntries!AR3</f>
+        <f>AllEntries!AS3</f>
         <v>0</v>
       </c>
       <c r="AV3" s="29">
-        <f>AllEntries!AS3</f>
+        <f>AllEntries!AT3</f>
         <v>0</v>
       </c>
       <c r="AW3" s="29" t="e">
@@ -5694,11 +5703,11 @@
         <v>#REF!</v>
       </c>
       <c r="AX3" s="41">
-        <f>AllEntries!AT3</f>
+        <f>AllEntries!AU3</f>
         <v>0</v>
       </c>
       <c r="AY3" s="27">
-        <f>AllEntries!AU3</f>
+        <f>AllEntries!AV3</f>
         <v>0</v>
       </c>
       <c r="AZ3" s="81"/>
@@ -5923,11 +5932,11 @@
         <v>DHMZ</v>
       </c>
       <c r="AF4" s="35" t="str">
-        <f>AllEntries!AD4</f>
+        <f>AllEntries!AE4</f>
         <v>GISS</v>
       </c>
       <c r="AG4" s="33" t="str">
-        <f>AllEntries!AE4</f>
+        <f>AllEntries!AF4</f>
         <v>CCCma</v>
       </c>
       <c r="AH4" s="75" t="str">
@@ -5935,59 +5944,59 @@
         <v>Data providing  center</v>
       </c>
       <c r="AI4" s="33" t="str">
-        <f>AllEntries!AF4</f>
-        <v>CSIR</v>
+        <f>AllEntries!AG4</f>
+        <v>CSIRO</v>
       </c>
       <c r="AJ4" s="35" t="str">
-        <f>AllEntries!AG4</f>
+        <f>AllEntries!AH4</f>
         <v>KAUST</v>
       </c>
       <c r="AK4" s="56" t="str">
-        <f>AllEntries!AH4</f>
-        <v>MOHC</v>
-      </c>
-      <c r="AL4" s="56" t="str">
         <f>AllEntries!AI4</f>
         <v>MOHC</v>
       </c>
+      <c r="AL4" s="56" t="str">
+        <f>AllEntries!AJ4</f>
+        <v>MOHC</v>
+      </c>
       <c r="AM4" s="35" t="str">
-        <f>AllEntries!AJ4</f>
+        <f>AllEntries!AK4</f>
         <v>MIUB</v>
       </c>
       <c r="AN4" s="35" t="str">
-        <f>AllEntries!AK4</f>
+        <f>AllEntries!AL4</f>
         <v>BCCR</v>
       </c>
       <c r="AO4" s="35" t="str">
-        <f>AllEntries!AL4</f>
+        <f>AllEntries!AM4</f>
         <v>CRP-GL</v>
       </c>
       <c r="AP4" s="35" t="str">
-        <f>AllEntries!AM4</f>
+        <f>AllEntries!AN4</f>
         <v>IDL</v>
       </c>
       <c r="AQ4" s="35" t="str">
-        <f>AllEntries!AN4</f>
+        <f>AllEntries!AO4</f>
         <v>IPSL/INERIS</v>
       </c>
       <c r="AR4" s="35" t="str">
-        <f>AllEntries!AO4</f>
+        <f>AllEntries!AP4</f>
         <v>AUTH-Met</v>
       </c>
       <c r="AS4" s="35" t="str">
-        <f>AllEntries!AP4</f>
+        <f>AllEntries!AQ4</f>
         <v>AUTH-LHTEE</v>
       </c>
       <c r="AT4" s="35" t="str">
-        <f>AllEntries!AQ4</f>
+        <f>AllEntries!AR4</f>
         <v>NUIM</v>
       </c>
       <c r="AU4" s="35" t="str">
-        <f>AllEntries!AR4</f>
+        <f>AllEntries!AS4</f>
         <v>UHOH</v>
       </c>
       <c r="AV4" s="35" t="str">
-        <f>AllEntries!AS4</f>
+        <f>AllEntries!AT4</f>
         <v>UM</v>
       </c>
       <c r="AW4" s="35" t="e">
@@ -5995,14 +6004,14 @@
         <v>#REF!</v>
       </c>
       <c r="AX4" s="42" t="str">
-        <f>AllEntries!AT4</f>
-        <v>UCAN</v>
-      </c>
-      <c r="AY4" s="33" t="str">
         <f>AllEntries!AU4</f>
         <v>UCAN</v>
       </c>
-      <c r="AZ4" s="197" t="s">
+      <c r="AY4" s="33" t="str">
+        <f>AllEntries!AV4</f>
+        <v>UCAN</v>
+      </c>
+      <c r="AZ4" s="198" t="s">
         <v>16</v>
       </c>
       <c r="BA4" s="75" t="s">
@@ -6226,11 +6235,11 @@
         <v>0</v>
       </c>
       <c r="AF5" s="35">
-        <f>AllEntries!AD6</f>
+        <f>AllEntries!AE6</f>
         <v>0</v>
       </c>
       <c r="AG5" s="33">
-        <f>AllEntries!AE6</f>
+        <f>AllEntries!AF6</f>
         <v>0</v>
       </c>
       <c r="AH5" s="75" t="str">
@@ -6238,59 +6247,59 @@
         <v>URL, path etc. to data**</v>
       </c>
       <c r="AI5" s="33">
-        <f>AllEntries!AF6</f>
+        <f>AllEntries!AG6</f>
         <v>0</v>
       </c>
       <c r="AJ5" s="35">
-        <f>AllEntries!AG6</f>
+        <f>AllEntries!AH6</f>
         <v>0</v>
       </c>
       <c r="AK5" s="56">
-        <f>AllEntries!AH6</f>
+        <f>AllEntries!AI6</f>
         <v>0</v>
       </c>
       <c r="AL5" s="56">
-        <f>AllEntries!AI6</f>
+        <f>AllEntries!AJ6</f>
         <v>0</v>
       </c>
       <c r="AM5" s="35">
-        <f>AllEntries!AJ6</f>
+        <f>AllEntries!AK6</f>
         <v>0</v>
       </c>
       <c r="AN5" s="35">
-        <f>AllEntries!AK6</f>
+        <f>AllEntries!AL6</f>
         <v>0</v>
       </c>
       <c r="AO5" s="35">
-        <f>AllEntries!AL6</f>
+        <f>AllEntries!AM6</f>
         <v>0</v>
       </c>
       <c r="AP5" s="35">
-        <f>AllEntries!AM6</f>
+        <f>AllEntries!AN6</f>
         <v>0</v>
       </c>
       <c r="AQ5" s="35">
-        <f>AllEntries!AN6</f>
+        <f>AllEntries!AO6</f>
         <v>0</v>
       </c>
       <c r="AR5" s="35">
-        <f>AllEntries!AO6</f>
+        <f>AllEntries!AP6</f>
         <v>0</v>
       </c>
       <c r="AS5" s="35">
-        <f>AllEntries!AP6</f>
+        <f>AllEntries!AQ6</f>
         <v>0</v>
       </c>
       <c r="AT5" s="35">
-        <f>AllEntries!AQ6</f>
+        <f>AllEntries!AR6</f>
         <v>0</v>
       </c>
       <c r="AU5" s="35">
-        <f>AllEntries!AR6</f>
+        <f>AllEntries!AS6</f>
         <v>0</v>
       </c>
       <c r="AV5" s="35">
-        <f>AllEntries!AS6</f>
+        <f>AllEntries!AT6</f>
         <v>0</v>
       </c>
       <c r="AW5" s="35" t="e">
@@ -6298,14 +6307,14 @@
         <v>#REF!</v>
       </c>
       <c r="AX5" s="42">
-        <f>AllEntries!AT6</f>
+        <f>AllEntries!AU6</f>
         <v>0</v>
       </c>
       <c r="AY5" s="33">
-        <f>AllEntries!AU6</f>
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="198"/>
+        <f>AllEntries!AV6</f>
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="199"/>
       <c r="BA5" s="75"/>
       <c r="BB5" s="2"/>
       <c r="BC5" s="2"/>
@@ -6525,11 +6534,11 @@
         <v>RegCM4-2</v>
       </c>
       <c r="AF6" s="25" t="str">
-        <f>AllEntries!AD8</f>
+        <f>AllEntries!AE8</f>
         <v>RM3</v>
       </c>
       <c r="AG6" s="124" t="str">
-        <f>AllEntries!AE8</f>
+        <f>AllEntries!AF8</f>
         <v>CanRCM4</v>
       </c>
       <c r="AH6" s="76" t="str">
@@ -6537,59 +6546,59 @@
         <v xml:space="preserve">RCM name </v>
       </c>
       <c r="AI6" s="124" t="str">
-        <f>AllEntries!AF8</f>
+        <f>AllEntries!AG8</f>
         <v>CCAM</v>
       </c>
       <c r="AJ6" s="24" t="str">
-        <f>AllEntries!AG8</f>
+        <f>AllEntries!AH8</f>
         <v>GFDL</v>
       </c>
       <c r="AK6" s="57" t="str">
-        <f>AllEntries!AH8</f>
+        <f>AllEntries!AI8</f>
         <v>HadGEM3-RA</v>
       </c>
       <c r="AL6" s="57" t="str">
-        <f>AllEntries!AI8</f>
+        <f>AllEntries!AJ8</f>
         <v>HadRM3P</v>
       </c>
       <c r="AM6" s="38" t="str">
-        <f>AllEntries!AJ8</f>
+        <f>AllEntries!AK8</f>
         <v>WRF331A</v>
       </c>
       <c r="AN6" s="38" t="str">
-        <f>AllEntries!AK8</f>
+        <f>AllEntries!AL8</f>
         <v>WRF331C</v>
       </c>
       <c r="AO6" s="39" t="str">
-        <f>AllEntries!AL8</f>
+        <f>AllEntries!AM8</f>
         <v>WRF331A</v>
       </c>
       <c r="AP6" s="39" t="str">
-        <f>AllEntries!AM8</f>
+        <f>AllEntries!AN8</f>
         <v>WRF331D</v>
       </c>
       <c r="AQ6" s="39" t="str">
-        <f>AllEntries!AN8</f>
+        <f>AllEntries!AO8</f>
         <v>WRF331F</v>
       </c>
       <c r="AR6" s="25" t="str">
-        <f>AllEntries!AO8</f>
+        <f>AllEntries!AP8</f>
         <v>WRF331A</v>
       </c>
       <c r="AS6" s="24" t="str">
-        <f>AllEntries!AP8</f>
+        <f>AllEntries!AQ8</f>
         <v>WRF321B</v>
       </c>
       <c r="AT6" s="25" t="str">
-        <f>AllEntries!AQ8</f>
+        <f>AllEntries!AR8</f>
         <v>WRF341E</v>
       </c>
       <c r="AU6" s="25" t="str">
-        <f>AllEntries!AR8</f>
+        <f>AllEntries!AS8</f>
         <v>WRF331H</v>
       </c>
       <c r="AV6" s="25" t="str">
-        <f>AllEntries!AS8</f>
+        <f>AllEntries!AT8</f>
         <v>WRF331</v>
       </c>
       <c r="AW6" s="37" t="e">
@@ -6597,14 +6606,14 @@
         <v>#REF!</v>
       </c>
       <c r="AX6" s="43" t="str">
-        <f>AllEntries!AT8</f>
+        <f>AllEntries!AU8</f>
         <v>WRF331G</v>
       </c>
       <c r="AY6" s="84" t="str">
-        <f>AllEntries!AU8</f>
+        <f>AllEntries!AV8</f>
         <v>WRF350I</v>
       </c>
-      <c r="AZ6" s="199"/>
+      <c r="AZ6" s="200"/>
       <c r="BA6" s="76" t="s">
         <v>19</v>
       </c>
@@ -10200,25 +10209,25 @@
       <c r="EN27" s="26"/>
     </row>
     <row r="28" spans="1:144" s="26" customFormat="1" ht="37.200000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="200" t="s">
+      <c r="A28" s="201" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="200"/>
-      <c r="C28" s="200"/>
-      <c r="D28" s="200"/>
-      <c r="E28" s="200"/>
-      <c r="F28" s="200"/>
-      <c r="G28" s="200"/>
-      <c r="H28" s="200"/>
-      <c r="I28" s="200"/>
-      <c r="J28" s="200"/>
-      <c r="K28" s="200"/>
-      <c r="L28" s="200"/>
-      <c r="M28" s="200"/>
-      <c r="N28" s="200"/>
-      <c r="O28" s="200"/>
-      <c r="P28" s="200"/>
-      <c r="Q28" s="200"/>
+      <c r="B28" s="201"/>
+      <c r="C28" s="201"/>
+      <c r="D28" s="201"/>
+      <c r="E28" s="201"/>
+      <c r="F28" s="201"/>
+      <c r="G28" s="201"/>
+      <c r="H28" s="201"/>
+      <c r="I28" s="201"/>
+      <c r="J28" s="201"/>
+      <c r="K28" s="201"/>
+      <c r="L28" s="201"/>
+      <c r="M28" s="201"/>
+      <c r="N28" s="201"/>
+      <c r="O28" s="201"/>
+      <c r="P28" s="201"/>
+      <c r="Q28" s="201"/>
       <c r="R28" s="40"/>
       <c r="S28" s="40"/>
       <c r="T28" s="40"/>
@@ -10254,69 +10263,69 @@
       <c r="AX28" s="30"/>
     </row>
     <row r="29" spans="1:144" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="201" t="s">
+      <c r="A29" s="202" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="201"/>
-      <c r="C29" s="201"/>
-      <c r="D29" s="201"/>
-      <c r="E29" s="201"/>
-      <c r="F29" s="201"/>
-      <c r="G29" s="201"/>
-      <c r="H29" s="201"/>
-      <c r="I29" s="201"/>
-      <c r="J29" s="201"/>
-      <c r="K29" s="201"/>
-      <c r="L29" s="201"/>
-      <c r="M29" s="201"/>
-      <c r="N29" s="201"/>
-      <c r="O29" s="201"/>
-      <c r="P29" s="201"/>
-      <c r="Q29" s="201"/>
-      <c r="R29" s="201"/>
-      <c r="S29" s="201"/>
-      <c r="T29" s="201"/>
-      <c r="U29" s="201"/>
-      <c r="V29" s="201"/>
-      <c r="W29" s="201"/>
-      <c r="X29" s="201"/>
-      <c r="Y29" s="201"/>
-      <c r="Z29" s="201"/>
-      <c r="AA29" s="201"/>
-      <c r="AB29" s="201"/>
-      <c r="AC29" s="201"/>
-      <c r="AD29" s="201"/>
-      <c r="AE29" s="201"/>
-      <c r="AF29" s="201"/>
-      <c r="AG29" s="201"/>
-      <c r="AH29" s="201"/>
-      <c r="AI29" s="201"/>
-      <c r="AJ29" s="201"/>
-      <c r="AK29" s="201"/>
-      <c r="AL29" s="201"/>
-      <c r="AM29" s="201"/>
-      <c r="AN29" s="201"/>
-      <c r="AO29" s="201"/>
-      <c r="AP29" s="201"/>
-      <c r="AQ29" s="201"/>
-      <c r="AR29" s="201"/>
-      <c r="AS29" s="201"/>
-      <c r="AT29" s="201"/>
-      <c r="AU29" s="201"/>
-      <c r="AV29" s="201"/>
-      <c r="AW29" s="201"/>
-      <c r="AX29" s="201"/>
+      <c r="B29" s="202"/>
+      <c r="C29" s="202"/>
+      <c r="D29" s="202"/>
+      <c r="E29" s="202"/>
+      <c r="F29" s="202"/>
+      <c r="G29" s="202"/>
+      <c r="H29" s="202"/>
+      <c r="I29" s="202"/>
+      <c r="J29" s="202"/>
+      <c r="K29" s="202"/>
+      <c r="L29" s="202"/>
+      <c r="M29" s="202"/>
+      <c r="N29" s="202"/>
+      <c r="O29" s="202"/>
+      <c r="P29" s="202"/>
+      <c r="Q29" s="202"/>
+      <c r="R29" s="202"/>
+      <c r="S29" s="202"/>
+      <c r="T29" s="202"/>
+      <c r="U29" s="202"/>
+      <c r="V29" s="202"/>
+      <c r="W29" s="202"/>
+      <c r="X29" s="202"/>
+      <c r="Y29" s="202"/>
+      <c r="Z29" s="202"/>
+      <c r="AA29" s="202"/>
+      <c r="AB29" s="202"/>
+      <c r="AC29" s="202"/>
+      <c r="AD29" s="202"/>
+      <c r="AE29" s="202"/>
+      <c r="AF29" s="202"/>
+      <c r="AG29" s="202"/>
+      <c r="AH29" s="202"/>
+      <c r="AI29" s="202"/>
+      <c r="AJ29" s="202"/>
+      <c r="AK29" s="202"/>
+      <c r="AL29" s="202"/>
+      <c r="AM29" s="202"/>
+      <c r="AN29" s="202"/>
+      <c r="AO29" s="202"/>
+      <c r="AP29" s="202"/>
+      <c r="AQ29" s="202"/>
+      <c r="AR29" s="202"/>
+      <c r="AS29" s="202"/>
+      <c r="AT29" s="202"/>
+      <c r="AU29" s="202"/>
+      <c r="AV29" s="202"/>
+      <c r="AW29" s="202"/>
+      <c r="AX29" s="202"/>
     </row>
     <row r="30" spans="1:144" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="202" t="s">
+      <c r="A30" s="203" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="202"/>
-      <c r="C30" s="202"/>
-      <c r="D30" s="202"/>
-      <c r="E30" s="202"/>
-      <c r="F30" s="201"/>
-      <c r="G30" s="201"/>
+      <c r="B30" s="203"/>
+      <c r="C30" s="203"/>
+      <c r="D30" s="203"/>
+      <c r="E30" s="203"/>
+      <c r="F30" s="202"/>
+      <c r="G30" s="202"/>
       <c r="H30" s="19"/>
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
@@ -10358,10 +10367,10 @@
       <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="203" t="s">
+      <c r="D31" s="204" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="204"/>
+      <c r="E31" s="205"/>
       <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:144" x14ac:dyDescent="0.3">
@@ -10376,11 +10385,11 @@
         <f>C33*98*63/194/201</f>
         <v>460.27127250346206</v>
       </c>
-      <c r="D32" s="205">
+      <c r="D32" s="206">
         <f t="shared" ref="D32:D37" si="33">(B32+C32)/1</f>
         <v>476.23114325280812</v>
       </c>
-      <c r="E32" s="206"/>
+      <c r="E32" s="207"/>
       <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.3">
@@ -10394,11 +10403,11 @@
       <c r="C33" s="10">
         <v>2907</v>
       </c>
-      <c r="D33" s="207">
+      <c r="D33" s="208">
         <f t="shared" si="33"/>
         <v>3007.8</v>
       </c>
-      <c r="E33" s="208"/>
+      <c r="E33" s="209"/>
       <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:49" x14ac:dyDescent="0.3">
@@ -10413,11 +10422,11 @@
         <f>4*AFR44tier1</f>
         <v>11628</v>
       </c>
-      <c r="D34" s="207">
+      <c r="D34" s="208">
         <f t="shared" si="33"/>
         <v>12031.2</v>
       </c>
-      <c r="E34" s="208"/>
+      <c r="E34" s="209"/>
       <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:49" x14ac:dyDescent="0.3">
@@ -10431,11 +10440,11 @@
       <c r="C35" s="98">
         <v>13005</v>
       </c>
-      <c r="D35" s="207">
+      <c r="D35" s="208">
         <f t="shared" si="33"/>
         <v>13475.4</v>
       </c>
-      <c r="E35" s="208"/>
+      <c r="E35" s="209"/>
       <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:49" x14ac:dyDescent="0.3">
@@ -10450,11 +10459,11 @@
         <f>C33*125*97/194/201</f>
         <v>903.91791044776119</v>
       </c>
-      <c r="D36" s="207">
+      <c r="D36" s="208">
         <f t="shared" si="33"/>
         <v>932.02992768118168</v>
       </c>
-      <c r="E36" s="208"/>
+      <c r="E36" s="209"/>
       <c r="F36" s="26"/>
     </row>
     <row r="37" spans="1:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10469,34 +10478,34 @@
         <f>C33*116*133/194/201</f>
         <v>1150.1563317433452</v>
       </c>
-      <c r="D37" s="209">
+      <c r="D37" s="210">
         <f t="shared" si="33"/>
         <v>1190.0379135251578</v>
       </c>
-      <c r="E37" s="210"/>
+      <c r="E37" s="211"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A38" s="195" t="s">
+      <c r="A38" s="196" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="195"/>
-      <c r="C38" s="195"/>
-      <c r="D38" s="195"/>
-      <c r="E38" s="195"/>
-      <c r="F38" s="196"/>
-      <c r="G38" s="196"/>
+      <c r="B38" s="196"/>
+      <c r="C38" s="196"/>
+      <c r="D38" s="196"/>
+      <c r="E38" s="196"/>
+      <c r="F38" s="197"/>
+      <c r="G38" s="197"/>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A39" s="196" t="s">
+      <c r="A39" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="196"/>
-      <c r="C39" s="196"/>
-      <c r="D39" s="196"/>
-      <c r="E39" s="196"/>
-      <c r="F39" s="196"/>
-      <c r="G39" s="196"/>
+      <c r="B39" s="197"/>
+      <c r="C39" s="197"/>
+      <c r="D39" s="197"/>
+      <c r="E39" s="197"/>
+      <c r="F39" s="197"/>
+      <c r="G39" s="197"/>
       <c r="H39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
@@ -10559,10 +10568,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW18"/>
+  <dimension ref="A1:BX18"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AH3" sqref="AH3:AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10594,49 +10603,49 @@
     <col min="26" max="26" width="17.6640625" customWidth="1"/>
     <col min="27" max="28" width="18.88671875" customWidth="1"/>
     <col min="29" max="29" width="18.33203125" customWidth="1"/>
-    <col min="30" max="30" width="18.44140625" customWidth="1"/>
-    <col min="31" max="31" width="12.88671875" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="19.5546875" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="15.109375" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="15.21875" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="22.44140625" customWidth="1"/>
-    <col min="36" max="36" width="23" customWidth="1"/>
-    <col min="37" max="37" width="19.44140625" customWidth="1"/>
-    <col min="38" max="38" width="22.21875" customWidth="1"/>
-    <col min="39" max="39" width="20.109375" customWidth="1"/>
-    <col min="40" max="40" width="22.109375" customWidth="1"/>
-    <col min="41" max="41" width="21" customWidth="1"/>
-    <col min="42" max="42" width="16.88671875" customWidth="1"/>
-    <col min="43" max="43" width="18.44140625" customWidth="1"/>
-    <col min="44" max="44" width="17.44140625" customWidth="1"/>
-    <col min="45" max="45" width="23" customWidth="1"/>
-    <col min="46" max="46" width="21.44140625" customWidth="1"/>
-    <col min="47" max="48" width="19.44140625" customWidth="1"/>
-    <col min="70" max="75" width="8.88671875" style="26"/>
+    <col min="30" max="31" width="18.44140625" customWidth="1"/>
+    <col min="32" max="32" width="12.88671875" customWidth="1"/>
+    <col min="33" max="33" width="19.5546875" customWidth="1"/>
+    <col min="34" max="34" width="15.109375" customWidth="1"/>
+    <col min="35" max="35" width="15.21875" customWidth="1"/>
+    <col min="36" max="36" width="22.44140625" customWidth="1"/>
+    <col min="37" max="37" width="23" customWidth="1"/>
+    <col min="38" max="38" width="19.44140625" customWidth="1"/>
+    <col min="39" max="39" width="22.21875" customWidth="1"/>
+    <col min="40" max="40" width="20.109375" customWidth="1"/>
+    <col min="41" max="41" width="22.109375" customWidth="1"/>
+    <col min="42" max="42" width="21" customWidth="1"/>
+    <col min="43" max="43" width="16.88671875" customWidth="1"/>
+    <col min="44" max="44" width="18.44140625" customWidth="1"/>
+    <col min="45" max="45" width="17.44140625" customWidth="1"/>
+    <col min="46" max="46" width="23" customWidth="1"/>
+    <col min="47" max="47" width="21.44140625" customWidth="1"/>
+    <col min="48" max="49" width="19.44140625" customWidth="1"/>
+    <col min="71" max="76" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="211" t="s">
+    <row r="1" spans="1:76" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="212" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="211"/>
-      <c r="C1" s="211"/>
-      <c r="D1" s="211"/>
-      <c r="E1" s="211"/>
-      <c r="F1" s="211"/>
-      <c r="G1" s="211"/>
-      <c r="H1" s="211"/>
-      <c r="I1" s="211"/>
-      <c r="J1" s="211"/>
-      <c r="K1" s="211"/>
-      <c r="L1" s="211"/>
-      <c r="M1" s="211"/>
-      <c r="N1" s="211"/>
-      <c r="O1" s="211"/>
-      <c r="P1" s="211"/>
-      <c r="Q1" s="211"/>
-      <c r="R1" s="211"/>
-      <c r="S1" s="211"/>
+      <c r="B1" s="212"/>
+      <c r="C1" s="212"/>
+      <c r="D1" s="212"/>
+      <c r="E1" s="212"/>
+      <c r="F1" s="212"/>
+      <c r="G1" s="212"/>
+      <c r="H1" s="212"/>
+      <c r="I1" s="212"/>
+      <c r="J1" s="212"/>
+      <c r="K1" s="212"/>
+      <c r="L1" s="212"/>
+      <c r="M1" s="212"/>
+      <c r="N1" s="212"/>
+      <c r="O1" s="212"/>
+      <c r="P1" s="212"/>
+      <c r="Q1" s="212"/>
+      <c r="R1" s="212"/>
+      <c r="S1" s="212"/>
       <c r="T1" s="104"/>
       <c r="U1" s="64"/>
       <c r="V1" s="20"/>
@@ -10654,36 +10663,37 @@
       <c r="AH1" s="20"/>
       <c r="AI1" s="20"/>
       <c r="AJ1" s="20"/>
-      <c r="AK1" s="26"/>
-      <c r="AM1" s="20"/>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="26"/>
       <c r="AN1" s="20"/>
       <c r="AO1" s="20"/>
       <c r="AP1" s="20"/>
       <c r="AQ1" s="20"/>
       <c r="AR1" s="20"/>
       <c r="AS1" s="20"/>
-      <c r="AU1" s="26"/>
+      <c r="AT1" s="20"/>
       <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
     </row>
-    <row r="2" spans="1:75" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:76" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="54">
         <f>GeneralRemarks!A2</f>
-        <v>41731</v>
-      </c>
-      <c r="B2" s="212"/>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
+        <v>41901</v>
+      </c>
+      <c r="B2" s="213"/>
+      <c r="C2" s="213"/>
+      <c r="D2" s="213"/>
       <c r="E2" s="138"/>
       <c r="F2" s="138"/>
       <c r="G2" s="138"/>
       <c r="H2" s="138"/>
       <c r="I2" s="138"/>
-      <c r="J2" s="212"/>
-      <c r="K2" s="212"/>
-      <c r="L2" s="212"/>
-      <c r="M2" s="212"/>
-      <c r="N2" s="212"/>
-      <c r="O2" s="212"/>
+      <c r="J2" s="213"/>
+      <c r="K2" s="213"/>
+      <c r="L2" s="213"/>
+      <c r="M2" s="213"/>
+      <c r="N2" s="213"/>
+      <c r="O2" s="213"/>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
       <c r="R2" s="20"/>
@@ -10705,21 +10715,22 @@
       <c r="AH2" s="20"/>
       <c r="AI2" s="20"/>
       <c r="AJ2" s="20"/>
-      <c r="AK2" s="26"/>
-      <c r="AM2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="26"/>
       <c r="AN2" s="20"/>
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
       <c r="AQ2" s="20"/>
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
-      <c r="AU2" s="52">
+      <c r="AT2" s="20"/>
+      <c r="AV2" s="52">
         <f>A2</f>
-        <v>41731</v>
-      </c>
-      <c r="AV2" s="26"/>
+        <v>41901</v>
+      </c>
+      <c r="AW2" s="26"/>
     </row>
-    <row r="3" spans="1:75" s="1" customFormat="1" ht="32.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:76" s="1" customFormat="1" ht="32.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="79" t="s">
         <v>88</v>
       </c>
@@ -10836,25 +10847,25 @@
         <f>AllEntries!AC7</f>
         <v>DHMZ</v>
       </c>
-      <c r="AE3" s="139" t="str">
+      <c r="AE3" s="80" t="str">
         <f>AllEntries!AD7</f>
-        <v>GISS</v>
+        <v>IITM</v>
       </c>
       <c r="AF3" s="139" t="str">
         <f>AllEntries!AE7</f>
-        <v>CCCma</v>
+        <v>GISS</v>
       </c>
       <c r="AG3" s="139" t="str">
         <f>AllEntries!AF7</f>
-        <v>CSIR</v>
-      </c>
-      <c r="AH3" s="139" t="str">
+        <v>CCCma</v>
+      </c>
+      <c r="AH3" s="80" t="str">
         <f>AllEntries!AG7</f>
+        <v>CSIRO</v>
+      </c>
+      <c r="AI3" s="139" t="str">
+        <f>AllEntries!AH7</f>
         <v>KAUST</v>
-      </c>
-      <c r="AI3" s="80" t="str">
-        <f>AllEntries!AH7</f>
-        <v>MOHC</v>
       </c>
       <c r="AJ3" s="80" t="str">
         <f>AllEntries!AI7</f>
@@ -10862,54 +10873,57 @@
       </c>
       <c r="AK3" s="80" t="str">
         <f>AllEntries!AJ7</f>
+        <v>MOHC</v>
+      </c>
+      <c r="AL3" s="80" t="str">
+        <f>AllEntries!AK7</f>
         <v>MIUB</v>
       </c>
-      <c r="AL3" s="125" t="str">
-        <f>AllEntries!AK7</f>
+      <c r="AM3" s="125" t="str">
+        <f>AllEntries!AL7</f>
         <v>BCCR</v>
-      </c>
-      <c r="AM3" s="80" t="str">
-        <f>AllEntries!AL7</f>
-        <v>CRP-GL</v>
       </c>
       <c r="AN3" s="80" t="str">
         <f>AllEntries!AM7</f>
-        <v>IDL</v>
+        <v>CRP-GL</v>
       </c>
       <c r="AO3" s="80" t="str">
         <f>AllEntries!AN7</f>
-        <v>IPSL-INERIS</v>
+        <v>IDL</v>
       </c>
       <c r="AP3" s="80" t="str">
         <f>AllEntries!AO7</f>
-        <v>AUTH-Met</v>
+        <v>IPSL-INERIS</v>
       </c>
       <c r="AQ3" s="80" t="str">
         <f>AllEntries!AP7</f>
-        <v>AUTH-LHTEE</v>
+        <v>AUTH-Met</v>
       </c>
       <c r="AR3" s="80" t="str">
         <f>AllEntries!AQ7</f>
-        <v>NUIM</v>
+        <v>AUTH-LHTEE</v>
       </c>
       <c r="AS3" s="80" t="str">
         <f>AllEntries!AR7</f>
-        <v>UHOH</v>
+        <v>NUIM</v>
       </c>
       <c r="AT3" s="80" t="str">
         <f>AllEntries!AS7</f>
-        <v>UM</v>
+        <v>UHOH</v>
       </c>
       <c r="AU3" s="80" t="str">
         <f>AllEntries!AT7</f>
-        <v>UCAN</v>
-      </c>
-      <c r="AV3" s="162" t="str">
+        <v>UM</v>
+      </c>
+      <c r="AV3" s="80" t="str">
         <f>AllEntries!AU7</f>
         <v>UCAN</v>
       </c>
-      <c r="AW3" s="198"/>
-      <c r="AX3" s="2"/>
+      <c r="AW3" s="162" t="str">
+        <f>AllEntries!AV7</f>
+        <v>UCAN</v>
+      </c>
+      <c r="AX3" s="199"/>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
@@ -10935,10 +10949,11 @@
       <c r="BU3" s="2"/>
       <c r="BV3" s="2"/>
       <c r="BW3" s="2"/>
+      <c r="BX3" s="2"/>
     </row>
-    <row r="4" spans="1:75" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:76" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="149" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!B9),"",AllEntries!B9)</f>
@@ -11058,23 +11073,23 @@
       </c>
       <c r="AE4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AD9),"",AllEntries!AD9)</f>
-        <v/>
+        <v>Indian Institute of Tropical Meteorology</v>
       </c>
       <c r="AF4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AE9),"",AllEntries!AE9)</f>
-        <v>CCCma (Canadian Centre for Climate Modelling and Analysis, Victoria, BC, Canada)</v>
+        <v/>
       </c>
       <c r="AG4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AF9),"",AllEntries!AF9)</f>
-        <v/>
+        <v>CCCma (Canadian Centre for Climate Modelling and Analysis, Victoria, BC, Canada)</v>
       </c>
       <c r="AH4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AG9),"",AllEntries!AG9)</f>
-        <v/>
+        <v>Commonwealth Scientific and Industrial Research Organisation</v>
       </c>
       <c r="AI4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AH9),"",AllEntries!AH9)</f>
-        <v>Met Office Hadley Centre</v>
+        <v/>
       </c>
       <c r="AJ4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AI9),"",AllEntries!AI9)</f>
@@ -11082,15 +11097,15 @@
       </c>
       <c r="AK4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AJ9),"",AllEntries!AJ9)</f>
-        <v/>
+        <v>Met Office Hadley Centre</v>
       </c>
       <c r="AL4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AK9),"",AllEntries!AK9)</f>
-        <v>Bjerknes Centre for Climate Research</v>
+        <v/>
       </c>
       <c r="AM4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AL9),"",AllEntries!AL9)</f>
-        <v/>
+        <v>Bjerknes Centre for Climate Research</v>
       </c>
       <c r="AN4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AM9),"",AllEntries!AM9)</f>
@@ -11114,7 +11129,7 @@
       </c>
       <c r="AS4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AR9),"",AllEntries!AR9)</f>
-        <v/>
+        <v>National University of Ireland Maynooth</v>
       </c>
       <c r="AT4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AS9),"",AllEntries!AS9)</f>
@@ -11124,12 +11139,15 @@
         <f>IF(ISBLANK(AllEntries!AT9),"",AllEntries!AT9)</f>
         <v/>
       </c>
-      <c r="AV4" s="163" t="str">
+      <c r="AV4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AU9),"",AllEntries!AU9)</f>
         <v/>
       </c>
-      <c r="AW4" s="198"/>
-      <c r="AX4" s="2"/>
+      <c r="AW4" s="163" t="str">
+        <f>IF(ISBLANK(AllEntries!AV9),"",AllEntries!AV9)</f>
+        <v/>
+      </c>
+      <c r="AX4" s="199"/>
       <c r="AY4" s="2"/>
       <c r="AZ4" s="2"/>
       <c r="BA4" s="2"/>
@@ -11155,8 +11173,9 @@
       <c r="BU4" s="2"/>
       <c r="BV4" s="2"/>
       <c r="BW4" s="2"/>
+      <c r="BX4" s="2"/>
     </row>
-    <row r="5" spans="1:75" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:76" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="155" t="s">
         <v>86</v>
       </c>
@@ -11273,80 +11292,83 @@
         <f>AllEntries!AC8</f>
         <v>RegCM4-2</v>
       </c>
-      <c r="AE5" s="140" t="str">
+      <c r="AE5" s="65" t="str">
         <f>AllEntries!AD8</f>
-        <v>RM3</v>
+        <v>RegCM4-1</v>
       </c>
       <c r="AF5" s="140" t="str">
         <f>AllEntries!AE8</f>
-        <v>CanRCM4</v>
+        <v>RM3</v>
       </c>
       <c r="AG5" s="140" t="str">
         <f>AllEntries!AF8</f>
+        <v>CanRCM4</v>
+      </c>
+      <c r="AH5" s="65" t="str">
+        <f>AllEntries!AG8</f>
         <v>CCAM</v>
       </c>
-      <c r="AH5" s="140" t="str">
-        <f>AllEntries!AG8</f>
+      <c r="AI5" s="140" t="str">
+        <f>AllEntries!AH8</f>
         <v>GFDL</v>
-      </c>
-      <c r="AI5" s="65" t="str">
-        <f>AllEntries!AH8</f>
-        <v>HadGEM3-RA</v>
       </c>
       <c r="AJ5" s="65" t="str">
         <f>AllEntries!AI8</f>
-        <v>HadRM3P</v>
+        <v>HadGEM3-RA</v>
       </c>
       <c r="AK5" s="65" t="str">
         <f>AllEntries!AJ8</f>
+        <v>HadRM3P</v>
+      </c>
+      <c r="AL5" s="65" t="str">
+        <f>AllEntries!AK8</f>
         <v>WRF331A</v>
       </c>
-      <c r="AL5" s="126" t="str">
-        <f>AllEntries!AK8</f>
+      <c r="AM5" s="126" t="str">
+        <f>AllEntries!AL8</f>
         <v>WRF331C</v>
-      </c>
-      <c r="AM5" s="65" t="str">
-        <f>AllEntries!AL8</f>
-        <v>WRF331A</v>
       </c>
       <c r="AN5" s="65" t="str">
         <f>AllEntries!AM8</f>
-        <v>WRF331D</v>
+        <v>WRF331A</v>
       </c>
       <c r="AO5" s="65" t="str">
         <f>AllEntries!AN8</f>
-        <v>WRF331F</v>
+        <v>WRF331D</v>
       </c>
       <c r="AP5" s="65" t="str">
         <f>AllEntries!AO8</f>
-        <v>WRF331A</v>
+        <v>WRF331F</v>
       </c>
       <c r="AQ5" s="65" t="str">
         <f>AllEntries!AP8</f>
-        <v>WRF321B</v>
+        <v>WRF331A</v>
       </c>
       <c r="AR5" s="65" t="str">
         <f>AllEntries!AQ8</f>
-        <v>WRF341E</v>
+        <v>WRF321B</v>
       </c>
       <c r="AS5" s="65" t="str">
         <f>AllEntries!AR8</f>
-        <v>WRF331H</v>
+        <v>WRF341E</v>
       </c>
       <c r="AT5" s="65" t="str">
         <f>AllEntries!AS8</f>
-        <v>WRF331</v>
+        <v>WRF331H</v>
       </c>
       <c r="AU5" s="65" t="str">
         <f>AllEntries!AT8</f>
+        <v>WRF331</v>
+      </c>
+      <c r="AV5" s="65" t="str">
+        <f>AllEntries!AU8</f>
         <v>WRF331G</v>
       </c>
-      <c r="AV5" s="164" t="str">
-        <f>AllEntries!AU8</f>
+      <c r="AW5" s="164" t="str">
+        <f>AllEntries!AV8</f>
         <v>WRF350I</v>
       </c>
-      <c r="AW5" s="198"/>
-      <c r="AX5" s="2"/>
+      <c r="AX5" s="199"/>
       <c r="AY5" s="2"/>
       <c r="AZ5" s="2"/>
       <c r="BA5" s="2"/>
@@ -11372,8 +11394,9 @@
       <c r="BU5" s="2"/>
       <c r="BV5" s="2"/>
       <c r="BW5" s="2"/>
+      <c r="BX5" s="2"/>
     </row>
-    <row r="6" spans="1:75" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:76" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="76" t="s">
         <v>87</v>
       </c>
@@ -11490,83 +11513,86 @@
         <v>CUNI-RegCM4-2</v>
       </c>
       <c r="AD6" s="65" t="str">
-        <f t="shared" ref="AD6" si="26">IF(ISBLANK(AD9),"",CONCATENATE(AD3,"-",AD5))</f>
+        <f t="shared" ref="AD6:AF6" si="26">IF(ISBLANK(AD9),"",CONCATENATE(AD3,"-",AD5))</f>
         <v>DHMZ-RegCM4-2</v>
       </c>
-      <c r="AE6" s="140" t="str">
+      <c r="AE6" s="65" t="str">
         <f t="shared" ref="AE6" si="27">IF(ISBLANK(AE9),"",CONCATENATE(AE3,"-",AE5))</f>
+        <v>IITM-RegCM4-1</v>
+      </c>
+      <c r="AF6" s="140" t="str">
+        <f>IF(ISBLANK(AF9),"",CONCATENATE(AF3,"-",AF5))</f>
         <v/>
       </c>
-      <c r="AF6" s="140" t="str">
-        <f t="shared" ref="AF6" si="28">IF(ISBLANK(AF9),"",CONCATENATE(AF3,"-",AF5))</f>
+      <c r="AG6" s="140" t="str">
+        <f>IF(ISBLANK(AG9),"",CONCATENATE(AG3,"-",AG5))</f>
         <v/>
       </c>
-      <c r="AG6" s="140" t="str">
-        <f t="shared" ref="AG6" si="29">IF(ISBLANK(AG9),"",CONCATENATE(AG3,"-",AG5))</f>
+      <c r="AH6" s="65" t="str">
+        <f>IF(ISBLANK(AH9),"",CONCATENATE(AH3,"-",AH5))</f>
+        <v>CSIRO-CCAM</v>
+      </c>
+      <c r="AI6" s="140" t="str">
+        <f>IF(ISBLANK(AI9),"",CONCATENATE(AI3,"-",AI5))</f>
         <v/>
       </c>
-      <c r="AH6" s="140" t="str">
-        <f t="shared" ref="AH6" si="30">IF(ISBLANK(AH9),"",CONCATENATE(AH3,"-",AH5))</f>
-        <v/>
-      </c>
-      <c r="AI6" s="65" t="str">
-        <f t="shared" ref="AI6" si="31">IF(ISBLANK(AI9),"",CONCATENATE(AI3,"-",AI5))</f>
+      <c r="AJ6" s="65" t="str">
+        <f>IF(ISBLANK(AJ9),"",CONCATENATE(AJ3,"-",AJ5))</f>
         <v>MOHC-HadGEM3-RA</v>
       </c>
-      <c r="AJ6" s="65" t="str">
-        <f t="shared" ref="AJ6" si="32">IF(ISBLANK(AJ9),"",CONCATENATE(AJ3,"-",AJ5))</f>
+      <c r="AK6" s="65" t="str">
+        <f>IF(ISBLANK(AK9),"",CONCATENATE(AK3,"-",AK5))</f>
         <v>MOHC-HadRM3P</v>
       </c>
-      <c r="AK6" s="65" t="str">
-        <f t="shared" ref="AK6" si="33">IF(ISBLANK(AK9),"",CONCATENATE(AK3,"-",AK5))</f>
+      <c r="AL6" s="65" t="str">
+        <f>IF(ISBLANK(AL9),"",CONCATENATE(AL3,"-",AL5))</f>
         <v>MIUB-WRF331A</v>
       </c>
-      <c r="AL6" s="65" t="str">
-        <f t="shared" ref="AL6" si="34">IF(ISBLANK(AL9),"",CONCATENATE(AL3,"-",AL5))</f>
+      <c r="AM6" s="65" t="str">
+        <f>IF(ISBLANK(AM9),"",CONCATENATE(AM3,"-",AM5))</f>
         <v>BCCR-WRF331C</v>
       </c>
-      <c r="AM6" s="65" t="str">
-        <f t="shared" ref="AM6:AN6" si="35">IF(ISBLANK(AM9),"",CONCATENATE(AM3,"-",AM5))</f>
+      <c r="AN6" s="65" t="str">
+        <f>IF(ISBLANK(AN9),"",CONCATENATE(AN3,"-",AN5))</f>
         <v>CRP-GL-WRF331A</v>
-      </c>
-      <c r="AN6" s="65" t="str">
-        <f t="shared" si="35"/>
-        <v>IDL-WRF331D</v>
       </c>
       <c r="AO6" s="65" t="str">
         <f>IF(ISBLANK(AO9),"",CONCATENATE(AO3,"-",AO5))</f>
+        <v>IDL-WRF331D</v>
+      </c>
+      <c r="AP6" s="65" t="str">
+        <f>IF(ISBLANK(AP9),"",CONCATENATE(AP3,"-",AP5))</f>
         <v>IPSL-INERIS-WRF331F</v>
       </c>
-      <c r="AP6" s="65" t="str">
-        <f t="shared" ref="AP6:AQ6" si="36">IF(ISBLANK(AP9),"",CONCATENATE(AP3,"-",AP5))</f>
+      <c r="AQ6" s="65" t="str">
+        <f>IF(ISBLANK(AQ9),"",CONCATENATE(AQ3,"-",AQ5))</f>
         <v>AUTH-Met-WRF331A</v>
       </c>
-      <c r="AQ6" s="65" t="str">
-        <f t="shared" si="36"/>
+      <c r="AR6" s="65" t="str">
+        <f>IF(ISBLANK(AR9),"",CONCATENATE(AR3,"-",AR5))</f>
         <v>AUTH-LHTEE-WRF321B</v>
       </c>
-      <c r="AR6" s="65" t="str">
-        <f t="shared" ref="AR6" si="37">IF(ISBLANK(AR9),"",CONCATENATE(AR3,"-",AR5))</f>
+      <c r="AS6" s="65" t="str">
+        <f>IF(ISBLANK(AS9),"",CONCATENATE(AS3,"-",AS5))</f>
         <v>NUIM-WRF341E</v>
       </c>
-      <c r="AS6" s="65" t="str">
-        <f t="shared" ref="AS6" si="38">IF(ISBLANK(AS9),"",CONCATENATE(AS3,"-",AS5))</f>
+      <c r="AT6" s="65" t="str">
+        <f>IF(ISBLANK(AT9),"",CONCATENATE(AT3,"-",AT5))</f>
         <v>UHOH-WRF331H</v>
       </c>
-      <c r="AT6" s="65" t="str">
-        <f t="shared" ref="AT6" si="39">IF(ISBLANK(AT9),"",CONCATENATE(AT3,"-",AT5))</f>
+      <c r="AU6" s="65" t="str">
+        <f>IF(ISBLANK(AU9),"",CONCATENATE(AU3,"-",AU5))</f>
         <v>UM-WRF331</v>
       </c>
-      <c r="AU6" s="65" t="str">
-        <f t="shared" ref="AU6" si="40">IF(ISBLANK(AU9),"",CONCATENATE(AU3,"-",AU5))</f>
+      <c r="AV6" s="65" t="str">
+        <f>IF(ISBLANK(AV9),"",CONCATENATE(AV3,"-",AV5))</f>
         <v>UCAN-WRF331G</v>
       </c>
-      <c r="AV6" s="164" t="str">
-        <f t="shared" ref="AV6" si="41">IF(ISBLANK(AV9),"",CONCATENATE(AV3,"-",AV5))</f>
+      <c r="AW6" s="164" t="str">
+        <f>IF(ISBLANK(AW9),"",CONCATENATE(AW3,"-",AW5))</f>
         <v>UCAN-WRF350I</v>
       </c>
-      <c r="AW6" s="105"/>
-      <c r="AX6" s="2"/>
+      <c r="AX6" s="105"/>
       <c r="AY6" s="2"/>
       <c r="AZ6" s="2"/>
       <c r="BA6" s="2"/>
@@ -11592,8 +11618,9 @@
       <c r="BU6" s="2"/>
       <c r="BV6" s="2"/>
       <c r="BW6" s="2"/>
+      <c r="BX6" s="2"/>
     </row>
-    <row r="7" spans="1:75" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:76" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="153" t="s">
         <v>151</v>
       </c>
@@ -11712,15 +11739,15 @@
       </c>
       <c r="AE7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AD11),"unknown",AllEntries!AD11)</f>
-        <v>unknown</v>
+        <v>non-commercial only</v>
       </c>
       <c r="AF7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AE11),"unknown",AllEntries!AE11)</f>
-        <v>unrestricted</v>
+        <v>unknown</v>
       </c>
       <c r="AG7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AF11),"unknown",AllEntries!AF11)</f>
-        <v>unknown</v>
+        <v>unrestricted</v>
       </c>
       <c r="AH7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AG11),"unknown",AllEntries!AG11)</f>
@@ -11728,7 +11755,7 @@
       </c>
       <c r="AI7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AH11),"unknown",AllEntries!AH11)</f>
-        <v>unrestricted</v>
+        <v>unknown</v>
       </c>
       <c r="AJ7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AI11),"unknown",AllEntries!AI11)</f>
@@ -11736,11 +11763,11 @@
       </c>
       <c r="AK7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AJ11),"unknown",AllEntries!AJ11)</f>
-        <v>unknown</v>
+        <v>unrestricted</v>
       </c>
       <c r="AL7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AK11),"unknown",AllEntries!AK11)</f>
-        <v>unrestricted</v>
+        <v>unknown</v>
       </c>
       <c r="AM7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AL11),"unknown",AllEntries!AL11)</f>
@@ -11748,7 +11775,7 @@
       </c>
       <c r="AN7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AM11),"unknown",AllEntries!AM11)</f>
-        <v>unknown</v>
+        <v>unrestricted</v>
       </c>
       <c r="AO7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AN11),"unknown",AllEntries!AN11)</f>
@@ -11768,7 +11795,7 @@
       </c>
       <c r="AS7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AR11),"unknown",AllEntries!AR11)</f>
-        <v>unknown</v>
+        <v>non-commercial only</v>
       </c>
       <c r="AT7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AS11),"unknown",AllEntries!AS11)</f>
@@ -11776,14 +11803,17 @@
       </c>
       <c r="AU7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AT11),"unknown",AllEntries!AT11)</f>
+        <v>unknown</v>
+      </c>
+      <c r="AV7" s="137" t="str">
+        <f>IF(ISBLANK(AllEntries!AU11),"unknown",AllEntries!AU11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AV7" s="165" t="str">
-        <f>IF(ISBLANK(AllEntries!AU11),"unknown",AllEntries!AU11)</f>
+      <c r="AW7" s="165" t="str">
+        <f>IF(ISBLANK(AllEntries!AV11),"unknown",AllEntries!AV11)</f>
         <v>unknown</v>
       </c>
-      <c r="AW7" s="128"/>
-      <c r="AX7" s="2"/>
+      <c r="AX7" s="128"/>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
@@ -11809,150 +11839,153 @@
       <c r="BU7" s="2"/>
       <c r="BV7" s="2"/>
       <c r="BW7" s="2"/>
+      <c r="BX7" s="2"/>
     </row>
-    <row r="8" spans="1:75" s="36" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:76" s="36" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="154" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="M8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="O8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="P8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Q8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="R8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="S8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="T8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="U8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="V8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="W8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="X8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Y8" s="142"/>
       <c r="Z8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AA8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AB8" s="142"/>
       <c r="AC8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AD8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AE8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AF8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AG8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AH8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AI8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AJ8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AK8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AL8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AM8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AN8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AO8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AP8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AQ8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AR8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AS8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AT8" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AU8" s="142" t="s">
-        <v>188</v>
-      </c>
-      <c r="AV8" s="166" t="s">
-        <v>188</v>
-      </c>
-      <c r="AW8" s="145"/>
-      <c r="AX8" s="146"/>
+        <v>186</v>
+      </c>
+      <c r="AV8" s="142" t="s">
+        <v>186</v>
+      </c>
+      <c r="AW8" s="166" t="s">
+        <v>186</v>
+      </c>
+      <c r="AX8" s="145"/>
       <c r="AY8" s="146"/>
       <c r="AZ8" s="146"/>
       <c r="BA8" s="146"/>
@@ -11978,8 +12011,9 @@
       <c r="BU8" s="146"/>
       <c r="BV8" s="146"/>
       <c r="BW8" s="146"/>
+      <c r="BX8" s="146"/>
     </row>
-    <row r="9" spans="1:75" s="36" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:76" s="36" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="154" t="s">
         <v>96</v>
       </c>
@@ -12064,18 +12098,20 @@
       <c r="AD9" s="142" t="s">
         <v>157</v>
       </c>
-      <c r="AE9" s="142"/>
+      <c r="AE9" s="142" t="s">
+        <v>225</v>
+      </c>
       <c r="AF9" s="142"/>
       <c r="AG9" s="142"/>
-      <c r="AH9" s="142"/>
-      <c r="AI9" s="142" t="s">
-        <v>158</v>
-      </c>
+      <c r="AH9" s="221" t="s">
+        <v>229</v>
+      </c>
+      <c r="AI9" s="142"/>
       <c r="AJ9" s="142" t="s">
         <v>158</v>
       </c>
       <c r="AK9" s="142" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AL9" s="142" t="s">
         <v>159</v>
@@ -12087,10 +12123,10 @@
         <v>159</v>
       </c>
       <c r="AO9" s="142" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="AP9" s="142" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="AQ9" s="142" t="s">
         <v>159</v>
@@ -12099,7 +12135,7 @@
         <v>159</v>
       </c>
       <c r="AS9" s="142" t="s">
-        <v>159</v>
+        <v>224</v>
       </c>
       <c r="AT9" s="142" t="s">
         <v>159</v>
@@ -12107,11 +12143,13 @@
       <c r="AU9" s="142" t="s">
         <v>159</v>
       </c>
-      <c r="AV9" s="166" t="s">
+      <c r="AV9" s="142" t="s">
         <v>159</v>
       </c>
-      <c r="AW9" s="145"/>
-      <c r="AX9" s="146"/>
+      <c r="AW9" s="166" t="s">
+        <v>159</v>
+      </c>
+      <c r="AX9" s="145"/>
       <c r="AY9" s="146"/>
       <c r="AZ9" s="146"/>
       <c r="BA9" s="146"/>
@@ -12137,9 +12175,10 @@
       <c r="BU9" s="146"/>
       <c r="BV9" s="146"/>
       <c r="BW9" s="146"/>
+      <c r="BX9" s="146"/>
     </row>
-    <row r="10" spans="1:75" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:76" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A11" s="63"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
@@ -12147,7 +12186,7 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="AW3:AW5"/>
+    <mergeCell ref="AX3:AX5"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J2:O2"/>
@@ -12159,7 +12198,7 @@
     <brk id="17" max="9" man="1"/>
   </colBreaks>
   <ignoredErrors>
-    <ignoredError sqref="AO6" formula="1"/>
+    <ignoredError sqref="AP6" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -12168,8 +12207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12186,19 +12225,19 @@
     </row>
     <row r="3" spans="2:6" ht="25.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="173" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="174" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="174" t="s">
         <v>195</v>
       </c>
-      <c r="C3" s="174" t="s">
+      <c r="E3" s="175" t="s">
+        <v>199</v>
+      </c>
+      <c r="F3" s="176" t="s">
         <v>196</v>
-      </c>
-      <c r="D3" s="174" t="s">
-        <v>197</v>
-      </c>
-      <c r="E3" s="175" t="s">
-        <v>201</v>
-      </c>
-      <c r="F3" s="176" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30.6" x14ac:dyDescent="0.3">
@@ -12210,13 +12249,13 @@
       </c>
       <c r="D4" s="116"/>
       <c r="E4" s="181" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F4" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="177" t="s">
         <v>104</v>
       </c>
@@ -12224,7 +12263,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="116" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E5" s="181"/>
       <c r="F5" s="116"/>
@@ -12237,13 +12276,13 @@
         <v>58</v>
       </c>
       <c r="D6" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E6" s="181" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F6" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -12254,11 +12293,11 @@
         <v>58</v>
       </c>
       <c r="D7" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" s="181"/>
       <c r="F7" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -12269,11 +12308,11 @@
         <v>58</v>
       </c>
       <c r="D8" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E8" s="181"/>
       <c r="F8" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -12284,11 +12323,11 @@
         <v>58</v>
       </c>
       <c r="D9" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E9" s="181"/>
       <c r="F9" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
@@ -12299,11 +12338,11 @@
         <v>58</v>
       </c>
       <c r="D10" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E10" s="181"/>
       <c r="F10" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
@@ -12314,14 +12353,14 @@
         <v>58</v>
       </c>
       <c r="D11" s="116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E11" s="181"/>
       <c r="F11" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="178" t="s">
         <v>121</v>
       </c>
@@ -12329,11 +12368,11 @@
         <v>124</v>
       </c>
       <c r="D12" s="116" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E12" s="189"/>
       <c r="F12" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
@@ -12344,16 +12383,16 @@
         <v>124</v>
       </c>
       <c r="D13" s="116" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E13" s="189" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F13" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="178" t="s">
         <v>121</v>
       </c>
@@ -12361,14 +12400,14 @@
         <v>124</v>
       </c>
       <c r="D14" s="116" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E14" s="189"/>
       <c r="F14" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="178" t="s">
         <v>42</v>
       </c>
@@ -12376,11 +12415,11 @@
         <v>115</v>
       </c>
       <c r="D15" s="116" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E15" s="189"/>
       <c r="F15" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
@@ -12391,16 +12430,16 @@
         <v>116</v>
       </c>
       <c r="D16" s="116" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E16" s="189" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F16" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="178" t="s">
         <v>42</v>
       </c>
@@ -12408,11 +12447,11 @@
         <v>109</v>
       </c>
       <c r="D17" s="116" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E17" s="189"/>
       <c r="F17" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="61.2" x14ac:dyDescent="0.3">
@@ -12423,13 +12462,13 @@
         <v>25</v>
       </c>
       <c r="D18" s="116" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E18" s="181" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F18" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -12451,13 +12490,13 @@
         <v>26</v>
       </c>
       <c r="D20" s="116" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E20" s="116" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F20" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -12468,11 +12507,11 @@
         <v>26</v>
       </c>
       <c r="D21" s="116" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E21" s="181"/>
       <c r="F21" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -12483,11 +12522,11 @@
         <v>130</v>
       </c>
       <c r="D22" s="185" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E22" s="181"/>
       <c r="F22" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
@@ -12498,13 +12537,13 @@
         <v>148</v>
       </c>
       <c r="D23" s="185" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E23" s="181" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F23" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
@@ -12515,13 +12554,13 @@
         <v>111</v>
       </c>
       <c r="D24" s="185" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E24" s="181" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F24" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
@@ -12532,13 +12571,13 @@
         <v>97</v>
       </c>
       <c r="D25" s="185" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E25" s="181" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F25" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
@@ -12549,11 +12588,11 @@
         <v>93</v>
       </c>
       <c r="D26" s="116" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E26" s="116"/>
       <c r="F26" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
@@ -12564,7 +12603,7 @@
         <v>94</v>
       </c>
       <c r="D27" s="116" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E27" s="116"/>
       <c r="F27" s="116"/>
@@ -12576,20 +12615,28 @@
       <c r="C28" s="180" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="116"/>
+      <c r="D28" s="116" t="s">
+        <v>202</v>
+      </c>
       <c r="E28" s="116"/>
-      <c r="F28" s="116"/>
+      <c r="F28" s="116" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="178" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C29" s="180" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="116"/>
+      <c r="D29" s="116" t="s">
+        <v>204</v>
+      </c>
       <c r="E29" s="116"/>
-      <c r="F29" s="116"/>
+      <c r="F29" s="116" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="178" t="s">
@@ -12610,11 +12657,11 @@
         <v>134</v>
       </c>
       <c r="D31" s="116" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E31" s="116"/>
       <c r="F31" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
@@ -12636,11 +12683,11 @@
         <v>28</v>
       </c>
       <c r="D33" s="116" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E33" s="116"/>
       <c r="F33" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
@@ -12673,11 +12720,11 @@
         <v>114</v>
       </c>
       <c r="D36" s="116" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E36" s="116"/>
       <c r="F36" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="30.6" x14ac:dyDescent="0.3">
@@ -12688,13 +12735,13 @@
         <v>128</v>
       </c>
       <c r="D37" s="116" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E37" s="116" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F37" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
@@ -12716,11 +12763,11 @@
         <v>136</v>
       </c>
       <c r="D39" s="185" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E39" s="116"/>
       <c r="F39" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
@@ -12733,7 +12780,7 @@
       <c r="D40" s="185"/>
       <c r="E40" s="116"/>
       <c r="F40" s="116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
@@ -12756,7 +12803,7 @@
       </c>
       <c r="D42" s="185"/>
       <c r="E42" s="116" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F42" s="116"/>
     </row>
@@ -12787,7 +12834,7 @@
         <v>56</v>
       </c>
       <c r="C45" s="182" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="116"/>
@@ -12824,10 +12871,10 @@
       </c>
       <c r="D48" s="116"/>
       <c r="E48" s="116" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F48" s="116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
@@ -12842,72 +12889,87 @@
       <c r="F49" s="116"/>
     </row>
   </sheetData>
+  <autoFilter ref="B3:F49">
+    <sortState ref="B42:F42">
+      <sortCondition descending="1" ref="F3:F49"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="B4:E49">
     <sortCondition ref="C4:C49"/>
   </sortState>
-  <conditionalFormatting sqref="B5:F5 B21:F22 B7:F12 B26:F36 B38:F41 B19:F19 B17:F17 B14:F15 B49:F49 B43:F47">
-    <cfRule type="containsText" dxfId="42" priority="13" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="B5:F5 B21:F22 B7:F12 B26:F27 B38:F41 B19:F19 B17:F17 B14:F15 B49:F49 B43:F47 B30:F36">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:F20">
-    <cfRule type="containsText" dxfId="36" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:F6">
-    <cfRule type="containsText" dxfId="32" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:F24">
-    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37:F37">
-    <cfRule type="containsText" dxfId="24" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:F23">
-    <cfRule type="containsText" dxfId="21" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:F25">
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:F18">
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:F16">
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:F13">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:F48">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:F42">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:F29">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:F28">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
A wrong dash is deleted (led to 2 CLMcom versions)
</commit_message>
<xml_diff>
--- a/CORDEX_ESGF_coordination_issues.xlsx
+++ b/CORDEX_ESGF_coordination_issues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="768" windowWidth="16608" windowHeight="8676" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="768" windowWidth="16608" windowHeight="8676" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralRemarks" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="ARC_44">DatVol!$B$37</definedName>
     <definedName name="ARC44tier1">DatVol!$C$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$AW$13</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AX$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AW$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">DatVol!$A$1:$BA$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$4</definedName>
     <definedName name="EUR_11" localSheetId="3">ControlledVocabulary!#REF!</definedName>
@@ -56,7 +56,7 @@
     <definedName name="MED44tier1" localSheetId="0">GeneralRemarks!#REF!</definedName>
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
     <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AW$9</definedName>
-    <definedName name="Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AU$5</definedName>
+    <definedName name="Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AT$5</definedName>
     <definedName name="Print_Area" localSheetId="2">DatVol!$A$1:$AZ$39</definedName>
     <definedName name="Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$2</definedName>
   </definedNames>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="230">
   <si>
     <t>Domain</t>
   </si>
@@ -2992,6 +2992,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3060,30 +3084,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3093,47 +3093,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color auto="1"/>
@@ -3620,20 +3580,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="199" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
-      <c r="F1" s="191"/>
-      <c r="G1" s="191"/>
-      <c r="H1" s="191"/>
-      <c r="I1" s="191"/>
-      <c r="J1" s="191"/>
-      <c r="K1" s="191"/>
-      <c r="L1" s="191"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="199"/>
+      <c r="L1" s="199"/>
       <c r="M1" s="21"/>
       <c r="N1" s="20"/>
       <c r="O1" s="20"/>
@@ -3658,12 +3618,12 @@
       <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" s="148" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="200" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="192"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
       <c r="E3" s="147"/>
       <c r="F3" s="147"/>
       <c r="G3" s="147"/>
@@ -3701,8 +3661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BZ38"/>
   <sheetViews>
-    <sheetView topLeftCell="U2" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3740,24 +3700,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="201" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
-      <c r="F1" s="191"/>
-      <c r="G1" s="191"/>
-      <c r="H1" s="191"/>
-      <c r="I1" s="191"/>
-      <c r="J1" s="191"/>
-      <c r="K1" s="191"/>
-      <c r="L1" s="191"/>
-      <c r="M1" s="191"/>
-      <c r="N1" s="191"/>
-      <c r="O1" s="191"/>
-      <c r="P1" s="191"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="199"/>
+      <c r="L1" s="199"/>
+      <c r="M1" s="199"/>
+      <c r="N1" s="199"/>
+      <c r="O1" s="199"/>
+      <c r="P1" s="199"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="20"/>
       <c r="S1" s="20"/>
@@ -3805,13 +3765,13 @@
         <f>GeneralRemarks!A2</f>
         <v>41901</v>
       </c>
-      <c r="B2" s="195"/>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
+      <c r="B2" s="203"/>
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="203"/>
+      <c r="H2" s="203"/>
       <c r="I2" s="51"/>
       <c r="J2" s="51"/>
       <c r="K2" s="51"/>
@@ -3955,7 +3915,7 @@
       <c r="AC3" s="112" t="s">
         <v>135</v>
       </c>
-      <c r="AD3" s="214" t="s">
+      <c r="AD3" s="191" t="s">
         <v>223</v>
       </c>
       <c r="AE3" s="112"/>
@@ -3981,7 +3941,7 @@
       </c>
       <c r="AP3" s="112"/>
       <c r="AQ3" s="112"/>
-      <c r="AR3" s="214" t="s">
+      <c r="AR3" s="191" t="s">
         <v>217</v>
       </c>
       <c r="AS3" s="112"/>
@@ -4120,7 +4080,7 @@
         <f t="shared" si="2"/>
         <v>DHMZ</v>
       </c>
-      <c r="AD4" s="215"/>
+      <c r="AD4" s="192"/>
       <c r="AE4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>GISS</v>
@@ -4263,7 +4223,7 @@
       <c r="AA5" s="131"/>
       <c r="AB5" s="131"/>
       <c r="AC5" s="131"/>
-      <c r="AD5" s="216"/>
+      <c r="AD5" s="193"/>
       <c r="AE5" s="131"/>
       <c r="AF5" s="131"/>
       <c r="AG5" s="131"/>
@@ -4347,7 +4307,7 @@
       <c r="AA6" s="115"/>
       <c r="AB6" s="115"/>
       <c r="AC6" s="115"/>
-      <c r="AD6" s="215"/>
+      <c r="AD6" s="192"/>
       <c r="AE6" s="115"/>
       <c r="AF6" s="115"/>
       <c r="AG6" s="115"/>
@@ -4410,7 +4370,7 @@
         <v>104</v>
       </c>
       <c r="D7" s="177" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E7" s="177" t="s">
         <v>50</v>
@@ -4487,7 +4447,7 @@
       <c r="AC7" s="178" t="s">
         <v>48</v>
       </c>
-      <c r="AD7" s="217" t="s">
+      <c r="AD7" s="194" t="s">
         <v>221</v>
       </c>
       <c r="AE7" s="178" t="s">
@@ -4665,7 +4625,7 @@
       <c r="AC8" s="180" t="s">
         <v>134</v>
       </c>
-      <c r="AD8" s="218" t="s">
+      <c r="AD8" s="195" t="s">
         <v>222</v>
       </c>
       <c r="AE8" s="182" t="s">
@@ -4837,7 +4797,7 @@
       <c r="AC9" s="116" t="s">
         <v>188</v>
       </c>
-      <c r="AD9" s="219" t="s">
+      <c r="AD9" s="196" t="s">
         <v>220</v>
       </c>
       <c r="AE9" s="116"/>
@@ -4863,7 +4823,7 @@
       <c r="AO9" s="185"/>
       <c r="AP9" s="116"/>
       <c r="AQ9" s="116"/>
-      <c r="AR9" s="219" t="s">
+      <c r="AR9" s="196" t="s">
         <v>216</v>
       </c>
       <c r="AS9" s="116"/>
@@ -4953,7 +4913,7 @@
       <c r="AA10" s="116"/>
       <c r="AB10" s="116"/>
       <c r="AC10" s="116"/>
-      <c r="AD10" s="219"/>
+      <c r="AD10" s="196"/>
       <c r="AE10" s="116"/>
       <c r="AF10" s="116"/>
       <c r="AG10" s="116"/>
@@ -5126,7 +5086,7 @@
         <v>181</v>
       </c>
       <c r="AV11" s="116"/>
-      <c r="AW11" s="220" t="s">
+      <c r="AW11" s="197" t="s">
         <v>153</v>
       </c>
       <c r="AX11" s="135"/>
@@ -5160,16 +5120,16 @@
       <c r="BZ11" s="135"/>
     </row>
     <row r="12" spans="1:78" s="26" customFormat="1" ht="21.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="194" t="s">
+      <c r="A12" s="202" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="194"/>
-      <c r="C12" s="194"/>
-      <c r="D12" s="194"/>
-      <c r="E12" s="194"/>
-      <c r="F12" s="194"/>
-      <c r="G12" s="194"/>
-      <c r="H12" s="194"/>
+      <c r="B12" s="202"/>
+      <c r="C12" s="202"/>
+      <c r="D12" s="202"/>
+      <c r="E12" s="202"/>
+      <c r="F12" s="202"/>
+      <c r="G12" s="202"/>
+      <c r="H12" s="202"/>
       <c r="I12" s="127"/>
       <c r="J12" s="127"/>
       <c r="K12" s="127"/>
@@ -5212,14 +5172,14 @@
       <c r="AV12" s="127"/>
     </row>
     <row r="13" spans="1:78" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="194" t="s">
+      <c r="A13" s="202" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="194"/>
-      <c r="C13" s="194"/>
-      <c r="D13" s="194"/>
-      <c r="E13" s="194"/>
-      <c r="F13" s="194"/>
+      <c r="B13" s="202"/>
+      <c r="C13" s="202"/>
+      <c r="D13" s="202"/>
+      <c r="E13" s="202"/>
+      <c r="F13" s="202"/>
       <c r="G13" s="141"/>
       <c r="H13" s="141"/>
       <c r="I13" s="141"/>
@@ -5357,25 +5317,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:144" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="199" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
-      <c r="F1" s="191"/>
-      <c r="G1" s="191"/>
-      <c r="H1" s="191"/>
-      <c r="I1" s="191"/>
-      <c r="J1" s="191"/>
-      <c r="K1" s="191"/>
-      <c r="L1" s="191"/>
-      <c r="M1" s="191"/>
-      <c r="N1" s="191"/>
-      <c r="O1" s="191"/>
-      <c r="P1" s="191"/>
-      <c r="Q1" s="191"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="199"/>
+      <c r="L1" s="199"/>
+      <c r="M1" s="199"/>
+      <c r="N1" s="199"/>
+      <c r="O1" s="199"/>
+      <c r="P1" s="199"/>
+      <c r="Q1" s="199"/>
       <c r="R1" s="21"/>
       <c r="S1" s="20"/>
       <c r="T1" s="20"/>
@@ -6011,7 +5971,7 @@
         <f>AllEntries!AV4</f>
         <v>UCAN</v>
       </c>
-      <c r="AZ4" s="198" t="s">
+      <c r="AZ4" s="206" t="s">
         <v>16</v>
       </c>
       <c r="BA4" s="75" t="s">
@@ -6314,7 +6274,7 @@
         <f>AllEntries!AV6</f>
         <v>0</v>
       </c>
-      <c r="AZ5" s="199"/>
+      <c r="AZ5" s="207"/>
       <c r="BA5" s="75"/>
       <c r="BB5" s="2"/>
       <c r="BC5" s="2"/>
@@ -6613,7 +6573,7 @@
         <f>AllEntries!AV8</f>
         <v>WRF350I</v>
       </c>
-      <c r="AZ6" s="200"/>
+      <c r="AZ6" s="208"/>
       <c r="BA6" s="76" t="s">
         <v>19</v>
       </c>
@@ -10209,25 +10169,25 @@
       <c r="EN27" s="26"/>
     </row>
     <row r="28" spans="1:144" s="26" customFormat="1" ht="37.200000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="201" t="s">
+      <c r="A28" s="209" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="201"/>
-      <c r="C28" s="201"/>
-      <c r="D28" s="201"/>
-      <c r="E28" s="201"/>
-      <c r="F28" s="201"/>
-      <c r="G28" s="201"/>
-      <c r="H28" s="201"/>
-      <c r="I28" s="201"/>
-      <c r="J28" s="201"/>
-      <c r="K28" s="201"/>
-      <c r="L28" s="201"/>
-      <c r="M28" s="201"/>
-      <c r="N28" s="201"/>
-      <c r="O28" s="201"/>
-      <c r="P28" s="201"/>
-      <c r="Q28" s="201"/>
+      <c r="B28" s="209"/>
+      <c r="C28" s="209"/>
+      <c r="D28" s="209"/>
+      <c r="E28" s="209"/>
+      <c r="F28" s="209"/>
+      <c r="G28" s="209"/>
+      <c r="H28" s="209"/>
+      <c r="I28" s="209"/>
+      <c r="J28" s="209"/>
+      <c r="K28" s="209"/>
+      <c r="L28" s="209"/>
+      <c r="M28" s="209"/>
+      <c r="N28" s="209"/>
+      <c r="O28" s="209"/>
+      <c r="P28" s="209"/>
+      <c r="Q28" s="209"/>
       <c r="R28" s="40"/>
       <c r="S28" s="40"/>
       <c r="T28" s="40"/>
@@ -10263,69 +10223,69 @@
       <c r="AX28" s="30"/>
     </row>
     <row r="29" spans="1:144" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="202" t="s">
+      <c r="A29" s="210" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="202"/>
-      <c r="C29" s="202"/>
-      <c r="D29" s="202"/>
-      <c r="E29" s="202"/>
-      <c r="F29" s="202"/>
-      <c r="G29" s="202"/>
-      <c r="H29" s="202"/>
-      <c r="I29" s="202"/>
-      <c r="J29" s="202"/>
-      <c r="K29" s="202"/>
-      <c r="L29" s="202"/>
-      <c r="M29" s="202"/>
-      <c r="N29" s="202"/>
-      <c r="O29" s="202"/>
-      <c r="P29" s="202"/>
-      <c r="Q29" s="202"/>
-      <c r="R29" s="202"/>
-      <c r="S29" s="202"/>
-      <c r="T29" s="202"/>
-      <c r="U29" s="202"/>
-      <c r="V29" s="202"/>
-      <c r="W29" s="202"/>
-      <c r="X29" s="202"/>
-      <c r="Y29" s="202"/>
-      <c r="Z29" s="202"/>
-      <c r="AA29" s="202"/>
-      <c r="AB29" s="202"/>
-      <c r="AC29" s="202"/>
-      <c r="AD29" s="202"/>
-      <c r="AE29" s="202"/>
-      <c r="AF29" s="202"/>
-      <c r="AG29" s="202"/>
-      <c r="AH29" s="202"/>
-      <c r="AI29" s="202"/>
-      <c r="AJ29" s="202"/>
-      <c r="AK29" s="202"/>
-      <c r="AL29" s="202"/>
-      <c r="AM29" s="202"/>
-      <c r="AN29" s="202"/>
-      <c r="AO29" s="202"/>
-      <c r="AP29" s="202"/>
-      <c r="AQ29" s="202"/>
-      <c r="AR29" s="202"/>
-      <c r="AS29" s="202"/>
-      <c r="AT29" s="202"/>
-      <c r="AU29" s="202"/>
-      <c r="AV29" s="202"/>
-      <c r="AW29" s="202"/>
-      <c r="AX29" s="202"/>
+      <c r="B29" s="210"/>
+      <c r="C29" s="210"/>
+      <c r="D29" s="210"/>
+      <c r="E29" s="210"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="210"/>
+      <c r="H29" s="210"/>
+      <c r="I29" s="210"/>
+      <c r="J29" s="210"/>
+      <c r="K29" s="210"/>
+      <c r="L29" s="210"/>
+      <c r="M29" s="210"/>
+      <c r="N29" s="210"/>
+      <c r="O29" s="210"/>
+      <c r="P29" s="210"/>
+      <c r="Q29" s="210"/>
+      <c r="R29" s="210"/>
+      <c r="S29" s="210"/>
+      <c r="T29" s="210"/>
+      <c r="U29" s="210"/>
+      <c r="V29" s="210"/>
+      <c r="W29" s="210"/>
+      <c r="X29" s="210"/>
+      <c r="Y29" s="210"/>
+      <c r="Z29" s="210"/>
+      <c r="AA29" s="210"/>
+      <c r="AB29" s="210"/>
+      <c r="AC29" s="210"/>
+      <c r="AD29" s="210"/>
+      <c r="AE29" s="210"/>
+      <c r="AF29" s="210"/>
+      <c r="AG29" s="210"/>
+      <c r="AH29" s="210"/>
+      <c r="AI29" s="210"/>
+      <c r="AJ29" s="210"/>
+      <c r="AK29" s="210"/>
+      <c r="AL29" s="210"/>
+      <c r="AM29" s="210"/>
+      <c r="AN29" s="210"/>
+      <c r="AO29" s="210"/>
+      <c r="AP29" s="210"/>
+      <c r="AQ29" s="210"/>
+      <c r="AR29" s="210"/>
+      <c r="AS29" s="210"/>
+      <c r="AT29" s="210"/>
+      <c r="AU29" s="210"/>
+      <c r="AV29" s="210"/>
+      <c r="AW29" s="210"/>
+      <c r="AX29" s="210"/>
     </row>
     <row r="30" spans="1:144" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="203" t="s">
+      <c r="A30" s="211" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="203"/>
-      <c r="C30" s="203"/>
-      <c r="D30" s="203"/>
-      <c r="E30" s="203"/>
-      <c r="F30" s="202"/>
-      <c r="G30" s="202"/>
+      <c r="B30" s="211"/>
+      <c r="C30" s="211"/>
+      <c r="D30" s="211"/>
+      <c r="E30" s="211"/>
+      <c r="F30" s="210"/>
+      <c r="G30" s="210"/>
       <c r="H30" s="19"/>
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
@@ -10367,10 +10327,10 @@
       <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="204" t="s">
+      <c r="D31" s="212" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="205"/>
+      <c r="E31" s="213"/>
       <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:144" x14ac:dyDescent="0.3">
@@ -10385,11 +10345,11 @@
         <f>C33*98*63/194/201</f>
         <v>460.27127250346206</v>
       </c>
-      <c r="D32" s="206">
+      <c r="D32" s="214">
         <f t="shared" ref="D32:D37" si="33">(B32+C32)/1</f>
         <v>476.23114325280812</v>
       </c>
-      <c r="E32" s="207"/>
+      <c r="E32" s="215"/>
       <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.3">
@@ -10403,11 +10363,11 @@
       <c r="C33" s="10">
         <v>2907</v>
       </c>
-      <c r="D33" s="208">
+      <c r="D33" s="216">
         <f t="shared" si="33"/>
         <v>3007.8</v>
       </c>
-      <c r="E33" s="209"/>
+      <c r="E33" s="217"/>
       <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:49" x14ac:dyDescent="0.3">
@@ -10422,11 +10382,11 @@
         <f>4*AFR44tier1</f>
         <v>11628</v>
       </c>
-      <c r="D34" s="208">
+      <c r="D34" s="216">
         <f t="shared" si="33"/>
         <v>12031.2</v>
       </c>
-      <c r="E34" s="209"/>
+      <c r="E34" s="217"/>
       <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:49" x14ac:dyDescent="0.3">
@@ -10440,11 +10400,11 @@
       <c r="C35" s="98">
         <v>13005</v>
       </c>
-      <c r="D35" s="208">
+      <c r="D35" s="216">
         <f t="shared" si="33"/>
         <v>13475.4</v>
       </c>
-      <c r="E35" s="209"/>
+      <c r="E35" s="217"/>
       <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:49" x14ac:dyDescent="0.3">
@@ -10459,11 +10419,11 @@
         <f>C33*125*97/194/201</f>
         <v>903.91791044776119</v>
       </c>
-      <c r="D36" s="208">
+      <c r="D36" s="216">
         <f t="shared" si="33"/>
         <v>932.02992768118168</v>
       </c>
-      <c r="E36" s="209"/>
+      <c r="E36" s="217"/>
       <c r="F36" s="26"/>
     </row>
     <row r="37" spans="1:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10478,34 +10438,34 @@
         <f>C33*116*133/194/201</f>
         <v>1150.1563317433452</v>
       </c>
-      <c r="D37" s="210">
+      <c r="D37" s="218">
         <f t="shared" si="33"/>
         <v>1190.0379135251578</v>
       </c>
-      <c r="E37" s="211"/>
+      <c r="E37" s="219"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A38" s="196" t="s">
+      <c r="A38" s="204" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="196"/>
-      <c r="C38" s="196"/>
-      <c r="D38" s="196"/>
-      <c r="E38" s="196"/>
-      <c r="F38" s="197"/>
-      <c r="G38" s="197"/>
+      <c r="B38" s="204"/>
+      <c r="C38" s="204"/>
+      <c r="D38" s="204"/>
+      <c r="E38" s="204"/>
+      <c r="F38" s="205"/>
+      <c r="G38" s="205"/>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A39" s="197" t="s">
+      <c r="A39" s="205" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="197"/>
-      <c r="C39" s="197"/>
-      <c r="D39" s="197"/>
-      <c r="E39" s="197"/>
-      <c r="F39" s="197"/>
-      <c r="G39" s="197"/>
+      <c r="B39" s="205"/>
+      <c r="C39" s="205"/>
+      <c r="D39" s="205"/>
+      <c r="E39" s="205"/>
+      <c r="F39" s="205"/>
+      <c r="G39" s="205"/>
       <c r="H39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
@@ -10568,10 +10528,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BX18"/>
+  <dimension ref="A1:BW18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3:AH6"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10592,62 +10552,61 @@
     <col min="14" max="14" width="16.33203125" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
     <col min="16" max="16" width="14.109375" customWidth="1"/>
-    <col min="17" max="17" width="14.109375" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="19.6640625" customWidth="1"/>
-    <col min="19" max="19" width="26.33203125" customWidth="1"/>
-    <col min="20" max="20" width="17.88671875" customWidth="1"/>
-    <col min="21" max="21" width="16.6640625" style="62" customWidth="1"/>
-    <col min="22" max="23" width="19" customWidth="1"/>
-    <col min="24" max="24" width="23.6640625" customWidth="1"/>
-    <col min="25" max="25" width="16.6640625" customWidth="1"/>
-    <col min="26" max="26" width="17.6640625" customWidth="1"/>
-    <col min="27" max="28" width="18.88671875" customWidth="1"/>
-    <col min="29" max="29" width="18.33203125" customWidth="1"/>
-    <col min="30" max="31" width="18.44140625" customWidth="1"/>
-    <col min="32" max="32" width="12.88671875" customWidth="1"/>
-    <col min="33" max="33" width="19.5546875" customWidth="1"/>
-    <col min="34" max="34" width="15.109375" customWidth="1"/>
-    <col min="35" max="35" width="15.21875" customWidth="1"/>
-    <col min="36" max="36" width="22.44140625" customWidth="1"/>
-    <col min="37" max="37" width="23" customWidth="1"/>
-    <col min="38" max="38" width="19.44140625" customWidth="1"/>
-    <col min="39" max="39" width="22.21875" customWidth="1"/>
-    <col min="40" max="40" width="20.109375" customWidth="1"/>
-    <col min="41" max="41" width="22.109375" customWidth="1"/>
-    <col min="42" max="42" width="21" customWidth="1"/>
-    <col min="43" max="43" width="16.88671875" customWidth="1"/>
-    <col min="44" max="44" width="18.44140625" customWidth="1"/>
-    <col min="45" max="45" width="17.44140625" customWidth="1"/>
-    <col min="46" max="46" width="23" customWidth="1"/>
-    <col min="47" max="47" width="21.44140625" customWidth="1"/>
-    <col min="48" max="49" width="19.44140625" customWidth="1"/>
-    <col min="71" max="76" width="8.88671875" style="26"/>
+    <col min="17" max="17" width="19.6640625" customWidth="1"/>
+    <col min="18" max="18" width="26.33203125" customWidth="1"/>
+    <col min="19" max="19" width="17.88671875" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" style="62" customWidth="1"/>
+    <col min="21" max="22" width="19" customWidth="1"/>
+    <col min="23" max="23" width="23.6640625" customWidth="1"/>
+    <col min="24" max="24" width="16.6640625" customWidth="1"/>
+    <col min="25" max="25" width="17.6640625" customWidth="1"/>
+    <col min="26" max="27" width="18.88671875" customWidth="1"/>
+    <col min="28" max="28" width="18.33203125" customWidth="1"/>
+    <col min="29" max="30" width="18.44140625" customWidth="1"/>
+    <col min="31" max="31" width="12.88671875" customWidth="1"/>
+    <col min="32" max="32" width="19.5546875" customWidth="1"/>
+    <col min="33" max="33" width="15.109375" customWidth="1"/>
+    <col min="34" max="34" width="15.21875" customWidth="1"/>
+    <col min="35" max="35" width="22.44140625" customWidth="1"/>
+    <col min="36" max="36" width="23" customWidth="1"/>
+    <col min="37" max="37" width="19.44140625" customWidth="1"/>
+    <col min="38" max="38" width="22.21875" customWidth="1"/>
+    <col min="39" max="39" width="20.109375" customWidth="1"/>
+    <col min="40" max="40" width="22.109375" customWidth="1"/>
+    <col min="41" max="41" width="21" customWidth="1"/>
+    <col min="42" max="42" width="16.88671875" customWidth="1"/>
+    <col min="43" max="43" width="18.44140625" customWidth="1"/>
+    <col min="44" max="44" width="17.44140625" customWidth="1"/>
+    <col min="45" max="45" width="23" customWidth="1"/>
+    <col min="46" max="46" width="21.44140625" customWidth="1"/>
+    <col min="47" max="48" width="19.44140625" customWidth="1"/>
+    <col min="70" max="75" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="212" t="s">
+    <row r="1" spans="1:75" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="220" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="212"/>
-      <c r="H1" s="212"/>
-      <c r="I1" s="212"/>
-      <c r="J1" s="212"/>
-      <c r="K1" s="212"/>
-      <c r="L1" s="212"/>
-      <c r="M1" s="212"/>
-      <c r="N1" s="212"/>
-      <c r="O1" s="212"/>
-      <c r="P1" s="212"/>
-      <c r="Q1" s="212"/>
-      <c r="R1" s="212"/>
-      <c r="S1" s="212"/>
-      <c r="T1" s="104"/>
-      <c r="U1" s="64"/>
+      <c r="B1" s="220"/>
+      <c r="C1" s="220"/>
+      <c r="D1" s="220"/>
+      <c r="E1" s="220"/>
+      <c r="F1" s="220"/>
+      <c r="G1" s="220"/>
+      <c r="H1" s="220"/>
+      <c r="I1" s="220"/>
+      <c r="J1" s="220"/>
+      <c r="K1" s="220"/>
+      <c r="L1" s="220"/>
+      <c r="M1" s="220"/>
+      <c r="N1" s="220"/>
+      <c r="O1" s="220"/>
+      <c r="P1" s="220"/>
+      <c r="Q1" s="220"/>
+      <c r="R1" s="220"/>
+      <c r="S1" s="104"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="20"/>
       <c r="V1" s="20"/>
       <c r="W1" s="20"/>
       <c r="X1" s="20"/>
@@ -10663,46 +10622,45 @@
       <c r="AH1" s="20"/>
       <c r="AI1" s="20"/>
       <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AM1" s="20"/>
       <c r="AN1" s="20"/>
       <c r="AO1" s="20"/>
       <c r="AP1" s="20"/>
       <c r="AQ1" s="20"/>
       <c r="AR1" s="20"/>
       <c r="AS1" s="20"/>
-      <c r="AT1" s="20"/>
+      <c r="AU1" s="26"/>
       <c r="AV1" s="26"/>
-      <c r="AW1" s="26"/>
     </row>
-    <row r="2" spans="1:76" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:75" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="54">
         <f>GeneralRemarks!A2</f>
         <v>41901</v>
       </c>
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="213"/>
+      <c r="B2" s="221"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
       <c r="E2" s="138"/>
       <c r="F2" s="138"/>
       <c r="G2" s="138"/>
       <c r="H2" s="138"/>
       <c r="I2" s="138"/>
-      <c r="J2" s="213"/>
-      <c r="K2" s="213"/>
-      <c r="L2" s="213"/>
-      <c r="M2" s="213"/>
-      <c r="N2" s="213"/>
-      <c r="O2" s="213"/>
+      <c r="J2" s="221"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
+      <c r="M2" s="221"/>
+      <c r="N2" s="221"/>
+      <c r="O2" s="221"/>
       <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
+      <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
       <c r="T2" s="20"/>
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="20"/>
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
       <c r="AA2" s="20"/>
@@ -10715,22 +10673,21 @@
       <c r="AH2" s="20"/>
       <c r="AI2" s="20"/>
       <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AM2" s="20"/>
       <c r="AN2" s="20"/>
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
       <c r="AQ2" s="20"/>
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AV2" s="52">
+      <c r="AU2" s="52">
         <f>A2</f>
         <v>41901</v>
       </c>
-      <c r="AW2" s="26"/>
+      <c r="AV2" s="26"/>
     </row>
-    <row r="3" spans="1:76" s="1" customFormat="1" ht="32.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:75" s="1" customFormat="1" ht="32.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="79" t="s">
         <v>88</v>
       </c>
@@ -10744,7 +10701,7 @@
       </c>
       <c r="D3" s="80" t="str">
         <f>AllEntries!D7</f>
-        <v xml:space="preserve">CLMcom </v>
+        <v>CLMcom</v>
       </c>
       <c r="E3" s="80" t="str">
         <f>AllEntries!E7</f>
@@ -10794,136 +10751,136 @@
         <f>AllEntries!P7</f>
         <v>SMHI</v>
       </c>
-      <c r="Q3" s="139"/>
-      <c r="R3" s="80" t="str">
+      <c r="Q3" s="80" t="str">
         <f>AllEntries!Q7</f>
         <v>CHMI</v>
       </c>
-      <c r="S3" s="80" t="str">
+      <c r="R3" s="80" t="str">
         <f>AllEntries!R7</f>
         <v>HMS</v>
       </c>
-      <c r="T3" s="80" t="str">
+      <c r="S3" s="80" t="str">
         <f>AllEntries!S7</f>
         <v>CNRM</v>
       </c>
-      <c r="U3" s="80" t="str">
+      <c r="T3" s="80" t="str">
         <f>AllEntries!T7</f>
         <v>CNRM</v>
       </c>
-      <c r="V3" s="110" t="str">
+      <c r="U3" s="110" t="str">
         <f>AllEntries!U7</f>
         <v>KNMI</v>
       </c>
-      <c r="W3" s="110" t="str">
+      <c r="V3" s="110" t="str">
         <f>AllEntries!V7</f>
         <v>KNMI</v>
       </c>
-      <c r="X3" s="125" t="str">
+      <c r="W3" s="125" t="str">
         <f>AllEntries!W7</f>
         <v>KNMI</v>
       </c>
-      <c r="Y3" s="139" t="str">
+      <c r="X3" s="139" t="str">
         <f>AllEntries!X7</f>
         <v>UQAM</v>
       </c>
-      <c r="Z3" s="80" t="str">
+      <c r="Y3" s="80" t="str">
         <f>AllEntries!Y7</f>
         <v>UCLM</v>
       </c>
-      <c r="AA3" s="80" t="str">
+      <c r="Z3" s="80" t="str">
         <f>AllEntries!Z7</f>
         <v>ICTP</v>
       </c>
-      <c r="AB3" s="139" t="str">
+      <c r="AA3" s="139" t="str">
         <f>AllEntries!AA7</f>
         <v>ENEA</v>
       </c>
-      <c r="AC3" s="80" t="str">
+      <c r="AB3" s="80" t="str">
         <f>AllEntries!AB7</f>
         <v>CUNI</v>
       </c>
-      <c r="AD3" s="80" t="str">
+      <c r="AC3" s="80" t="str">
         <f>AllEntries!AC7</f>
         <v>DHMZ</v>
       </c>
-      <c r="AE3" s="80" t="str">
+      <c r="AD3" s="80" t="str">
         <f>AllEntries!AD7</f>
         <v>IITM</v>
       </c>
-      <c r="AF3" s="139" t="str">
+      <c r="AE3" s="139" t="str">
         <f>AllEntries!AE7</f>
         <v>GISS</v>
       </c>
-      <c r="AG3" s="139" t="str">
+      <c r="AF3" s="139" t="str">
         <f>AllEntries!AF7</f>
         <v>CCCma</v>
       </c>
-      <c r="AH3" s="80" t="str">
+      <c r="AG3" s="80" t="str">
         <f>AllEntries!AG7</f>
         <v>CSIRO</v>
       </c>
-      <c r="AI3" s="139" t="str">
+      <c r="AH3" s="139" t="str">
         <f>AllEntries!AH7</f>
         <v>KAUST</v>
       </c>
-      <c r="AJ3" s="80" t="str">
+      <c r="AI3" s="80" t="str">
         <f>AllEntries!AI7</f>
         <v>MOHC</v>
       </c>
-      <c r="AK3" s="80" t="str">
+      <c r="AJ3" s="80" t="str">
         <f>AllEntries!AJ7</f>
         <v>MOHC</v>
       </c>
-      <c r="AL3" s="80" t="str">
+      <c r="AK3" s="80" t="str">
         <f>AllEntries!AK7</f>
         <v>MIUB</v>
       </c>
-      <c r="AM3" s="125" t="str">
+      <c r="AL3" s="125" t="str">
         <f>AllEntries!AL7</f>
         <v>BCCR</v>
       </c>
-      <c r="AN3" s="80" t="str">
+      <c r="AM3" s="80" t="str">
         <f>AllEntries!AM7</f>
         <v>CRP-GL</v>
       </c>
-      <c r="AO3" s="80" t="str">
+      <c r="AN3" s="80" t="str">
         <f>AllEntries!AN7</f>
         <v>IDL</v>
       </c>
-      <c r="AP3" s="80" t="str">
+      <c r="AO3" s="80" t="str">
         <f>AllEntries!AO7</f>
         <v>IPSL-INERIS</v>
       </c>
-      <c r="AQ3" s="80" t="str">
+      <c r="AP3" s="80" t="str">
         <f>AllEntries!AP7</f>
         <v>AUTH-Met</v>
       </c>
-      <c r="AR3" s="80" t="str">
+      <c r="AQ3" s="80" t="str">
         <f>AllEntries!AQ7</f>
         <v>AUTH-LHTEE</v>
       </c>
-      <c r="AS3" s="80" t="str">
+      <c r="AR3" s="80" t="str">
         <f>AllEntries!AR7</f>
         <v>NUIM</v>
       </c>
-      <c r="AT3" s="80" t="str">
+      <c r="AS3" s="80" t="str">
         <f>AllEntries!AS7</f>
         <v>UHOH</v>
       </c>
-      <c r="AU3" s="80" t="str">
+      <c r="AT3" s="80" t="str">
         <f>AllEntries!AT7</f>
         <v>UM</v>
       </c>
-      <c r="AV3" s="80" t="str">
+      <c r="AU3" s="80" t="str">
         <f>AllEntries!AU7</f>
         <v>UCAN</v>
       </c>
-      <c r="AW3" s="162" t="str">
+      <c r="AV3" s="162" t="str">
         <f>AllEntries!AV7</f>
         <v>UCAN</v>
       </c>
-      <c r="AX3" s="199"/>
+      <c r="AW3" s="207"/>
+      <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
@@ -10949,9 +10906,8 @@
       <c r="BU3" s="2"/>
       <c r="BV3" s="2"/>
       <c r="BW3" s="2"/>
-      <c r="BX3" s="2"/>
     </row>
-    <row r="4" spans="1:76" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:75" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="149" t="s">
         <v>182</v>
       </c>
@@ -11015,139 +10971,136 @@
         <f>IF(ISBLANK(AllEntries!P9),"",AllEntries!P9)</f>
         <v>Swedish Meteorological and Hydrological Institute, Rossby Centre</v>
       </c>
-      <c r="Q4" s="150" t="e">
-        <f>IF(ISBLANK(AllEntries!#REF!),"",AllEntries!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R4" s="150" t="str">
+      <c r="Q4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!Q9),"",AllEntries!Q9)</f>
         <v/>
       </c>
-      <c r="S4" s="150" t="str">
+      <c r="R4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!R9),"",AllEntries!R9)</f>
         <v>Hungarian Meteorological Service</v>
       </c>
-      <c r="T4" s="150" t="str">
+      <c r="S4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!S9),"",AllEntries!S9)</f>
         <v>Centre National de Recherches Meteorologiques</v>
       </c>
-      <c r="U4" s="150" t="str">
+      <c r="T4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!T9),"",AllEntries!T9)</f>
         <v>Centre National de Recherches Meteorologiques</v>
       </c>
-      <c r="V4" s="150" t="str">
+      <c r="U4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!U9),"",AllEntries!U9)</f>
         <v>Royal Netherlands Meteorological Institute, De Bilt, The Netherlands</v>
       </c>
-      <c r="W4" s="150" t="str">
+      <c r="V4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!V9),"",AllEntries!V9)</f>
         <v>Royal Netherlands Meteorological Institute, De Bilt, The Netherlands</v>
       </c>
-      <c r="X4" s="150" t="str">
+      <c r="W4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!W9),"",AllEntries!W9)</f>
         <v>Royal Netherlands Meteorological Institute, De Bilt, The Netherlands</v>
       </c>
-      <c r="Y4" s="152" t="str">
+      <c r="X4" s="152" t="str">
         <f>IF(ISBLANK(AllEntries!X9),"",AllEntries!X9)</f>
         <v>Universite du Quebec a Montreal</v>
       </c>
-      <c r="Z4" s="150" t="str">
+      <c r="Y4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!Y9),"",AllEntries!Y9)</f>
         <v>University of Castilla-La Mancha, Toledo, Spain</v>
       </c>
-      <c r="AA4" s="150" t="str">
+      <c r="Z4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!Z9),"",AllEntries!Z9)</f>
         <v xml:space="preserve"> Abdus Salam International Centre for Theoretical Physics</v>
       </c>
-      <c r="AB4" s="152" t="str">
+      <c r="AA4" s="152" t="str">
         <f>IF(ISBLANK(AllEntries!AA9),"",AllEntries!AA9)</f>
         <v>Italian National Agency for New Technologies, Energy and Sustainable Economic Development</v>
       </c>
-      <c r="AC4" s="150" t="str">
+      <c r="AB4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AB9),"",AllEntries!AB9)</f>
         <v/>
       </c>
-      <c r="AD4" s="150" t="str">
+      <c r="AC4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AC9),"",AllEntries!AC9)</f>
         <v>Meteorological and Hydrological Service of Croatia</v>
       </c>
-      <c r="AE4" s="150" t="str">
+      <c r="AD4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AD9),"",AllEntries!AD9)</f>
         <v>Indian Institute of Tropical Meteorology</v>
       </c>
-      <c r="AF4" s="150" t="str">
+      <c r="AE4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AE9),"",AllEntries!AE9)</f>
         <v/>
       </c>
-      <c r="AG4" s="150" t="str">
+      <c r="AF4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AF9),"",AllEntries!AF9)</f>
         <v>CCCma (Canadian Centre for Climate Modelling and Analysis, Victoria, BC, Canada)</v>
       </c>
-      <c r="AH4" s="150" t="str">
+      <c r="AG4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AG9),"",AllEntries!AG9)</f>
         <v>Commonwealth Scientific and Industrial Research Organisation</v>
       </c>
-      <c r="AI4" s="150" t="str">
+      <c r="AH4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AH9),"",AllEntries!AH9)</f>
         <v/>
       </c>
-      <c r="AJ4" s="150" t="str">
+      <c r="AI4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AI9),"",AllEntries!AI9)</f>
         <v>Met Office Hadley Centre</v>
       </c>
-      <c r="AK4" s="150" t="str">
+      <c r="AJ4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AJ9),"",AllEntries!AJ9)</f>
         <v>Met Office Hadley Centre</v>
       </c>
-      <c r="AL4" s="150" t="str">
+      <c r="AK4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AK9),"",AllEntries!AK9)</f>
         <v/>
       </c>
-      <c r="AM4" s="150" t="str">
+      <c r="AL4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AL9),"",AllEntries!AL9)</f>
         <v>Bjerknes Centre for Climate Research</v>
       </c>
-      <c r="AN4" s="150" t="str">
+      <c r="AM4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AM9),"",AllEntries!AM9)</f>
         <v/>
       </c>
-      <c r="AO4" s="150" t="str">
+      <c r="AN4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AN9),"",AllEntries!AN9)</f>
         <v/>
       </c>
-      <c r="AP4" s="150" t="str">
+      <c r="AO4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AO9),"",AllEntries!AO9)</f>
         <v/>
       </c>
-      <c r="AQ4" s="150" t="str">
+      <c r="AP4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AP9),"",AllEntries!AP9)</f>
         <v/>
       </c>
-      <c r="AR4" s="150" t="str">
+      <c r="AQ4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AQ9),"",AllEntries!AQ9)</f>
         <v/>
       </c>
-      <c r="AS4" s="150" t="str">
+      <c r="AR4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AR9),"",AllEntries!AR9)</f>
         <v>National University of Ireland Maynooth</v>
       </c>
-      <c r="AT4" s="150" t="str">
+      <c r="AS4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AS9),"",AllEntries!AS9)</f>
         <v/>
       </c>
-      <c r="AU4" s="150" t="str">
+      <c r="AT4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AT9),"",AllEntries!AT9)</f>
         <v/>
       </c>
-      <c r="AV4" s="150" t="str">
+      <c r="AU4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AU9),"",AllEntries!AU9)</f>
         <v/>
       </c>
-      <c r="AW4" s="163" t="str">
+      <c r="AV4" s="163" t="str">
         <f>IF(ISBLANK(AllEntries!AV9),"",AllEntries!AV9)</f>
         <v/>
       </c>
-      <c r="AX4" s="199"/>
+      <c r="AW4" s="207"/>
+      <c r="AX4" s="2"/>
       <c r="AY4" s="2"/>
       <c r="AZ4" s="2"/>
       <c r="BA4" s="2"/>
@@ -11173,9 +11126,8 @@
       <c r="BU4" s="2"/>
       <c r="BV4" s="2"/>
       <c r="BW4" s="2"/>
-      <c r="BX4" s="2"/>
     </row>
-    <row r="5" spans="1:76" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:75" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="155" t="s">
         <v>86</v>
       </c>
@@ -11239,136 +11191,136 @@
         <f>AllEntries!P8</f>
         <v>RCA4</v>
       </c>
-      <c r="Q5" s="140"/>
-      <c r="R5" s="65" t="str">
+      <c r="Q5" s="65" t="str">
         <f>AllEntries!Q8</f>
         <v>ALADIN52</v>
       </c>
-      <c r="S5" s="65" t="str">
+      <c r="R5" s="65" t="str">
         <f>AllEntries!R8</f>
         <v>ALADIN52</v>
       </c>
-      <c r="T5" s="65" t="str">
+      <c r="S5" s="65" t="str">
         <f>AllEntries!S8</f>
         <v>ALADIN52</v>
       </c>
-      <c r="U5" s="65" t="str">
+      <c r="T5" s="65" t="str">
         <f>AllEntries!T8</f>
         <v>ARPEGE52</v>
       </c>
-      <c r="V5" s="111" t="str">
+      <c r="U5" s="111" t="str">
         <f>AllEntries!U8</f>
         <v>RACMO22E</v>
       </c>
-      <c r="W5" s="111" t="str">
+      <c r="V5" s="111" t="str">
         <f>AllEntries!V8</f>
         <v>RACMO21P</v>
       </c>
-      <c r="X5" s="126" t="str">
+      <c r="W5" s="126" t="str">
         <f>AllEntries!W8</f>
         <v>RACMO22T</v>
       </c>
-      <c r="Y5" s="140" t="str">
+      <c r="X5" s="140" t="str">
         <f>AllEntries!X8</f>
         <v>CRCM5</v>
       </c>
-      <c r="Z5" s="65" t="str">
+      <c r="Y5" s="65" t="str">
         <f>AllEntries!Y8</f>
         <v>PROMES</v>
       </c>
-      <c r="AA5" s="65" t="str">
+      <c r="Z5" s="65" t="str">
         <f>AllEntries!Z8</f>
         <v>RegCM4-3</v>
       </c>
-      <c r="AB5" s="140" t="str">
+      <c r="AA5" s="140" t="str">
         <f>AllEntries!AA8</f>
         <v>RegCM4-3</v>
       </c>
-      <c r="AC5" s="65" t="str">
+      <c r="AB5" s="65" t="str">
         <f>AllEntries!AB8</f>
         <v>RegCM4-2</v>
       </c>
-      <c r="AD5" s="65" t="str">
+      <c r="AC5" s="65" t="str">
         <f>AllEntries!AC8</f>
         <v>RegCM4-2</v>
       </c>
-      <c r="AE5" s="65" t="str">
+      <c r="AD5" s="65" t="str">
         <f>AllEntries!AD8</f>
         <v>RegCM4-1</v>
       </c>
-      <c r="AF5" s="140" t="str">
+      <c r="AE5" s="140" t="str">
         <f>AllEntries!AE8</f>
         <v>RM3</v>
       </c>
-      <c r="AG5" s="140" t="str">
+      <c r="AF5" s="140" t="str">
         <f>AllEntries!AF8</f>
         <v>CanRCM4</v>
       </c>
-      <c r="AH5" s="65" t="str">
+      <c r="AG5" s="65" t="str">
         <f>AllEntries!AG8</f>
         <v>CCAM</v>
       </c>
-      <c r="AI5" s="140" t="str">
+      <c r="AH5" s="140" t="str">
         <f>AllEntries!AH8</f>
         <v>GFDL</v>
       </c>
-      <c r="AJ5" s="65" t="str">
+      <c r="AI5" s="65" t="str">
         <f>AllEntries!AI8</f>
         <v>HadGEM3-RA</v>
       </c>
-      <c r="AK5" s="65" t="str">
+      <c r="AJ5" s="65" t="str">
         <f>AllEntries!AJ8</f>
         <v>HadRM3P</v>
       </c>
-      <c r="AL5" s="65" t="str">
+      <c r="AK5" s="65" t="str">
         <f>AllEntries!AK8</f>
         <v>WRF331A</v>
       </c>
-      <c r="AM5" s="126" t="str">
+      <c r="AL5" s="126" t="str">
         <f>AllEntries!AL8</f>
         <v>WRF331C</v>
       </c>
-      <c r="AN5" s="65" t="str">
+      <c r="AM5" s="65" t="str">
         <f>AllEntries!AM8</f>
         <v>WRF331A</v>
       </c>
-      <c r="AO5" s="65" t="str">
+      <c r="AN5" s="65" t="str">
         <f>AllEntries!AN8</f>
         <v>WRF331D</v>
       </c>
-      <c r="AP5" s="65" t="str">
+      <c r="AO5" s="65" t="str">
         <f>AllEntries!AO8</f>
         <v>WRF331F</v>
       </c>
-      <c r="AQ5" s="65" t="str">
+      <c r="AP5" s="65" t="str">
         <f>AllEntries!AP8</f>
         <v>WRF331A</v>
       </c>
-      <c r="AR5" s="65" t="str">
+      <c r="AQ5" s="65" t="str">
         <f>AllEntries!AQ8</f>
         <v>WRF321B</v>
       </c>
-      <c r="AS5" s="65" t="str">
+      <c r="AR5" s="65" t="str">
         <f>AllEntries!AR8</f>
         <v>WRF341E</v>
       </c>
-      <c r="AT5" s="65" t="str">
+      <c r="AS5" s="65" t="str">
         <f>AllEntries!AS8</f>
         <v>WRF331H</v>
       </c>
-      <c r="AU5" s="65" t="str">
+      <c r="AT5" s="65" t="str">
         <f>AllEntries!AT8</f>
         <v>WRF331</v>
       </c>
-      <c r="AV5" s="65" t="str">
+      <c r="AU5" s="65" t="str">
         <f>AllEntries!AU8</f>
         <v>WRF331G</v>
       </c>
-      <c r="AW5" s="164" t="str">
+      <c r="AV5" s="164" t="str">
         <f>AllEntries!AV8</f>
         <v>WRF350I</v>
       </c>
-      <c r="AX5" s="199"/>
+      <c r="AW5" s="207"/>
+      <c r="AX5" s="2"/>
       <c r="AY5" s="2"/>
       <c r="AZ5" s="2"/>
       <c r="BA5" s="2"/>
@@ -11394,9 +11346,8 @@
       <c r="BU5" s="2"/>
       <c r="BV5" s="2"/>
       <c r="BW5" s="2"/>
-      <c r="BX5" s="2"/>
     </row>
-    <row r="6" spans="1:76" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:75" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="76" t="s">
         <v>87</v>
       </c>
@@ -11410,7 +11361,7 @@
       </c>
       <c r="D6" s="65" t="str">
         <f t="shared" ref="D6" si="1">IF(ISBLANK(D9),"",CONCATENATE(D3,"-",D5))</f>
-        <v>CLMcom -CCLM4-8-17</v>
+        <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="E6" s="65" t="str">
         <f t="shared" ref="E6" si="2">IF(ISBLANK(E9),"",CONCATENATE(E3,"-",E5))</f>
@@ -11460,139 +11411,136 @@
         <f t="shared" ref="P6" si="13">IF(ISBLANK(P9),"",CONCATENATE(P3,"-",P5))</f>
         <v>SMHI-RCA4</v>
       </c>
-      <c r="Q6" s="140" t="str">
+      <c r="Q6" s="65" t="str">
         <f t="shared" ref="Q6" si="14">IF(ISBLANK(Q9),"",CONCATENATE(Q3,"-",Q5))</f>
-        <v/>
+        <v>CHMI-ALADIN52</v>
       </c>
       <c r="R6" s="65" t="str">
         <f t="shared" ref="R6" si="15">IF(ISBLANK(R9),"",CONCATENATE(R3,"-",R5))</f>
-        <v>CHMI-ALADIN52</v>
+        <v>HMS-ALADIN52</v>
       </c>
       <c r="S6" s="65" t="str">
         <f t="shared" ref="S6" si="16">IF(ISBLANK(S9),"",CONCATENATE(S3,"-",S5))</f>
-        <v>HMS-ALADIN52</v>
+        <v>CNRM-ALADIN52</v>
       </c>
       <c r="T6" s="65" t="str">
         <f t="shared" ref="T6" si="17">IF(ISBLANK(T9),"",CONCATENATE(T3,"-",T5))</f>
-        <v>CNRM-ALADIN52</v>
+        <v>CNRM-ARPEGE52</v>
       </c>
       <c r="U6" s="65" t="str">
         <f t="shared" ref="U6" si="18">IF(ISBLANK(U9),"",CONCATENATE(U3,"-",U5))</f>
-        <v>CNRM-ARPEGE52</v>
+        <v>KNMI-RACMO22E</v>
       </c>
       <c r="V6" s="65" t="str">
         <f t="shared" ref="V6" si="19">IF(ISBLANK(V9),"",CONCATENATE(V3,"-",V5))</f>
-        <v>KNMI-RACMO22E</v>
+        <v>KNMI-RACMO21P</v>
       </c>
       <c r="W6" s="65" t="str">
         <f t="shared" ref="W6" si="20">IF(ISBLANK(W9),"",CONCATENATE(W3,"-",W5))</f>
-        <v>KNMI-RACMO21P</v>
-      </c>
-      <c r="X6" s="65" t="str">
+        <v>KNMI-RACMO22T</v>
+      </c>
+      <c r="X6" s="140" t="str">
         <f t="shared" ref="X6" si="21">IF(ISBLANK(X9),"",CONCATENATE(X3,"-",X5))</f>
-        <v>KNMI-RACMO22T</v>
-      </c>
-      <c r="Y6" s="140" t="str">
+        <v/>
+      </c>
+      <c r="Y6" s="65" t="str">
         <f t="shared" ref="Y6" si="22">IF(ISBLANK(Y9),"",CONCATENATE(Y3,"-",Y5))</f>
+        <v>UCLM-PROMES</v>
+      </c>
+      <c r="Z6" s="65" t="str">
+        <f t="shared" ref="Z6:AA6" si="23">IF(ISBLANK(Z9),"",CONCATENATE(Z3,"-",Z5))</f>
+        <v>ICTP-RegCM4-3</v>
+      </c>
+      <c r="AA6" s="140" t="str">
+        <f t="shared" si="23"/>
         <v/>
       </c>
-      <c r="Z6" s="65" t="str">
-        <f t="shared" ref="Z6" si="23">IF(ISBLANK(Z9),"",CONCATENATE(Z3,"-",Z5))</f>
-        <v>UCLM-PROMES</v>
-      </c>
-      <c r="AA6" s="65" t="str">
-        <f t="shared" ref="AA6:AB6" si="24">IF(ISBLANK(AA9),"",CONCATENATE(AA3,"-",AA5))</f>
-        <v>ICTP-RegCM4-3</v>
-      </c>
-      <c r="AB6" s="140" t="str">
-        <f t="shared" si="24"/>
-        <v/>
+      <c r="AB6" s="65" t="str">
+        <f t="shared" ref="AB6" si="24">IF(ISBLANK(AB9),"",CONCATENATE(AB3,"-",AB5))</f>
+        <v>CUNI-RegCM4-2</v>
       </c>
       <c r="AC6" s="65" t="str">
         <f t="shared" ref="AC6" si="25">IF(ISBLANK(AC9),"",CONCATENATE(AC3,"-",AC5))</f>
-        <v>CUNI-RegCM4-2</v>
+        <v>DHMZ-RegCM4-2</v>
       </c>
       <c r="AD6" s="65" t="str">
-        <f t="shared" ref="AD6:AF6" si="26">IF(ISBLANK(AD9),"",CONCATENATE(AD3,"-",AD5))</f>
-        <v>DHMZ-RegCM4-2</v>
-      </c>
-      <c r="AE6" s="65" t="str">
-        <f t="shared" ref="AE6" si="27">IF(ISBLANK(AE9),"",CONCATENATE(AE3,"-",AE5))</f>
+        <f t="shared" ref="AD6" si="26">IF(ISBLANK(AD9),"",CONCATENATE(AD3,"-",AD5))</f>
         <v>IITM-RegCM4-1</v>
       </c>
+      <c r="AE6" s="140" t="str">
+        <f t="shared" ref="AE6:AV6" si="27">IF(ISBLANK(AE9),"",CONCATENATE(AE3,"-",AE5))</f>
+        <v/>
+      </c>
       <c r="AF6" s="140" t="str">
-        <f>IF(ISBLANK(AF9),"",CONCATENATE(AF3,"-",AF5))</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
-      <c r="AG6" s="140" t="str">
-        <f>IF(ISBLANK(AG9),"",CONCATENATE(AG3,"-",AG5))</f>
+      <c r="AG6" s="65" t="str">
+        <f t="shared" si="27"/>
+        <v>CSIRO-CCAM</v>
+      </c>
+      <c r="AH6" s="140" t="str">
+        <f t="shared" si="27"/>
         <v/>
       </c>
-      <c r="AH6" s="65" t="str">
-        <f>IF(ISBLANK(AH9),"",CONCATENATE(AH3,"-",AH5))</f>
-        <v>CSIRO-CCAM</v>
-      </c>
-      <c r="AI6" s="140" t="str">
-        <f>IF(ISBLANK(AI9),"",CONCATENATE(AI3,"-",AI5))</f>
-        <v/>
+      <c r="AI6" s="65" t="str">
+        <f t="shared" si="27"/>
+        <v>MOHC-HadGEM3-RA</v>
       </c>
       <c r="AJ6" s="65" t="str">
-        <f>IF(ISBLANK(AJ9),"",CONCATENATE(AJ3,"-",AJ5))</f>
-        <v>MOHC-HadGEM3-RA</v>
+        <f t="shared" si="27"/>
+        <v>MOHC-HadRM3P</v>
       </c>
       <c r="AK6" s="65" t="str">
-        <f>IF(ISBLANK(AK9),"",CONCATENATE(AK3,"-",AK5))</f>
-        <v>MOHC-HadRM3P</v>
+        <f t="shared" si="27"/>
+        <v>MIUB-WRF331A</v>
       </c>
       <c r="AL6" s="65" t="str">
-        <f>IF(ISBLANK(AL9),"",CONCATENATE(AL3,"-",AL5))</f>
-        <v>MIUB-WRF331A</v>
+        <f t="shared" si="27"/>
+        <v>BCCR-WRF331C</v>
       </c>
       <c r="AM6" s="65" t="str">
-        <f>IF(ISBLANK(AM9),"",CONCATENATE(AM3,"-",AM5))</f>
-        <v>BCCR-WRF331C</v>
+        <f t="shared" si="27"/>
+        <v>CRP-GL-WRF331A</v>
       </c>
       <c r="AN6" s="65" t="str">
-        <f>IF(ISBLANK(AN9),"",CONCATENATE(AN3,"-",AN5))</f>
-        <v>CRP-GL-WRF331A</v>
+        <f t="shared" si="27"/>
+        <v>IDL-WRF331D</v>
       </c>
       <c r="AO6" s="65" t="str">
-        <f>IF(ISBLANK(AO9),"",CONCATENATE(AO3,"-",AO5))</f>
-        <v>IDL-WRF331D</v>
+        <f t="shared" si="27"/>
+        <v>IPSL-INERIS-WRF331F</v>
       </c>
       <c r="AP6" s="65" t="str">
-        <f>IF(ISBLANK(AP9),"",CONCATENATE(AP3,"-",AP5))</f>
-        <v>IPSL-INERIS-WRF331F</v>
+        <f t="shared" si="27"/>
+        <v>AUTH-Met-WRF331A</v>
       </c>
       <c r="AQ6" s="65" t="str">
-        <f>IF(ISBLANK(AQ9),"",CONCATENATE(AQ3,"-",AQ5))</f>
-        <v>AUTH-Met-WRF331A</v>
+        <f t="shared" si="27"/>
+        <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="AR6" s="65" t="str">
-        <f>IF(ISBLANK(AR9),"",CONCATENATE(AR3,"-",AR5))</f>
-        <v>AUTH-LHTEE-WRF321B</v>
+        <f t="shared" si="27"/>
+        <v>NUIM-WRF341E</v>
       </c>
       <c r="AS6" s="65" t="str">
-        <f>IF(ISBLANK(AS9),"",CONCATENATE(AS3,"-",AS5))</f>
-        <v>NUIM-WRF341E</v>
+        <f t="shared" si="27"/>
+        <v>UHOH-WRF331H</v>
       </c>
       <c r="AT6" s="65" t="str">
-        <f>IF(ISBLANK(AT9),"",CONCATENATE(AT3,"-",AT5))</f>
-        <v>UHOH-WRF331H</v>
+        <f t="shared" si="27"/>
+        <v>UM-WRF331</v>
       </c>
       <c r="AU6" s="65" t="str">
-        <f>IF(ISBLANK(AU9),"",CONCATENATE(AU3,"-",AU5))</f>
-        <v>UM-WRF331</v>
-      </c>
-      <c r="AV6" s="65" t="str">
-        <f>IF(ISBLANK(AV9),"",CONCATENATE(AV3,"-",AV5))</f>
+        <f t="shared" si="27"/>
         <v>UCAN-WRF331G</v>
       </c>
-      <c r="AW6" s="164" t="str">
-        <f>IF(ISBLANK(AW9),"",CONCATENATE(AW3,"-",AW5))</f>
+      <c r="AV6" s="164" t="str">
+        <f t="shared" si="27"/>
         <v>UCAN-WRF350I</v>
       </c>
-      <c r="AX6" s="105"/>
+      <c r="AW6" s="105"/>
+      <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
       <c r="AZ6" s="2"/>
       <c r="BA6" s="2"/>
@@ -11618,9 +11566,8 @@
       <c r="BU6" s="2"/>
       <c r="BV6" s="2"/>
       <c r="BW6" s="2"/>
-      <c r="BX6" s="2"/>
     </row>
-    <row r="7" spans="1:76" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:75" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="153" t="s">
         <v>151</v>
       </c>
@@ -11684,136 +11631,136 @@
         <f>IF(ISBLANK(AllEntries!P11),"",AllEntries!P11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="Q7" s="137"/>
-      <c r="R7" s="137" t="str">
+      <c r="Q7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!Q11),"unknown",AllEntries!Q11)</f>
         <v>unknown</v>
       </c>
-      <c r="S7" s="137" t="str">
+      <c r="R7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!R11),"unknown",AllEntries!R11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="T7" s="137" t="str">
+      <c r="S7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!S11),"unknown",AllEntries!S11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="U7" s="137" t="str">
+      <c r="T7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!T11),"unknown",AllEntries!T11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="V7" s="137" t="str">
+      <c r="U7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!U11),"unknown",AllEntries!U11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="W7" s="137" t="str">
+      <c r="V7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!V11),"unknown",AllEntries!V11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="X7" s="137" t="str">
+      <c r="W7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!W11),"unknown",AllEntries!W11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="Y7" s="137" t="str">
+      <c r="X7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!X11),"unknown",AllEntries!X11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="Z7" s="137" t="str">
+      <c r="Y7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!Y11),"unknown",AllEntries!Y11)</f>
         <v>unknown</v>
       </c>
-      <c r="AA7" s="137" t="str">
+      <c r="Z7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!Z11),"unknown",AllEntries!Z11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AB7" s="137" t="str">
+      <c r="AA7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AA11),"unknown",AllEntries!AA11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AC7" s="137" t="str">
+      <c r="AB7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AB11),"unknown",AllEntries!AB11)</f>
         <v>unknown</v>
       </c>
-      <c r="AD7" s="137" t="str">
+      <c r="AC7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AC11),"unknown",AllEntries!AC11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AE7" s="137" t="str">
+      <c r="AD7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AD11),"unknown",AllEntries!AD11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AF7" s="137" t="str">
+      <c r="AE7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AE11),"unknown",AllEntries!AE11)</f>
         <v>unknown</v>
       </c>
-      <c r="AG7" s="137" t="str">
+      <c r="AF7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AF11),"unknown",AllEntries!AF11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AH7" s="137" t="str">
+      <c r="AG7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AG11),"unknown",AllEntries!AG11)</f>
         <v>unknown</v>
       </c>
-      <c r="AI7" s="137" t="str">
+      <c r="AH7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AH11),"unknown",AllEntries!AH11)</f>
         <v>unknown</v>
       </c>
-      <c r="AJ7" s="137" t="str">
+      <c r="AI7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AI11),"unknown",AllEntries!AI11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AK7" s="137" t="str">
+      <c r="AJ7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AJ11),"unknown",AllEntries!AJ11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AL7" s="137" t="str">
+      <c r="AK7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AK11),"unknown",AllEntries!AK11)</f>
         <v>unknown</v>
       </c>
-      <c r="AM7" s="137" t="str">
+      <c r="AL7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AL11),"unknown",AllEntries!AL11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AN7" s="137" t="str">
+      <c r="AM7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AM11),"unknown",AllEntries!AM11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AO7" s="137" t="str">
+      <c r="AN7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AN11),"unknown",AllEntries!AN11)</f>
         <v>unknown</v>
       </c>
-      <c r="AP7" s="137" t="str">
+      <c r="AO7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AO11),"unknown",AllEntries!AO11)</f>
         <v>unknown</v>
       </c>
-      <c r="AQ7" s="137" t="str">
+      <c r="AP7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AP11),"unknown",AllEntries!AP11)</f>
         <v>unknown</v>
       </c>
-      <c r="AR7" s="137" t="str">
+      <c r="AQ7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AQ11),"unknown",AllEntries!AQ11)</f>
         <v>unknown</v>
       </c>
-      <c r="AS7" s="137" t="str">
+      <c r="AR7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AR11),"unknown",AllEntries!AR11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AT7" s="137" t="str">
+      <c r="AS7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AS11),"unknown",AllEntries!AS11)</f>
         <v>unknown</v>
       </c>
-      <c r="AU7" s="137" t="str">
+      <c r="AT7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AT11),"unknown",AllEntries!AT11)</f>
         <v>unknown</v>
       </c>
-      <c r="AV7" s="137" t="str">
+      <c r="AU7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AU11),"unknown",AllEntries!AU11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AW7" s="165" t="str">
+      <c r="AV7" s="165" t="str">
         <f>IF(ISBLANK(AllEntries!AV11),"unknown",AllEntries!AV11)</f>
         <v>unknown</v>
       </c>
-      <c r="AX7" s="128"/>
+      <c r="AW7" s="128"/>
+      <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
@@ -11839,9 +11786,8 @@
       <c r="BU7" s="2"/>
       <c r="BV7" s="2"/>
       <c r="BW7" s="2"/>
-      <c r="BX7" s="2"/>
     </row>
-    <row r="8" spans="1:76" s="36" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" s="36" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="154" t="s">
         <v>187</v>
       </c>
@@ -11911,17 +11857,17 @@
       <c r="W8" s="142" t="s">
         <v>186</v>
       </c>
-      <c r="X8" s="142" t="s">
+      <c r="X8" s="142"/>
+      <c r="Y8" s="142" t="s">
         <v>186</v>
       </c>
-      <c r="Y8" s="142"/>
       <c r="Z8" s="142" t="s">
         <v>186</v>
       </c>
-      <c r="AA8" s="142" t="s">
+      <c r="AA8" s="142"/>
+      <c r="AB8" s="142" t="s">
         <v>186</v>
       </c>
-      <c r="AB8" s="142"/>
       <c r="AC8" s="142" t="s">
         <v>186</v>
       </c>
@@ -11979,13 +11925,11 @@
       <c r="AU8" s="142" t="s">
         <v>186</v>
       </c>
-      <c r="AV8" s="142" t="s">
+      <c r="AV8" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="AW8" s="166" t="s">
-        <v>186</v>
-      </c>
-      <c r="AX8" s="145"/>
+      <c r="AW8" s="145"/>
+      <c r="AX8" s="146"/>
       <c r="AY8" s="146"/>
       <c r="AZ8" s="146"/>
       <c r="BA8" s="146"/>
@@ -12011,9 +11955,8 @@
       <c r="BU8" s="146"/>
       <c r="BV8" s="146"/>
       <c r="BW8" s="146"/>
-      <c r="BX8" s="146"/>
     </row>
-    <row r="9" spans="1:76" s="36" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:75" s="36" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="154" t="s">
         <v>96</v>
       </c>
@@ -12062,56 +12005,58 @@
       <c r="P9" s="142" t="s">
         <v>155</v>
       </c>
-      <c r="Q9" s="143"/>
-      <c r="R9" s="143" t="s">
+      <c r="Q9" s="143" t="s">
         <v>132</v>
       </c>
-      <c r="S9" s="142" t="s">
+      <c r="R9" s="142" t="s">
         <v>156</v>
+      </c>
+      <c r="S9" s="143" t="s">
+        <v>131</v>
       </c>
       <c r="T9" s="143" t="s">
         <v>131</v>
       </c>
       <c r="U9" s="143" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="V9" s="143" t="s">
         <v>118</v>
       </c>
-      <c r="W9" s="143" t="s">
-        <v>118</v>
-      </c>
-      <c r="X9" s="144" t="s">
+      <c r="W9" s="144" t="s">
         <v>119</v>
       </c>
-      <c r="Y9" s="142"/>
+      <c r="X9" s="142"/>
+      <c r="Y9" s="142" t="s">
+        <v>162</v>
+      </c>
       <c r="Z9" s="142" t="s">
-        <v>162</v>
-      </c>
-      <c r="AA9" s="142" t="s">
         <v>157</v>
       </c>
-      <c r="AB9" s="142"/>
+      <c r="AA9" s="142"/>
+      <c r="AB9" s="142" t="s">
+        <v>157</v>
+      </c>
       <c r="AC9" s="142" t="s">
         <v>157</v>
       </c>
       <c r="AD9" s="142" t="s">
-        <v>157</v>
-      </c>
-      <c r="AE9" s="142" t="s">
         <v>225</v>
       </c>
+      <c r="AE9" s="142"/>
       <c r="AF9" s="142"/>
-      <c r="AG9" s="142"/>
-      <c r="AH9" s="221" t="s">
+      <c r="AG9" s="198" t="s">
         <v>229</v>
       </c>
-      <c r="AI9" s="142"/>
+      <c r="AH9" s="142"/>
+      <c r="AI9" s="142" t="s">
+        <v>158</v>
+      </c>
       <c r="AJ9" s="142" t="s">
         <v>158</v>
       </c>
       <c r="AK9" s="142" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AL9" s="142" t="s">
         <v>159</v>
@@ -12123,19 +12068,19 @@
         <v>159</v>
       </c>
       <c r="AO9" s="142" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP9" s="142" t="s">
         <v>159</v>
-      </c>
-      <c r="AP9" s="142" t="s">
-        <v>166</v>
       </c>
       <c r="AQ9" s="142" t="s">
         <v>159</v>
       </c>
       <c r="AR9" s="142" t="s">
+        <v>224</v>
+      </c>
+      <c r="AS9" s="142" t="s">
         <v>159</v>
-      </c>
-      <c r="AS9" s="142" t="s">
-        <v>224</v>
       </c>
       <c r="AT9" s="142" t="s">
         <v>159</v>
@@ -12143,13 +12088,11 @@
       <c r="AU9" s="142" t="s">
         <v>159</v>
       </c>
-      <c r="AV9" s="142" t="s">
+      <c r="AV9" s="166" t="s">
         <v>159</v>
       </c>
-      <c r="AW9" s="166" t="s">
-        <v>159</v>
-      </c>
-      <c r="AX9" s="145"/>
+      <c r="AW9" s="145"/>
+      <c r="AX9" s="146"/>
       <c r="AY9" s="146"/>
       <c r="AZ9" s="146"/>
       <c r="BA9" s="146"/>
@@ -12175,10 +12118,9 @@
       <c r="BU9" s="146"/>
       <c r="BV9" s="146"/>
       <c r="BW9" s="146"/>
-      <c r="BX9" s="146"/>
     </row>
-    <row r="10" spans="1:76" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:75" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A11" s="63"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
@@ -12186,19 +12128,18 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="AX3:AX5"/>
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="AW3:AW5"/>
+    <mergeCell ref="A1:R1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J2:O2"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="46" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <colBreaks count="2" manualBreakCount="2">
+  <pageSetup paperSize="9" scale="46" fitToHeight="0" orientation="landscape" verticalDpi="4" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
     <brk id="16" max="9" man="1"/>
-    <brk id="17" max="9" man="1"/>
   </colBreaks>
   <ignoredErrors>
-    <ignoredError sqref="AP6" formula="1"/>
+    <ignoredError sqref="AO6" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added ALADIN53 / CNRM / Clothilde D.
</commit_message>
<xml_diff>
--- a/CORDEX_ESGF_coordination_issues.xlsx
+++ b/CORDEX_ESGF_coordination_issues.xlsx
@@ -35,8 +35,8 @@
     <definedName name="ANT44tier1">DatVol!$C$36</definedName>
     <definedName name="ARC_44">DatVol!$B$37</definedName>
     <definedName name="ARC44tier1">DatVol!$C$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$AW$13</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AW$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$AX$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AX$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">DatVol!$A$1:$BA$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$4</definedName>
     <definedName name="EUR_11" localSheetId="3">ControlledVocabulary!#REF!</definedName>
@@ -55,8 +55,8 @@
     <definedName name="MED44tier1" localSheetId="2">DatVol!$C$32</definedName>
     <definedName name="MED44tier1" localSheetId="0">GeneralRemarks!#REF!</definedName>
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
-    <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AW$9</definedName>
-    <definedName name="Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AT$5</definedName>
+    <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AX$9</definedName>
+    <definedName name="Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$AU$5</definedName>
     <definedName name="Print_Area" localSheetId="2">DatVol!$A$1:$AZ$39</definedName>
     <definedName name="Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$2</definedName>
   </definedNames>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="235">
   <si>
     <t>Domain</t>
   </si>
@@ -1250,6 +1250,23 @@
     <t>confirmed by 
 Jack Katzfey</t>
   </si>
+  <si>
+    <t>King Abdullah University, Thuwal, Saudi Arabien</t>
+  </si>
+  <si>
+    <t>ALADIN53</t>
+  </si>
+  <si>
+    <t>clotilde.dubois
+@meteo.fr</t>
+  </si>
+  <si>
+    <t>confirmed by 
+Clothilde D.</t>
+  </si>
+  <si>
+    <t>EUR-??</t>
+  </si>
 </sst>
 </file>
 
@@ -1259,7 +1276,7 @@
     <numFmt numFmtId="164" formatCode="[$-407]d/\ mmm\ yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1514,6 +1531,13 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2542,7 +2566,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3015,6 +3039,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3570,7 +3600,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3580,27 +3610,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="201" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
-      <c r="L1" s="199"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
       <c r="M1" s="21"/>
       <c r="N1" s="20"/>
       <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="54">
-        <v>41901</v>
+        <v>41954</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -3618,12 +3648,12 @@
       <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" s="148" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="202" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
       <c r="E3" s="147"/>
       <c r="F3" s="147"/>
       <c r="G3" s="147"/>
@@ -3659,10 +3689,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BZ38"/>
+  <dimension ref="A1:CA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="Q2" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3680,44 +3710,44 @@
     <col min="12" max="16" width="13.77734375" customWidth="1"/>
     <col min="17" max="17" width="16.77734375" customWidth="1"/>
     <col min="18" max="18" width="18.77734375" customWidth="1"/>
-    <col min="19" max="19" width="13.77734375" customWidth="1"/>
-    <col min="20" max="20" width="12.77734375" customWidth="1"/>
-    <col min="21" max="22" width="13.77734375" customWidth="1"/>
-    <col min="23" max="23" width="15.5546875" customWidth="1"/>
-    <col min="24" max="24" width="13.109375" customWidth="1"/>
-    <col min="25" max="25" width="13.88671875" customWidth="1"/>
-    <col min="26" max="26" width="14.44140625" customWidth="1"/>
-    <col min="27" max="27" width="20" customWidth="1"/>
-    <col min="28" max="28" width="13.88671875" customWidth="1"/>
-    <col min="29" max="29" width="13.109375" customWidth="1"/>
-    <col min="30" max="30" width="13.77734375" customWidth="1"/>
-    <col min="31" max="31" width="12.5546875" customWidth="1"/>
-    <col min="32" max="32" width="13.109375" customWidth="1"/>
-    <col min="33" max="33" width="12" customWidth="1"/>
-    <col min="34" max="36" width="16.6640625" customWidth="1"/>
-    <col min="37" max="48" width="13.77734375" customWidth="1"/>
-    <col min="49" max="49" width="22.44140625" customWidth="1"/>
+    <col min="19" max="20" width="13.77734375" customWidth="1"/>
+    <col min="21" max="21" width="12.77734375" customWidth="1"/>
+    <col min="22" max="23" width="13.77734375" customWidth="1"/>
+    <col min="24" max="24" width="15.5546875" customWidth="1"/>
+    <col min="25" max="25" width="13.109375" customWidth="1"/>
+    <col min="26" max="26" width="13.88671875" customWidth="1"/>
+    <col min="27" max="27" width="14.44140625" customWidth="1"/>
+    <col min="28" max="28" width="20" customWidth="1"/>
+    <col min="29" max="29" width="13.88671875" customWidth="1"/>
+    <col min="30" max="30" width="13.109375" customWidth="1"/>
+    <col min="31" max="31" width="13.77734375" customWidth="1"/>
+    <col min="32" max="32" width="12.5546875" customWidth="1"/>
+    <col min="33" max="33" width="13.109375" customWidth="1"/>
+    <col min="34" max="34" width="12" customWidth="1"/>
+    <col min="35" max="37" width="16.6640625" customWidth="1"/>
+    <col min="38" max="49" width="13.77734375" customWidth="1"/>
+    <col min="50" max="50" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="201" t="s">
+    <row r="1" spans="1:79" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="203" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
-      <c r="L1" s="199"/>
-      <c r="M1" s="199"/>
-      <c r="N1" s="199"/>
-      <c r="O1" s="199"/>
-      <c r="P1" s="199"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
+      <c r="N1" s="201"/>
+      <c r="O1" s="201"/>
+      <c r="P1" s="201"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="20"/>
       <c r="S1" s="20"/>
@@ -3750,7 +3780,7 @@
       <c r="AT1" s="20"/>
       <c r="AU1" s="20"/>
       <c r="AV1" s="20"/>
-      <c r="BR1" s="26"/>
+      <c r="AW1" s="20"/>
       <c r="BS1" s="26"/>
       <c r="BT1" s="26"/>
       <c r="BU1" s="26"/>
@@ -3759,19 +3789,20 @@
       <c r="BX1" s="26"/>
       <c r="BY1" s="26"/>
       <c r="BZ1" s="26"/>
+      <c r="CA1" s="26"/>
     </row>
-    <row r="2" spans="1:78" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:79" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="53">
         <f>GeneralRemarks!A2</f>
-        <v>41901</v>
-      </c>
-      <c r="B2" s="203"/>
-      <c r="C2" s="203"/>
-      <c r="D2" s="203"/>
-      <c r="E2" s="203"/>
-      <c r="F2" s="203"/>
-      <c r="G2" s="203"/>
-      <c r="H2" s="203"/>
+        <v>41954</v>
+      </c>
+      <c r="B2" s="205"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="205"/>
+      <c r="H2" s="205"/>
       <c r="I2" s="51"/>
       <c r="J2" s="51"/>
       <c r="K2" s="51"/>
@@ -3786,11 +3817,11 @@
       <c r="T2" s="20"/>
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
-      <c r="W2" s="54">
+      <c r="W2" s="20"/>
+      <c r="X2" s="54">
         <f>A2</f>
-        <v>41901</v>
-      </c>
-      <c r="X2" s="20"/>
+        <v>41954</v>
+      </c>
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
       <c r="AA2" s="20"/>
@@ -3815,11 +3846,11 @@
       <c r="AT2" s="20"/>
       <c r="AU2" s="20"/>
       <c r="AV2" s="20"/>
-      <c r="AW2" s="73">
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="73">
         <f>A2</f>
-        <v>41901</v>
-      </c>
-      <c r="BR2" s="26"/>
+        <v>41954</v>
+      </c>
       <c r="BS2" s="26"/>
       <c r="BT2" s="26"/>
       <c r="BU2" s="26"/>
@@ -3828,8 +3859,9 @@
       <c r="BX2" s="26"/>
       <c r="BY2" s="26"/>
       <c r="BZ2" s="26"/>
+      <c r="CA2" s="26"/>
     </row>
-    <row r="3" spans="1:78" s="1" customFormat="1" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:79" s="1" customFormat="1" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="168" t="s">
         <v>57</v>
       </c>
@@ -3887,11 +3919,11 @@
       <c r="S3" s="112" t="s">
         <v>89</v>
       </c>
-      <c r="T3" s="112" t="s">
+      <c r="T3" s="72" t="s">
+        <v>232</v>
+      </c>
+      <c r="U3" s="112" t="s">
         <v>129</v>
-      </c>
-      <c r="U3" s="112" t="s">
-        <v>117</v>
       </c>
       <c r="V3" s="112" t="s">
         <v>117</v>
@@ -3900,58 +3932,60 @@
         <v>117</v>
       </c>
       <c r="X3" s="112" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y3" s="112" t="s">
         <v>180</v>
       </c>
-      <c r="Y3" s="112" t="s">
+      <c r="Z3" s="112" t="s">
         <v>219</v>
       </c>
-      <c r="Z3" s="112" t="s">
+      <c r="AA3" s="112" t="s">
         <v>203</v>
       </c>
-      <c r="AA3" s="112" t="s">
+      <c r="AB3" s="112" t="s">
         <v>205</v>
       </c>
-      <c r="AB3" s="112"/>
-      <c r="AC3" s="112" t="s">
+      <c r="AC3" s="112"/>
+      <c r="AD3" s="112" t="s">
         <v>135</v>
       </c>
-      <c r="AD3" s="191" t="s">
+      <c r="AE3" s="191" t="s">
         <v>223</v>
       </c>
-      <c r="AE3" s="112"/>
-      <c r="AF3" s="167" t="s">
+      <c r="AF3" s="112"/>
+      <c r="AG3" s="167" t="s">
         <v>178</v>
       </c>
-      <c r="AG3" s="112" t="s">
+      <c r="AH3" s="112" t="s">
         <v>228</v>
       </c>
-      <c r="AH3" s="112"/>
-      <c r="AI3" s="113" t="s">
-        <v>98</v>
-      </c>
+      <c r="AI3" s="112"/>
       <c r="AJ3" s="113" t="s">
         <v>98</v>
       </c>
-      <c r="AK3" s="112"/>
+      <c r="AK3" s="113" t="s">
+        <v>98</v>
+      </c>
       <c r="AL3" s="112"/>
       <c r="AM3" s="112"/>
       <c r="AN3" s="112"/>
-      <c r="AO3" s="112" t="s">
+      <c r="AO3" s="112"/>
+      <c r="AP3" s="112" t="s">
         <v>218</v>
       </c>
-      <c r="AP3" s="112"/>
       <c r="AQ3" s="112"/>
-      <c r="AR3" s="191" t="s">
+      <c r="AR3" s="112"/>
+      <c r="AS3" s="191" t="s">
         <v>217</v>
       </c>
-      <c r="AS3" s="112"/>
       <c r="AT3" s="112"/>
       <c r="AU3" s="112"/>
       <c r="AV3" s="112"/>
-      <c r="AW3" s="168" t="s">
+      <c r="AW3" s="112"/>
+      <c r="AX3" s="168" t="s">
         <v>57</v>
       </c>
-      <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
@@ -3980,8 +4014,9 @@
       <c r="BX3" s="2"/>
       <c r="BY3" s="2"/>
       <c r="BZ3" s="2"/>
+      <c r="CA3" s="2"/>
     </row>
-    <row r="4" spans="1:78" s="1" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:79" s="1" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="170" t="s">
         <v>41</v>
       </c>
@@ -4032,7 +4067,7 @@
         <v>42</v>
       </c>
       <c r="Q4" s="115" t="str">
-        <f t="shared" ref="Q4:W4" si="0">Q7</f>
+        <f t="shared" ref="Q4:X4" si="0">Q7</f>
         <v>CHMI</v>
       </c>
       <c r="R4" s="115" t="str">
@@ -4043,119 +4078,121 @@
         <f t="shared" si="0"/>
         <v>CNRM</v>
       </c>
-      <c r="T4" s="115" t="str">
+      <c r="T4" s="115" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="115" t="str">
         <f t="shared" si="0"/>
         <v>CNRM</v>
       </c>
-      <c r="U4" s="115" t="str">
-        <f t="shared" ref="U4:V4" si="1">U7</f>
+      <c r="V4" s="115" t="str">
+        <f t="shared" ref="V4:W4" si="1">V7</f>
         <v>KNMI</v>
       </c>
-      <c r="V4" s="115" t="str">
+      <c r="W4" s="115" t="str">
         <f t="shared" si="1"/>
         <v>KNMI</v>
       </c>
-      <c r="W4" s="115" t="str">
+      <c r="X4" s="115" t="str">
         <f t="shared" si="0"/>
         <v>KNMI</v>
       </c>
-      <c r="X4" s="115" t="str">
-        <f t="shared" ref="X4:AI4" si="2">X7</f>
+      <c r="Y4" s="115" t="str">
+        <f t="shared" ref="Y4:AJ4" si="2">Y7</f>
         <v>UQAM</v>
       </c>
-      <c r="Y4" s="115" t="str">
+      <c r="Z4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>UCLM</v>
       </c>
-      <c r="Z4" s="115" t="str">
+      <c r="AA4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>ICTP</v>
       </c>
-      <c r="AA4" s="115"/>
-      <c r="AB4" s="115" t="str">
+      <c r="AB4" s="115"/>
+      <c r="AC4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>CUNI</v>
       </c>
-      <c r="AC4" s="115" t="str">
+      <c r="AD4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>DHMZ</v>
       </c>
-      <c r="AD4" s="192"/>
-      <c r="AE4" s="115" t="str">
+      <c r="AE4" s="192"/>
+      <c r="AF4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>GISS</v>
       </c>
-      <c r="AF4" s="115" t="str">
+      <c r="AG4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>CCCma</v>
       </c>
-      <c r="AG4" s="115" t="str">
-        <f>AG7</f>
+      <c r="AH4" s="115" t="str">
+        <f>AH7</f>
         <v>CSIRO</v>
       </c>
-      <c r="AH4" s="115" t="str">
+      <c r="AI4" s="115" t="str">
         <f t="shared" si="2"/>
         <v>KAUST</v>
       </c>
-      <c r="AI4" s="116" t="str">
+      <c r="AJ4" s="116" t="str">
         <f t="shared" si="2"/>
         <v>MOHC</v>
       </c>
-      <c r="AJ4" s="116" t="str">
-        <f t="shared" ref="AJ4" si="3">AJ7</f>
+      <c r="AK4" s="116" t="str">
+        <f t="shared" ref="AK4" si="3">AK7</f>
         <v>MOHC</v>
       </c>
-      <c r="AK4" s="115" t="str">
-        <f>AK7</f>
+      <c r="AL4" s="115" t="str">
+        <f>AL7</f>
         <v>MIUB</v>
       </c>
-      <c r="AL4" s="115" t="str">
-        <f t="shared" ref="AL4:AV4" si="4">AL7</f>
+      <c r="AM4" s="115" t="str">
+        <f t="shared" ref="AM4:AW4" si="4">AM7</f>
         <v>BCCR</v>
       </c>
-      <c r="AM4" s="115" t="str">
+      <c r="AN4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>CRP-GL</v>
       </c>
-      <c r="AN4" s="115" t="str">
+      <c r="AO4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>IDL</v>
       </c>
-      <c r="AO4" s="115" t="s">
+      <c r="AP4" s="115" t="s">
         <v>165</v>
       </c>
-      <c r="AP4" s="115" t="str">
+      <c r="AQ4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>AUTH-Met</v>
       </c>
-      <c r="AQ4" s="115" t="str">
+      <c r="AR4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>AUTH-LHTEE</v>
       </c>
-      <c r="AR4" s="115" t="str">
+      <c r="AS4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>NUIM</v>
       </c>
-      <c r="AS4" s="115" t="str">
+      <c r="AT4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>UHOH</v>
       </c>
-      <c r="AT4" s="115" t="str">
+      <c r="AU4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>UM</v>
-      </c>
-      <c r="AU4" s="115" t="str">
-        <f t="shared" si="4"/>
-        <v>UCAN</v>
       </c>
       <c r="AV4" s="115" t="str">
         <f t="shared" si="4"/>
         <v>UCAN</v>
       </c>
-      <c r="AW4" s="170" t="s">
+      <c r="AW4" s="115" t="str">
+        <f t="shared" si="4"/>
+        <v>UCAN</v>
+      </c>
+      <c r="AX4" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="AX4" s="2"/>
       <c r="AY4" s="2"/>
       <c r="AZ4" s="2"/>
       <c r="BA4" s="2"/>
@@ -4184,8 +4221,9 @@
       <c r="BX4" s="2"/>
       <c r="BY4" s="2"/>
       <c r="BZ4" s="2"/>
+      <c r="CA4" s="2"/>
     </row>
-    <row r="5" spans="1:78" s="136" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:79" s="136" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="171" t="s">
         <v>126</v>
       </c>
@@ -4213,39 +4251,39 @@
       <c r="Q5" s="129"/>
       <c r="R5" s="131"/>
       <c r="S5" s="129"/>
-      <c r="T5" s="130"/>
+      <c r="T5" s="129"/>
       <c r="U5" s="130"/>
       <c r="V5" s="130"/>
       <c r="W5" s="130"/>
-      <c r="X5" s="131"/>
+      <c r="X5" s="130"/>
       <c r="Y5" s="131"/>
       <c r="Z5" s="131"/>
       <c r="AA5" s="131"/>
       <c r="AB5" s="131"/>
       <c r="AC5" s="131"/>
-      <c r="AD5" s="193"/>
-      <c r="AE5" s="131"/>
+      <c r="AD5" s="131"/>
+      <c r="AE5" s="193"/>
       <c r="AF5" s="131"/>
       <c r="AG5" s="131"/>
       <c r="AH5" s="131"/>
-      <c r="AI5" s="132"/>
+      <c r="AI5" s="131"/>
       <c r="AJ5" s="132"/>
-      <c r="AK5" s="133"/>
+      <c r="AK5" s="132"/>
       <c r="AL5" s="133"/>
-      <c r="AM5" s="134"/>
+      <c r="AM5" s="133"/>
       <c r="AN5" s="134"/>
       <c r="AO5" s="134"/>
-      <c r="AP5" s="131"/>
+      <c r="AP5" s="134"/>
       <c r="AQ5" s="131"/>
       <c r="AR5" s="131"/>
       <c r="AS5" s="131"/>
       <c r="AT5" s="131"/>
       <c r="AU5" s="131"/>
       <c r="AV5" s="131"/>
-      <c r="AW5" s="171" t="s">
+      <c r="AW5" s="131"/>
+      <c r="AX5" s="171" t="s">
         <v>126</v>
       </c>
-      <c r="AX5" s="135"/>
       <c r="AY5" s="135"/>
       <c r="AZ5" s="135"/>
       <c r="BA5" s="135"/>
@@ -4274,8 +4312,9 @@
       <c r="BX5" s="135"/>
       <c r="BY5" s="135"/>
       <c r="BZ5" s="135"/>
+      <c r="CA5" s="135"/>
     </row>
-    <row r="6" spans="1:78" s="1" customFormat="1" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:79" s="1" customFormat="1" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="170" t="s">
         <v>64</v>
       </c>
@@ -4301,20 +4340,20 @@
       <c r="U6" s="117"/>
       <c r="V6" s="117"/>
       <c r="W6" s="117"/>
-      <c r="X6" s="115"/>
+      <c r="X6" s="117"/>
       <c r="Y6" s="115"/>
       <c r="Z6" s="115"/>
       <c r="AA6" s="115"/>
       <c r="AB6" s="115"/>
       <c r="AC6" s="115"/>
-      <c r="AD6" s="192"/>
-      <c r="AE6" s="115"/>
+      <c r="AD6" s="115"/>
+      <c r="AE6" s="192"/>
       <c r="AF6" s="115"/>
       <c r="AG6" s="115"/>
       <c r="AH6" s="115"/>
-      <c r="AI6" s="116"/>
+      <c r="AI6" s="115"/>
       <c r="AJ6" s="116"/>
-      <c r="AK6" s="115"/>
+      <c r="AK6" s="116"/>
       <c r="AL6" s="115"/>
       <c r="AM6" s="115"/>
       <c r="AN6" s="115"/>
@@ -4326,10 +4365,10 @@
       <c r="AT6" s="115"/>
       <c r="AU6" s="115"/>
       <c r="AV6" s="115"/>
-      <c r="AW6" s="170" t="s">
+      <c r="AW6" s="115"/>
+      <c r="AX6" s="170" t="s">
         <v>64</v>
       </c>
-      <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
       <c r="AZ6" s="2"/>
       <c r="BA6" s="2"/>
@@ -4358,8 +4397,9 @@
       <c r="BX6" s="2"/>
       <c r="BY6" s="2"/>
       <c r="BZ6" s="2"/>
+      <c r="CA6" s="2"/>
     </row>
-    <row r="7" spans="1:78" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:79" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="171" t="s">
         <v>185</v>
       </c>
@@ -4417,11 +4457,11 @@
       <c r="S7" s="178" t="s">
         <v>39</v>
       </c>
-      <c r="T7" s="186" t="s">
+      <c r="T7" s="178" t="s">
         <v>39</v>
       </c>
       <c r="U7" s="186" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="V7" s="186" t="s">
         <v>52</v>
@@ -4429,85 +4469,87 @@
       <c r="W7" s="186" t="s">
         <v>52</v>
       </c>
-      <c r="X7" s="178" t="s">
+      <c r="X7" s="186" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y7" s="178" t="s">
         <v>31</v>
       </c>
-      <c r="Y7" s="178" t="s">
+      <c r="Z7" s="178" t="s">
         <v>34</v>
       </c>
-      <c r="Z7" s="178" t="s">
+      <c r="AA7" s="178" t="s">
         <v>38</v>
       </c>
-      <c r="AA7" s="178" t="s">
+      <c r="AB7" s="178" t="s">
         <v>174</v>
       </c>
-      <c r="AB7" s="178" t="s">
+      <c r="AC7" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="AC7" s="178" t="s">
+      <c r="AD7" s="178" t="s">
         <v>48</v>
       </c>
-      <c r="AD7" s="194" t="s">
+      <c r="AE7" s="194" t="s">
         <v>221</v>
       </c>
-      <c r="AE7" s="178" t="s">
+      <c r="AF7" s="178" t="s">
         <v>37</v>
       </c>
-      <c r="AF7" s="178" t="s">
+      <c r="AG7" s="178" t="s">
         <v>120</v>
       </c>
-      <c r="AG7" s="178" t="s">
+      <c r="AH7" s="178" t="s">
         <v>226</v>
       </c>
-      <c r="AH7" s="178" t="s">
+      <c r="AI7" s="178" t="s">
         <v>55</v>
-      </c>
-      <c r="AI7" s="178" t="s">
-        <v>53</v>
       </c>
       <c r="AJ7" s="178" t="s">
         <v>53</v>
       </c>
-      <c r="AK7" s="183" t="s">
+      <c r="AK7" s="178" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL7" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="AL7" s="183" t="s">
+      <c r="AM7" s="183" t="s">
         <v>45</v>
       </c>
-      <c r="AM7" s="186" t="s">
+      <c r="AN7" s="186" t="s">
         <v>36</v>
       </c>
-      <c r="AN7" s="186" t="s">
+      <c r="AO7" s="186" t="s">
         <v>46</v>
       </c>
-      <c r="AO7" s="186" t="s">
+      <c r="AP7" s="186" t="s">
         <v>164</v>
       </c>
-      <c r="AP7" s="178" t="s">
+      <c r="AQ7" s="178" t="s">
         <v>144</v>
       </c>
-      <c r="AQ7" s="178" t="s">
+      <c r="AR7" s="178" t="s">
         <v>145</v>
       </c>
-      <c r="AR7" s="178" t="s">
+      <c r="AS7" s="178" t="s">
         <v>56</v>
       </c>
-      <c r="AS7" s="178" t="s">
+      <c r="AT7" s="178" t="s">
         <v>33</v>
       </c>
-      <c r="AT7" s="178" t="s">
+      <c r="AU7" s="178" t="s">
         <v>32</v>
-      </c>
-      <c r="AU7" s="178" t="s">
-        <v>140</v>
       </c>
       <c r="AV7" s="178" t="s">
         <v>140</v>
       </c>
-      <c r="AW7" s="171" t="s">
+      <c r="AW7" s="178" t="s">
+        <v>140</v>
+      </c>
+      <c r="AX7" s="171" t="s">
         <v>185</v>
       </c>
-      <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
@@ -4536,8 +4578,9 @@
       <c r="BX7" s="2"/>
       <c r="BY7" s="2"/>
       <c r="BZ7" s="2"/>
+      <c r="CA7" s="2"/>
     </row>
-    <row r="8" spans="1:78" s="121" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:79" s="121" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="171" t="s">
         <v>86</v>
       </c>
@@ -4595,97 +4638,99 @@
       <c r="S8" s="180" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="188" t="s">
+      <c r="T8" s="200" t="s">
+        <v>231</v>
+      </c>
+      <c r="U8" s="188" t="s">
         <v>130</v>
       </c>
-      <c r="U8" s="188" t="s">
+      <c r="V8" s="188" t="s">
         <v>148</v>
       </c>
-      <c r="V8" s="188" t="s">
+      <c r="W8" s="188" t="s">
         <v>111</v>
       </c>
-      <c r="W8" s="188" t="s">
+      <c r="X8" s="188" t="s">
         <v>97</v>
       </c>
-      <c r="X8" s="180" t="s">
+      <c r="Y8" s="180" t="s">
         <v>93</v>
       </c>
-      <c r="Y8" s="180" t="s">
+      <c r="Z8" s="180" t="s">
         <v>94</v>
-      </c>
-      <c r="Z8" s="180" t="s">
-        <v>95</v>
       </c>
       <c r="AA8" s="180" t="s">
         <v>95</v>
       </c>
       <c r="AB8" s="180" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="AC8" s="180" t="s">
         <v>134</v>
       </c>
-      <c r="AD8" s="195" t="s">
+      <c r="AD8" s="180" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE8" s="195" t="s">
         <v>222</v>
       </c>
-      <c r="AE8" s="182" t="s">
+      <c r="AF8" s="182" t="s">
         <v>27</v>
       </c>
-      <c r="AF8" s="180" t="s">
+      <c r="AG8" s="180" t="s">
         <v>28</v>
       </c>
-      <c r="AG8" s="180" t="s">
+      <c r="AH8" s="180" t="s">
         <v>29</v>
       </c>
-      <c r="AH8" s="180" t="s">
+      <c r="AI8" s="180" t="s">
         <v>30</v>
       </c>
-      <c r="AI8" s="179" t="s">
+      <c r="AJ8" s="179" t="s">
         <v>114</v>
       </c>
-      <c r="AJ8" s="179" t="s">
+      <c r="AK8" s="179" t="s">
         <v>128</v>
       </c>
-      <c r="AK8" s="184" t="s">
+      <c r="AL8" s="184" t="s">
         <v>137</v>
       </c>
-      <c r="AL8" s="184" t="s">
+      <c r="AM8" s="184" t="s">
         <v>136</v>
       </c>
-      <c r="AM8" s="187" t="s">
+      <c r="AN8" s="187" t="s">
         <v>137</v>
       </c>
-      <c r="AN8" s="187" t="s">
+      <c r="AO8" s="187" t="s">
         <v>138</v>
       </c>
-      <c r="AO8" s="187" t="s">
+      <c r="AP8" s="187" t="s">
         <v>139</v>
       </c>
-      <c r="AP8" s="182" t="s">
+      <c r="AQ8" s="182" t="s">
         <v>137</v>
       </c>
-      <c r="AQ8" s="180" t="s">
+      <c r="AR8" s="180" t="s">
         <v>146</v>
       </c>
-      <c r="AR8" s="182" t="s">
+      <c r="AS8" s="182" t="s">
         <v>175</v>
       </c>
-      <c r="AS8" s="182" t="s">
+      <c r="AT8" s="182" t="s">
         <v>142</v>
       </c>
-      <c r="AT8" s="182" t="s">
+      <c r="AU8" s="182" t="s">
         <v>24</v>
       </c>
-      <c r="AU8" s="188" t="s">
+      <c r="AV8" s="188" t="s">
         <v>141</v>
       </c>
-      <c r="AV8" s="182" t="s">
+      <c r="AW8" s="182" t="s">
         <v>147</v>
       </c>
-      <c r="AW8" s="171" t="s">
+      <c r="AX8" s="171" t="s">
         <v>86</v>
       </c>
-      <c r="AX8" s="120"/>
       <c r="AY8" s="120"/>
       <c r="AZ8" s="120"/>
       <c r="BA8" s="120"/>
@@ -4714,8 +4759,9 @@
       <c r="BX8" s="120"/>
       <c r="BY8" s="120"/>
       <c r="BZ8" s="120"/>
+      <c r="CA8" s="120"/>
     </row>
-    <row r="9" spans="1:78" s="35" customFormat="1" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:79" s="35" customFormat="1" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="170" t="s">
         <v>167</v>
       </c>
@@ -4773,7 +4819,7 @@
         <v>190</v>
       </c>
       <c r="U9" s="185" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="V9" s="185" t="s">
         <v>169</v>
@@ -4781,59 +4827,63 @@
       <c r="W9" s="185" t="s">
         <v>169</v>
       </c>
-      <c r="X9" s="116" t="s">
+      <c r="X9" s="185" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y9" s="116" t="s">
         <v>179</v>
       </c>
-      <c r="Y9" s="116" t="s">
+      <c r="Z9" s="116" t="s">
         <v>171</v>
       </c>
-      <c r="Z9" s="116" t="s">
+      <c r="AA9" s="116" t="s">
         <v>202</v>
       </c>
-      <c r="AA9" s="116" t="s">
+      <c r="AB9" s="116" t="s">
         <v>204</v>
       </c>
-      <c r="AB9" s="116"/>
-      <c r="AC9" s="116" t="s">
+      <c r="AC9" s="116"/>
+      <c r="AD9" s="116" t="s">
         <v>188</v>
       </c>
-      <c r="AD9" s="196" t="s">
+      <c r="AE9" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="AE9" s="116"/>
-      <c r="AF9" s="116" t="s">
+      <c r="AF9" s="116"/>
+      <c r="AG9" s="116" t="s">
         <v>177</v>
       </c>
-      <c r="AG9" s="116" t="s">
+      <c r="AH9" s="116" t="s">
         <v>227</v>
       </c>
-      <c r="AH9" s="116"/>
       <c r="AI9" s="116" t="s">
-        <v>189</v>
+        <v>230</v>
       </c>
       <c r="AJ9" s="116" t="s">
         <v>189</v>
       </c>
-      <c r="AK9" s="185"/>
-      <c r="AL9" s="185" t="s">
+      <c r="AK9" s="116" t="s">
+        <v>189</v>
+      </c>
+      <c r="AL9" s="185"/>
+      <c r="AM9" s="185" t="s">
         <v>191</v>
       </c>
-      <c r="AM9" s="185"/>
       <c r="AN9" s="185"/>
       <c r="AO9" s="185"/>
-      <c r="AP9" s="116"/>
+      <c r="AP9" s="185"/>
       <c r="AQ9" s="116"/>
-      <c r="AR9" s="196" t="s">
+      <c r="AR9" s="116"/>
+      <c r="AS9" s="196" t="s">
         <v>216</v>
       </c>
-      <c r="AS9" s="116"/>
       <c r="AT9" s="116"/>
       <c r="AU9" s="116"/>
       <c r="AV9" s="116"/>
-      <c r="AW9" s="170" t="s">
+      <c r="AW9" s="116"/>
+      <c r="AX9" s="170" t="s">
         <v>167</v>
       </c>
-      <c r="AX9" s="72"/>
       <c r="AY9" s="72"/>
       <c r="AZ9" s="72"/>
       <c r="BA9" s="72"/>
@@ -4862,8 +4912,9 @@
       <c r="BX9" s="72"/>
       <c r="BY9" s="72"/>
       <c r="BZ9" s="72"/>
+      <c r="CA9" s="72"/>
     </row>
-    <row r="10" spans="1:78" s="1" customFormat="1" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:79" s="1" customFormat="1" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="170" t="s">
         <v>197</v>
       </c>
@@ -4897,51 +4948,53 @@
         <v>206</v>
       </c>
       <c r="S10" s="181"/>
-      <c r="T10" s="181"/>
-      <c r="U10" s="181" t="s">
+      <c r="T10" s="181" t="s">
+        <v>234</v>
+      </c>
+      <c r="U10" s="181"/>
+      <c r="V10" s="181" t="s">
         <v>211</v>
       </c>
-      <c r="V10" s="181" t="s">
+      <c r="W10" s="181" t="s">
         <v>210</v>
       </c>
-      <c r="W10" s="181" t="s">
+      <c r="X10" s="181" t="s">
         <v>212</v>
       </c>
-      <c r="X10" s="116"/>
       <c r="Y10" s="116"/>
       <c r="Z10" s="116"/>
       <c r="AA10" s="116"/>
       <c r="AB10" s="116"/>
       <c r="AC10" s="116"/>
-      <c r="AD10" s="196"/>
-      <c r="AE10" s="116"/>
+      <c r="AD10" s="116"/>
+      <c r="AE10" s="196"/>
       <c r="AF10" s="116"/>
       <c r="AG10" s="116"/>
       <c r="AH10" s="116"/>
       <c r="AI10" s="116"/>
-      <c r="AJ10" s="116" t="s">
+      <c r="AJ10" s="116"/>
+      <c r="AK10" s="116" t="s">
         <v>209</v>
       </c>
-      <c r="AK10" s="116"/>
       <c r="AL10" s="116"/>
       <c r="AM10" s="116"/>
       <c r="AN10" s="116"/>
-      <c r="AO10" s="116" t="s">
+      <c r="AO10" s="116"/>
+      <c r="AP10" s="116" t="s">
         <v>198</v>
       </c>
-      <c r="AP10" s="116"/>
       <c r="AQ10" s="116"/>
       <c r="AR10" s="116"/>
       <c r="AS10" s="116"/>
       <c r="AT10" s="116"/>
-      <c r="AU10" s="116" t="s">
+      <c r="AU10" s="116"/>
+      <c r="AV10" s="116" t="s">
         <v>200</v>
       </c>
-      <c r="AV10" s="116"/>
-      <c r="AW10" s="170" t="s">
+      <c r="AW10" s="116"/>
+      <c r="AX10" s="170" t="s">
         <v>197</v>
       </c>
-      <c r="AX10" s="2"/>
       <c r="AY10" s="2"/>
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
@@ -4970,8 +5023,9 @@
       <c r="BX10" s="2"/>
       <c r="BY10" s="2"/>
       <c r="BZ10" s="2"/>
+      <c r="CA10" s="2"/>
     </row>
-    <row r="11" spans="1:78" s="136" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:79" s="136" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="172" t="s">
         <v>153</v>
       </c>
@@ -5026,7 +5080,7 @@
         <v>176</v>
       </c>
       <c r="T11" s="116" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="U11" s="116" t="s">
         <v>176</v>
@@ -5040,56 +5094,58 @@
       <c r="X11" s="116" t="s">
         <v>176</v>
       </c>
-      <c r="Y11" s="116"/>
-      <c r="Z11" s="116" t="s">
+      <c r="Y11" s="116" t="s">
         <v>176</v>
       </c>
+      <c r="Z11" s="116"/>
       <c r="AA11" s="116" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB11" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="AB11" s="116"/>
-      <c r="AC11" s="116" t="s">
-        <v>181</v>
-      </c>
+      <c r="AC11" s="116"/>
       <c r="AD11" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="AE11" s="116"/>
-      <c r="AF11" s="116" t="s">
+      <c r="AE11" s="116" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF11" s="116"/>
+      <c r="AG11" s="116" t="s">
         <v>176</v>
       </c>
-      <c r="AG11" s="116"/>
       <c r="AH11" s="116"/>
-      <c r="AI11" s="116" t="s">
-        <v>176</v>
-      </c>
+      <c r="AI11" s="116"/>
       <c r="AJ11" s="116" t="s">
         <v>176</v>
       </c>
-      <c r="AK11" s="116"/>
-      <c r="AL11" s="116" t="s">
+      <c r="AK11" s="116" t="s">
         <v>176</v>
       </c>
+      <c r="AL11" s="116"/>
       <c r="AM11" s="116" t="s">
         <v>176</v>
       </c>
-      <c r="AN11" s="116"/>
+      <c r="AN11" s="116" t="s">
+        <v>176</v>
+      </c>
       <c r="AO11" s="116"/>
       <c r="AP11" s="116"/>
       <c r="AQ11" s="116"/>
-      <c r="AR11" s="116" t="s">
+      <c r="AR11" s="116"/>
+      <c r="AS11" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="AS11" s="116"/>
       <c r="AT11" s="116"/>
-      <c r="AU11" s="116" t="s">
+      <c r="AU11" s="116"/>
+      <c r="AV11" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="AV11" s="116"/>
-      <c r="AW11" s="197" t="s">
+      <c r="AW11" s="116"/>
+      <c r="AX11" s="197" t="s">
         <v>153</v>
       </c>
-      <c r="AX11" s="135"/>
       <c r="AY11" s="135"/>
       <c r="AZ11" s="135"/>
       <c r="BA11" s="135"/>
@@ -5118,18 +5174,19 @@
       <c r="BX11" s="135"/>
       <c r="BY11" s="135"/>
       <c r="BZ11" s="135"/>
+      <c r="CA11" s="135"/>
     </row>
-    <row r="12" spans="1:78" s="26" customFormat="1" ht="21.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="202" t="s">
+    <row r="12" spans="1:79" s="26" customFormat="1" ht="21.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="204" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="202"/>
-      <c r="C12" s="202"/>
-      <c r="D12" s="202"/>
-      <c r="E12" s="202"/>
-      <c r="F12" s="202"/>
-      <c r="G12" s="202"/>
-      <c r="H12" s="202"/>
+      <c r="B12" s="204"/>
+      <c r="C12" s="204"/>
+      <c r="D12" s="204"/>
+      <c r="E12" s="204"/>
+      <c r="F12" s="204"/>
+      <c r="G12" s="204"/>
+      <c r="H12" s="204"/>
       <c r="I12" s="127"/>
       <c r="J12" s="127"/>
       <c r="K12" s="127"/>
@@ -5141,18 +5198,18 @@
       <c r="Q12" s="127"/>
       <c r="R12" s="127"/>
       <c r="S12" s="127"/>
-      <c r="T12" s="127"/>
+      <c r="T12" s="199"/>
       <c r="U12" s="127"/>
       <c r="V12" s="127"/>
       <c r="W12" s="127"/>
       <c r="X12" s="127"/>
       <c r="Y12" s="127"/>
       <c r="Z12" s="127"/>
-      <c r="AA12" s="151"/>
-      <c r="AB12" s="127"/>
+      <c r="AA12" s="127"/>
+      <c r="AB12" s="151"/>
       <c r="AC12" s="127"/>
-      <c r="AD12" s="190"/>
-      <c r="AE12" s="127"/>
+      <c r="AD12" s="127"/>
+      <c r="AE12" s="190"/>
       <c r="AF12" s="127"/>
       <c r="AG12" s="127"/>
       <c r="AH12" s="127"/>
@@ -5170,16 +5227,17 @@
       <c r="AT12" s="127"/>
       <c r="AU12" s="127"/>
       <c r="AV12" s="127"/>
+      <c r="AW12" s="127"/>
     </row>
-    <row r="13" spans="1:78" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="202" t="s">
+    <row r="13" spans="1:79" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="204" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="202"/>
-      <c r="C13" s="202"/>
-      <c r="D13" s="202"/>
-      <c r="E13" s="202"/>
-      <c r="F13" s="202"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="204"/>
+      <c r="D13" s="204"/>
+      <c r="E13" s="204"/>
+      <c r="F13" s="204"/>
       <c r="G13" s="141"/>
       <c r="H13" s="141"/>
       <c r="I13" s="141"/>
@@ -5194,7 +5252,6 @@
       <c r="R13" s="141"/>
       <c r="S13" s="141"/>
       <c r="T13" s="141"/>
-      <c r="U13" s="141"/>
       <c r="V13" s="141"/>
       <c r="W13" s="141"/>
       <c r="X13" s="141"/>
@@ -5222,9 +5279,10 @@
       <c r="AT13" s="141"/>
       <c r="AU13" s="141"/>
       <c r="AV13" s="141"/>
+      <c r="AW13" s="141"/>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="AW14" s="72"/>
+    <row r="14" spans="1:79" x14ac:dyDescent="0.3">
+      <c r="AX14" s="72"/>
     </row>
     <row r="22" spans="4:14" x14ac:dyDescent="0.3">
       <c r="N22" s="122"/>
@@ -5244,23 +5302,23 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A13:F13"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:AC11 AE11:AV11 AD7:AV10">
+  <conditionalFormatting sqref="B7:AD7 AF11:AW11 AE7:AW10 B8:S8 U8:AD8 B9:AD11">
     <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD11">
+  <conditionalFormatting sqref="AE11">
     <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",AD11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",AE11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="AF3" r:id="rId1" display="mailto:John.Scinocca@ec.gc.ca"/>
+    <hyperlink ref="AG3" r:id="rId1" display="mailto:John.Scinocca@ec.gc.ca"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="47" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="34" max="8" man="1"/>
+    <brk id="35" max="8" man="1"/>
   </colBreaks>
 </worksheet>
 </file>
@@ -5317,25 +5375,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:144" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="201" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
-      <c r="L1" s="199"/>
-      <c r="M1" s="199"/>
-      <c r="N1" s="199"/>
-      <c r="O1" s="199"/>
-      <c r="P1" s="199"/>
-      <c r="Q1" s="199"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
+      <c r="N1" s="201"/>
+      <c r="O1" s="201"/>
+      <c r="P1" s="201"/>
+      <c r="Q1" s="201"/>
       <c r="R1" s="21"/>
       <c r="S1" s="20"/>
       <c r="T1" s="20"/>
@@ -5373,7 +5431,7 @@
     <row r="2" spans="1:144" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="53">
         <f>GeneralRemarks!A2</f>
-        <v>41901</v>
+        <v>41954</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -5399,7 +5457,7 @@
       <c r="W2" s="20"/>
       <c r="X2" s="54">
         <f>GeneralRemarks!A2</f>
-        <v>41901</v>
+        <v>41954</v>
       </c>
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
@@ -5429,7 +5487,7 @@
       <c r="AX2" s="20"/>
       <c r="AZ2" s="73">
         <f>A2</f>
-        <v>41901</v>
+        <v>41954</v>
       </c>
     </row>
     <row r="3" spans="1:144" s="1" customFormat="1" ht="36.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5538,59 +5596,59 @@
 @meteo.fr</v>
       </c>
       <c r="V3" s="29" t="str">
-        <f>AllEntries!T3</f>
+        <f>AllEntries!U3</f>
         <v>Michel.DEQUE
 @meteo.fr</v>
       </c>
       <c r="W3" s="29" t="str">
-        <f>AllEntries!U3</f>
-        <v>Erik van Meijgaard 
-vanmeijg@knmi.nl</v>
-      </c>
-      <c r="X3" s="29" t="str">
         <f>AllEntries!V3</f>
         <v>Erik van Meijgaard 
 vanmeijg@knmi.nl</v>
       </c>
-      <c r="Y3" s="29" t="str">
+      <c r="X3" s="29" t="str">
         <f>AllEntries!W3</f>
         <v>Erik van Meijgaard 
 vanmeijg@knmi.nl</v>
       </c>
+      <c r="Y3" s="29" t="str">
+        <f>AllEntries!X3</f>
+        <v>Erik van Meijgaard 
+vanmeijg@knmi.nl</v>
+      </c>
       <c r="Z3" s="29" t="str">
-        <f>AllEntries!X3</f>
+        <f>AllEntries!Y3</f>
         <v>Winger.Katja
 @uqam.ca</v>
       </c>
       <c r="AA3" s="29" t="str">
-        <f>AllEntries!Y3</f>
+        <f>AllEntries!Z3</f>
         <v>marta.dominguez@uclm.es; miguel.gaertner
 @uclm.es</v>
       </c>
       <c r="AB3" s="29" t="str">
-        <f>AllEntries!Z3</f>
+        <f>AllEntries!AA3</f>
         <v>Erika Coppola coppolae@ictp.it</v>
       </c>
       <c r="AC3" s="29" t="str">
-        <f>AllEntries!AA3</f>
+        <f>AllEntries!AB3</f>
         <v>Sandro Calmanti sandro.calmanti
 @enea.it</v>
       </c>
       <c r="AD3" s="29">
-        <f>AllEntries!AB3</f>
+        <f>AllEntries!AC3</f>
         <v>0</v>
       </c>
       <c r="AE3" s="29" t="str">
-        <f>AllEntries!AC3</f>
+        <f>AllEntries!AD3</f>
         <v>ivan.guettler @gmail.com
 Cedo Brankovic</v>
       </c>
       <c r="AF3" s="29">
-        <f>AllEntries!AE3</f>
+        <f>AllEntries!AF3</f>
         <v>0</v>
       </c>
       <c r="AG3" s="27" t="str">
-        <f>AllEntries!AF3</f>
+        <f>AllEntries!AG3</f>
         <v>John.Scinocca
 @ec.gc.ca</v>
       </c>
@@ -5599,63 +5657,63 @@
         <v>Contact</v>
       </c>
       <c r="AI3" s="27" t="str">
-        <f>AllEntries!AG3</f>
+        <f>AllEntries!AH3</f>
         <v>Jack.Katzfey@csiro.au</v>
       </c>
       <c r="AJ3" s="29">
-        <f>AllEntries!AH3</f>
+        <f>AllEntries!AI3</f>
         <v>0</v>
       </c>
       <c r="AK3" s="55" t="str">
-        <f>AllEntries!AI3</f>
-        <v>carlo.buontempo
-@metoffice.gov.uk</v>
-      </c>
-      <c r="AL3" s="55" t="str">
         <f>AllEntries!AJ3</f>
         <v>carlo.buontempo
 @metoffice.gov.uk</v>
       </c>
+      <c r="AL3" s="55" t="str">
+        <f>AllEntries!AK3</f>
+        <v>carlo.buontempo
+@metoffice.gov.uk</v>
+      </c>
       <c r="AM3" s="29">
-        <f>AllEntries!AK3</f>
+        <f>AllEntries!AL3</f>
         <v>0</v>
       </c>
       <c r="AN3" s="29">
-        <f>AllEntries!AL3</f>
+        <f>AllEntries!AM3</f>
         <v>0</v>
       </c>
       <c r="AO3" s="29">
-        <f>AllEntries!AM3</f>
+        <f>AllEntries!AN3</f>
         <v>0</v>
       </c>
       <c r="AP3" s="29">
-        <f>AllEntries!AN3</f>
+        <f>AllEntries!AO3</f>
         <v>0</v>
       </c>
       <c r="AQ3" s="29" t="str">
-        <f>AllEntries!AO3</f>
+        <f>AllEntries!AP3</f>
         <v>robert.vautard
 @lsce.ipsl.fr</v>
       </c>
       <c r="AR3" s="29">
-        <f>AllEntries!AP3</f>
+        <f>AllEntries!AQ3</f>
         <v>0</v>
       </c>
       <c r="AS3" s="29">
-        <f>AllEntries!AQ3</f>
+        <f>AllEntries!AR3</f>
         <v>0</v>
       </c>
       <c r="AT3" s="29" t="str">
-        <f>AllEntries!AR3</f>
+        <f>AllEntries!AS3</f>
         <v>Rowan Fealy : rowan.fealy
 @nuim.ie</v>
       </c>
       <c r="AU3" s="29">
-        <f>AllEntries!AS3</f>
+        <f>AllEntries!AT3</f>
         <v>0</v>
       </c>
       <c r="AV3" s="29">
-        <f>AllEntries!AT3</f>
+        <f>AllEntries!AU3</f>
         <v>0</v>
       </c>
       <c r="AW3" s="29" t="e">
@@ -5663,11 +5721,11 @@
         <v>#REF!</v>
       </c>
       <c r="AX3" s="41">
-        <f>AllEntries!AU3</f>
+        <f>AllEntries!AV3</f>
         <v>0</v>
       </c>
       <c r="AY3" s="27">
-        <f>AllEntries!AV3</f>
+        <f>AllEntries!AW3</f>
         <v>0</v>
       </c>
       <c r="AZ3" s="81"/>
@@ -5852,51 +5910,51 @@
         <v>CNRM</v>
       </c>
       <c r="V4" s="35" t="str">
-        <f>AllEntries!T4</f>
+        <f>AllEntries!U4</f>
         <v>CNRM</v>
       </c>
       <c r="W4" s="35" t="str">
-        <f>AllEntries!U4</f>
-        <v>KNMI</v>
-      </c>
-      <c r="X4" s="35" t="str">
         <f>AllEntries!V4</f>
         <v>KNMI</v>
       </c>
-      <c r="Y4" s="35" t="str">
+      <c r="X4" s="35" t="str">
         <f>AllEntries!W4</f>
         <v>KNMI</v>
       </c>
+      <c r="Y4" s="35" t="str">
+        <f>AllEntries!X4</f>
+        <v>KNMI</v>
+      </c>
       <c r="Z4" s="35" t="str">
-        <f>AllEntries!X4</f>
+        <f>AllEntries!Y4</f>
         <v>UQAM</v>
       </c>
       <c r="AA4" s="35" t="str">
-        <f>AllEntries!Y4</f>
+        <f>AllEntries!Z4</f>
         <v>UCLM</v>
       </c>
       <c r="AB4" s="35" t="str">
-        <f>AllEntries!Z4</f>
+        <f>AllEntries!AA4</f>
         <v>ICTP</v>
       </c>
       <c r="AC4" s="35">
-        <f>AllEntries!AA4</f>
+        <f>AllEntries!AB4</f>
         <v>0</v>
       </c>
       <c r="AD4" s="35" t="str">
-        <f>AllEntries!AB4</f>
+        <f>AllEntries!AC4</f>
         <v>CUNI</v>
       </c>
       <c r="AE4" s="35" t="str">
-        <f>AllEntries!AC4</f>
+        <f>AllEntries!AD4</f>
         <v>DHMZ</v>
       </c>
       <c r="AF4" s="35" t="str">
-        <f>AllEntries!AE4</f>
+        <f>AllEntries!AF4</f>
         <v>GISS</v>
       </c>
       <c r="AG4" s="33" t="str">
-        <f>AllEntries!AF4</f>
+        <f>AllEntries!AG4</f>
         <v>CCCma</v>
       </c>
       <c r="AH4" s="75" t="str">
@@ -5904,59 +5962,59 @@
         <v>Data providing  center</v>
       </c>
       <c r="AI4" s="33" t="str">
-        <f>AllEntries!AG4</f>
+        <f>AllEntries!AH4</f>
         <v>CSIRO</v>
       </c>
       <c r="AJ4" s="35" t="str">
-        <f>AllEntries!AH4</f>
+        <f>AllEntries!AI4</f>
         <v>KAUST</v>
       </c>
       <c r="AK4" s="56" t="str">
-        <f>AllEntries!AI4</f>
-        <v>MOHC</v>
-      </c>
-      <c r="AL4" s="56" t="str">
         <f>AllEntries!AJ4</f>
         <v>MOHC</v>
       </c>
+      <c r="AL4" s="56" t="str">
+        <f>AllEntries!AK4</f>
+        <v>MOHC</v>
+      </c>
       <c r="AM4" s="35" t="str">
-        <f>AllEntries!AK4</f>
+        <f>AllEntries!AL4</f>
         <v>MIUB</v>
       </c>
       <c r="AN4" s="35" t="str">
-        <f>AllEntries!AL4</f>
+        <f>AllEntries!AM4</f>
         <v>BCCR</v>
       </c>
       <c r="AO4" s="35" t="str">
-        <f>AllEntries!AM4</f>
+        <f>AllEntries!AN4</f>
         <v>CRP-GL</v>
       </c>
       <c r="AP4" s="35" t="str">
-        <f>AllEntries!AN4</f>
+        <f>AllEntries!AO4</f>
         <v>IDL</v>
       </c>
       <c r="AQ4" s="35" t="str">
-        <f>AllEntries!AO4</f>
+        <f>AllEntries!AP4</f>
         <v>IPSL/INERIS</v>
       </c>
       <c r="AR4" s="35" t="str">
-        <f>AllEntries!AP4</f>
+        <f>AllEntries!AQ4</f>
         <v>AUTH-Met</v>
       </c>
       <c r="AS4" s="35" t="str">
-        <f>AllEntries!AQ4</f>
+        <f>AllEntries!AR4</f>
         <v>AUTH-LHTEE</v>
       </c>
       <c r="AT4" s="35" t="str">
-        <f>AllEntries!AR4</f>
+        <f>AllEntries!AS4</f>
         <v>NUIM</v>
       </c>
       <c r="AU4" s="35" t="str">
-        <f>AllEntries!AS4</f>
+        <f>AllEntries!AT4</f>
         <v>UHOH</v>
       </c>
       <c r="AV4" s="35" t="str">
-        <f>AllEntries!AT4</f>
+        <f>AllEntries!AU4</f>
         <v>UM</v>
       </c>
       <c r="AW4" s="35" t="e">
@@ -5964,14 +6022,14 @@
         <v>#REF!</v>
       </c>
       <c r="AX4" s="42" t="str">
-        <f>AllEntries!AU4</f>
-        <v>UCAN</v>
-      </c>
-      <c r="AY4" s="33" t="str">
         <f>AllEntries!AV4</f>
         <v>UCAN</v>
       </c>
-      <c r="AZ4" s="206" t="s">
+      <c r="AY4" s="33" t="str">
+        <f>AllEntries!AW4</f>
+        <v>UCAN</v>
+      </c>
+      <c r="AZ4" s="208" t="s">
         <v>16</v>
       </c>
       <c r="BA4" s="75" t="s">
@@ -6155,51 +6213,51 @@
         <v>0</v>
       </c>
       <c r="V5" s="70">
-        <f>AllEntries!T6</f>
+        <f>AllEntries!U6</f>
         <v>0</v>
       </c>
       <c r="W5" s="70">
-        <f>AllEntries!U6</f>
+        <f>AllEntries!V6</f>
         <v>0</v>
       </c>
       <c r="X5" s="70">
-        <f>AllEntries!V6</f>
+        <f>AllEntries!W6</f>
         <v>0</v>
       </c>
       <c r="Y5" s="70">
-        <f>AllEntries!W6</f>
+        <f>AllEntries!X6</f>
         <v>0</v>
       </c>
       <c r="Z5" s="35">
-        <f>AllEntries!X6</f>
+        <f>AllEntries!Y6</f>
         <v>0</v>
       </c>
       <c r="AA5" s="35">
-        <f>AllEntries!Y6</f>
+        <f>AllEntries!Z6</f>
         <v>0</v>
       </c>
       <c r="AB5" s="35">
-        <f>AllEntries!Z6</f>
+        <f>AllEntries!AA6</f>
         <v>0</v>
       </c>
       <c r="AC5" s="35">
-        <f>AllEntries!AA6</f>
+        <f>AllEntries!AB6</f>
         <v>0</v>
       </c>
       <c r="AD5" s="35">
-        <f>AllEntries!AB6</f>
+        <f>AllEntries!AC6</f>
         <v>0</v>
       </c>
       <c r="AE5" s="35">
-        <f>AllEntries!AC6</f>
+        <f>AllEntries!AD6</f>
         <v>0</v>
       </c>
       <c r="AF5" s="35">
-        <f>AllEntries!AE6</f>
+        <f>AllEntries!AF6</f>
         <v>0</v>
       </c>
       <c r="AG5" s="33">
-        <f>AllEntries!AF6</f>
+        <f>AllEntries!AG6</f>
         <v>0</v>
       </c>
       <c r="AH5" s="75" t="str">
@@ -6207,59 +6265,59 @@
         <v>URL, path etc. to data**</v>
       </c>
       <c r="AI5" s="33">
-        <f>AllEntries!AG6</f>
+        <f>AllEntries!AH6</f>
         <v>0</v>
       </c>
       <c r="AJ5" s="35">
-        <f>AllEntries!AH6</f>
+        <f>AllEntries!AI6</f>
         <v>0</v>
       </c>
       <c r="AK5" s="56">
-        <f>AllEntries!AI6</f>
+        <f>AllEntries!AJ6</f>
         <v>0</v>
       </c>
       <c r="AL5" s="56">
-        <f>AllEntries!AJ6</f>
+        <f>AllEntries!AK6</f>
         <v>0</v>
       </c>
       <c r="AM5" s="35">
-        <f>AllEntries!AK6</f>
+        <f>AllEntries!AL6</f>
         <v>0</v>
       </c>
       <c r="AN5" s="35">
-        <f>AllEntries!AL6</f>
+        <f>AllEntries!AM6</f>
         <v>0</v>
       </c>
       <c r="AO5" s="35">
-        <f>AllEntries!AM6</f>
+        <f>AllEntries!AN6</f>
         <v>0</v>
       </c>
       <c r="AP5" s="35">
-        <f>AllEntries!AN6</f>
+        <f>AllEntries!AO6</f>
         <v>0</v>
       </c>
       <c r="AQ5" s="35">
-        <f>AllEntries!AO6</f>
+        <f>AllEntries!AP6</f>
         <v>0</v>
       </c>
       <c r="AR5" s="35">
-        <f>AllEntries!AP6</f>
+        <f>AllEntries!AQ6</f>
         <v>0</v>
       </c>
       <c r="AS5" s="35">
-        <f>AllEntries!AQ6</f>
+        <f>AllEntries!AR6</f>
         <v>0</v>
       </c>
       <c r="AT5" s="35">
-        <f>AllEntries!AR6</f>
+        <f>AllEntries!AS6</f>
         <v>0</v>
       </c>
       <c r="AU5" s="35">
-        <f>AllEntries!AS6</f>
+        <f>AllEntries!AT6</f>
         <v>0</v>
       </c>
       <c r="AV5" s="35">
-        <f>AllEntries!AT6</f>
+        <f>AllEntries!AU6</f>
         <v>0</v>
       </c>
       <c r="AW5" s="35" t="e">
@@ -6267,14 +6325,14 @@
         <v>#REF!</v>
       </c>
       <c r="AX5" s="42">
-        <f>AllEntries!AU6</f>
+        <f>AllEntries!AV6</f>
         <v>0</v>
       </c>
       <c r="AY5" s="33">
-        <f>AllEntries!AV6</f>
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="207"/>
+        <f>AllEntries!AW6</f>
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="209"/>
       <c r="BA5" s="75"/>
       <c r="BB5" s="2"/>
       <c r="BC5" s="2"/>
@@ -6454,51 +6512,51 @@
         <v>ALADIN52</v>
       </c>
       <c r="V6" s="37" t="str">
-        <f>AllEntries!T8</f>
+        <f>AllEntries!U8</f>
         <v>ARPEGE52</v>
       </c>
       <c r="W6" s="37" t="str">
-        <f>AllEntries!U8</f>
+        <f>AllEntries!V8</f>
         <v>RACMO22E</v>
       </c>
       <c r="X6" s="37" t="str">
-        <f>AllEntries!V8</f>
+        <f>AllEntries!W8</f>
         <v>RACMO21P</v>
       </c>
       <c r="Y6" s="37" t="str">
-        <f>AllEntries!W8</f>
+        <f>AllEntries!X8</f>
         <v>RACMO22T</v>
       </c>
       <c r="Z6" s="24" t="str">
-        <f>AllEntries!X8</f>
+        <f>AllEntries!Y8</f>
         <v>CRCM5</v>
       </c>
       <c r="AA6" s="24" t="str">
-        <f>AllEntries!Y8</f>
+        <f>AllEntries!Z8</f>
         <v>PROMES</v>
       </c>
       <c r="AB6" s="24" t="str">
-        <f>AllEntries!Z8</f>
-        <v>RegCM4-3</v>
-      </c>
-      <c r="AC6" s="24" t="str">
         <f>AllEntries!AA8</f>
         <v>RegCM4-3</v>
       </c>
+      <c r="AC6" s="24" t="str">
+        <f>AllEntries!AB8</f>
+        <v>RegCM4-3</v>
+      </c>
       <c r="AD6" s="24" t="str">
-        <f>AllEntries!AB8</f>
-        <v>RegCM4-2</v>
-      </c>
-      <c r="AE6" s="24" t="str">
         <f>AllEntries!AC8</f>
         <v>RegCM4-2</v>
       </c>
+      <c r="AE6" s="24" t="str">
+        <f>AllEntries!AD8</f>
+        <v>RegCM4-2</v>
+      </c>
       <c r="AF6" s="25" t="str">
-        <f>AllEntries!AE8</f>
+        <f>AllEntries!AF8</f>
         <v>RM3</v>
       </c>
       <c r="AG6" s="124" t="str">
-        <f>AllEntries!AF8</f>
+        <f>AllEntries!AG8</f>
         <v>CanRCM4</v>
       </c>
       <c r="AH6" s="76" t="str">
@@ -6506,59 +6564,59 @@
         <v xml:space="preserve">RCM name </v>
       </c>
       <c r="AI6" s="124" t="str">
-        <f>AllEntries!AG8</f>
+        <f>AllEntries!AH8</f>
         <v>CCAM</v>
       </c>
       <c r="AJ6" s="24" t="str">
-        <f>AllEntries!AH8</f>
+        <f>AllEntries!AI8</f>
         <v>GFDL</v>
       </c>
       <c r="AK6" s="57" t="str">
-        <f>AllEntries!AI8</f>
+        <f>AllEntries!AJ8</f>
         <v>HadGEM3-RA</v>
       </c>
       <c r="AL6" s="57" t="str">
-        <f>AllEntries!AJ8</f>
+        <f>AllEntries!AK8</f>
         <v>HadRM3P</v>
       </c>
       <c r="AM6" s="38" t="str">
-        <f>AllEntries!AK8</f>
+        <f>AllEntries!AL8</f>
         <v>WRF331A</v>
       </c>
       <c r="AN6" s="38" t="str">
-        <f>AllEntries!AL8</f>
+        <f>AllEntries!AM8</f>
         <v>WRF331C</v>
       </c>
       <c r="AO6" s="39" t="str">
-        <f>AllEntries!AM8</f>
+        <f>AllEntries!AN8</f>
         <v>WRF331A</v>
       </c>
       <c r="AP6" s="39" t="str">
-        <f>AllEntries!AN8</f>
+        <f>AllEntries!AO8</f>
         <v>WRF331D</v>
       </c>
       <c r="AQ6" s="39" t="str">
-        <f>AllEntries!AO8</f>
+        <f>AllEntries!AP8</f>
         <v>WRF331F</v>
       </c>
       <c r="AR6" s="25" t="str">
-        <f>AllEntries!AP8</f>
+        <f>AllEntries!AQ8</f>
         <v>WRF331A</v>
       </c>
       <c r="AS6" s="24" t="str">
-        <f>AllEntries!AQ8</f>
+        <f>AllEntries!AR8</f>
         <v>WRF321B</v>
       </c>
       <c r="AT6" s="25" t="str">
-        <f>AllEntries!AR8</f>
+        <f>AllEntries!AS8</f>
         <v>WRF341E</v>
       </c>
       <c r="AU6" s="25" t="str">
-        <f>AllEntries!AS8</f>
+        <f>AllEntries!AT8</f>
         <v>WRF331H</v>
       </c>
       <c r="AV6" s="25" t="str">
-        <f>AllEntries!AT8</f>
+        <f>AllEntries!AU8</f>
         <v>WRF331</v>
       </c>
       <c r="AW6" s="37" t="e">
@@ -6566,14 +6624,14 @@
         <v>#REF!</v>
       </c>
       <c r="AX6" s="43" t="str">
-        <f>AllEntries!AU8</f>
+        <f>AllEntries!AV8</f>
         <v>WRF331G</v>
       </c>
       <c r="AY6" s="84" t="str">
-        <f>AllEntries!AV8</f>
+        <f>AllEntries!AW8</f>
         <v>WRF350I</v>
       </c>
-      <c r="AZ6" s="208"/>
+      <c r="AZ6" s="210"/>
       <c r="BA6" s="76" t="s">
         <v>19</v>
       </c>
@@ -10169,25 +10227,25 @@
       <c r="EN27" s="26"/>
     </row>
     <row r="28" spans="1:144" s="26" customFormat="1" ht="37.200000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="209" t="s">
+      <c r="A28" s="211" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="209"/>
-      <c r="C28" s="209"/>
-      <c r="D28" s="209"/>
-      <c r="E28" s="209"/>
-      <c r="F28" s="209"/>
-      <c r="G28" s="209"/>
-      <c r="H28" s="209"/>
-      <c r="I28" s="209"/>
-      <c r="J28" s="209"/>
-      <c r="K28" s="209"/>
-      <c r="L28" s="209"/>
-      <c r="M28" s="209"/>
-      <c r="N28" s="209"/>
-      <c r="O28" s="209"/>
-      <c r="P28" s="209"/>
-      <c r="Q28" s="209"/>
+      <c r="B28" s="211"/>
+      <c r="C28" s="211"/>
+      <c r="D28" s="211"/>
+      <c r="E28" s="211"/>
+      <c r="F28" s="211"/>
+      <c r="G28" s="211"/>
+      <c r="H28" s="211"/>
+      <c r="I28" s="211"/>
+      <c r="J28" s="211"/>
+      <c r="K28" s="211"/>
+      <c r="L28" s="211"/>
+      <c r="M28" s="211"/>
+      <c r="N28" s="211"/>
+      <c r="O28" s="211"/>
+      <c r="P28" s="211"/>
+      <c r="Q28" s="211"/>
       <c r="R28" s="40"/>
       <c r="S28" s="40"/>
       <c r="T28" s="40"/>
@@ -10223,69 +10281,69 @@
       <c r="AX28" s="30"/>
     </row>
     <row r="29" spans="1:144" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="210" t="s">
+      <c r="A29" s="212" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="210"/>
-      <c r="C29" s="210"/>
-      <c r="D29" s="210"/>
-      <c r="E29" s="210"/>
-      <c r="F29" s="210"/>
-      <c r="G29" s="210"/>
-      <c r="H29" s="210"/>
-      <c r="I29" s="210"/>
-      <c r="J29" s="210"/>
-      <c r="K29" s="210"/>
-      <c r="L29" s="210"/>
-      <c r="M29" s="210"/>
-      <c r="N29" s="210"/>
-      <c r="O29" s="210"/>
-      <c r="P29" s="210"/>
-      <c r="Q29" s="210"/>
-      <c r="R29" s="210"/>
-      <c r="S29" s="210"/>
-      <c r="T29" s="210"/>
-      <c r="U29" s="210"/>
-      <c r="V29" s="210"/>
-      <c r="W29" s="210"/>
-      <c r="X29" s="210"/>
-      <c r="Y29" s="210"/>
-      <c r="Z29" s="210"/>
-      <c r="AA29" s="210"/>
-      <c r="AB29" s="210"/>
-      <c r="AC29" s="210"/>
-      <c r="AD29" s="210"/>
-      <c r="AE29" s="210"/>
-      <c r="AF29" s="210"/>
-      <c r="AG29" s="210"/>
-      <c r="AH29" s="210"/>
-      <c r="AI29" s="210"/>
-      <c r="AJ29" s="210"/>
-      <c r="AK29" s="210"/>
-      <c r="AL29" s="210"/>
-      <c r="AM29" s="210"/>
-      <c r="AN29" s="210"/>
-      <c r="AO29" s="210"/>
-      <c r="AP29" s="210"/>
-      <c r="AQ29" s="210"/>
-      <c r="AR29" s="210"/>
-      <c r="AS29" s="210"/>
-      <c r="AT29" s="210"/>
-      <c r="AU29" s="210"/>
-      <c r="AV29" s="210"/>
-      <c r="AW29" s="210"/>
-      <c r="AX29" s="210"/>
+      <c r="B29" s="212"/>
+      <c r="C29" s="212"/>
+      <c r="D29" s="212"/>
+      <c r="E29" s="212"/>
+      <c r="F29" s="212"/>
+      <c r="G29" s="212"/>
+      <c r="H29" s="212"/>
+      <c r="I29" s="212"/>
+      <c r="J29" s="212"/>
+      <c r="K29" s="212"/>
+      <c r="L29" s="212"/>
+      <c r="M29" s="212"/>
+      <c r="N29" s="212"/>
+      <c r="O29" s="212"/>
+      <c r="P29" s="212"/>
+      <c r="Q29" s="212"/>
+      <c r="R29" s="212"/>
+      <c r="S29" s="212"/>
+      <c r="T29" s="212"/>
+      <c r="U29" s="212"/>
+      <c r="V29" s="212"/>
+      <c r="W29" s="212"/>
+      <c r="X29" s="212"/>
+      <c r="Y29" s="212"/>
+      <c r="Z29" s="212"/>
+      <c r="AA29" s="212"/>
+      <c r="AB29" s="212"/>
+      <c r="AC29" s="212"/>
+      <c r="AD29" s="212"/>
+      <c r="AE29" s="212"/>
+      <c r="AF29" s="212"/>
+      <c r="AG29" s="212"/>
+      <c r="AH29" s="212"/>
+      <c r="AI29" s="212"/>
+      <c r="AJ29" s="212"/>
+      <c r="AK29" s="212"/>
+      <c r="AL29" s="212"/>
+      <c r="AM29" s="212"/>
+      <c r="AN29" s="212"/>
+      <c r="AO29" s="212"/>
+      <c r="AP29" s="212"/>
+      <c r="AQ29" s="212"/>
+      <c r="AR29" s="212"/>
+      <c r="AS29" s="212"/>
+      <c r="AT29" s="212"/>
+      <c r="AU29" s="212"/>
+      <c r="AV29" s="212"/>
+      <c r="AW29" s="212"/>
+      <c r="AX29" s="212"/>
     </row>
     <row r="30" spans="1:144" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="211" t="s">
+      <c r="A30" s="213" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="211"/>
-      <c r="C30" s="211"/>
-      <c r="D30" s="211"/>
-      <c r="E30" s="211"/>
-      <c r="F30" s="210"/>
-      <c r="G30" s="210"/>
+      <c r="B30" s="213"/>
+      <c r="C30" s="213"/>
+      <c r="D30" s="213"/>
+      <c r="E30" s="213"/>
+      <c r="F30" s="212"/>
+      <c r="G30" s="212"/>
       <c r="H30" s="19"/>
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
@@ -10327,10 +10385,10 @@
       <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="212" t="s">
+      <c r="D31" s="214" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="213"/>
+      <c r="E31" s="215"/>
       <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:144" x14ac:dyDescent="0.3">
@@ -10345,11 +10403,11 @@
         <f>C33*98*63/194/201</f>
         <v>460.27127250346206</v>
       </c>
-      <c r="D32" s="214">
+      <c r="D32" s="216">
         <f t="shared" ref="D32:D37" si="33">(B32+C32)/1</f>
         <v>476.23114325280812</v>
       </c>
-      <c r="E32" s="215"/>
+      <c r="E32" s="217"/>
       <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.3">
@@ -10363,11 +10421,11 @@
       <c r="C33" s="10">
         <v>2907</v>
       </c>
-      <c r="D33" s="216">
+      <c r="D33" s="218">
         <f t="shared" si="33"/>
         <v>3007.8</v>
       </c>
-      <c r="E33" s="217"/>
+      <c r="E33" s="219"/>
       <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:49" x14ac:dyDescent="0.3">
@@ -10382,11 +10440,11 @@
         <f>4*AFR44tier1</f>
         <v>11628</v>
       </c>
-      <c r="D34" s="216">
+      <c r="D34" s="218">
         <f t="shared" si="33"/>
         <v>12031.2</v>
       </c>
-      <c r="E34" s="217"/>
+      <c r="E34" s="219"/>
       <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:49" x14ac:dyDescent="0.3">
@@ -10400,11 +10458,11 @@
       <c r="C35" s="98">
         <v>13005</v>
       </c>
-      <c r="D35" s="216">
+      <c r="D35" s="218">
         <f t="shared" si="33"/>
         <v>13475.4</v>
       </c>
-      <c r="E35" s="217"/>
+      <c r="E35" s="219"/>
       <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:49" x14ac:dyDescent="0.3">
@@ -10419,11 +10477,11 @@
         <f>C33*125*97/194/201</f>
         <v>903.91791044776119</v>
       </c>
-      <c r="D36" s="216">
+      <c r="D36" s="218">
         <f t="shared" si="33"/>
         <v>932.02992768118168</v>
       </c>
-      <c r="E36" s="217"/>
+      <c r="E36" s="219"/>
       <c r="F36" s="26"/>
     </row>
     <row r="37" spans="1:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10438,34 +10496,34 @@
         <f>C33*116*133/194/201</f>
         <v>1150.1563317433452</v>
       </c>
-      <c r="D37" s="218">
+      <c r="D37" s="220">
         <f t="shared" si="33"/>
         <v>1190.0379135251578</v>
       </c>
-      <c r="E37" s="219"/>
+      <c r="E37" s="221"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A38" s="204" t="s">
+      <c r="A38" s="206" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="204"/>
-      <c r="C38" s="204"/>
-      <c r="D38" s="204"/>
-      <c r="E38" s="204"/>
-      <c r="F38" s="205"/>
-      <c r="G38" s="205"/>
+      <c r="B38" s="206"/>
+      <c r="C38" s="206"/>
+      <c r="D38" s="206"/>
+      <c r="E38" s="206"/>
+      <c r="F38" s="207"/>
+      <c r="G38" s="207"/>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A39" s="205" t="s">
+      <c r="A39" s="207" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="205"/>
-      <c r="C39" s="205"/>
-      <c r="D39" s="205"/>
-      <c r="E39" s="205"/>
-      <c r="F39" s="205"/>
-      <c r="G39" s="205"/>
+      <c r="B39" s="207"/>
+      <c r="C39" s="207"/>
+      <c r="D39" s="207"/>
+      <c r="E39" s="207"/>
+      <c r="F39" s="207"/>
+      <c r="G39" s="207"/>
       <c r="H39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
@@ -10528,10 +10586,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW18"/>
+  <dimension ref="A1:BX18"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView view="pageBreakPreview" topLeftCell="P1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10555,58 +10613,58 @@
     <col min="17" max="17" width="19.6640625" customWidth="1"/>
     <col min="18" max="18" width="26.33203125" customWidth="1"/>
     <col min="19" max="19" width="17.88671875" customWidth="1"/>
-    <col min="20" max="20" width="16.6640625" style="62" customWidth="1"/>
-    <col min="21" max="22" width="19" customWidth="1"/>
-    <col min="23" max="23" width="23.6640625" customWidth="1"/>
-    <col min="24" max="24" width="16.6640625" customWidth="1"/>
-    <col min="25" max="25" width="17.6640625" customWidth="1"/>
-    <col min="26" max="27" width="18.88671875" customWidth="1"/>
-    <col min="28" max="28" width="18.33203125" customWidth="1"/>
-    <col min="29" max="30" width="18.44140625" customWidth="1"/>
-    <col min="31" max="31" width="12.88671875" customWidth="1"/>
-    <col min="32" max="32" width="19.5546875" customWidth="1"/>
-    <col min="33" max="33" width="15.109375" customWidth="1"/>
-    <col min="34" max="34" width="15.21875" customWidth="1"/>
-    <col min="35" max="35" width="22.44140625" customWidth="1"/>
-    <col min="36" max="36" width="23" customWidth="1"/>
-    <col min="37" max="37" width="19.44140625" customWidth="1"/>
-    <col min="38" max="38" width="22.21875" customWidth="1"/>
-    <col min="39" max="39" width="20.109375" customWidth="1"/>
-    <col min="40" max="40" width="22.109375" customWidth="1"/>
-    <col min="41" max="41" width="21" customWidth="1"/>
-    <col min="42" max="42" width="16.88671875" customWidth="1"/>
-    <col min="43" max="43" width="18.44140625" customWidth="1"/>
-    <col min="44" max="44" width="17.44140625" customWidth="1"/>
-    <col min="45" max="45" width="23" customWidth="1"/>
-    <col min="46" max="46" width="21.44140625" customWidth="1"/>
-    <col min="47" max="48" width="19.44140625" customWidth="1"/>
-    <col min="70" max="75" width="8.88671875" style="26"/>
+    <col min="20" max="21" width="16.6640625" style="62" customWidth="1"/>
+    <col min="22" max="23" width="19" customWidth="1"/>
+    <col min="24" max="24" width="23.6640625" customWidth="1"/>
+    <col min="25" max="25" width="16.6640625" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" customWidth="1"/>
+    <col min="27" max="28" width="18.88671875" customWidth="1"/>
+    <col min="29" max="29" width="18.33203125" customWidth="1"/>
+    <col min="30" max="31" width="18.44140625" customWidth="1"/>
+    <col min="32" max="32" width="12.88671875" customWidth="1"/>
+    <col min="33" max="33" width="19.5546875" customWidth="1"/>
+    <col min="34" max="34" width="15.109375" customWidth="1"/>
+    <col min="35" max="35" width="15.21875" customWidth="1"/>
+    <col min="36" max="36" width="22.44140625" customWidth="1"/>
+    <col min="37" max="37" width="23" customWidth="1"/>
+    <col min="38" max="38" width="19.44140625" customWidth="1"/>
+    <col min="39" max="39" width="22.21875" customWidth="1"/>
+    <col min="40" max="40" width="20.109375" customWidth="1"/>
+    <col min="41" max="41" width="22.109375" customWidth="1"/>
+    <col min="42" max="42" width="21" customWidth="1"/>
+    <col min="43" max="43" width="16.88671875" customWidth="1"/>
+    <col min="44" max="44" width="18.44140625" customWidth="1"/>
+    <col min="45" max="45" width="17.44140625" customWidth="1"/>
+    <col min="46" max="46" width="23" customWidth="1"/>
+    <col min="47" max="47" width="21.44140625" customWidth="1"/>
+    <col min="48" max="49" width="19.44140625" customWidth="1"/>
+    <col min="71" max="76" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="220" t="s">
+    <row r="1" spans="1:76" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="222" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
-      <c r="Q1" s="220"/>
-      <c r="R1" s="220"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="222"/>
+      <c r="K1" s="222"/>
+      <c r="L1" s="222"/>
+      <c r="M1" s="222"/>
+      <c r="N1" s="222"/>
+      <c r="O1" s="222"/>
+      <c r="P1" s="222"/>
+      <c r="Q1" s="222"/>
+      <c r="R1" s="222"/>
       <c r="S1" s="104"/>
       <c r="T1" s="64"/>
-      <c r="U1" s="20"/>
+      <c r="U1" s="64"/>
       <c r="V1" s="20"/>
       <c r="W1" s="20"/>
       <c r="X1" s="20"/>
@@ -10622,36 +10680,37 @@
       <c r="AH1" s="20"/>
       <c r="AI1" s="20"/>
       <c r="AJ1" s="20"/>
-      <c r="AK1" s="26"/>
-      <c r="AM1" s="20"/>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="26"/>
       <c r="AN1" s="20"/>
       <c r="AO1" s="20"/>
       <c r="AP1" s="20"/>
       <c r="AQ1" s="20"/>
       <c r="AR1" s="20"/>
       <c r="AS1" s="20"/>
-      <c r="AU1" s="26"/>
+      <c r="AT1" s="20"/>
       <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
     </row>
-    <row r="2" spans="1:75" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:76" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="54">
         <f>GeneralRemarks!A2</f>
-        <v>41901</v>
-      </c>
-      <c r="B2" s="221"/>
-      <c r="C2" s="221"/>
-      <c r="D2" s="221"/>
+        <v>41954</v>
+      </c>
+      <c r="B2" s="223"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
       <c r="E2" s="138"/>
       <c r="F2" s="138"/>
       <c r="G2" s="138"/>
       <c r="H2" s="138"/>
       <c r="I2" s="138"/>
-      <c r="J2" s="221"/>
-      <c r="K2" s="221"/>
-      <c r="L2" s="221"/>
-      <c r="M2" s="221"/>
-      <c r="N2" s="221"/>
-      <c r="O2" s="221"/>
+      <c r="J2" s="223"/>
+      <c r="K2" s="223"/>
+      <c r="L2" s="223"/>
+      <c r="M2" s="223"/>
+      <c r="N2" s="223"/>
+      <c r="O2" s="223"/>
       <c r="P2" s="21"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
@@ -10659,8 +10718,8 @@
       <c r="T2" s="20"/>
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="54"/>
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
       <c r="AA2" s="20"/>
@@ -10673,21 +10732,22 @@
       <c r="AH2" s="20"/>
       <c r="AI2" s="20"/>
       <c r="AJ2" s="20"/>
-      <c r="AK2" s="26"/>
-      <c r="AM2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="26"/>
       <c r="AN2" s="20"/>
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
       <c r="AQ2" s="20"/>
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
-      <c r="AU2" s="52">
+      <c r="AT2" s="20"/>
+      <c r="AV2" s="52">
         <f>A2</f>
-        <v>41901</v>
-      </c>
-      <c r="AV2" s="26"/>
+        <v>41954</v>
+      </c>
+      <c r="AW2" s="26"/>
     </row>
-    <row r="3" spans="1:75" s="1" customFormat="1" ht="32.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:76" s="1" customFormat="1" ht="32.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="79" t="s">
         <v>88</v>
       </c>
@@ -10767,65 +10827,65 @@
         <f>AllEntries!T7</f>
         <v>CNRM</v>
       </c>
-      <c r="U3" s="110" t="str">
+      <c r="U3" s="80" t="str">
         <f>AllEntries!U7</f>
-        <v>KNMI</v>
+        <v>CNRM</v>
       </c>
       <c r="V3" s="110" t="str">
         <f>AllEntries!V7</f>
         <v>KNMI</v>
       </c>
-      <c r="W3" s="125" t="str">
+      <c r="W3" s="110" t="str">
         <f>AllEntries!W7</f>
         <v>KNMI</v>
       </c>
-      <c r="X3" s="139" t="str">
+      <c r="X3" s="125" t="str">
         <f>AllEntries!X7</f>
+        <v>KNMI</v>
+      </c>
+      <c r="Y3" s="139" t="str">
+        <f>AllEntries!Y7</f>
         <v>UQAM</v>
-      </c>
-      <c r="Y3" s="80" t="str">
-        <f>AllEntries!Y7</f>
-        <v>UCLM</v>
       </c>
       <c r="Z3" s="80" t="str">
         <f>AllEntries!Z7</f>
+        <v>UCLM</v>
+      </c>
+      <c r="AA3" s="80" t="str">
+        <f>AllEntries!AA7</f>
         <v>ICTP</v>
       </c>
-      <c r="AA3" s="139" t="str">
-        <f>AllEntries!AA7</f>
+      <c r="AB3" s="139" t="str">
+        <f>AllEntries!AB7</f>
         <v>ENEA</v>
-      </c>
-      <c r="AB3" s="80" t="str">
-        <f>AllEntries!AB7</f>
-        <v>CUNI</v>
       </c>
       <c r="AC3" s="80" t="str">
         <f>AllEntries!AC7</f>
-        <v>DHMZ</v>
+        <v>CUNI</v>
       </c>
       <c r="AD3" s="80" t="str">
         <f>AllEntries!AD7</f>
+        <v>DHMZ</v>
+      </c>
+      <c r="AE3" s="80" t="str">
+        <f>AllEntries!AE7</f>
         <v>IITM</v>
-      </c>
-      <c r="AE3" s="139" t="str">
-        <f>AllEntries!AE7</f>
-        <v>GISS</v>
       </c>
       <c r="AF3" s="139" t="str">
         <f>AllEntries!AF7</f>
+        <v>GISS</v>
+      </c>
+      <c r="AG3" s="139" t="str">
+        <f>AllEntries!AG7</f>
         <v>CCCma</v>
       </c>
-      <c r="AG3" s="80" t="str">
-        <f>AllEntries!AG7</f>
+      <c r="AH3" s="80" t="str">
+        <f>AllEntries!AH7</f>
         <v>CSIRO</v>
       </c>
-      <c r="AH3" s="139" t="str">
-        <f>AllEntries!AH7</f>
+      <c r="AI3" s="139" t="str">
+        <f>AllEntries!AI7</f>
         <v>KAUST</v>
-      </c>
-      <c r="AI3" s="80" t="str">
-        <f>AllEntries!AI7</f>
-        <v>MOHC</v>
       </c>
       <c r="AJ3" s="80" t="str">
         <f>AllEntries!AJ7</f>
@@ -10833,54 +10893,57 @@
       </c>
       <c r="AK3" s="80" t="str">
         <f>AllEntries!AK7</f>
+        <v>MOHC</v>
+      </c>
+      <c r="AL3" s="80" t="str">
+        <f>AllEntries!AL7</f>
         <v>MIUB</v>
       </c>
-      <c r="AL3" s="125" t="str">
-        <f>AllEntries!AL7</f>
+      <c r="AM3" s="125" t="str">
+        <f>AllEntries!AM7</f>
         <v>BCCR</v>
-      </c>
-      <c r="AM3" s="80" t="str">
-        <f>AllEntries!AM7</f>
-        <v>CRP-GL</v>
       </c>
       <c r="AN3" s="80" t="str">
         <f>AllEntries!AN7</f>
-        <v>IDL</v>
+        <v>CRP-GL</v>
       </c>
       <c r="AO3" s="80" t="str">
         <f>AllEntries!AO7</f>
-        <v>IPSL-INERIS</v>
+        <v>IDL</v>
       </c>
       <c r="AP3" s="80" t="str">
         <f>AllEntries!AP7</f>
-        <v>AUTH-Met</v>
+        <v>IPSL-INERIS</v>
       </c>
       <c r="AQ3" s="80" t="str">
         <f>AllEntries!AQ7</f>
-        <v>AUTH-LHTEE</v>
+        <v>AUTH-Met</v>
       </c>
       <c r="AR3" s="80" t="str">
         <f>AllEntries!AR7</f>
-        <v>NUIM</v>
+        <v>AUTH-LHTEE</v>
       </c>
       <c r="AS3" s="80" t="str">
         <f>AllEntries!AS7</f>
-        <v>UHOH</v>
+        <v>NUIM</v>
       </c>
       <c r="AT3" s="80" t="str">
         <f>AllEntries!AT7</f>
-        <v>UM</v>
+        <v>UHOH</v>
       </c>
       <c r="AU3" s="80" t="str">
         <f>AllEntries!AU7</f>
-        <v>UCAN</v>
-      </c>
-      <c r="AV3" s="162" t="str">
+        <v>UM</v>
+      </c>
+      <c r="AV3" s="80" t="str">
         <f>AllEntries!AV7</f>
         <v>UCAN</v>
       </c>
-      <c r="AW3" s="207"/>
-      <c r="AX3" s="2"/>
+      <c r="AW3" s="162" t="str">
+        <f>AllEntries!AW7</f>
+        <v>UCAN</v>
+      </c>
+      <c r="AX3" s="209"/>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
@@ -10906,8 +10969,9 @@
       <c r="BU3" s="2"/>
       <c r="BV3" s="2"/>
       <c r="BW3" s="2"/>
+      <c r="BX3" s="2"/>
     </row>
-    <row r="4" spans="1:75" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:76" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="149" t="s">
         <v>182</v>
       </c>
@@ -10989,7 +11053,7 @@
       </c>
       <c r="U4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!U9),"",AllEntries!U9)</f>
-        <v>Royal Netherlands Meteorological Institute, De Bilt, The Netherlands</v>
+        <v>Centre National de Recherches Meteorologiques</v>
       </c>
       <c r="V4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!V9),"",AllEntries!V9)</f>
@@ -10999,53 +11063,53 @@
         <f>IF(ISBLANK(AllEntries!W9),"",AllEntries!W9)</f>
         <v>Royal Netherlands Meteorological Institute, De Bilt, The Netherlands</v>
       </c>
-      <c r="X4" s="152" t="str">
+      <c r="X4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!X9),"",AllEntries!X9)</f>
+        <v>Royal Netherlands Meteorological Institute, De Bilt, The Netherlands</v>
+      </c>
+      <c r="Y4" s="152" t="str">
+        <f>IF(ISBLANK(AllEntries!Y9),"",AllEntries!Y9)</f>
         <v>Universite du Quebec a Montreal</v>
-      </c>
-      <c r="Y4" s="150" t="str">
-        <f>IF(ISBLANK(AllEntries!Y9),"",AllEntries!Y9)</f>
-        <v>University of Castilla-La Mancha, Toledo, Spain</v>
       </c>
       <c r="Z4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!Z9),"",AllEntries!Z9)</f>
+        <v>University of Castilla-La Mancha, Toledo, Spain</v>
+      </c>
+      <c r="AA4" s="150" t="str">
+        <f>IF(ISBLANK(AllEntries!AA9),"",AllEntries!AA9)</f>
         <v xml:space="preserve"> Abdus Salam International Centre for Theoretical Physics</v>
       </c>
-      <c r="AA4" s="152" t="str">
-        <f>IF(ISBLANK(AllEntries!AA9),"",AllEntries!AA9)</f>
+      <c r="AB4" s="152" t="str">
+        <f>IF(ISBLANK(AllEntries!AB9),"",AllEntries!AB9)</f>
         <v>Italian National Agency for New Technologies, Energy and Sustainable Economic Development</v>
-      </c>
-      <c r="AB4" s="150" t="str">
-        <f>IF(ISBLANK(AllEntries!AB9),"",AllEntries!AB9)</f>
-        <v/>
       </c>
       <c r="AC4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AC9),"",AllEntries!AC9)</f>
-        <v>Meteorological and Hydrological Service of Croatia</v>
+        <v/>
       </c>
       <c r="AD4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AD9),"",AllEntries!AD9)</f>
-        <v>Indian Institute of Tropical Meteorology</v>
+        <v>Meteorological and Hydrological Service of Croatia</v>
       </c>
       <c r="AE4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AE9),"",AllEntries!AE9)</f>
-        <v/>
+        <v>Indian Institute of Tropical Meteorology</v>
       </c>
       <c r="AF4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AF9),"",AllEntries!AF9)</f>
-        <v>CCCma (Canadian Centre for Climate Modelling and Analysis, Victoria, BC, Canada)</v>
+        <v/>
       </c>
       <c r="AG4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AG9),"",AllEntries!AG9)</f>
-        <v>Commonwealth Scientific and Industrial Research Organisation</v>
+        <v>CCCma (Canadian Centre for Climate Modelling and Analysis, Victoria, BC, Canada)</v>
       </c>
       <c r="AH4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AH9),"",AllEntries!AH9)</f>
-        <v/>
+        <v>Commonwealth Scientific and Industrial Research Organisation</v>
       </c>
       <c r="AI4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AI9),"",AllEntries!AI9)</f>
-        <v>Met Office Hadley Centre</v>
+        <v>King Abdullah University, Thuwal, Saudi Arabien</v>
       </c>
       <c r="AJ4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AJ9),"",AllEntries!AJ9)</f>
@@ -11053,15 +11117,15 @@
       </c>
       <c r="AK4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AK9),"",AllEntries!AK9)</f>
-        <v/>
+        <v>Met Office Hadley Centre</v>
       </c>
       <c r="AL4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AL9),"",AllEntries!AL9)</f>
-        <v>Bjerknes Centre for Climate Research</v>
+        <v/>
       </c>
       <c r="AM4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AM9),"",AllEntries!AM9)</f>
-        <v/>
+        <v>Bjerknes Centre for Climate Research</v>
       </c>
       <c r="AN4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AN9),"",AllEntries!AN9)</f>
@@ -11081,11 +11145,11 @@
       </c>
       <c r="AR4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AR9),"",AllEntries!AR9)</f>
-        <v>National University of Ireland Maynooth</v>
+        <v/>
       </c>
       <c r="AS4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AS9),"",AllEntries!AS9)</f>
-        <v/>
+        <v>National University of Ireland Maynooth</v>
       </c>
       <c r="AT4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AT9),"",AllEntries!AT9)</f>
@@ -11095,12 +11159,15 @@
         <f>IF(ISBLANK(AllEntries!AU9),"",AllEntries!AU9)</f>
         <v/>
       </c>
-      <c r="AV4" s="163" t="str">
+      <c r="AV4" s="150" t="str">
         <f>IF(ISBLANK(AllEntries!AV9),"",AllEntries!AV9)</f>
         <v/>
       </c>
-      <c r="AW4" s="207"/>
-      <c r="AX4" s="2"/>
+      <c r="AW4" s="163" t="str">
+        <f>IF(ISBLANK(AllEntries!AW9),"",AllEntries!AW9)</f>
+        <v/>
+      </c>
+      <c r="AX4" s="209"/>
       <c r="AY4" s="2"/>
       <c r="AZ4" s="2"/>
       <c r="BA4" s="2"/>
@@ -11126,8 +11193,9 @@
       <c r="BU4" s="2"/>
       <c r="BV4" s="2"/>
       <c r="BW4" s="2"/>
+      <c r="BX4" s="2"/>
     </row>
-    <row r="5" spans="1:75" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:76" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="155" t="s">
         <v>86</v>
       </c>
@@ -11205,39 +11273,39 @@
       </c>
       <c r="T5" s="65" t="str">
         <f>AllEntries!T8</f>
+        <v>ALADIN53</v>
+      </c>
+      <c r="U5" s="65" t="str">
+        <f>AllEntries!U8</f>
         <v>ARPEGE52</v>
-      </c>
-      <c r="U5" s="111" t="str">
-        <f>AllEntries!U8</f>
-        <v>RACMO22E</v>
       </c>
       <c r="V5" s="111" t="str">
         <f>AllEntries!V8</f>
+        <v>RACMO22E</v>
+      </c>
+      <c r="W5" s="111" t="str">
+        <f>AllEntries!W8</f>
         <v>RACMO21P</v>
       </c>
-      <c r="W5" s="126" t="str">
-        <f>AllEntries!W8</f>
+      <c r="X5" s="126" t="str">
+        <f>AllEntries!X8</f>
         <v>RACMO22T</v>
       </c>
-      <c r="X5" s="140" t="str">
-        <f>AllEntries!X8</f>
+      <c r="Y5" s="140" t="str">
+        <f>AllEntries!Y8</f>
         <v>CRCM5</v>
-      </c>
-      <c r="Y5" s="65" t="str">
-        <f>AllEntries!Y8</f>
-        <v>PROMES</v>
       </c>
       <c r="Z5" s="65" t="str">
         <f>AllEntries!Z8</f>
-        <v>RegCM4-3</v>
-      </c>
-      <c r="AA5" s="140" t="str">
+        <v>PROMES</v>
+      </c>
+      <c r="AA5" s="65" t="str">
         <f>AllEntries!AA8</f>
         <v>RegCM4-3</v>
       </c>
-      <c r="AB5" s="65" t="str">
+      <c r="AB5" s="140" t="str">
         <f>AllEntries!AB8</f>
-        <v>RegCM4-2</v>
+        <v>RegCM4-3</v>
       </c>
       <c r="AC5" s="65" t="str">
         <f>AllEntries!AC8</f>
@@ -11245,82 +11313,85 @@
       </c>
       <c r="AD5" s="65" t="str">
         <f>AllEntries!AD8</f>
+        <v>RegCM4-2</v>
+      </c>
+      <c r="AE5" s="65" t="str">
+        <f>AllEntries!AE8</f>
         <v>RegCM4-1</v>
-      </c>
-      <c r="AE5" s="140" t="str">
-        <f>AllEntries!AE8</f>
-        <v>RM3</v>
       </c>
       <c r="AF5" s="140" t="str">
         <f>AllEntries!AF8</f>
+        <v>RM3</v>
+      </c>
+      <c r="AG5" s="140" t="str">
+        <f>AllEntries!AG8</f>
         <v>CanRCM4</v>
       </c>
-      <c r="AG5" s="65" t="str">
-        <f>AllEntries!AG8</f>
+      <c r="AH5" s="65" t="str">
+        <f>AllEntries!AH8</f>
         <v>CCAM</v>
       </c>
-      <c r="AH5" s="140" t="str">
-        <f>AllEntries!AH8</f>
+      <c r="AI5" s="140" t="str">
+        <f>AllEntries!AI8</f>
         <v>GFDL</v>
-      </c>
-      <c r="AI5" s="65" t="str">
-        <f>AllEntries!AI8</f>
-        <v>HadGEM3-RA</v>
       </c>
       <c r="AJ5" s="65" t="str">
         <f>AllEntries!AJ8</f>
-        <v>HadRM3P</v>
+        <v>HadGEM3-RA</v>
       </c>
       <c r="AK5" s="65" t="str">
         <f>AllEntries!AK8</f>
+        <v>HadRM3P</v>
+      </c>
+      <c r="AL5" s="65" t="str">
+        <f>AllEntries!AL8</f>
         <v>WRF331A</v>
       </c>
-      <c r="AL5" s="126" t="str">
-        <f>AllEntries!AL8</f>
+      <c r="AM5" s="126" t="str">
+        <f>AllEntries!AM8</f>
         <v>WRF331C</v>
-      </c>
-      <c r="AM5" s="65" t="str">
-        <f>AllEntries!AM8</f>
-        <v>WRF331A</v>
       </c>
       <c r="AN5" s="65" t="str">
         <f>AllEntries!AN8</f>
-        <v>WRF331D</v>
+        <v>WRF331A</v>
       </c>
       <c r="AO5" s="65" t="str">
         <f>AllEntries!AO8</f>
-        <v>WRF331F</v>
+        <v>WRF331D</v>
       </c>
       <c r="AP5" s="65" t="str">
         <f>AllEntries!AP8</f>
-        <v>WRF331A</v>
+        <v>WRF331F</v>
       </c>
       <c r="AQ5" s="65" t="str">
         <f>AllEntries!AQ8</f>
-        <v>WRF321B</v>
+        <v>WRF331A</v>
       </c>
       <c r="AR5" s="65" t="str">
         <f>AllEntries!AR8</f>
-        <v>WRF341E</v>
+        <v>WRF321B</v>
       </c>
       <c r="AS5" s="65" t="str">
         <f>AllEntries!AS8</f>
-        <v>WRF331H</v>
+        <v>WRF341E</v>
       </c>
       <c r="AT5" s="65" t="str">
         <f>AllEntries!AT8</f>
-        <v>WRF331</v>
+        <v>WRF331H</v>
       </c>
       <c r="AU5" s="65" t="str">
         <f>AllEntries!AU8</f>
+        <v>WRF331</v>
+      </c>
+      <c r="AV5" s="65" t="str">
+        <f>AllEntries!AV8</f>
         <v>WRF331G</v>
       </c>
-      <c r="AV5" s="164" t="str">
-        <f>AllEntries!AV8</f>
+      <c r="AW5" s="164" t="str">
+        <f>AllEntries!AW8</f>
         <v>WRF350I</v>
       </c>
-      <c r="AW5" s="207"/>
-      <c r="AX5" s="2"/>
+      <c r="AX5" s="209"/>
       <c r="AY5" s="2"/>
       <c r="AZ5" s="2"/>
       <c r="BA5" s="2"/>
@@ -11346,8 +11417,9 @@
       <c r="BU5" s="2"/>
       <c r="BV5" s="2"/>
       <c r="BW5" s="2"/>
+      <c r="BX5" s="2"/>
     </row>
-    <row r="6" spans="1:75" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:76" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="76" t="s">
         <v>87</v>
       </c>
@@ -11424,123 +11496,126 @@
         <v>CNRM-ALADIN52</v>
       </c>
       <c r="T6" s="65" t="str">
-        <f t="shared" ref="T6" si="17">IF(ISBLANK(T9),"",CONCATENATE(T3,"-",T5))</f>
+        <f t="shared" ref="T6:U6" si="17">IF(ISBLANK(T9),"",CONCATENATE(T3,"-",T5))</f>
+        <v>CNRM-ALADIN53</v>
+      </c>
+      <c r="U6" s="65" t="str">
+        <f t="shared" si="17"/>
         <v>CNRM-ARPEGE52</v>
       </c>
-      <c r="U6" s="65" t="str">
-        <f t="shared" ref="U6" si="18">IF(ISBLANK(U9),"",CONCATENATE(U3,"-",U5))</f>
+      <c r="V6" s="65" t="str">
+        <f t="shared" ref="V6" si="18">IF(ISBLANK(V9),"",CONCATENATE(V3,"-",V5))</f>
         <v>KNMI-RACMO22E</v>
       </c>
-      <c r="V6" s="65" t="str">
-        <f t="shared" ref="V6" si="19">IF(ISBLANK(V9),"",CONCATENATE(V3,"-",V5))</f>
+      <c r="W6" s="65" t="str">
+        <f t="shared" ref="W6" si="19">IF(ISBLANK(W9),"",CONCATENATE(W3,"-",W5))</f>
         <v>KNMI-RACMO21P</v>
       </c>
-      <c r="W6" s="65" t="str">
-        <f t="shared" ref="W6" si="20">IF(ISBLANK(W9),"",CONCATENATE(W3,"-",W5))</f>
+      <c r="X6" s="65" t="str">
+        <f t="shared" ref="X6" si="20">IF(ISBLANK(X9),"",CONCATENATE(X3,"-",X5))</f>
         <v>KNMI-RACMO22T</v>
       </c>
-      <c r="X6" s="140" t="str">
-        <f t="shared" ref="X6" si="21">IF(ISBLANK(X9),"",CONCATENATE(X3,"-",X5))</f>
+      <c r="Y6" s="140" t="str">
+        <f t="shared" ref="Y6" si="21">IF(ISBLANK(Y9),"",CONCATENATE(Y3,"-",Y5))</f>
         <v/>
       </c>
-      <c r="Y6" s="65" t="str">
-        <f t="shared" ref="Y6" si="22">IF(ISBLANK(Y9),"",CONCATENATE(Y3,"-",Y5))</f>
+      <c r="Z6" s="65" t="str">
+        <f t="shared" ref="Z6" si="22">IF(ISBLANK(Z9),"",CONCATENATE(Z3,"-",Z5))</f>
         <v>UCLM-PROMES</v>
       </c>
-      <c r="Z6" s="65" t="str">
-        <f t="shared" ref="Z6:AA6" si="23">IF(ISBLANK(Z9),"",CONCATENATE(Z3,"-",Z5))</f>
+      <c r="AA6" s="65" t="str">
+        <f t="shared" ref="AA6:AB6" si="23">IF(ISBLANK(AA9),"",CONCATENATE(AA3,"-",AA5))</f>
         <v>ICTP-RegCM4-3</v>
       </c>
-      <c r="AA6" s="140" t="str">
+      <c r="AB6" s="140" t="str">
         <f t="shared" si="23"/>
         <v/>
       </c>
-      <c r="AB6" s="65" t="str">
-        <f t="shared" ref="AB6" si="24">IF(ISBLANK(AB9),"",CONCATENATE(AB3,"-",AB5))</f>
+      <c r="AC6" s="65" t="str">
+        <f t="shared" ref="AC6" si="24">IF(ISBLANK(AC9),"",CONCATENATE(AC3,"-",AC5))</f>
         <v>CUNI-RegCM4-2</v>
       </c>
-      <c r="AC6" s="65" t="str">
-        <f t="shared" ref="AC6" si="25">IF(ISBLANK(AC9),"",CONCATENATE(AC3,"-",AC5))</f>
+      <c r="AD6" s="65" t="str">
+        <f t="shared" ref="AD6" si="25">IF(ISBLANK(AD9),"",CONCATENATE(AD3,"-",AD5))</f>
         <v>DHMZ-RegCM4-2</v>
       </c>
-      <c r="AD6" s="65" t="str">
-        <f t="shared" ref="AD6" si="26">IF(ISBLANK(AD9),"",CONCATENATE(AD3,"-",AD5))</f>
+      <c r="AE6" s="65" t="str">
+        <f t="shared" ref="AE6" si="26">IF(ISBLANK(AE9),"",CONCATENATE(AE3,"-",AE5))</f>
         <v>IITM-RegCM4-1</v>
       </c>
-      <c r="AE6" s="140" t="str">
-        <f t="shared" ref="AE6:AV6" si="27">IF(ISBLANK(AE9),"",CONCATENATE(AE3,"-",AE5))</f>
+      <c r="AF6" s="140" t="str">
+        <f t="shared" ref="AF6:AW6" si="27">IF(ISBLANK(AF9),"",CONCATENATE(AF3,"-",AF5))</f>
         <v/>
       </c>
-      <c r="AF6" s="140" t="str">
+      <c r="AG6" s="140" t="str">
         <f t="shared" si="27"/>
         <v/>
       </c>
-      <c r="AG6" s="65" t="str">
+      <c r="AH6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>CSIRO-CCAM</v>
       </c>
-      <c r="AH6" s="140" t="str">
+      <c r="AI6" s="140" t="str">
         <f t="shared" si="27"/>
         <v/>
       </c>
-      <c r="AI6" s="65" t="str">
+      <c r="AJ6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>MOHC-HadGEM3-RA</v>
       </c>
-      <c r="AJ6" s="65" t="str">
+      <c r="AK6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>MOHC-HadRM3P</v>
       </c>
-      <c r="AK6" s="65" t="str">
+      <c r="AL6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>MIUB-WRF331A</v>
       </c>
-      <c r="AL6" s="65" t="str">
+      <c r="AM6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>BCCR-WRF331C</v>
       </c>
-      <c r="AM6" s="65" t="str">
+      <c r="AN6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>CRP-GL-WRF331A</v>
       </c>
-      <c r="AN6" s="65" t="str">
+      <c r="AO6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>IDL-WRF331D</v>
       </c>
-      <c r="AO6" s="65" t="str">
+      <c r="AP6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>IPSL-INERIS-WRF331F</v>
       </c>
-      <c r="AP6" s="65" t="str">
+      <c r="AQ6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>AUTH-Met-WRF331A</v>
       </c>
-      <c r="AQ6" s="65" t="str">
+      <c r="AR6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>AUTH-LHTEE-WRF321B</v>
       </c>
-      <c r="AR6" s="65" t="str">
+      <c r="AS6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>NUIM-WRF341E</v>
       </c>
-      <c r="AS6" s="65" t="str">
+      <c r="AT6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>UHOH-WRF331H</v>
       </c>
-      <c r="AT6" s="65" t="str">
+      <c r="AU6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>UM-WRF331</v>
       </c>
-      <c r="AU6" s="65" t="str">
+      <c r="AV6" s="65" t="str">
         <f t="shared" si="27"/>
         <v>UCAN-WRF331G</v>
       </c>
-      <c r="AV6" s="164" t="str">
+      <c r="AW6" s="164" t="str">
         <f t="shared" si="27"/>
         <v>UCAN-WRF350I</v>
       </c>
-      <c r="AW6" s="105"/>
-      <c r="AX6" s="2"/>
+      <c r="AX6" s="105"/>
       <c r="AY6" s="2"/>
       <c r="AZ6" s="2"/>
       <c r="BA6" s="2"/>
@@ -11566,8 +11641,9 @@
       <c r="BU6" s="2"/>
       <c r="BV6" s="2"/>
       <c r="BW6" s="2"/>
+      <c r="BX6" s="2"/>
     </row>
-    <row r="7" spans="1:75" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:76" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="153" t="s">
         <v>151</v>
       </c>
@@ -11645,7 +11721,7 @@
       </c>
       <c r="T7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!T11),"unknown",AllEntries!T11)</f>
-        <v>unrestricted</v>
+        <v>non-commercial only</v>
       </c>
       <c r="U7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!U11),"unknown",AllEntries!U11)</f>
@@ -11665,23 +11741,23 @@
       </c>
       <c r="Y7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!Y11),"unknown",AllEntries!Y11)</f>
-        <v>unknown</v>
+        <v>unrestricted</v>
       </c>
       <c r="Z7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!Z11),"unknown",AllEntries!Z11)</f>
-        <v>unrestricted</v>
+        <v>unknown</v>
       </c>
       <c r="AA7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AA11),"unknown",AllEntries!AA11)</f>
-        <v>non-commercial only</v>
+        <v>unrestricted</v>
       </c>
       <c r="AB7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AB11),"unknown",AllEntries!AB11)</f>
-        <v>unknown</v>
+        <v>non-commercial only</v>
       </c>
       <c r="AC7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AC11),"unknown",AllEntries!AC11)</f>
-        <v>non-commercial only</v>
+        <v>unknown</v>
       </c>
       <c r="AD7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AD11),"unknown",AllEntries!AD11)</f>
@@ -11689,15 +11765,15 @@
       </c>
       <c r="AE7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AE11),"unknown",AllEntries!AE11)</f>
-        <v>unknown</v>
+        <v>non-commercial only</v>
       </c>
       <c r="AF7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AF11),"unknown",AllEntries!AF11)</f>
-        <v>unrestricted</v>
+        <v>unknown</v>
       </c>
       <c r="AG7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AG11),"unknown",AllEntries!AG11)</f>
-        <v>unknown</v>
+        <v>unrestricted</v>
       </c>
       <c r="AH7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AH11),"unknown",AllEntries!AH11)</f>
@@ -11705,7 +11781,7 @@
       </c>
       <c r="AI7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AI11),"unknown",AllEntries!AI11)</f>
-        <v>unrestricted</v>
+        <v>unknown</v>
       </c>
       <c r="AJ7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AJ11),"unknown",AllEntries!AJ11)</f>
@@ -11713,11 +11789,11 @@
       </c>
       <c r="AK7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AK11),"unknown",AllEntries!AK11)</f>
-        <v>unknown</v>
+        <v>unrestricted</v>
       </c>
       <c r="AL7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AL11),"unknown",AllEntries!AL11)</f>
-        <v>unrestricted</v>
+        <v>unknown</v>
       </c>
       <c r="AM7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AM11),"unknown",AllEntries!AM11)</f>
@@ -11725,7 +11801,7 @@
       </c>
       <c r="AN7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AN11),"unknown",AllEntries!AN11)</f>
-        <v>unknown</v>
+        <v>unrestricted</v>
       </c>
       <c r="AO7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AO11),"unknown",AllEntries!AO11)</f>
@@ -11741,11 +11817,11 @@
       </c>
       <c r="AR7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AR11),"unknown",AllEntries!AR11)</f>
-        <v>non-commercial only</v>
+        <v>unknown</v>
       </c>
       <c r="AS7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AS11),"unknown",AllEntries!AS11)</f>
-        <v>unknown</v>
+        <v>non-commercial only</v>
       </c>
       <c r="AT7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AT11),"unknown",AllEntries!AT11)</f>
@@ -11753,14 +11829,17 @@
       </c>
       <c r="AU7" s="137" t="str">
         <f>IF(ISBLANK(AllEntries!AU11),"unknown",AllEntries!AU11)</f>
+        <v>unknown</v>
+      </c>
+      <c r="AV7" s="137" t="str">
+        <f>IF(ISBLANK(AllEntries!AV11),"unknown",AllEntries!AV11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AV7" s="165" t="str">
-        <f>IF(ISBLANK(AllEntries!AV11),"unknown",AllEntries!AV11)</f>
+      <c r="AW7" s="165" t="str">
+        <f>IF(ISBLANK(AllEntries!AW11),"unknown",AllEntries!AW11)</f>
         <v>unknown</v>
       </c>
-      <c r="AW7" s="128"/>
-      <c r="AX7" s="2"/>
+      <c r="AX7" s="128"/>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
@@ -11786,8 +11865,9 @@
       <c r="BU7" s="2"/>
       <c r="BV7" s="2"/>
       <c r="BW7" s="2"/>
+      <c r="BX7" s="2"/>
     </row>
-    <row r="8" spans="1:75" s="36" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:76" s="36" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="154" t="s">
         <v>187</v>
       </c>
@@ -11857,17 +11937,17 @@
       <c r="W8" s="142" t="s">
         <v>186</v>
       </c>
-      <c r="X8" s="142"/>
-      <c r="Y8" s="142" t="s">
+      <c r="X8" s="142" t="s">
         <v>186</v>
       </c>
+      <c r="Y8" s="142"/>
       <c r="Z8" s="142" t="s">
         <v>186</v>
       </c>
-      <c r="AA8" s="142"/>
-      <c r="AB8" s="142" t="s">
+      <c r="AA8" s="142" t="s">
         <v>186</v>
       </c>
+      <c r="AB8" s="142"/>
       <c r="AC8" s="142" t="s">
         <v>186</v>
       </c>
@@ -11925,11 +12005,13 @@
       <c r="AU8" s="142" t="s">
         <v>186</v>
       </c>
-      <c r="AV8" s="166" t="s">
+      <c r="AV8" s="142" t="s">
         <v>186</v>
       </c>
-      <c r="AW8" s="145"/>
-      <c r="AX8" s="146"/>
+      <c r="AW8" s="166" t="s">
+        <v>186</v>
+      </c>
+      <c r="AX8" s="145"/>
       <c r="AY8" s="146"/>
       <c r="AZ8" s="146"/>
       <c r="BA8" s="146"/>
@@ -11955,8 +12037,9 @@
       <c r="BU8" s="146"/>
       <c r="BV8" s="146"/>
       <c r="BW8" s="146"/>
+      <c r="BX8" s="146"/>
     </row>
-    <row r="9" spans="1:75" s="36" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:76" s="36" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="154" t="s">
         <v>96</v>
       </c>
@@ -12015,48 +12098,48 @@
         <v>131</v>
       </c>
       <c r="T9" s="143" t="s">
+        <v>233</v>
+      </c>
+      <c r="U9" s="143" t="s">
         <v>131</v>
-      </c>
-      <c r="U9" s="143" t="s">
-        <v>118</v>
       </c>
       <c r="V9" s="143" t="s">
         <v>118</v>
       </c>
-      <c r="W9" s="144" t="s">
+      <c r="W9" s="143" t="s">
+        <v>118</v>
+      </c>
+      <c r="X9" s="144" t="s">
         <v>119</v>
       </c>
-      <c r="X9" s="142"/>
-      <c r="Y9" s="142" t="s">
+      <c r="Y9" s="142"/>
+      <c r="Z9" s="142" t="s">
         <v>162</v>
       </c>
-      <c r="Z9" s="142" t="s">
+      <c r="AA9" s="142" t="s">
         <v>157</v>
       </c>
-      <c r="AA9" s="142"/>
-      <c r="AB9" s="142" t="s">
-        <v>157</v>
-      </c>
+      <c r="AB9" s="142"/>
       <c r="AC9" s="142" t="s">
         <v>157</v>
       </c>
       <c r="AD9" s="142" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE9" s="142" t="s">
         <v>225</v>
       </c>
-      <c r="AE9" s="142"/>
       <c r="AF9" s="142"/>
-      <c r="AG9" s="198" t="s">
+      <c r="AG9" s="142"/>
+      <c r="AH9" s="198" t="s">
         <v>229</v>
       </c>
-      <c r="AH9" s="142"/>
-      <c r="AI9" s="142" t="s">
-        <v>158</v>
-      </c>
+      <c r="AI9" s="142"/>
       <c r="AJ9" s="142" t="s">
         <v>158</v>
       </c>
       <c r="AK9" s="142" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AL9" s="142" t="s">
         <v>159</v>
@@ -12068,19 +12151,19 @@
         <v>159</v>
       </c>
       <c r="AO9" s="142" t="s">
+        <v>159</v>
+      </c>
+      <c r="AP9" s="142" t="s">
         <v>166</v>
-      </c>
-      <c r="AP9" s="142" t="s">
-        <v>159</v>
       </c>
       <c r="AQ9" s="142" t="s">
         <v>159</v>
       </c>
       <c r="AR9" s="142" t="s">
+        <v>159</v>
+      </c>
+      <c r="AS9" s="142" t="s">
         <v>224</v>
-      </c>
-      <c r="AS9" s="142" t="s">
-        <v>159</v>
       </c>
       <c r="AT9" s="142" t="s">
         <v>159</v>
@@ -12088,11 +12171,13 @@
       <c r="AU9" s="142" t="s">
         <v>159</v>
       </c>
-      <c r="AV9" s="166" t="s">
+      <c r="AV9" s="142" t="s">
         <v>159</v>
       </c>
-      <c r="AW9" s="145"/>
-      <c r="AX9" s="146"/>
+      <c r="AW9" s="166" t="s">
+        <v>159</v>
+      </c>
+      <c r="AX9" s="145"/>
       <c r="AY9" s="146"/>
       <c r="AZ9" s="146"/>
       <c r="BA9" s="146"/>
@@ -12118,9 +12203,10 @@
       <c r="BU9" s="146"/>
       <c r="BV9" s="146"/>
       <c r="BW9" s="146"/>
+      <c r="BX9" s="146"/>
     </row>
-    <row r="10" spans="1:75" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:76" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A11" s="63"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
@@ -12128,7 +12214,7 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="AW3:AW5"/>
+    <mergeCell ref="AX3:AX5"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J2:O2"/>
@@ -12139,7 +12225,7 @@
     <brk id="16" max="9" man="1"/>
   </colBreaks>
   <ignoredErrors>
-    <ignoredError sqref="AO6" formula="1"/>
+    <ignoredError sqref="AP6" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added new info for UHOH
</commit_message>
<xml_diff>
--- a/CORDEX_ESGF_coordination_issues.xlsx
+++ b/CORDEX_ESGF_coordination_issues.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="243">
   <si>
     <t>Domain</t>
   </si>
@@ -1266,6 +1266,31 @@
   </si>
   <si>
     <t>EUR-??</t>
+  </si>
+  <si>
+    <t>NASA Goddard Institute for Space Studies (GISS)</t>
+  </si>
+  <si>
+    <t>Ruben Worrell                     Howard Spergel                   Crae Sosa               Kush Dave</t>
+  </si>
+  <si>
+    <t>not confirmed</t>
+  </si>
+  <si>
+    <t>georgiy.stenchikov@ kaust.edu.sa</t>
+  </si>
+  <si>
+    <t>Kirsten.Warrach-Sagi@uni-hohenheim.de</t>
+  </si>
+  <si>
+    <t>WRF361H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Hohenheim </t>
+  </si>
+  <si>
+    <t>confirmed by 
+Kirsten Warrach-Sagi</t>
   </si>
 </sst>
 </file>
@@ -2512,7 +2537,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2796,12 +2821,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2824,9 +2843,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2947,9 +2963,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2965,21 +2978,51 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3047,7 +3090,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3057,7 +3103,17 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -3544,27 +3600,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="203" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="197"/>
-      <c r="C1" s="197"/>
-      <c r="D1" s="197"/>
-      <c r="E1" s="197"/>
-      <c r="F1" s="197"/>
-      <c r="G1" s="197"/>
-      <c r="H1" s="197"/>
-      <c r="I1" s="197"/>
-      <c r="J1" s="197"/>
-      <c r="K1" s="197"/>
-      <c r="L1" s="197"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="203"/>
+      <c r="I1" s="203"/>
+      <c r="J1" s="203"/>
+      <c r="K1" s="203"/>
+      <c r="L1" s="203"/>
       <c r="M1" s="21"/>
       <c r="N1" s="20"/>
       <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="54">
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -3581,21 +3637,21 @@
       <c r="N2" s="20"/>
       <c r="O2" s="20"/>
     </row>
-    <row r="3" spans="1:15" s="139" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="198" t="s">
+    <row r="3" spans="1:15" s="137" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="204" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="198"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="138"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="138"/>
+      <c r="B3" s="204"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="136"/>
+      <c r="L3" s="136"/>
     </row>
     <row r="4" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
@@ -3625,8 +3681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA38"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ2" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Z23" sqref="Z23"/>
+    <sheetView topLeftCell="AL1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AU10" sqref="AU10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3664,24 +3720,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="205" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="197"/>
-      <c r="C1" s="197"/>
-      <c r="D1" s="197"/>
-      <c r="E1" s="197"/>
-      <c r="F1" s="197"/>
-      <c r="G1" s="197"/>
-      <c r="H1" s="197"/>
-      <c r="I1" s="197"/>
-      <c r="J1" s="197"/>
-      <c r="K1" s="197"/>
-      <c r="L1" s="197"/>
-      <c r="M1" s="197"/>
-      <c r="N1" s="197"/>
-      <c r="O1" s="197"/>
-      <c r="P1" s="197"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="203"/>
+      <c r="I1" s="203"/>
+      <c r="J1" s="203"/>
+      <c r="K1" s="203"/>
+      <c r="L1" s="203"/>
+      <c r="M1" s="203"/>
+      <c r="N1" s="203"/>
+      <c r="O1" s="203"/>
+      <c r="P1" s="203"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="20"/>
       <c r="S1" s="20"/>
@@ -3728,15 +3784,15 @@
     <row r="2" spans="1:79" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="53">
         <f>GeneralRemarks!A2</f>
-        <v>41985</v>
-      </c>
-      <c r="B2" s="201"/>
-      <c r="C2" s="201"/>
-      <c r="D2" s="201"/>
-      <c r="E2" s="201"/>
-      <c r="F2" s="201"/>
-      <c r="G2" s="201"/>
-      <c r="H2" s="201"/>
+        <v>41991</v>
+      </c>
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
       <c r="I2" s="51"/>
       <c r="J2" s="51"/>
       <c r="K2" s="51"/>
@@ -3754,7 +3810,7 @@
       <c r="W2" s="20"/>
       <c r="X2" s="54">
         <f>A2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
@@ -3783,7 +3839,7 @@
       <c r="AW2" s="20"/>
       <c r="AX2" s="71">
         <f>A2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="BS2" s="26"/>
       <c r="BT2" s="26"/>
@@ -3796,7 +3852,7 @@
       <c r="CA2" s="26"/>
     </row>
     <row r="3" spans="1:79" s="1" customFormat="1" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="150" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="105" t="s">
@@ -3844,7 +3900,7 @@
       <c r="P3" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="Q3" s="154" t="s">
+      <c r="Q3" s="151" t="s">
         <v>90</v>
       </c>
       <c r="R3" s="105" t="s">
@@ -3884,17 +3940,21 @@
       <c r="AD3" s="105" t="s">
         <v>135</v>
       </c>
-      <c r="AE3" s="176" t="s">
+      <c r="AE3" s="173" t="s">
         <v>223</v>
       </c>
-      <c r="AF3" s="105"/>
-      <c r="AG3" s="152" t="s">
+      <c r="AF3" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="AG3" s="149" t="s">
         <v>178</v>
       </c>
       <c r="AH3" s="105" t="s">
         <v>228</v>
       </c>
-      <c r="AI3" s="105"/>
+      <c r="AI3" s="105" t="s">
+        <v>238</v>
+      </c>
       <c r="AJ3" s="106" t="s">
         <v>98</v>
       </c>
@@ -3910,14 +3970,16 @@
       </c>
       <c r="AQ3" s="105"/>
       <c r="AR3" s="105"/>
-      <c r="AS3" s="176" t="s">
+      <c r="AS3" s="173" t="s">
         <v>217</v>
       </c>
-      <c r="AT3" s="105"/>
+      <c r="AT3" s="105" t="s">
+        <v>239</v>
+      </c>
       <c r="AU3" s="105"/>
       <c r="AV3" s="105"/>
       <c r="AW3" s="105"/>
-      <c r="AX3" s="153" t="s">
+      <c r="AX3" s="150" t="s">
         <v>57</v>
       </c>
       <c r="AY3" s="2"/>
@@ -3951,7 +4013,7 @@
       <c r="CA3" s="2"/>
     </row>
     <row r="4" spans="1:79" s="1" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="155" t="s">
+      <c r="A4" s="152" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="108" t="str">
@@ -4052,7 +4114,7 @@
         <f t="shared" si="2"/>
         <v>DHMZ</v>
       </c>
-      <c r="AE4" s="177"/>
+      <c r="AE4" s="174"/>
       <c r="AF4" s="108" t="str">
         <f t="shared" si="2"/>
         <v>GISS</v>
@@ -4124,7 +4186,7 @@
         <f t="shared" si="4"/>
         <v>UCAN</v>
       </c>
-      <c r="AX4" s="155" t="s">
+      <c r="AX4" s="152" t="s">
         <v>41</v>
       </c>
       <c r="AY4" s="2"/>
@@ -4158,7 +4220,7 @@
       <c r="CA4" s="2"/>
     </row>
     <row r="5" spans="1:79" s="128" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="156" t="s">
+      <c r="A5" s="153" t="s">
         <v>126</v>
       </c>
       <c r="B5" s="107"/>
@@ -4196,7 +4258,7 @@
       <c r="AB5" s="123"/>
       <c r="AC5" s="123"/>
       <c r="AD5" s="123"/>
-      <c r="AE5" s="178"/>
+      <c r="AE5" s="175"/>
       <c r="AF5" s="123"/>
       <c r="AG5" s="123"/>
       <c r="AH5" s="123"/>
@@ -4215,7 +4277,7 @@
       <c r="AU5" s="123"/>
       <c r="AV5" s="123"/>
       <c r="AW5" s="123"/>
-      <c r="AX5" s="156" t="s">
+      <c r="AX5" s="153" t="s">
         <v>126</v>
       </c>
       <c r="AY5" s="127"/>
@@ -4249,7 +4311,7 @@
       <c r="CA5" s="127"/>
     </row>
     <row r="6" spans="1:79" s="1" customFormat="1" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="155" t="s">
+      <c r="A6" s="152" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="110"/>
@@ -4281,7 +4343,7 @@
       <c r="AB6" s="108"/>
       <c r="AC6" s="108"/>
       <c r="AD6" s="108"/>
-      <c r="AE6" s="177"/>
+      <c r="AE6" s="174"/>
       <c r="AF6" s="108"/>
       <c r="AG6" s="108"/>
       <c r="AH6" s="108"/>
@@ -4300,7 +4362,7 @@
       <c r="AU6" s="108"/>
       <c r="AV6" s="108"/>
       <c r="AW6" s="108"/>
-      <c r="AX6" s="155" t="s">
+      <c r="AX6" s="152" t="s">
         <v>64</v>
       </c>
       <c r="AY6" s="2"/>
@@ -4334,154 +4396,154 @@
       <c r="CA6" s="2"/>
     </row>
     <row r="7" spans="1:79" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="156" t="s">
+      <c r="A7" s="153" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="159" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="162" t="s">
+      <c r="C7" s="159" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="162" t="s">
+      <c r="D7" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="162" t="s">
+      <c r="E7" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="162" t="s">
+      <c r="F7" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="163" t="s">
+      <c r="G7" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="163" t="s">
+      <c r="H7" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="163" t="s">
+      <c r="I7" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="163" t="s">
+      <c r="J7" s="160" t="s">
         <v>121</v>
       </c>
-      <c r="K7" s="163" t="s">
+      <c r="K7" s="160" t="s">
         <v>121</v>
       </c>
-      <c r="L7" s="163" t="s">
+      <c r="L7" s="160" t="s">
         <v>121</v>
       </c>
-      <c r="M7" s="163" t="s">
+      <c r="M7" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="N7" s="163" t="s">
+      <c r="N7" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="163" t="s">
+      <c r="O7" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="163" t="s">
+      <c r="P7" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="Q7" s="163" t="s">
+      <c r="Q7" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="163" t="s">
+      <c r="R7" s="160" t="s">
         <v>47</v>
       </c>
-      <c r="S7" s="163" t="s">
+      <c r="S7" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="T7" s="163" t="s">
+      <c r="T7" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="U7" s="171" t="s">
+      <c r="U7" s="168" t="s">
         <v>39</v>
       </c>
-      <c r="V7" s="171" t="s">
+      <c r="V7" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="W7" s="171" t="s">
+      <c r="W7" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="X7" s="171" t="s">
+      <c r="X7" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="Y7" s="163" t="s">
+      <c r="Y7" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="Z7" s="163" t="s">
+      <c r="Z7" s="160" t="s">
         <v>34</v>
       </c>
-      <c r="AA7" s="163" t="s">
+      <c r="AA7" s="160" t="s">
         <v>38</v>
       </c>
-      <c r="AB7" s="163" t="s">
+      <c r="AB7" s="160" t="s">
         <v>174</v>
       </c>
-      <c r="AC7" s="163" t="s">
+      <c r="AC7" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="AD7" s="163" t="s">
+      <c r="AD7" s="160" t="s">
         <v>48</v>
       </c>
-      <c r="AE7" s="179" t="s">
+      <c r="AE7" s="176" t="s">
         <v>221</v>
       </c>
-      <c r="AF7" s="163" t="s">
+      <c r="AF7" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="AG7" s="163" t="s">
+      <c r="AG7" s="160" t="s">
         <v>120</v>
       </c>
-      <c r="AH7" s="163" t="s">
+      <c r="AH7" s="160" t="s">
         <v>226</v>
       </c>
-      <c r="AI7" s="163" t="s">
+      <c r="AI7" s="160" t="s">
         <v>55</v>
       </c>
-      <c r="AJ7" s="163" t="s">
+      <c r="AJ7" s="160" t="s">
         <v>53</v>
       </c>
-      <c r="AK7" s="163" t="s">
+      <c r="AK7" s="160" t="s">
         <v>53</v>
       </c>
-      <c r="AL7" s="168" t="s">
+      <c r="AL7" s="165" t="s">
         <v>143</v>
       </c>
-      <c r="AM7" s="168" t="s">
+      <c r="AM7" s="165" t="s">
         <v>45</v>
       </c>
-      <c r="AN7" s="171" t="s">
+      <c r="AN7" s="168" t="s">
         <v>36</v>
       </c>
-      <c r="AO7" s="171" t="s">
+      <c r="AO7" s="168" t="s">
         <v>46</v>
       </c>
-      <c r="AP7" s="171" t="s">
+      <c r="AP7" s="168" t="s">
         <v>164</v>
       </c>
-      <c r="AQ7" s="163" t="s">
+      <c r="AQ7" s="160" t="s">
         <v>144</v>
       </c>
-      <c r="AR7" s="163" t="s">
+      <c r="AR7" s="160" t="s">
         <v>145</v>
       </c>
-      <c r="AS7" s="163" t="s">
+      <c r="AS7" s="160" t="s">
         <v>56</v>
       </c>
-      <c r="AT7" s="163" t="s">
+      <c r="AT7" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="AU7" s="163" t="s">
+      <c r="AU7" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="AV7" s="163" t="s">
+      <c r="AV7" s="160" t="s">
         <v>140</v>
       </c>
-      <c r="AW7" s="163" t="s">
+      <c r="AW7" s="160" t="s">
         <v>140</v>
       </c>
-      <c r="AX7" s="156" t="s">
+      <c r="AX7" s="153" t="s">
         <v>185</v>
       </c>
       <c r="AY7" s="2"/>
@@ -4515,154 +4577,154 @@
       <c r="CA7" s="2"/>
     </row>
     <row r="8" spans="1:79" s="114" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="156" t="s">
+      <c r="A8" s="153" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="164" t="s">
+      <c r="B8" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="164" t="s">
+      <c r="C8" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="164" t="s">
+      <c r="D8" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="164" t="s">
+      <c r="E8" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="164" t="s">
+      <c r="F8" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="165" t="s">
+      <c r="G8" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="165" t="s">
+      <c r="H8" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="165" t="s">
+      <c r="I8" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="165" t="s">
+      <c r="J8" s="162" t="s">
         <v>124</v>
       </c>
-      <c r="K8" s="165" t="s">
+      <c r="K8" s="162" t="s">
         <v>124</v>
       </c>
-      <c r="L8" s="165" t="s">
+      <c r="L8" s="162" t="s">
         <v>124</v>
       </c>
-      <c r="M8" s="165" t="s">
+      <c r="M8" s="162" t="s">
         <v>115</v>
       </c>
-      <c r="N8" s="165" t="s">
+      <c r="N8" s="162" t="s">
         <v>116</v>
       </c>
-      <c r="O8" s="165" t="s">
+      <c r="O8" s="162" t="s">
         <v>109</v>
       </c>
-      <c r="P8" s="167" t="s">
+      <c r="P8" s="164" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="165" t="s">
+      <c r="Q8" s="162" t="s">
         <v>26</v>
       </c>
-      <c r="R8" s="164" t="s">
+      <c r="R8" s="161" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="165" t="s">
+      <c r="S8" s="162" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="184" t="s">
+      <c r="T8" s="181" t="s">
         <v>231</v>
       </c>
-      <c r="U8" s="173" t="s">
+      <c r="U8" s="170" t="s">
         <v>130</v>
       </c>
-      <c r="V8" s="173" t="s">
+      <c r="V8" s="170" t="s">
         <v>148</v>
       </c>
-      <c r="W8" s="173" t="s">
+      <c r="W8" s="170" t="s">
         <v>111</v>
       </c>
-      <c r="X8" s="173" t="s">
+      <c r="X8" s="170" t="s">
         <v>97</v>
       </c>
-      <c r="Y8" s="165" t="s">
+      <c r="Y8" s="162" t="s">
         <v>93</v>
       </c>
-      <c r="Z8" s="165" t="s">
+      <c r="Z8" s="162" t="s">
         <v>94</v>
       </c>
-      <c r="AA8" s="165" t="s">
+      <c r="AA8" s="162" t="s">
         <v>95</v>
       </c>
-      <c r="AB8" s="165" t="s">
+      <c r="AB8" s="162" t="s">
         <v>95</v>
       </c>
-      <c r="AC8" s="165" t="s">
+      <c r="AC8" s="162" t="s">
         <v>134</v>
       </c>
-      <c r="AD8" s="165" t="s">
+      <c r="AD8" s="162" t="s">
         <v>134</v>
       </c>
-      <c r="AE8" s="180" t="s">
+      <c r="AE8" s="177" t="s">
         <v>222</v>
       </c>
-      <c r="AF8" s="167" t="s">
+      <c r="AF8" s="164" t="s">
         <v>27</v>
       </c>
-      <c r="AG8" s="165" t="s">
+      <c r="AG8" s="162" t="s">
         <v>28</v>
       </c>
-      <c r="AH8" s="165" t="s">
+      <c r="AH8" s="162" t="s">
         <v>29</v>
       </c>
-      <c r="AI8" s="165" t="s">
+      <c r="AI8" s="162" t="s">
         <v>30</v>
       </c>
-      <c r="AJ8" s="164" t="s">
+      <c r="AJ8" s="161" t="s">
         <v>114</v>
       </c>
-      <c r="AK8" s="164" t="s">
+      <c r="AK8" s="161" t="s">
         <v>128</v>
       </c>
-      <c r="AL8" s="169" t="s">
+      <c r="AL8" s="166" t="s">
         <v>137</v>
       </c>
-      <c r="AM8" s="169" t="s">
+      <c r="AM8" s="166" t="s">
         <v>136</v>
       </c>
-      <c r="AN8" s="172" t="s">
+      <c r="AN8" s="169" t="s">
         <v>137</v>
       </c>
-      <c r="AO8" s="172" t="s">
+      <c r="AO8" s="169" t="s">
         <v>138</v>
       </c>
-      <c r="AP8" s="172" t="s">
+      <c r="AP8" s="169" t="s">
         <v>139</v>
       </c>
-      <c r="AQ8" s="167" t="s">
+      <c r="AQ8" s="164" t="s">
         <v>137</v>
       </c>
-      <c r="AR8" s="165" t="s">
+      <c r="AR8" s="162" t="s">
         <v>146</v>
       </c>
-      <c r="AS8" s="167" t="s">
+      <c r="AS8" s="164" t="s">
         <v>175</v>
       </c>
-      <c r="AT8" s="167" t="s">
-        <v>142</v>
-      </c>
-      <c r="AU8" s="167" t="s">
+      <c r="AT8" s="164" t="s">
+        <v>240</v>
+      </c>
+      <c r="AU8" s="164" t="s">
         <v>24</v>
       </c>
-      <c r="AV8" s="173" t="s">
+      <c r="AV8" s="170" t="s">
         <v>141</v>
       </c>
-      <c r="AW8" s="167" t="s">
+      <c r="AW8" s="164" t="s">
         <v>147</v>
       </c>
-      <c r="AX8" s="156" t="s">
+      <c r="AX8" s="153" t="s">
         <v>86</v>
       </c>
       <c r="AY8" s="113"/>
@@ -4696,7 +4758,7 @@
       <c r="CA8" s="113"/>
     </row>
     <row r="9" spans="1:79" s="35" customFormat="1" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="155" t="s">
+      <c r="A9" s="152" t="s">
         <v>167</v>
       </c>
       <c r="B9" s="109"/>
@@ -4749,19 +4811,19 @@
       <c r="S9" s="109" t="s">
         <v>190</v>
       </c>
-      <c r="T9" s="170" t="s">
+      <c r="T9" s="167" t="s">
         <v>190</v>
       </c>
-      <c r="U9" s="170" t="s">
+      <c r="U9" s="167" t="s">
         <v>190</v>
       </c>
-      <c r="V9" s="170" t="s">
+      <c r="V9" s="167" t="s">
         <v>169</v>
       </c>
-      <c r="W9" s="170" t="s">
+      <c r="W9" s="167" t="s">
         <v>169</v>
       </c>
-      <c r="X9" s="170" t="s">
+      <c r="X9" s="167" t="s">
         <v>169</v>
       </c>
       <c r="Y9" s="109" t="s">
@@ -4780,10 +4842,12 @@
       <c r="AD9" s="109" t="s">
         <v>188</v>
       </c>
-      <c r="AE9" s="181" t="s">
+      <c r="AE9" s="178" t="s">
         <v>220</v>
       </c>
-      <c r="AF9" s="109"/>
+      <c r="AF9" s="109" t="s">
+        <v>235</v>
+      </c>
       <c r="AG9" s="109" t="s">
         <v>177</v>
       </c>
@@ -4799,23 +4863,25 @@
       <c r="AK9" s="109" t="s">
         <v>189</v>
       </c>
-      <c r="AL9" s="170"/>
-      <c r="AM9" s="170" t="s">
+      <c r="AL9" s="167"/>
+      <c r="AM9" s="167" t="s">
         <v>191</v>
       </c>
-      <c r="AN9" s="170"/>
-      <c r="AO9" s="170"/>
-      <c r="AP9" s="170"/>
+      <c r="AN9" s="167"/>
+      <c r="AO9" s="167"/>
+      <c r="AP9" s="167"/>
       <c r="AQ9" s="109"/>
       <c r="AR9" s="109"/>
-      <c r="AS9" s="181" t="s">
+      <c r="AS9" s="178" t="s">
         <v>216</v>
       </c>
-      <c r="AT9" s="109"/>
+      <c r="AT9" s="109" t="s">
+        <v>241</v>
+      </c>
       <c r="AU9" s="109"/>
       <c r="AV9" s="109"/>
       <c r="AW9" s="109"/>
-      <c r="AX9" s="155" t="s">
+      <c r="AX9" s="152" t="s">
         <v>167</v>
       </c>
       <c r="AY9" s="70"/>
@@ -4849,50 +4915,50 @@
       <c r="CA9" s="70"/>
     </row>
     <row r="10" spans="1:79" s="1" customFormat="1" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="155" t="s">
+      <c r="A10" s="152" t="s">
         <v>197</v>
       </c>
-      <c r="B10" s="166" t="s">
+      <c r="B10" s="163" t="s">
         <v>208</v>
       </c>
-      <c r="C10" s="166"/>
-      <c r="D10" s="166" t="s">
+      <c r="C10" s="163"/>
+      <c r="D10" s="163" t="s">
         <v>207</v>
       </c>
-      <c r="E10" s="166"/>
-      <c r="F10" s="166"/>
-      <c r="G10" s="166"/>
-      <c r="H10" s="166"/>
-      <c r="I10" s="166"/>
-      <c r="J10" s="174"/>
-      <c r="K10" s="174" t="s">
+      <c r="E10" s="163"/>
+      <c r="F10" s="163"/>
+      <c r="G10" s="163"/>
+      <c r="H10" s="163"/>
+      <c r="I10" s="163"/>
+      <c r="J10" s="171"/>
+      <c r="K10" s="171" t="s">
         <v>215</v>
       </c>
-      <c r="L10" s="174"/>
-      <c r="M10" s="174"/>
-      <c r="N10" s="174" t="s">
+      <c r="L10" s="171"/>
+      <c r="M10" s="171"/>
+      <c r="N10" s="171" t="s">
         <v>214</v>
       </c>
-      <c r="O10" s="174"/>
-      <c r="P10" s="166" t="s">
+      <c r="O10" s="171"/>
+      <c r="P10" s="163" t="s">
         <v>213</v>
       </c>
-      <c r="Q10" s="166"/>
+      <c r="Q10" s="163"/>
       <c r="R10" s="109" t="s">
         <v>206</v>
       </c>
-      <c r="S10" s="166"/>
-      <c r="T10" s="166" t="s">
+      <c r="S10" s="163"/>
+      <c r="T10" s="163" t="s">
         <v>234</v>
       </c>
-      <c r="U10" s="166"/>
-      <c r="V10" s="166" t="s">
+      <c r="U10" s="163"/>
+      <c r="V10" s="163" t="s">
         <v>211</v>
       </c>
-      <c r="W10" s="166" t="s">
+      <c r="W10" s="163" t="s">
         <v>210</v>
       </c>
-      <c r="X10" s="166" t="s">
+      <c r="X10" s="163" t="s">
         <v>212</v>
       </c>
       <c r="Y10" s="109"/>
@@ -4901,7 +4967,7 @@
       <c r="AB10" s="109"/>
       <c r="AC10" s="109"/>
       <c r="AD10" s="109"/>
-      <c r="AE10" s="181"/>
+      <c r="AE10" s="178"/>
       <c r="AF10" s="109"/>
       <c r="AG10" s="109"/>
       <c r="AH10" s="109"/>
@@ -4926,7 +4992,7 @@
         <v>200</v>
       </c>
       <c r="AW10" s="109"/>
-      <c r="AX10" s="155" t="s">
+      <c r="AX10" s="152" t="s">
         <v>197</v>
       </c>
       <c r="AY10" s="2"/>
@@ -4960,7 +5026,7 @@
       <c r="CA10" s="2"/>
     </row>
     <row r="11" spans="1:79" s="128" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="157" t="s">
+      <c r="A11" s="154" t="s">
         <v>153</v>
       </c>
       <c r="B11" s="109" t="s">
@@ -5071,13 +5137,15 @@
       <c r="AS11" s="109" t="s">
         <v>181</v>
       </c>
-      <c r="AT11" s="109"/>
+      <c r="AT11" s="109" t="s">
+        <v>181</v>
+      </c>
       <c r="AU11" s="109"/>
       <c r="AV11" s="109" t="s">
         <v>181</v>
       </c>
       <c r="AW11" s="109"/>
-      <c r="AX11" s="182" t="s">
+      <c r="AX11" s="179" t="s">
         <v>153</v>
       </c>
       <c r="AY11" s="127"/>
@@ -5111,16 +5179,16 @@
       <c r="CA11" s="127"/>
     </row>
     <row r="12" spans="1:79" s="26" customFormat="1" ht="21.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="200" t="s">
+      <c r="A12" s="206" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="200"/>
-      <c r="C12" s="200"/>
-      <c r="D12" s="200"/>
-      <c r="E12" s="200"/>
-      <c r="F12" s="200"/>
-      <c r="G12" s="200"/>
-      <c r="H12" s="200"/>
+      <c r="B12" s="206"/>
+      <c r="C12" s="206"/>
+      <c r="D12" s="206"/>
+      <c r="E12" s="206"/>
+      <c r="F12" s="206"/>
+      <c r="G12" s="206"/>
+      <c r="H12" s="206"/>
       <c r="I12" s="120"/>
       <c r="J12" s="120"/>
       <c r="K12" s="120"/>
@@ -5132,7 +5200,7 @@
       <c r="Q12" s="120"/>
       <c r="R12" s="120"/>
       <c r="S12" s="120"/>
-      <c r="T12" s="183"/>
+      <c r="T12" s="180"/>
       <c r="U12" s="120"/>
       <c r="V12" s="120"/>
       <c r="W12" s="120"/>
@@ -5140,10 +5208,10 @@
       <c r="Y12" s="120"/>
       <c r="Z12" s="120"/>
       <c r="AA12" s="120"/>
-      <c r="AB12" s="141"/>
+      <c r="AB12" s="139"/>
       <c r="AC12" s="120"/>
       <c r="AD12" s="120"/>
-      <c r="AE12" s="175"/>
+      <c r="AE12" s="172"/>
       <c r="AF12" s="120"/>
       <c r="AG12" s="120"/>
       <c r="AH12" s="120"/>
@@ -5164,56 +5232,56 @@
       <c r="AW12" s="120"/>
     </row>
     <row r="13" spans="1:79" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="200" t="s">
+      <c r="A13" s="206" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="200"/>
-      <c r="C13" s="200"/>
-      <c r="D13" s="200"/>
-      <c r="E13" s="200"/>
-      <c r="F13" s="200"/>
-      <c r="G13" s="133"/>
-      <c r="H13" s="133"/>
-      <c r="I13" s="133"/>
-      <c r="J13" s="133"/>
-      <c r="K13" s="133"/>
-      <c r="L13" s="133"/>
-      <c r="M13" s="133"/>
-      <c r="N13" s="133"/>
-      <c r="O13" s="133"/>
-      <c r="P13" s="133"/>
-      <c r="Q13" s="133"/>
-      <c r="R13" s="133"/>
-      <c r="S13" s="133"/>
-      <c r="T13" s="133"/>
-      <c r="V13" s="133"/>
-      <c r="W13" s="133"/>
-      <c r="X13" s="133"/>
-      <c r="Y13" s="133"/>
-      <c r="Z13" s="133"/>
-      <c r="AA13" s="133"/>
-      <c r="AB13" s="133"/>
-      <c r="AC13" s="133"/>
-      <c r="AD13" s="133"/>
-      <c r="AE13" s="133"/>
-      <c r="AF13" s="133"/>
-      <c r="AG13" s="133"/>
-      <c r="AH13" s="133"/>
-      <c r="AI13" s="133"/>
-      <c r="AJ13" s="133"/>
-      <c r="AK13" s="133"/>
-      <c r="AL13" s="133"/>
-      <c r="AM13" s="133"/>
-      <c r="AN13" s="133"/>
-      <c r="AO13" s="133"/>
-      <c r="AP13" s="133"/>
-      <c r="AQ13" s="133"/>
-      <c r="AR13" s="133"/>
-      <c r="AS13" s="133"/>
-      <c r="AT13" s="133"/>
-      <c r="AU13" s="133"/>
-      <c r="AV13" s="133"/>
-      <c r="AW13" s="133"/>
+      <c r="B13" s="206"/>
+      <c r="C13" s="206"/>
+      <c r="D13" s="206"/>
+      <c r="E13" s="206"/>
+      <c r="F13" s="206"/>
+      <c r="G13" s="131"/>
+      <c r="H13" s="131"/>
+      <c r="I13" s="131"/>
+      <c r="J13" s="131"/>
+      <c r="K13" s="131"/>
+      <c r="L13" s="131"/>
+      <c r="M13" s="131"/>
+      <c r="N13" s="131"/>
+      <c r="O13" s="131"/>
+      <c r="P13" s="131"/>
+      <c r="Q13" s="131"/>
+      <c r="R13" s="131"/>
+      <c r="S13" s="131"/>
+      <c r="T13" s="131"/>
+      <c r="V13" s="131"/>
+      <c r="W13" s="131"/>
+      <c r="X13" s="131"/>
+      <c r="Y13" s="131"/>
+      <c r="Z13" s="131"/>
+      <c r="AA13" s="131"/>
+      <c r="AB13" s="131"/>
+      <c r="AC13" s="131"/>
+      <c r="AD13" s="131"/>
+      <c r="AE13" s="131"/>
+      <c r="AF13" s="131"/>
+      <c r="AG13" s="131"/>
+      <c r="AH13" s="131"/>
+      <c r="AI13" s="131"/>
+      <c r="AJ13" s="131"/>
+      <c r="AK13" s="131"/>
+      <c r="AL13" s="131"/>
+      <c r="AM13" s="131"/>
+      <c r="AN13" s="131"/>
+      <c r="AO13" s="131"/>
+      <c r="AP13" s="131"/>
+      <c r="AQ13" s="131"/>
+      <c r="AR13" s="131"/>
+      <c r="AS13" s="131"/>
+      <c r="AT13" s="131"/>
+      <c r="AU13" s="131"/>
+      <c r="AV13" s="131"/>
+      <c r="AW13" s="131"/>
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.3">
       <c r="AX14" s="70"/>
@@ -5236,13 +5304,13 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A13:F13"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:AD7 AF11:AW11 AE7:AW10 B8:S8 U8:AD8 B9:AD11">
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="B7:AD7 AE7:AW10 B8:S8 U8:AD8 B9:AD11 AF11:AW11">
+    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE11">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",AE11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5309,25 +5377,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:144" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="203" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="197"/>
-      <c r="C1" s="197"/>
-      <c r="D1" s="197"/>
-      <c r="E1" s="197"/>
-      <c r="F1" s="197"/>
-      <c r="G1" s="197"/>
-      <c r="H1" s="197"/>
-      <c r="I1" s="197"/>
-      <c r="J1" s="197"/>
-      <c r="K1" s="197"/>
-      <c r="L1" s="197"/>
-      <c r="M1" s="197"/>
-      <c r="N1" s="197"/>
-      <c r="O1" s="197"/>
-      <c r="P1" s="197"/>
-      <c r="Q1" s="197"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="203"/>
+      <c r="I1" s="203"/>
+      <c r="J1" s="203"/>
+      <c r="K1" s="203"/>
+      <c r="L1" s="203"/>
+      <c r="M1" s="203"/>
+      <c r="N1" s="203"/>
+      <c r="O1" s="203"/>
+      <c r="P1" s="203"/>
+      <c r="Q1" s="203"/>
       <c r="R1" s="21"/>
       <c r="S1" s="20"/>
       <c r="T1" s="20"/>
@@ -5365,7 +5433,7 @@
     <row r="2" spans="1:144" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="53">
         <f>GeneralRemarks!A2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -5391,7 +5459,7 @@
       <c r="W2" s="20"/>
       <c r="X2" s="54">
         <f>GeneralRemarks!A2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
@@ -5421,7 +5489,7 @@
       <c r="AX2" s="20"/>
       <c r="AZ2" s="71">
         <f>A2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
     </row>
     <row r="3" spans="1:144" s="1" customFormat="1" ht="36.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5518,7 +5586,7 @@
         <v>Petr Skalak
 skalak@chmi.cz</v>
       </c>
-      <c r="T3" s="147" t="str">
+      <c r="T3" s="144" t="str">
         <f>AllEntries!R3</f>
         <v>Gabriella Szepszo szepszo.g@met.hu
 Ilona Krüzselyi
@@ -5577,9 +5645,9 @@
         <v>ivan.guettler @gmail.com
 Cedo Brankovic</v>
       </c>
-      <c r="AF3" s="29">
+      <c r="AF3" s="29" t="str">
         <f>AllEntries!AF3</f>
-        <v>0</v>
+        <v>Ruben Worrell                     Howard Spergel                   Crae Sosa               Kush Dave</v>
       </c>
       <c r="AG3" s="27" t="str">
         <f>AllEntries!AG3</f>
@@ -5594,9 +5662,9 @@
         <f>AllEntries!AH3</f>
         <v>Jack.Katzfey@csiro.au</v>
       </c>
-      <c r="AJ3" s="29">
+      <c r="AJ3" s="29" t="str">
         <f>AllEntries!AI3</f>
-        <v>0</v>
+        <v>georgiy.stenchikov@ kaust.edu.sa</v>
       </c>
       <c r="AK3" s="55" t="str">
         <f>AllEntries!AJ3</f>
@@ -5642,9 +5710,9 @@
         <v>Rowan Fealy : rowan.fealy
 @nuim.ie</v>
       </c>
-      <c r="AU3" s="29">
+      <c r="AU3" s="29" t="str">
         <f>AllEntries!AT3</f>
-        <v>0</v>
+        <v>Kirsten.Warrach-Sagi@uni-hohenheim.de</v>
       </c>
       <c r="AV3" s="29">
         <f>AllEntries!AU3</f>
@@ -5963,7 +6031,7 @@
         <f>AllEntries!AW4</f>
         <v>UCAN</v>
       </c>
-      <c r="AZ4" s="204" t="s">
+      <c r="AZ4" s="210" t="s">
         <v>16</v>
       </c>
       <c r="BA4" s="73" t="s">
@@ -6266,7 +6334,7 @@
         <f>AllEntries!AW6</f>
         <v>0</v>
       </c>
-      <c r="AZ5" s="205"/>
+      <c r="AZ5" s="211"/>
       <c r="BA5" s="73"/>
       <c r="BB5" s="2"/>
       <c r="BC5" s="2"/>
@@ -6547,7 +6615,7 @@
       </c>
       <c r="AU6" s="25" t="str">
         <f>AllEntries!AT8</f>
-        <v>WRF331H</v>
+        <v>WRF361H</v>
       </c>
       <c r="AV6" s="25" t="str">
         <f>AllEntries!AU8</f>
@@ -6565,7 +6633,7 @@
         <f>AllEntries!AW8</f>
         <v>WRF350I</v>
       </c>
-      <c r="AZ6" s="206"/>
+      <c r="AZ6" s="212"/>
       <c r="BA6" s="74" t="s">
         <v>19</v>
       </c>
@@ -6768,7 +6836,7 @@
       <c r="AH7" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AI7" s="148"/>
+      <c r="AI7" s="145"/>
       <c r="AJ7" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6946,7 +7014,7 @@
       <c r="AH8" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="AI8" s="149"/>
+      <c r="AI8" s="146"/>
       <c r="AJ8" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -7124,7 +7192,7 @@
       <c r="AH9" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="AI9" s="149"/>
+      <c r="AI9" s="146"/>
       <c r="AJ9" s="15">
         <f>(1*56+0*95+0)*AFR_22/1000</f>
         <v>22.5792</v>
@@ -7302,7 +7370,7 @@
       <c r="AH10" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="AI10" s="149"/>
+      <c r="AI10" s="146"/>
       <c r="AJ10" s="15">
         <f>(1*56+0*95+0)*AFR22tier1/1000</f>
         <v>651.16800000000001</v>
@@ -7482,7 +7550,7 @@
       <c r="AH11" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="AI11" s="149"/>
+      <c r="AI11" s="146"/>
       <c r="AJ11" s="15">
         <f>(0*56+0*95+0)*EUR_11/16/1000</f>
         <v>0</v>
@@ -7662,7 +7730,7 @@
       <c r="AH12" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="AI12" s="149"/>
+      <c r="AI12" s="146"/>
       <c r="AJ12" s="15">
         <f>(0*56+0*95+0)*EUR11tier1/16/1000</f>
         <v>0</v>
@@ -7843,7 +7911,7 @@
       <c r="AH13" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="AI13" s="149"/>
+      <c r="AI13" s="146"/>
       <c r="AJ13" s="15">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -8023,7 +8091,7 @@
       <c r="AH14" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="AI14" s="149"/>
+      <c r="AI14" s="146"/>
       <c r="AJ14" s="15">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -8201,7 +8269,7 @@
       <c r="AH15" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="AI15" s="149"/>
+      <c r="AI15" s="146"/>
       <c r="AJ15" s="15">
         <f t="shared" si="13"/>
         <v>0</v>
@@ -8379,7 +8447,7 @@
       <c r="AH16" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="AI16" s="149"/>
+      <c r="AI16" s="146"/>
       <c r="AJ16" s="15">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -8557,7 +8625,7 @@
       <c r="AH17" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="AI17" s="149"/>
+      <c r="AI17" s="146"/>
       <c r="AJ17" s="15">
         <f t="shared" si="15"/>
         <v>0</v>
@@ -8735,7 +8803,7 @@
       <c r="AH18" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="AI18" s="149"/>
+      <c r="AI18" s="146"/>
       <c r="AJ18" s="15">
         <f t="shared" si="16"/>
         <v>0</v>
@@ -8913,7 +8981,7 @@
       <c r="AH19" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="AI19" s="149"/>
+      <c r="AI19" s="146"/>
       <c r="AJ19" s="15">
         <f t="shared" si="17"/>
         <v>0</v>
@@ -9091,7 +9159,7 @@
       <c r="AH20" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="AI20" s="149"/>
+      <c r="AI20" s="146"/>
       <c r="AJ20" s="15">
         <f t="shared" si="18"/>
         <v>0</v>
@@ -9205,7 +9273,7 @@
       <c r="AH21" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="AI21" s="149"/>
+      <c r="AI21" s="146"/>
       <c r="AJ21" s="15"/>
       <c r="AK21" s="59"/>
       <c r="AL21" s="59"/>
@@ -9274,7 +9342,7 @@
       <c r="AH22" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="AI22" s="150"/>
+      <c r="AI22" s="147"/>
       <c r="AJ22" s="87"/>
       <c r="AK22" s="90"/>
       <c r="AL22" s="90"/>
@@ -9344,7 +9412,7 @@
       <c r="AH23" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="AI23" s="149"/>
+      <c r="AI23" s="146"/>
       <c r="AJ23" s="15"/>
       <c r="AK23" s="59"/>
       <c r="AL23" s="59"/>
@@ -9504,7 +9572,7 @@
       <c r="AH24" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="AI24" s="149"/>
+      <c r="AI24" s="146"/>
       <c r="AJ24" s="15"/>
       <c r="AK24" s="59"/>
       <c r="AL24" s="59"/>
@@ -9676,7 +9744,7 @@
       <c r="AH25" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="AI25" s="149"/>
+      <c r="AI25" s="146"/>
       <c r="AJ25" s="15"/>
       <c r="AK25" s="59"/>
       <c r="AL25" s="59"/>
@@ -9848,7 +9916,7 @@
       <c r="AH26" s="85" t="s">
         <v>106</v>
       </c>
-      <c r="AI26" s="150"/>
+      <c r="AI26" s="147"/>
       <c r="AJ26" s="87"/>
       <c r="AK26" s="90"/>
       <c r="AL26" s="90"/>
@@ -10039,7 +10107,7 @@
         <f t="shared" si="20"/>
         <v>0.2829834</v>
       </c>
-      <c r="T27" s="146"/>
+      <c r="T27" s="143"/>
       <c r="U27" s="98">
         <f t="shared" si="20"/>
         <v>3.0588391124480689</v>
@@ -10089,7 +10157,7 @@
       <c r="AH27" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="AI27" s="151"/>
+      <c r="AI27" s="148"/>
       <c r="AJ27" s="99">
         <f t="shared" ref="AJ27" si="28">SUM(AJ7:AJ26)/1000</f>
         <v>0.67374719999999999</v>
@@ -10161,25 +10229,25 @@
       <c r="EN27" s="26"/>
     </row>
     <row r="28" spans="1:144" s="26" customFormat="1" ht="37.200000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="207" t="s">
+      <c r="A28" s="213" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="207"/>
-      <c r="C28" s="207"/>
-      <c r="D28" s="207"/>
-      <c r="E28" s="207"/>
-      <c r="F28" s="207"/>
-      <c r="G28" s="207"/>
-      <c r="H28" s="207"/>
-      <c r="I28" s="207"/>
-      <c r="J28" s="207"/>
-      <c r="K28" s="207"/>
-      <c r="L28" s="207"/>
-      <c r="M28" s="207"/>
-      <c r="N28" s="207"/>
-      <c r="O28" s="207"/>
-      <c r="P28" s="207"/>
-      <c r="Q28" s="207"/>
+      <c r="B28" s="213"/>
+      <c r="C28" s="213"/>
+      <c r="D28" s="213"/>
+      <c r="E28" s="213"/>
+      <c r="F28" s="213"/>
+      <c r="G28" s="213"/>
+      <c r="H28" s="213"/>
+      <c r="I28" s="213"/>
+      <c r="J28" s="213"/>
+      <c r="K28" s="213"/>
+      <c r="L28" s="213"/>
+      <c r="M28" s="213"/>
+      <c r="N28" s="213"/>
+      <c r="O28" s="213"/>
+      <c r="P28" s="213"/>
+      <c r="Q28" s="213"/>
       <c r="R28" s="40"/>
       <c r="S28" s="40"/>
       <c r="T28" s="40"/>
@@ -10215,69 +10283,69 @@
       <c r="AX28" s="30"/>
     </row>
     <row r="29" spans="1:144" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="208" t="s">
+      <c r="A29" s="214" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="208"/>
-      <c r="C29" s="208"/>
-      <c r="D29" s="208"/>
-      <c r="E29" s="208"/>
-      <c r="F29" s="208"/>
-      <c r="G29" s="208"/>
-      <c r="H29" s="208"/>
-      <c r="I29" s="208"/>
-      <c r="J29" s="208"/>
-      <c r="K29" s="208"/>
-      <c r="L29" s="208"/>
-      <c r="M29" s="208"/>
-      <c r="N29" s="208"/>
-      <c r="O29" s="208"/>
-      <c r="P29" s="208"/>
-      <c r="Q29" s="208"/>
-      <c r="R29" s="208"/>
-      <c r="S29" s="208"/>
-      <c r="T29" s="208"/>
-      <c r="U29" s="208"/>
-      <c r="V29" s="208"/>
-      <c r="W29" s="208"/>
-      <c r="X29" s="208"/>
-      <c r="Y29" s="208"/>
-      <c r="Z29" s="208"/>
-      <c r="AA29" s="208"/>
-      <c r="AB29" s="208"/>
-      <c r="AC29" s="208"/>
-      <c r="AD29" s="208"/>
-      <c r="AE29" s="208"/>
-      <c r="AF29" s="208"/>
-      <c r="AG29" s="208"/>
-      <c r="AH29" s="208"/>
-      <c r="AI29" s="208"/>
-      <c r="AJ29" s="208"/>
-      <c r="AK29" s="208"/>
-      <c r="AL29" s="208"/>
-      <c r="AM29" s="208"/>
-      <c r="AN29" s="208"/>
-      <c r="AO29" s="208"/>
-      <c r="AP29" s="208"/>
-      <c r="AQ29" s="208"/>
-      <c r="AR29" s="208"/>
-      <c r="AS29" s="208"/>
-      <c r="AT29" s="208"/>
-      <c r="AU29" s="208"/>
-      <c r="AV29" s="208"/>
-      <c r="AW29" s="208"/>
-      <c r="AX29" s="208"/>
+      <c r="B29" s="214"/>
+      <c r="C29" s="214"/>
+      <c r="D29" s="214"/>
+      <c r="E29" s="214"/>
+      <c r="F29" s="214"/>
+      <c r="G29" s="214"/>
+      <c r="H29" s="214"/>
+      <c r="I29" s="214"/>
+      <c r="J29" s="214"/>
+      <c r="K29" s="214"/>
+      <c r="L29" s="214"/>
+      <c r="M29" s="214"/>
+      <c r="N29" s="214"/>
+      <c r="O29" s="214"/>
+      <c r="P29" s="214"/>
+      <c r="Q29" s="214"/>
+      <c r="R29" s="214"/>
+      <c r="S29" s="214"/>
+      <c r="T29" s="214"/>
+      <c r="U29" s="214"/>
+      <c r="V29" s="214"/>
+      <c r="W29" s="214"/>
+      <c r="X29" s="214"/>
+      <c r="Y29" s="214"/>
+      <c r="Z29" s="214"/>
+      <c r="AA29" s="214"/>
+      <c r="AB29" s="214"/>
+      <c r="AC29" s="214"/>
+      <c r="AD29" s="214"/>
+      <c r="AE29" s="214"/>
+      <c r="AF29" s="214"/>
+      <c r="AG29" s="214"/>
+      <c r="AH29" s="214"/>
+      <c r="AI29" s="214"/>
+      <c r="AJ29" s="214"/>
+      <c r="AK29" s="214"/>
+      <c r="AL29" s="214"/>
+      <c r="AM29" s="214"/>
+      <c r="AN29" s="214"/>
+      <c r="AO29" s="214"/>
+      <c r="AP29" s="214"/>
+      <c r="AQ29" s="214"/>
+      <c r="AR29" s="214"/>
+      <c r="AS29" s="214"/>
+      <c r="AT29" s="214"/>
+      <c r="AU29" s="214"/>
+      <c r="AV29" s="214"/>
+      <c r="AW29" s="214"/>
+      <c r="AX29" s="214"/>
     </row>
     <row r="30" spans="1:144" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="209" t="s">
+      <c r="A30" s="215" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="209"/>
-      <c r="C30" s="209"/>
-      <c r="D30" s="209"/>
-      <c r="E30" s="209"/>
-      <c r="F30" s="208"/>
-      <c r="G30" s="208"/>
+      <c r="B30" s="215"/>
+      <c r="C30" s="215"/>
+      <c r="D30" s="215"/>
+      <c r="E30" s="215"/>
+      <c r="F30" s="214"/>
+      <c r="G30" s="214"/>
       <c r="H30" s="19"/>
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
@@ -10319,10 +10387,10 @@
       <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="210" t="s">
+      <c r="D31" s="216" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="211"/>
+      <c r="E31" s="217"/>
       <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:144" x14ac:dyDescent="0.3">
@@ -10337,11 +10405,11 @@
         <f>C33*98*63/194/201</f>
         <v>460.27127250346206</v>
       </c>
-      <c r="D32" s="212">
+      <c r="D32" s="218">
         <f t="shared" ref="D32:D37" si="33">(B32+C32)/1</f>
         <v>476.23114325280812</v>
       </c>
-      <c r="E32" s="213"/>
+      <c r="E32" s="219"/>
       <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.3">
@@ -10355,11 +10423,11 @@
       <c r="C33" s="10">
         <v>2907</v>
       </c>
-      <c r="D33" s="214">
+      <c r="D33" s="220">
         <f t="shared" si="33"/>
         <v>3007.8</v>
       </c>
-      <c r="E33" s="215"/>
+      <c r="E33" s="221"/>
       <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:49" x14ac:dyDescent="0.3">
@@ -10374,11 +10442,11 @@
         <f>4*AFR44tier1</f>
         <v>11628</v>
       </c>
-      <c r="D34" s="214">
+      <c r="D34" s="220">
         <f t="shared" si="33"/>
         <v>12031.2</v>
       </c>
-      <c r="E34" s="215"/>
+      <c r="E34" s="221"/>
       <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:49" x14ac:dyDescent="0.3">
@@ -10392,11 +10460,11 @@
       <c r="C35" s="95">
         <v>13005</v>
       </c>
-      <c r="D35" s="214">
+      <c r="D35" s="220">
         <f t="shared" si="33"/>
         <v>13475.4</v>
       </c>
-      <c r="E35" s="215"/>
+      <c r="E35" s="221"/>
       <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:49" x14ac:dyDescent="0.3">
@@ -10411,11 +10479,11 @@
         <f>C33*125*97/194/201</f>
         <v>903.91791044776119</v>
       </c>
-      <c r="D36" s="214">
+      <c r="D36" s="220">
         <f t="shared" si="33"/>
         <v>932.02992768118168</v>
       </c>
-      <c r="E36" s="215"/>
+      <c r="E36" s="221"/>
       <c r="F36" s="26"/>
     </row>
     <row r="37" spans="1:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10430,34 +10498,34 @@
         <f>C33*116*133/194/201</f>
         <v>1150.1563317433452</v>
       </c>
-      <c r="D37" s="216">
+      <c r="D37" s="222">
         <f t="shared" si="33"/>
         <v>1190.0379135251578</v>
       </c>
-      <c r="E37" s="217"/>
+      <c r="E37" s="223"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A38" s="202" t="s">
+      <c r="A38" s="208" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="202"/>
-      <c r="C38" s="202"/>
-      <c r="D38" s="202"/>
-      <c r="E38" s="202"/>
-      <c r="F38" s="203"/>
-      <c r="G38" s="203"/>
+      <c r="B38" s="208"/>
+      <c r="C38" s="208"/>
+      <c r="D38" s="208"/>
+      <c r="E38" s="208"/>
+      <c r="F38" s="209"/>
+      <c r="G38" s="209"/>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A39" s="203" t="s">
+      <c r="A39" s="209" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="203"/>
-      <c r="C39" s="203"/>
-      <c r="D39" s="203"/>
-      <c r="E39" s="203"/>
-      <c r="F39" s="203"/>
-      <c r="G39" s="203"/>
+      <c r="B39" s="209"/>
+      <c r="C39" s="209"/>
+      <c r="D39" s="209"/>
+      <c r="E39" s="209"/>
+      <c r="F39" s="209"/>
+      <c r="G39" s="209"/>
       <c r="H39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
@@ -10522,8 +10590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="AY1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="BB6" sqref="BB6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="AP1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="BA3" sqref="BA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10552,7 +10620,7 @@
     <col min="22" max="22" width="21.109375" customWidth="1"/>
     <col min="23" max="23" width="15.6640625" customWidth="1"/>
     <col min="24" max="24" width="26.5546875" customWidth="1"/>
-    <col min="25" max="25" width="12.88671875" customWidth="1"/>
+    <col min="25" max="25" width="19.21875" customWidth="1"/>
     <col min="26" max="26" width="21.33203125" customWidth="1"/>
     <col min="27" max="27" width="18.88671875" customWidth="1"/>
     <col min="28" max="28" width="17.77734375" customWidth="1"/>
@@ -10577,84 +10645,97 @@
     <col min="48" max="48" width="19.109375" customWidth="1"/>
     <col min="49" max="50" width="19.44140625" customWidth="1"/>
     <col min="51" max="51" width="17.6640625" customWidth="1"/>
-    <col min="52" max="52" width="23" customWidth="1"/>
+    <col min="52" max="52" width="19.5546875" customWidth="1"/>
     <col min="53" max="53" width="21.44140625" customWidth="1"/>
     <col min="54" max="54" width="16.6640625" customWidth="1"/>
     <col min="76" max="81" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:81" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="225" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="219"/>
-      <c r="C1" s="219"/>
-      <c r="D1" s="219"/>
-      <c r="E1" s="219"/>
-      <c r="F1" s="219"/>
-      <c r="G1" s="219"/>
-      <c r="H1" s="219"/>
-      <c r="I1" s="219"/>
-      <c r="J1" s="219"/>
-      <c r="K1" s="219"/>
-      <c r="L1" s="219"/>
-      <c r="M1" s="219"/>
-      <c r="N1" s="219"/>
-      <c r="O1" s="219"/>
-      <c r="P1" s="219"/>
-      <c r="Q1" s="219"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="186"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="186"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20"/>
-      <c r="AN1" s="186"/>
-      <c r="AO1" s="186"/>
-      <c r="AP1" s="186"/>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="186"/>
-      <c r="AS1" s="186"/>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="186"/>
-      <c r="AV1" s="186"/>
-      <c r="AW1" s="26"/>
-      <c r="AX1" s="26"/>
-      <c r="AY1" s="20"/>
-      <c r="AZ1" s="20"/>
-      <c r="BB1" s="20"/>
+      <c r="B1" s="225"/>
+      <c r="C1" s="225"/>
+      <c r="D1" s="225"/>
+      <c r="E1" s="225"/>
+      <c r="F1" s="225"/>
+      <c r="G1" s="225"/>
+      <c r="H1" s="225"/>
+      <c r="I1" s="225"/>
+      <c r="J1" s="225" t="str">
+        <f>A1</f>
+        <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
+      </c>
+      <c r="K1" s="225"/>
+      <c r="L1" s="225"/>
+      <c r="M1" s="225"/>
+      <c r="N1" s="225"/>
+      <c r="O1" s="225"/>
+      <c r="P1" s="225"/>
+      <c r="Q1" s="225"/>
+      <c r="R1" s="225"/>
+      <c r="S1" s="226" t="str">
+        <f>A1</f>
+        <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
+      </c>
+      <c r="T1" s="226"/>
+      <c r="U1" s="226"/>
+      <c r="V1" s="226"/>
+      <c r="W1" s="226"/>
+      <c r="X1" s="226"/>
+      <c r="Y1" s="226"/>
+      <c r="Z1" s="226"/>
+      <c r="AA1" s="226"/>
+      <c r="AB1" s="190" t="str">
+        <f>A1</f>
+        <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
+      </c>
+      <c r="AC1" s="190"/>
+      <c r="AD1" s="190"/>
+      <c r="AE1" s="190"/>
+      <c r="AF1" s="190"/>
+      <c r="AG1" s="190"/>
+      <c r="AH1" s="190"/>
+      <c r="AI1" s="190"/>
+      <c r="AJ1" s="191"/>
+      <c r="AK1" s="226" t="str">
+        <f>A1</f>
+        <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
+      </c>
+      <c r="AL1" s="226"/>
+      <c r="AM1" s="226"/>
+      <c r="AN1" s="226"/>
+      <c r="AO1" s="226"/>
+      <c r="AP1" s="226"/>
+      <c r="AQ1" s="226"/>
+      <c r="AR1" s="226"/>
+      <c r="AS1" s="226"/>
+      <c r="AT1" s="190"/>
+      <c r="AU1" s="192"/>
+      <c r="AV1" s="192"/>
+      <c r="AW1" s="191"/>
+      <c r="AX1" s="191"/>
+      <c r="AY1" s="190"/>
+      <c r="AZ1" s="190"/>
+      <c r="BA1" s="193"/>
+      <c r="BB1" s="190"/>
     </row>
     <row r="2" spans="1:81" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="54">
         <f>GeneralRemarks!A2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
-      <c r="D2" s="187"/>
+      <c r="D2" s="183"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
-      <c r="H2" s="187"/>
+      <c r="H2" s="183"/>
       <c r="I2" s="130"/>
       <c r="J2" s="54">
         <f>A2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="K2" s="130"/>
       <c r="L2" s="130"/>
@@ -10666,19 +10747,19 @@
       <c r="R2" s="20"/>
       <c r="S2" s="54">
         <f>J2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="T2" s="20"/>
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
-      <c r="W2" s="187"/>
+      <c r="W2" s="183"/>
       <c r="X2" s="20"/>
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
       <c r="AA2" s="20"/>
       <c r="AB2" s="54">
         <f>S2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="AC2" s="20"/>
       <c r="AD2" s="20"/>
@@ -10690,25 +10771,25 @@
       <c r="AJ2" s="26"/>
       <c r="AK2" s="54">
         <f>AB2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="AL2" s="20"/>
       <c r="AM2" s="20"/>
-      <c r="AN2" s="187"/>
-      <c r="AO2" s="187"/>
-      <c r="AP2" s="187"/>
+      <c r="AN2" s="183"/>
+      <c r="AO2" s="183"/>
+      <c r="AP2" s="183"/>
       <c r="AQ2" s="20"/>
-      <c r="AR2" s="187"/>
-      <c r="AS2" s="187"/>
+      <c r="AR2" s="183"/>
+      <c r="AS2" s="183"/>
       <c r="AT2" s="54">
         <f>AK2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="AU2" s="21"/>
-      <c r="AV2" s="187"/>
+      <c r="AV2" s="183"/>
       <c r="AW2" s="52">
         <f>A2</f>
-        <v>41985</v>
+        <v>41991</v>
       </c>
       <c r="AX2" s="26"/>
       <c r="AY2" s="20"/>
@@ -10735,7 +10816,7 @@
         <f>AllEntries!AM7</f>
         <v>BCCR</v>
       </c>
-      <c r="F3" s="192" t="str">
+      <c r="F3" s="197" t="str">
         <f>AllEntries!AG7</f>
         <v>CCCma</v>
       </c>
@@ -10805,11 +10886,11 @@
         <f>AllEntries!B7</f>
         <v>DMI</v>
       </c>
-      <c r="X3" s="192" t="str">
+      <c r="X3" s="197" t="str">
         <f>AllEntries!AB7</f>
         <v>ENEA</v>
       </c>
-      <c r="Y3" s="192" t="str">
+      <c r="Y3" s="194" t="str">
         <f>AllEntries!AF7</f>
         <v>GISS</v>
       </c>
@@ -10836,7 +10917,7 @@
         <f>AllEntries!AP7</f>
         <v>IPSL-INERIS</v>
       </c>
-      <c r="AF3" s="192" t="str">
+      <c r="AF3" s="197" t="str">
         <f>AllEntries!AI7</f>
         <v>KAUST</v>
       </c>
@@ -10922,11 +11003,11 @@
         <f>AllEntries!AU7</f>
         <v>UM</v>
       </c>
-      <c r="BB3" s="131" t="str">
+      <c r="BB3" s="200" t="str">
         <f>AllEntries!Y7</f>
         <v>UQAM</v>
       </c>
-      <c r="BC3" s="218"/>
+      <c r="BC3" s="224"/>
       <c r="BD3" s="2"/>
       <c r="BE3" s="2"/>
       <c r="BF3" s="2"/>
@@ -10955,217 +11036,217 @@
       <c r="CC3" s="2"/>
     </row>
     <row r="4" spans="1:81" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="193" t="str">
+      <c r="B4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AR9),"",AllEntries!AR9)</f>
         <v/>
       </c>
-      <c r="C4" s="193" t="str">
+      <c r="C4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AQ9),"",AllEntries!AQ9)</f>
         <v/>
       </c>
-      <c r="D4" s="193" t="str">
+      <c r="D4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!C9),"",AllEntries!C9)</f>
         <v>Alfred Wegener Institute, Helmholtz Centre for Polar and Marine Research</v>
       </c>
-      <c r="E4" s="193" t="str">
+      <c r="E4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AM9),"",AllEntries!AM9)</f>
         <v>Bjerknes Centre for Climate Research</v>
       </c>
-      <c r="F4" s="193" t="str">
+      <c r="F4" s="195" t="str">
         <f>IF(ISBLANK(AllEntries!AG9),"",AllEntries!AG9)</f>
         <v>CCCma (Canadian Centre for Climate Modelling and Analysis, Victoria, BC, Canada)</v>
       </c>
-      <c r="G4" s="193" t="str">
+      <c r="G4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!Q9),"",AllEntries!Q9)</f>
         <v/>
       </c>
-      <c r="H4" s="193" t="str">
+      <c r="H4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!D9),"",AllEntries!D9)</f>
         <v>Climate Limited-area Modelling Community (CLM-Community)</v>
       </c>
-      <c r="I4" s="193" t="str">
+      <c r="I4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!E9),"",AllEntries!E9)</f>
         <v>Climate Limited-area Modelling Community (CLM-Community)</v>
       </c>
-      <c r="J4" s="140" t="s">
+      <c r="J4" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="K4" s="193" t="str">
+      <c r="K4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!F9),"",AllEntries!F9)</f>
         <v>Climate Limited-area Modelling Community (CLM-Community)</v>
       </c>
-      <c r="L4" s="193" t="str">
+      <c r="L4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!G9),"",AllEntries!G9)</f>
         <v>Climate Limited-area Modelling Community (CLM-Community)</v>
       </c>
-      <c r="M4" s="193" t="str">
+      <c r="M4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!H9),"",AllEntries!H9)</f>
         <v>Climate Limited-area Modelling Community (CLM-Community)</v>
       </c>
-      <c r="N4" s="193" t="str">
+      <c r="N4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!I9),"",AllEntries!I9)</f>
         <v>Climate Limited-area Modelling Community (CLM-Community)</v>
       </c>
-      <c r="O4" s="193" t="str">
+      <c r="O4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!S9),"",AllEntries!S9)</f>
         <v>Centre National de Recherches Meteorologiques</v>
       </c>
-      <c r="P4" s="193" t="str">
+      <c r="P4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!T9),"",AllEntries!T9)</f>
         <v>Centre National de Recherches Meteorologiques</v>
       </c>
-      <c r="Q4" s="193" t="str">
+      <c r="Q4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!U9),"",AllEntries!U9)</f>
         <v>Centre National de Recherches Meteorologiques</v>
       </c>
-      <c r="R4" s="193" t="str">
+      <c r="R4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AN9),"",AllEntries!AN9)</f>
         <v/>
       </c>
-      <c r="S4" s="140" t="s">
+      <c r="S4" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="T4" s="193" t="str">
+      <c r="T4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AH9),"",AllEntries!AH9)</f>
         <v>Commonwealth Scientific and Industrial Research Organisation</v>
       </c>
-      <c r="U4" s="193" t="str">
+      <c r="U4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AC9),"",AllEntries!AC9)</f>
         <v/>
       </c>
-      <c r="V4" s="193" t="str">
+      <c r="V4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AD9),"",AllEntries!AD9)</f>
         <v>Meteorological and Hydrological Service of Croatia</v>
       </c>
-      <c r="W4" s="193" t="str">
+      <c r="W4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!B9),"",AllEntries!B9)</f>
         <v/>
       </c>
-      <c r="X4" s="194" t="str">
+      <c r="X4" s="195" t="str">
         <f>IF(ISBLANK(AllEntries!AB9),"",AllEntries!AB9)</f>
         <v>Italian National Agency for New Technologies, Energy and Sustainable Economic Development</v>
       </c>
-      <c r="Y4" s="193" t="str">
+      <c r="Y4" s="199" t="str">
         <f>IF(ISBLANK(AllEntries!AF9),"",AllEntries!AF9)</f>
-        <v/>
-      </c>
-      <c r="Z4" s="193" t="str">
+        <v>NASA Goddard Institute for Space Studies (GISS)</v>
+      </c>
+      <c r="Z4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!R9),"",AllEntries!R9)</f>
         <v>Hungarian Meteorological Service</v>
       </c>
-      <c r="AA4" s="193" t="str">
+      <c r="AA4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AA9),"",AllEntries!AA9)</f>
         <v xml:space="preserve"> Abdus Salam International Centre for Theoretical Physics</v>
       </c>
-      <c r="AB4" s="140" t="s">
+      <c r="AB4" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="AC4" s="193" t="str">
+      <c r="AC4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AO9),"",AllEntries!AO9)</f>
         <v/>
       </c>
-      <c r="AD4" s="193" t="str">
+      <c r="AD4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AE9),"",AllEntries!AE9)</f>
         <v>Indian Institute of Tropical Meteorology</v>
       </c>
-      <c r="AE4" s="193" t="str">
+      <c r="AE4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AP9),"",AllEntries!AP9)</f>
         <v/>
       </c>
-      <c r="AF4" s="193" t="str">
+      <c r="AF4" s="195" t="str">
         <f>IF(ISBLANK(AllEntries!AI9),"",AllEntries!AI9)</f>
         <v>King Abdullah University, Thuwal, Saudi Arabien</v>
       </c>
-      <c r="AG4" s="193" t="str">
+      <c r="AG4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!W9),"",AllEntries!W9)</f>
         <v>Royal Netherlands Meteorological Institute, De Bilt, The Netherlands</v>
       </c>
-      <c r="AH4" s="193" t="str">
+      <c r="AH4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!V9),"",AllEntries!V9)</f>
         <v>Royal Netherlands Meteorological Institute, De Bilt, The Netherlands</v>
       </c>
-      <c r="AI4" s="193" t="str">
+      <c r="AI4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!X9),"",AllEntries!X9)</f>
         <v>Royal Netherlands Meteorological Institute, De Bilt, The Netherlands</v>
       </c>
-      <c r="AJ4" s="193" t="str">
+      <c r="AJ4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AL9),"",AllEntries!AL9)</f>
         <v/>
       </c>
-      <c r="AK4" s="140" t="s">
+      <c r="AK4" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="AL4" s="193" t="str">
+      <c r="AL4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AJ9),"",AllEntries!AJ9)</f>
         <v>Met Office Hadley Centre</v>
       </c>
-      <c r="AM4" s="193" t="str">
+      <c r="AM4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AK9),"",AllEntries!AK9)</f>
         <v>Met Office Hadley Centre</v>
       </c>
-      <c r="AN4" s="193" t="str">
+      <c r="AN4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!J9),"",AllEntries!J9)</f>
         <v>Helmholtz-Zentrum Geesthacht, Climate Service Center, Max Planck Institute for Meteorology</v>
       </c>
-      <c r="AO4" s="193" t="str">
+      <c r="AO4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!K9),"",AllEntries!K9)</f>
         <v>Helmholtz-Zentrum Geesthacht, Climate Service Center, Max Planck Institute for Meteorology</v>
       </c>
-      <c r="AP4" s="193" t="str">
+      <c r="AP4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!L9),"",AllEntries!L9)</f>
         <v>Helmholtz-Zentrum Geesthacht, Climate Service Center, Max Planck Institute for Meteorology</v>
       </c>
-      <c r="AQ4" s="193" t="str">
+      <c r="AQ4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AS9),"",AllEntries!AS9)</f>
         <v>National University of Ireland Maynooth</v>
       </c>
-      <c r="AR4" s="193" t="str">
+      <c r="AR4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!O9),"",AllEntries!O9)</f>
         <v>Swedish Meteorological and Hydrological Institute, Rossby Centre</v>
       </c>
-      <c r="AS4" s="193" t="str">
+      <c r="AS4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!M9),"",AllEntries!M9)</f>
         <v>Swedish Meteorological and Hydrological Institute, Rossby Centre</v>
       </c>
-      <c r="AT4" s="140" t="s">
+      <c r="AT4" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="AU4" s="193" t="str">
+      <c r="AU4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!P9),"",AllEntries!P9)</f>
         <v>Swedish Meteorological and Hydrological Institute, Rossby Centre</v>
       </c>
-      <c r="AV4" s="193" t="str">
+      <c r="AV4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!N9),"",AllEntries!N9)</f>
         <v>Swedish Meteorological and Hydrological Institute, Rossby Centre</v>
       </c>
-      <c r="AW4" s="193" t="str">
+      <c r="AW4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AV9),"",AllEntries!AV9)</f>
         <v/>
       </c>
-      <c r="AX4" s="193" t="str">
+      <c r="AX4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AW9),"",AllEntries!AW9)</f>
         <v/>
       </c>
-      <c r="AY4" s="193" t="str">
+      <c r="AY4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!Z9),"",AllEntries!Z9)</f>
         <v>University of Castilla-La Mancha, Toledo, Spain</v>
       </c>
-      <c r="AZ4" s="193" t="str">
+      <c r="AZ4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AT9),"",AllEntries!AT9)</f>
-        <v/>
-      </c>
-      <c r="BA4" s="193" t="str">
+        <v xml:space="preserve">University of Hohenheim </v>
+      </c>
+      <c r="BA4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AU9),"",AllEntries!AU9)</f>
         <v/>
       </c>
-      <c r="BB4" s="142" t="str">
+      <c r="BB4" s="201" t="str">
         <f>IF(ISBLANK(AllEntries!Y9),"",AllEntries!Y9)</f>
         <v>Universite du Quebec a Montreal</v>
       </c>
-      <c r="BC4" s="218"/>
+      <c r="BC4" s="224"/>
       <c r="BD4" s="2"/>
       <c r="BE4" s="2"/>
       <c r="BF4" s="2"/>
@@ -11194,7 +11275,7 @@
       <c r="CC4" s="2"/>
     </row>
     <row r="5" spans="1:81" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="145" t="s">
+      <c r="A5" s="142" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="119" t="str">
@@ -11213,7 +11294,7 @@
         <f>AllEntries!AM8</f>
         <v>WRF331C</v>
       </c>
-      <c r="F5" s="195" t="str">
+      <c r="F5" s="198" t="str">
         <f>AllEntries!AG8</f>
         <v>CanRCM4</v>
       </c>
@@ -11229,7 +11310,7 @@
         <f>AllEntries!E8</f>
         <v>CCLM4-8-17</v>
       </c>
-      <c r="J5" s="145" t="s">
+      <c r="J5" s="142" t="s">
         <v>86</v>
       </c>
       <c r="K5" s="119" t="str">
@@ -11264,7 +11345,7 @@
         <f>AllEntries!AN8</f>
         <v>WRF331A</v>
       </c>
-      <c r="S5" s="145" t="s">
+      <c r="S5" s="142" t="s">
         <v>86</v>
       </c>
       <c r="T5" s="119" t="str">
@@ -11283,11 +11364,11 @@
         <f>AllEntries!B8</f>
         <v>HIRHAM5</v>
       </c>
-      <c r="X5" s="195" t="str">
+      <c r="X5" s="198" t="str">
         <f>AllEntries!AB8</f>
         <v>RegCM4-3</v>
       </c>
-      <c r="Y5" s="195" t="str">
+      <c r="Y5" s="196" t="str">
         <f>AllEntries!AF8</f>
         <v>RM3</v>
       </c>
@@ -11299,7 +11380,7 @@
         <f>AllEntries!AA8</f>
         <v>RegCM4-3</v>
       </c>
-      <c r="AB5" s="145" t="s">
+      <c r="AB5" s="142" t="s">
         <v>86</v>
       </c>
       <c r="AC5" s="119" t="str">
@@ -11314,7 +11395,7 @@
         <f>AllEntries!AP8</f>
         <v>WRF331F</v>
       </c>
-      <c r="AF5" s="195" t="str">
+      <c r="AF5" s="198" t="str">
         <f>AllEntries!AI8</f>
         <v>GFDL</v>
       </c>
@@ -11334,7 +11415,7 @@
         <f>AllEntries!AL8</f>
         <v>WRF331A</v>
       </c>
-      <c r="AK5" s="145" t="s">
+      <c r="AK5" s="142" t="s">
         <v>86</v>
       </c>
       <c r="AL5" s="119" t="str">
@@ -11369,7 +11450,7 @@
         <f>AllEntries!M8</f>
         <v>RCAO-SN</v>
       </c>
-      <c r="AT5" s="145" t="s">
+      <c r="AT5" s="142" t="s">
         <v>86</v>
       </c>
       <c r="AU5" s="119" t="str">
@@ -11394,17 +11475,17 @@
       </c>
       <c r="AZ5" s="119" t="str">
         <f>AllEntries!AT8</f>
-        <v>WRF331H</v>
+        <v>WRF361H</v>
       </c>
       <c r="BA5" s="119" t="str">
         <f>AllEntries!AU8</f>
         <v>WRF331</v>
       </c>
-      <c r="BB5" s="132" t="str">
+      <c r="BB5" s="202" t="str">
         <f>AllEntries!Y8</f>
         <v>CRCM5</v>
       </c>
-      <c r="BC5" s="218"/>
+      <c r="BC5" s="224"/>
       <c r="BD5" s="2"/>
       <c r="BE5" s="2"/>
       <c r="BF5" s="2"/>
@@ -11452,7 +11533,7 @@
         <f>IF(ISBLANK(E9),"",CONCATENATE(E3,"-",E5))</f>
         <v>BCCR-WRF331C</v>
       </c>
-      <c r="F6" s="195" t="str">
+      <c r="F6" s="198" t="str">
         <f>CONCATENATE(F3,"-",F5)</f>
         <v>CCCma-CanRCM4</v>
       </c>
@@ -11522,11 +11603,11 @@
         <f>IF(ISBLANK(W9),"",CONCATENATE(W3,"-",W5))</f>
         <v>DMI-HIRHAM5</v>
       </c>
-      <c r="X6" s="195" t="str">
+      <c r="X6" s="198" t="str">
         <f>CONCATENATE(X3,"-",X5)</f>
         <v>ENEA-RegCM4-3</v>
       </c>
-      <c r="Y6" s="195" t="str">
+      <c r="Y6" s="196" t="str">
         <f>CONCATENATE(Y3,"-",Y5)</f>
         <v>GISS-RM3</v>
       </c>
@@ -11553,7 +11634,7 @@
         <f>IF(ISBLANK(AE9),"",CONCATENATE(AE3,"-",AE5))</f>
         <v>IPSL-INERIS-WRF331F</v>
       </c>
-      <c r="AF6" s="195" t="str">
+      <c r="AF6" s="198" t="str">
         <f>CONCATENATE(AF3,"-",AF5)</f>
         <v>KAUST-GFDL</v>
       </c>
@@ -11633,17 +11714,17 @@
       </c>
       <c r="AZ6" s="119" t="str">
         <f>IF(ISBLANK(AZ9),"",CONCATENATE(AZ3,"-",AZ5))</f>
-        <v>UHOH-WRF331H</v>
+        <v>UHOH-WRF361H</v>
       </c>
       <c r="BA6" s="119" t="str">
         <f>IF(ISBLANK(BA9),"",CONCATENATE(BA3,"-",BA5))</f>
         <v>UM-WRF331</v>
       </c>
-      <c r="BB6" s="132" t="str">
+      <c r="BB6" s="202" t="str">
         <f>CONCATENATE(BB3,"-",BB5)</f>
         <v>UQAM-CRCM5</v>
       </c>
-      <c r="BC6" s="185"/>
+      <c r="BC6" s="182"/>
       <c r="BD6" s="2"/>
       <c r="BE6" s="2"/>
       <c r="BF6" s="2"/>
@@ -11672,209 +11753,209 @@
       <c r="CC6" s="2"/>
     </row>
     <row r="7" spans="1:81" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="143" t="s">
+      <c r="A7" s="140" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="196" t="str">
+      <c r="B7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AR11),"unknown",AllEntries!AR11)</f>
         <v>unknown</v>
       </c>
-      <c r="C7" s="196" t="str">
+      <c r="C7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AQ11),"unknown",AllEntries!AQ11)</f>
         <v>unknown</v>
       </c>
-      <c r="D7" s="196" t="str">
+      <c r="D7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!C11),"unknown",AllEntries!C11)</f>
         <v>unknown</v>
       </c>
-      <c r="E7" s="196" t="str">
+      <c r="E7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AM11),"unknown",AllEntries!AM11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="F7" s="196" t="str">
+      <c r="F7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AG11),"unknown",AllEntries!AG11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="G7" s="196" t="str">
+      <c r="G7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!Q11),"unknown",AllEntries!Q11)</f>
         <v>unknown</v>
       </c>
-      <c r="H7" s="196" t="str">
+      <c r="H7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!D11),"unknown",AllEntries!D11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="I7" s="196" t="str">
+      <c r="I7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!E11),"unknown",AllEntries!E11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="J7" s="143" t="s">
+      <c r="J7" s="140" t="s">
         <v>151</v>
       </c>
-      <c r="K7" s="196" t="str">
+      <c r="K7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!F11),"unknown",AllEntries!F11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="L7" s="196" t="str">
+      <c r="L7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!G11),"unknown",AllEntries!G11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="M7" s="196" t="str">
+      <c r="M7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!H11),"unknown",AllEntries!H11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="N7" s="196" t="str">
+      <c r="N7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!I11),"unknown",AllEntries!I11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="O7" s="196" t="str">
+      <c r="O7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!S11),"unknown",AllEntries!S11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="P7" s="196" t="str">
+      <c r="P7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!T11),"unknown",AllEntries!T11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="Q7" s="196" t="str">
+      <c r="Q7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!U11),"unknown",AllEntries!U11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="R7" s="196" t="str">
+      <c r="R7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AN11),"unknown",AllEntries!AN11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="S7" s="143" t="s">
+      <c r="S7" s="140" t="s">
         <v>151</v>
       </c>
-      <c r="T7" s="196" t="str">
+      <c r="T7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AH11),"unknown",AllEntries!AH11)</f>
         <v>unknown</v>
       </c>
-      <c r="U7" s="196" t="str">
+      <c r="U7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AC11),"unknown",AllEntries!AC11)</f>
         <v>unknown</v>
       </c>
-      <c r="V7" s="196" t="str">
+      <c r="V7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AD11),"unknown",AllEntries!AD11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="W7" s="196" t="str">
+      <c r="W7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!B11),"unknown",AllEntries!B11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="X7" s="196" t="str">
+      <c r="X7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AB11),"unknown",AllEntries!AB11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="Y7" s="196" t="str">
+      <c r="Y7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AF11),"unknown",AllEntries!AF11)</f>
         <v>unknown</v>
       </c>
-      <c r="Z7" s="196" t="str">
+      <c r="Z7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!R11),"unknown",AllEntries!R11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AA7" s="196" t="str">
+      <c r="AA7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AA11),"unknown",AllEntries!AA11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AB7" s="143" t="s">
+      <c r="AB7" s="140" t="s">
         <v>151</v>
       </c>
-      <c r="AC7" s="196" t="str">
+      <c r="AC7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AO11),"unknown",AllEntries!AO11)</f>
         <v>unknown</v>
       </c>
-      <c r="AD7" s="196" t="str">
+      <c r="AD7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AE11),"unknown",AllEntries!AE11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AE7" s="196" t="str">
+      <c r="AE7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AP11),"unknown",AllEntries!AP11)</f>
         <v>unknown</v>
       </c>
-      <c r="AF7" s="196" t="str">
+      <c r="AF7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AI11),"unknown",AllEntries!AI11)</f>
         <v>unknown</v>
       </c>
-      <c r="AG7" s="196" t="str">
+      <c r="AG7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!W11),"unknown",AllEntries!W11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AH7" s="196" t="str">
+      <c r="AH7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!V11),"unknown",AllEntries!V11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AI7" s="196" t="str">
+      <c r="AI7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!X11),"unknown",AllEntries!X11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AJ7" s="196" t="str">
+      <c r="AJ7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AL11),"unknown",AllEntries!AL11)</f>
         <v>unknown</v>
       </c>
-      <c r="AK7" s="143" t="s">
+      <c r="AK7" s="140" t="s">
         <v>151</v>
       </c>
-      <c r="AL7" s="196" t="str">
+      <c r="AL7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AJ11),"unknown",AllEntries!AJ11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AM7" s="196" t="str">
+      <c r="AM7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AK11),"unknown",AllEntries!AK11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AN7" s="196" t="str">
+      <c r="AN7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!J11),"unknown",AllEntries!J11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AO7" s="196" t="str">
+      <c r="AO7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!K11),"unknown",AllEntries!K11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AP7" s="196" t="str">
+      <c r="AP7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!L11),"unknown",AllEntries!L11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AQ7" s="196" t="str">
+      <c r="AQ7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AS11),"unknown",AllEntries!AS11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AR7" s="196" t="str">
+      <c r="AR7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!O11),"",AllEntries!O11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AS7" s="196" t="str">
+      <c r="AS7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!M11),"",AllEntries!M11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AT7" s="143" t="s">
+      <c r="AT7" s="140" t="s">
         <v>151</v>
       </c>
-      <c r="AU7" s="196" t="str">
+      <c r="AU7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!P11),"",AllEntries!P11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AV7" s="196" t="str">
+      <c r="AV7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!N11),"",AllEntries!N11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="AW7" s="196" t="str">
+      <c r="AW7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AV11),"unknown",AllEntries!AV11)</f>
         <v>non-commercial only</v>
       </c>
-      <c r="AX7" s="196" t="str">
+      <c r="AX7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AW11),"unknown",AllEntries!AW11)</f>
         <v>unknown</v>
       </c>
-      <c r="AY7" s="196" t="str">
+      <c r="AY7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!Z11),"unknown",AllEntries!Z11)</f>
         <v>unknown</v>
       </c>
-      <c r="AZ7" s="196" t="str">
+      <c r="AZ7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AT11),"unknown",AllEntries!AT11)</f>
-        <v>unknown</v>
-      </c>
-      <c r="BA7" s="196" t="str">
+        <v>non-commercial only</v>
+      </c>
+      <c r="BA7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AU11),"unknown",AllEntries!AU11)</f>
         <v>unknown</v>
       </c>
@@ -11882,7 +11963,7 @@
         <f>IF(ISBLANK(AllEntries!Y11),"unknown",AllEntries!Y11)</f>
         <v>unrestricted</v>
       </c>
-      <c r="BC7" s="185"/>
+      <c r="BC7" s="182"/>
       <c r="BD7" s="2"/>
       <c r="BE7" s="2"/>
       <c r="BF7" s="2"/>
@@ -11911,372 +11992,374 @@
       <c r="CC7" s="2"/>
     </row>
     <row r="8" spans="1:81" s="36" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="144" t="s">
+      <c r="A8" s="141" t="s">
         <v>187</v>
       </c>
-      <c r="B8" s="135" t="s">
+      <c r="B8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="C8" s="135" t="s">
+      <c r="C8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="D8" s="135" t="s">
+      <c r="D8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="E8" s="135" t="s">
+      <c r="E8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="F8" s="135" t="s">
+      <c r="F8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="G8" s="135" t="s">
+      <c r="G8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="H8" s="135" t="s">
+      <c r="H8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="I8" s="135" t="s">
+      <c r="I8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="J8" s="144" t="s">
+      <c r="J8" s="141" t="s">
         <v>187</v>
       </c>
-      <c r="K8" s="135" t="s">
+      <c r="K8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="L8" s="135" t="s">
+      <c r="L8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="M8" s="135" t="s">
+      <c r="M8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="N8" s="135" t="s">
+      <c r="N8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="O8" s="135" t="s">
+      <c r="O8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="P8" s="135" t="s">
+      <c r="P8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="Q8" s="135" t="s">
+      <c r="Q8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="R8" s="135" t="s">
+      <c r="R8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="S8" s="144" t="s">
+      <c r="S8" s="141" t="s">
         <v>187</v>
       </c>
-      <c r="T8" s="135" t="s">
+      <c r="T8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="U8" s="135" t="s">
+      <c r="U8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="V8" s="135" t="s">
+      <c r="V8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="W8" s="135" t="s">
+      <c r="W8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="X8" s="135"/>
-      <c r="Y8" s="135" t="s">
+      <c r="X8" s="133"/>
+      <c r="Y8" s="133" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="Z8" s="135" t="s">
+      <c r="AA8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AA8" s="135" t="s">
+      <c r="AB8" s="141" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AB8" s="144" t="s">
+      <c r="AD8" s="133" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE8" s="133" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF8" s="133" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG8" s="133" t="s">
+        <v>186</v>
+      </c>
+      <c r="AH8" s="133" t="s">
+        <v>186</v>
+      </c>
+      <c r="AI8" s="133" t="s">
+        <v>186</v>
+      </c>
+      <c r="AJ8" s="133" t="s">
+        <v>186</v>
+      </c>
+      <c r="AK8" s="141" t="s">
         <v>187</v>
       </c>
-      <c r="AC8" s="135" t="s">
+      <c r="AL8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AD8" s="135" t="s">
+      <c r="AM8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AE8" s="135" t="s">
+      <c r="AN8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AF8" s="135" t="s">
+      <c r="AO8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AG8" s="135" t="s">
+      <c r="AP8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AH8" s="135" t="s">
+      <c r="AQ8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AI8" s="135" t="s">
+      <c r="AR8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AJ8" s="135" t="s">
+      <c r="AS8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AK8" s="144" t="s">
+      <c r="AT8" s="141" t="s">
         <v>187</v>
       </c>
-      <c r="AL8" s="135" t="s">
+      <c r="AU8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AM8" s="135" t="s">
+      <c r="AV8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AN8" s="135" t="s">
+      <c r="AW8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AO8" s="135" t="s">
+      <c r="AX8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AP8" s="135" t="s">
+      <c r="AY8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AQ8" s="135" t="s">
+      <c r="AZ8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AR8" s="135" t="s">
+      <c r="BA8" s="133" t="s">
         <v>186</v>
       </c>
-      <c r="AS8" s="135" t="s">
+      <c r="BB8" s="132" t="s">
         <v>186</v>
       </c>
-      <c r="AT8" s="144" t="s">
-        <v>187</v>
-      </c>
-      <c r="AU8" s="135" t="s">
-        <v>186</v>
-      </c>
-      <c r="AV8" s="135" t="s">
-        <v>186</v>
-      </c>
-      <c r="AW8" s="135" t="s">
-        <v>186</v>
-      </c>
-      <c r="AX8" s="135" t="s">
-        <v>186</v>
-      </c>
-      <c r="AY8" s="135" t="s">
-        <v>186</v>
-      </c>
-      <c r="AZ8" s="135" t="s">
-        <v>186</v>
-      </c>
-      <c r="BA8" s="135" t="s">
-        <v>186</v>
-      </c>
-      <c r="BB8" s="134"/>
-      <c r="BC8" s="136"/>
-      <c r="BD8" s="137"/>
-      <c r="BE8" s="137"/>
-      <c r="BF8" s="137"/>
-      <c r="BG8" s="137"/>
-      <c r="BH8" s="137"/>
-      <c r="BI8" s="137"/>
-      <c r="BJ8" s="137"/>
-      <c r="BK8" s="137"/>
-      <c r="BL8" s="137"/>
-      <c r="BM8" s="137"/>
-      <c r="BN8" s="137"/>
-      <c r="BO8" s="137"/>
-      <c r="BP8" s="137"/>
-      <c r="BQ8" s="137"/>
-      <c r="BR8" s="137"/>
-      <c r="BS8" s="137"/>
-      <c r="BT8" s="137"/>
-      <c r="BU8" s="137"/>
-      <c r="BV8" s="137"/>
-      <c r="BW8" s="137"/>
-      <c r="BX8" s="137"/>
-      <c r="BY8" s="137"/>
-      <c r="BZ8" s="137"/>
-      <c r="CA8" s="137"/>
-      <c r="CB8" s="137"/>
-      <c r="CC8" s="137"/>
+      <c r="BC8" s="134"/>
+      <c r="BD8" s="135"/>
+      <c r="BE8" s="135"/>
+      <c r="BF8" s="135"/>
+      <c r="BG8" s="135"/>
+      <c r="BH8" s="135"/>
+      <c r="BI8" s="135"/>
+      <c r="BJ8" s="135"/>
+      <c r="BK8" s="135"/>
+      <c r="BL8" s="135"/>
+      <c r="BM8" s="135"/>
+      <c r="BN8" s="135"/>
+      <c r="BO8" s="135"/>
+      <c r="BP8" s="135"/>
+      <c r="BQ8" s="135"/>
+      <c r="BR8" s="135"/>
+      <c r="BS8" s="135"/>
+      <c r="BT8" s="135"/>
+      <c r="BU8" s="135"/>
+      <c r="BV8" s="135"/>
+      <c r="BW8" s="135"/>
+      <c r="BX8" s="135"/>
+      <c r="BY8" s="135"/>
+      <c r="BZ8" s="135"/>
+      <c r="CA8" s="135"/>
+      <c r="CB8" s="135"/>
+      <c r="CC8" s="135"/>
     </row>
     <row r="9" spans="1:81" s="36" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="188" t="s">
+      <c r="A9" s="184" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="189" t="s">
+      <c r="B9" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="189" t="s">
+      <c r="C9" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="D9" s="189" t="s">
+      <c r="D9" s="185" t="s">
         <v>160</v>
       </c>
-      <c r="E9" s="189" t="s">
+      <c r="E9" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="F9" s="189"/>
-      <c r="G9" s="189" t="s">
+      <c r="F9" s="185"/>
+      <c r="G9" s="185" t="s">
         <v>132</v>
       </c>
-      <c r="H9" s="189" t="s">
+      <c r="H9" s="185" t="s">
         <v>161</v>
       </c>
-      <c r="I9" s="189" t="s">
+      <c r="I9" s="185" t="s">
         <v>161</v>
       </c>
-      <c r="J9" s="188" t="s">
+      <c r="J9" s="184" t="s">
         <v>96</v>
       </c>
-      <c r="K9" s="189" t="s">
+      <c r="K9" s="185" t="s">
         <v>161</v>
       </c>
-      <c r="L9" s="189" t="s">
+      <c r="L9" s="185" t="s">
         <v>161</v>
       </c>
-      <c r="M9" s="189" t="s">
+      <c r="M9" s="185" t="s">
         <v>161</v>
       </c>
-      <c r="N9" s="189" t="s">
+      <c r="N9" s="185" t="s">
         <v>161</v>
       </c>
-      <c r="O9" s="189" t="s">
+      <c r="O9" s="185" t="s">
         <v>131</v>
       </c>
-      <c r="P9" s="189" t="s">
+      <c r="P9" s="185" t="s">
         <v>233</v>
       </c>
-      <c r="Q9" s="189" t="s">
+      <c r="Q9" s="185" t="s">
         <v>131</v>
       </c>
-      <c r="R9" s="189" t="s">
+      <c r="R9" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="S9" s="188" t="s">
+      <c r="S9" s="184" t="s">
         <v>96</v>
       </c>
-      <c r="T9" s="190" t="s">
+      <c r="T9" s="186" t="s">
         <v>229</v>
       </c>
-      <c r="U9" s="189" t="s">
+      <c r="U9" s="185" t="s">
         <v>157</v>
       </c>
-      <c r="V9" s="189" t="s">
+      <c r="V9" s="185" t="s">
         <v>157</v>
       </c>
-      <c r="W9" s="189" t="s">
+      <c r="W9" s="185" t="s">
         <v>154</v>
       </c>
-      <c r="X9" s="189"/>
-      <c r="Y9" s="189"/>
-      <c r="Z9" s="189" t="s">
+      <c r="X9" s="185"/>
+      <c r="Y9" s="185"/>
+      <c r="Z9" s="185" t="s">
         <v>156</v>
       </c>
-      <c r="AA9" s="189" t="s">
+      <c r="AA9" s="185" t="s">
         <v>157</v>
       </c>
-      <c r="AB9" s="188" t="s">
+      <c r="AB9" s="184" t="s">
         <v>96</v>
       </c>
-      <c r="AC9" s="189" t="s">
+      <c r="AC9" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="AD9" s="189" t="s">
+      <c r="AD9" s="185" t="s">
         <v>225</v>
       </c>
-      <c r="AE9" s="189" t="s">
+      <c r="AE9" s="185" t="s">
         <v>166</v>
       </c>
-      <c r="AF9" s="189"/>
-      <c r="AG9" s="189" t="s">
+      <c r="AF9" s="185"/>
+      <c r="AG9" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="AH9" s="189" t="s">
+      <c r="AH9" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="AI9" s="189" t="s">
+      <c r="AI9" s="185" t="s">
         <v>119</v>
       </c>
-      <c r="AJ9" s="189" t="s">
+      <c r="AJ9" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="AK9" s="188" t="s">
+      <c r="AK9" s="184" t="s">
         <v>96</v>
       </c>
-      <c r="AL9" s="189" t="s">
+      <c r="AL9" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="AM9" s="189" t="s">
+      <c r="AM9" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="AN9" s="189" t="s">
+      <c r="AN9" s="185" t="s">
         <v>127</v>
       </c>
-      <c r="AO9" s="189" t="s">
+      <c r="AO9" s="185" t="s">
         <v>127</v>
       </c>
-      <c r="AP9" s="189" t="s">
+      <c r="AP9" s="185" t="s">
         <v>127</v>
       </c>
-      <c r="AQ9" s="189" t="s">
+      <c r="AQ9" s="185" t="s">
         <v>224</v>
       </c>
-      <c r="AR9" s="189" t="s">
+      <c r="AR9" s="185" t="s">
         <v>155</v>
       </c>
-      <c r="AS9" s="189" t="s">
+      <c r="AS9" s="185" t="s">
         <v>155</v>
       </c>
-      <c r="AT9" s="188" t="s">
+      <c r="AT9" s="184" t="s">
         <v>96</v>
       </c>
-      <c r="AU9" s="189" t="s">
+      <c r="AU9" s="185" t="s">
         <v>155</v>
       </c>
-      <c r="AV9" s="189" t="s">
+      <c r="AV9" s="185" t="s">
         <v>155</v>
       </c>
-      <c r="AW9" s="189" t="s">
+      <c r="AW9" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="AX9" s="189" t="s">
+      <c r="AX9" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="AY9" s="189" t="s">
+      <c r="AY9" s="185" t="s">
         <v>162</v>
       </c>
-      <c r="AZ9" s="189" t="s">
+      <c r="AZ9" s="185" t="s">
+        <v>242</v>
+      </c>
+      <c r="BA9" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="BA9" s="189" t="s">
-        <v>159</v>
-      </c>
-      <c r="BB9" s="191"/>
-      <c r="BC9" s="136"/>
-      <c r="BD9" s="137"/>
-      <c r="BE9" s="137"/>
-      <c r="BF9" s="137"/>
-      <c r="BG9" s="137"/>
-      <c r="BH9" s="137"/>
-      <c r="BI9" s="137"/>
-      <c r="BJ9" s="137"/>
-      <c r="BK9" s="137"/>
-      <c r="BL9" s="137"/>
-      <c r="BM9" s="137"/>
-      <c r="BN9" s="137"/>
-      <c r="BO9" s="137"/>
-      <c r="BP9" s="137"/>
-      <c r="BQ9" s="137"/>
-      <c r="BR9" s="137"/>
-      <c r="BS9" s="137"/>
-      <c r="BT9" s="137"/>
-      <c r="BU9" s="137"/>
-      <c r="BV9" s="137"/>
-      <c r="BW9" s="137"/>
-      <c r="BX9" s="137"/>
-      <c r="BY9" s="137"/>
-      <c r="BZ9" s="137"/>
-      <c r="CA9" s="137"/>
-      <c r="CB9" s="137"/>
-      <c r="CC9" s="137"/>
+      <c r="BB9" s="187"/>
+      <c r="BC9" s="134"/>
+      <c r="BD9" s="135"/>
+      <c r="BE9" s="135"/>
+      <c r="BF9" s="135"/>
+      <c r="BG9" s="135"/>
+      <c r="BH9" s="135"/>
+      <c r="BI9" s="135"/>
+      <c r="BJ9" s="135"/>
+      <c r="BK9" s="135"/>
+      <c r="BL9" s="135"/>
+      <c r="BM9" s="135"/>
+      <c r="BN9" s="135"/>
+      <c r="BO9" s="135"/>
+      <c r="BP9" s="135"/>
+      <c r="BQ9" s="135"/>
+      <c r="BR9" s="135"/>
+      <c r="BS9" s="135"/>
+      <c r="BT9" s="135"/>
+      <c r="BU9" s="135"/>
+      <c r="BV9" s="135"/>
+      <c r="BW9" s="135"/>
+      <c r="BX9" s="135"/>
+      <c r="BY9" s="135"/>
+      <c r="BZ9" s="135"/>
+      <c r="CA9" s="135"/>
+      <c r="CB9" s="135"/>
+      <c r="CC9" s="135"/>
     </row>
     <row r="11" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A11" s="63"/>
@@ -12290,8 +12373,12 @@
       <c r="D18" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="BC3:BC5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="S1:AA1"/>
+    <mergeCell ref="AK1:AS1"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" verticalDpi="4" r:id="rId1"/>
@@ -12311,8 +12398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12328,31 +12415,31 @@
       <c r="C2" s="26"/>
     </row>
     <row r="3" spans="2:6" ht="25.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="158" t="s">
+      <c r="B3" s="155" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="159" t="s">
+      <c r="C3" s="156" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="159" t="s">
+      <c r="D3" s="156" t="s">
         <v>195</v>
       </c>
-      <c r="E3" s="160" t="s">
+      <c r="E3" s="157" t="s">
         <v>199</v>
       </c>
-      <c r="F3" s="161" t="s">
+      <c r="F3" s="158" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="162" t="s">
+      <c r="B4" s="159" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="164" t="s">
+      <c r="C4" s="161" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="109"/>
-      <c r="E4" s="166" t="s">
+      <c r="E4" s="163" t="s">
         <v>208</v>
       </c>
       <c r="F4" s="109" t="s">
@@ -12360,29 +12447,29 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="162" t="s">
+      <c r="B5" s="159" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="164" t="s">
+      <c r="C5" s="161" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="109" t="s">
         <v>201</v>
       </c>
-      <c r="E5" s="166"/>
+      <c r="E5" s="163"/>
       <c r="F5" s="109"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="159" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="164" t="s">
+      <c r="C6" s="161" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="E6" s="166" t="s">
+      <c r="E6" s="163" t="s">
         <v>207</v>
       </c>
       <c r="F6" s="109" t="s">
@@ -12390,106 +12477,106 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="164" t="s">
+      <c r="C7" s="161" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="E7" s="166"/>
+      <c r="E7" s="163"/>
       <c r="F7" s="109" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="162" t="s">
+      <c r="B8" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="164" t="s">
+      <c r="C8" s="161" t="s">
         <v>58</v>
       </c>
       <c r="D8" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="E8" s="166"/>
+      <c r="E8" s="163"/>
       <c r="F8" s="109" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="163" t="s">
+      <c r="B9" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="165" t="s">
+      <c r="C9" s="162" t="s">
         <v>58</v>
       </c>
       <c r="D9" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="E9" s="166"/>
+      <c r="E9" s="163"/>
       <c r="F9" s="109" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="163" t="s">
+      <c r="B10" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="165" t="s">
+      <c r="C10" s="162" t="s">
         <v>58</v>
       </c>
       <c r="D10" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="E10" s="166"/>
+      <c r="E10" s="163"/>
       <c r="F10" s="109" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="163" t="s">
+      <c r="B11" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="165" t="s">
+      <c r="C11" s="162" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="E11" s="166"/>
+      <c r="E11" s="163"/>
       <c r="F11" s="109" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="163" t="s">
+      <c r="B12" s="160" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="165" t="s">
+      <c r="C12" s="162" t="s">
         <v>124</v>
       </c>
       <c r="D12" s="109" t="s">
         <v>172</v>
       </c>
-      <c r="E12" s="174"/>
+      <c r="E12" s="171"/>
       <c r="F12" s="109" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="163" t="s">
+      <c r="B13" s="160" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="165" t="s">
+      <c r="C13" s="162" t="s">
         <v>124</v>
       </c>
       <c r="D13" s="109" t="s">
         <v>172</v>
       </c>
-      <c r="E13" s="174" t="s">
+      <c r="E13" s="171" t="s">
         <v>215</v>
       </c>
       <c r="F13" s="109" t="s">
@@ -12497,46 +12584,46 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="163" t="s">
+      <c r="B14" s="160" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="165" t="s">
+      <c r="C14" s="162" t="s">
         <v>124</v>
       </c>
       <c r="D14" s="109" t="s">
         <v>172</v>
       </c>
-      <c r="E14" s="174"/>
+      <c r="E14" s="171"/>
       <c r="F14" s="109" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="163" t="s">
+      <c r="B15" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="165" t="s">
+      <c r="C15" s="162" t="s">
         <v>115</v>
       </c>
       <c r="D15" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="E15" s="174"/>
+      <c r="E15" s="171"/>
       <c r="F15" s="109" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="163" t="s">
+      <c r="B16" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="165" t="s">
+      <c r="C16" s="162" t="s">
         <v>116</v>
       </c>
       <c r="D16" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="E16" s="174" t="s">
+      <c r="E16" s="171" t="s">
         <v>214</v>
       </c>
       <c r="F16" s="109" t="s">
@@ -12544,31 +12631,31 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="163" t="s">
+      <c r="B17" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="165" t="s">
+      <c r="C17" s="162" t="s">
         <v>109</v>
       </c>
       <c r="D17" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="E17" s="174"/>
+      <c r="E17" s="171"/>
       <c r="F17" s="109" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="B18" s="163" t="s">
+      <c r="B18" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="167" t="s">
+      <c r="C18" s="164" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="E18" s="166" t="s">
+      <c r="E18" s="163" t="s">
         <v>213</v>
       </c>
       <c r="F18" s="109" t="s">
@@ -12576,21 +12663,21 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="163" t="s">
+      <c r="B19" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="165" t="s">
+      <c r="C19" s="162" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="109"/>
-      <c r="E19" s="166"/>
+      <c r="E19" s="163"/>
       <c r="F19" s="109"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="163" t="s">
+      <c r="B20" s="160" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="164" t="s">
+      <c r="C20" s="161" t="s">
         <v>26</v>
       </c>
       <c r="D20" s="109" t="s">
@@ -12604,46 +12691,46 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="163" t="s">
+      <c r="B21" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="165" t="s">
+      <c r="C21" s="162" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="109" t="s">
         <v>190</v>
       </c>
-      <c r="E21" s="166"/>
+      <c r="E21" s="163"/>
       <c r="F21" s="109" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="171" t="s">
+      <c r="B22" s="168" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="173" t="s">
+      <c r="C22" s="170" t="s">
         <v>130</v>
       </c>
-      <c r="D22" s="170" t="s">
+      <c r="D22" s="167" t="s">
         <v>190</v>
       </c>
-      <c r="E22" s="166"/>
+      <c r="E22" s="163"/>
       <c r="F22" s="109" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="171" t="s">
+      <c r="B23" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="173" t="s">
+      <c r="C23" s="170" t="s">
         <v>148</v>
       </c>
-      <c r="D23" s="170" t="s">
+      <c r="D23" s="167" t="s">
         <v>169</v>
       </c>
-      <c r="E23" s="166" t="s">
+      <c r="E23" s="163" t="s">
         <v>211</v>
       </c>
       <c r="F23" s="109" t="s">
@@ -12651,16 +12738,16 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="171" t="s">
+      <c r="B24" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="173" t="s">
+      <c r="C24" s="170" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="170" t="s">
+      <c r="D24" s="167" t="s">
         <v>169</v>
       </c>
-      <c r="E24" s="166" t="s">
+      <c r="E24" s="163" t="s">
         <v>210</v>
       </c>
       <c r="F24" s="109" t="s">
@@ -12668,16 +12755,16 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="171" t="s">
+      <c r="B25" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="173" t="s">
+      <c r="C25" s="170" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="170" t="s">
+      <c r="D25" s="167" t="s">
         <v>169</v>
       </c>
-      <c r="E25" s="166" t="s">
+      <c r="E25" s="163" t="s">
         <v>212</v>
       </c>
       <c r="F25" s="109" t="s">
@@ -12685,10 +12772,10 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="163" t="s">
+      <c r="B26" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="165" t="s">
+      <c r="C26" s="162" t="s">
         <v>93</v>
       </c>
       <c r="D26" s="109" t="s">
@@ -12700,10 +12787,10 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="163" t="s">
+      <c r="B27" s="160" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="165" t="s">
+      <c r="C27" s="162" t="s">
         <v>94</v>
       </c>
       <c r="D27" s="109" t="s">
@@ -12713,10 +12800,10 @@
       <c r="F27" s="109"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="163" t="s">
+      <c r="B28" s="160" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="165" t="s">
+      <c r="C28" s="162" t="s">
         <v>95</v>
       </c>
       <c r="D28" s="109" t="s">
@@ -12728,10 +12815,10 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="163" t="s">
+      <c r="B29" s="160" t="s">
         <v>174</v>
       </c>
-      <c r="C29" s="165" t="s">
+      <c r="C29" s="162" t="s">
         <v>95</v>
       </c>
       <c r="D29" s="109" t="s">
@@ -12743,10 +12830,10 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="163" t="s">
+      <c r="B30" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="165" t="s">
+      <c r="C30" s="162" t="s">
         <v>134</v>
       </c>
       <c r="D30" s="109"/>
@@ -12754,10 +12841,10 @@
       <c r="F30" s="109"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="163" t="s">
+      <c r="B31" s="160" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="165" t="s">
+      <c r="C31" s="162" t="s">
         <v>134</v>
       </c>
       <c r="D31" s="109" t="s">
@@ -12769,10 +12856,10 @@
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="163" t="s">
+      <c r="B32" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="167" t="s">
+      <c r="C32" s="164" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="109"/>
@@ -12780,10 +12867,10 @@
       <c r="F32" s="109"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="163" t="s">
+      <c r="B33" s="160" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="165" t="s">
+      <c r="C33" s="162" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="109" t="s">
@@ -12795,10 +12882,10 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="163" t="s">
+      <c r="B34" s="160" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="165" t="s">
+      <c r="C34" s="162" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="109"/>
@@ -12806,10 +12893,10 @@
       <c r="F34" s="109"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="163" t="s">
+      <c r="B35" s="160" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="165" t="s">
+      <c r="C35" s="162" t="s">
         <v>30</v>
       </c>
       <c r="D35" s="109"/>
@@ -12817,10 +12904,10 @@
       <c r="F35" s="109"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" s="163" t="s">
+      <c r="B36" s="160" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="164" t="s">
+      <c r="C36" s="161" t="s">
         <v>114</v>
       </c>
       <c r="D36" s="109" t="s">
@@ -12832,10 +12919,10 @@
       </c>
     </row>
     <row r="37" spans="2:6" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="B37" s="163" t="s">
+      <c r="B37" s="160" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="164" t="s">
+      <c r="C37" s="161" t="s">
         <v>128</v>
       </c>
       <c r="D37" s="109" t="s">
@@ -12849,24 +12936,24 @@
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="168" t="s">
+      <c r="B38" s="165" t="s">
         <v>143</v>
       </c>
-      <c r="C38" s="169" t="s">
+      <c r="C38" s="166" t="s">
         <v>137</v>
       </c>
-      <c r="D38" s="170"/>
+      <c r="D38" s="167"/>
       <c r="E38" s="109"/>
       <c r="F38" s="109"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="168" t="s">
+      <c r="B39" s="165" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="169" t="s">
+      <c r="C39" s="166" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="170" t="s">
+      <c r="D39" s="167" t="s">
         <v>191</v>
       </c>
       <c r="E39" s="109"/>
@@ -12875,47 +12962,47 @@
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="171" t="s">
+      <c r="B40" s="168" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="172" t="s">
+      <c r="C40" s="169" t="s">
         <v>137</v>
       </c>
-      <c r="D40" s="170"/>
+      <c r="D40" s="167"/>
       <c r="E40" s="109"/>
       <c r="F40" s="109" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="171" t="s">
+      <c r="B41" s="168" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="172" t="s">
+      <c r="C41" s="169" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="170"/>
+      <c r="D41" s="167"/>
       <c r="E41" s="109"/>
       <c r="F41" s="109"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="171" t="s">
+      <c r="B42" s="168" t="s">
         <v>164</v>
       </c>
-      <c r="C42" s="172" t="s">
+      <c r="C42" s="169" t="s">
         <v>139</v>
       </c>
-      <c r="D42" s="170"/>
+      <c r="D42" s="167"/>
       <c r="E42" s="109" t="s">
         <v>198</v>
       </c>
       <c r="F42" s="109"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="163" t="s">
+      <c r="B43" s="160" t="s">
         <v>144</v>
       </c>
-      <c r="C43" s="167" t="s">
+      <c r="C43" s="164" t="s">
         <v>137</v>
       </c>
       <c r="D43" s="109"/>
@@ -12923,10 +13010,10 @@
       <c r="F43" s="109"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="163" t="s">
+      <c r="B44" s="160" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="165" t="s">
+      <c r="C44" s="162" t="s">
         <v>146</v>
       </c>
       <c r="D44" s="109"/>
@@ -12934,10 +13021,10 @@
       <c r="F44" s="109"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="163" t="s">
+      <c r="B45" s="160" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="167" t="s">
+      <c r="C45" s="164" t="s">
         <v>175</v>
       </c>
       <c r="D45" s="109"/>
@@ -12945,10 +13032,10 @@
       <c r="F45" s="109"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="163" t="s">
+      <c r="B46" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="167" t="s">
+      <c r="C46" s="164" t="s">
         <v>142</v>
       </c>
       <c r="D46" s="109"/>
@@ -12956,10 +13043,10 @@
       <c r="F46" s="109"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="163" t="s">
+      <c r="B47" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="167" t="s">
+      <c r="C47" s="164" t="s">
         <v>24</v>
       </c>
       <c r="D47" s="109"/>
@@ -12967,10 +13054,10 @@
       <c r="F47" s="109"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="163" t="s">
+      <c r="B48" s="160" t="s">
         <v>140</v>
       </c>
-      <c r="C48" s="173" t="s">
+      <c r="C48" s="170" t="s">
         <v>141</v>
       </c>
       <c r="D48" s="109"/>
@@ -12982,10 +13069,10 @@
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="163" t="s">
+      <c r="B49" s="160" t="s">
         <v>140</v>
       </c>
-      <c r="C49" s="167" t="s">
+      <c r="C49" s="164" t="s">
         <v>147</v>
       </c>
       <c r="D49" s="109"/>
@@ -13002,77 +13089,77 @@
     <sortCondition ref="C4:C49"/>
   </sortState>
   <conditionalFormatting sqref="B5:F5 B21:F22 B7:F12 B26:F27 B38:F41 B19:F19 B17:F17 B14:F15 B49:F49 B43:F47 B30:F36">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:F20">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:F6">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:F24">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37:F37">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:F23">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:F25">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:F18">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:F16">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:F13">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:F48">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:F42">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:F29">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:F28">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B28)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added GMO St. Petersburg, University of Liege, Royal MI of Belgium
</commit_message>
<xml_diff>
--- a/CORDEX_ESGF_coordination_issues.xlsx
+++ b/CORDEX_ESGF_coordination_issues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="768" windowWidth="16608" windowHeight="8676" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="765" windowWidth="16605" windowHeight="8670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralRemarks" sheetId="7" r:id="rId1"/>
@@ -35,10 +35,6 @@
     <definedName name="ANT44tier1">DatVol!$C$36</definedName>
     <definedName name="ARC_44">DatVol!$B$37</definedName>
     <definedName name="ARC44tier1">DatVol!$C$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$AX$13</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$BB$9</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">DatVol!$A$1:$BA$39</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$4</definedName>
     <definedName name="EUR_11" localSheetId="3">ControlledVocabulary!#REF!</definedName>
     <definedName name="EUR_11" localSheetId="2">DatVol!$B$35</definedName>
     <definedName name="EUR_11" localSheetId="0">GeneralRemarks!#REF!</definedName>
@@ -55,17 +51,21 @@
     <definedName name="MED44tier1" localSheetId="2">DatVol!$C$32</definedName>
     <definedName name="MED44tier1" localSheetId="0">GeneralRemarks!#REF!</definedName>
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
-    <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AX$9</definedName>
+    <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$BA$9</definedName>
     <definedName name="Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$BA$5</definedName>
     <definedName name="Print_Area" localSheetId="2">DatVol!$A$1:$AZ$39</definedName>
     <definedName name="Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$BA$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$BB$9</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">DatVol!$A$1:$BA$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="258">
   <si>
     <t>Domain</t>
   </si>
@@ -446,10 +446,6 @@
 legutke@dkrz.de</t>
   </si>
   <si>
-    <t>O.B.Christensen
-obc@dmi.d</t>
-  </si>
-  <si>
     <t>URL, path etc. to data**</t>
   </si>
   <si>
@@ -1209,10 +1205,6 @@
 @nuim.ie</t>
   </si>
   <si>
-    <t>robert.vautard
-@lsce.ipsl.fr</t>
-  </si>
-  <si>
     <t>marta.dominguez@uclm.es; miguel.gaertner
 @uclm.es</t>
   </si>
@@ -1291,6 +1283,58 @@
   <si>
     <t>confirmed by 
 Kirsten Warrach-Sagi</t>
+  </si>
+  <si>
+    <t>O.B.Christensen
+obc@dmi.dk</t>
+  </si>
+  <si>
+    <t>Danish Meteorological Institute</t>
+  </si>
+  <si>
+    <t>MGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RRCM </t>
+  </si>
+  <si>
+    <t>Main Geophysical Observatory, St. Petersburg</t>
+  </si>
+  <si>
+    <t>Igor Shkolnik igor@main.mgo.rssi.ru</t>
+  </si>
+  <si>
+    <t>robert.vautard@lsce.ipsl.fr</t>
+  </si>
+  <si>
+    <t>Lesley De Cruz, lesley.decruz@meteo.be</t>
+  </si>
+  <si>
+    <t>RMIB</t>
+  </si>
+  <si>
+    <t>RMIB-UGENT</t>
+  </si>
+  <si>
+    <t>Alaro-0</t>
+  </si>
+  <si>
+    <t>Royal Meteorological Institute of Belgium</t>
+  </si>
+  <si>
+    <t>Eur-11, Eur-44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xavier Fettweis, xavier.fettweis@ulg.ac.be </t>
+  </si>
+  <si>
+    <t>MAR352</t>
+  </si>
+  <si>
+    <t>University of Liege</t>
+  </si>
+  <si>
+    <t>ULg</t>
   </si>
 </sst>
 </file>
@@ -2537,7 +2581,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3023,6 +3067,9 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3095,25 +3142,24 @@
     <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
+    <cellStyle name="Hyperlink 2" xfId="4"/>
     <cellStyle name="Hyperlänk 2" xfId="3"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="4"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color auto="1"/>
@@ -3301,9 +3347,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kontortema">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Kontor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3341,7 +3387,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Kontor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -3413,7 +3459,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Kontor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3593,27 +3639,27 @@
       <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="15" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="15" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="203" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
-      <c r="F1" s="203"/>
-      <c r="G1" s="203"/>
-      <c r="H1" s="203"/>
-      <c r="I1" s="203"/>
-      <c r="J1" s="203"/>
-      <c r="K1" s="203"/>
-      <c r="L1" s="203"/>
+    <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="204" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="204"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
+      <c r="I1" s="204"/>
+      <c r="J1" s="204"/>
+      <c r="K1" s="204"/>
+      <c r="L1" s="204"/>
       <c r="M1" s="21"/>
       <c r="N1" s="20"/>
       <c r="O1" s="20"/>
@@ -3637,13 +3683,13 @@
       <c r="N2" s="20"/>
       <c r="O2" s="20"/>
     </row>
-    <row r="3" spans="1:15" s="137" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="204" t="s">
-        <v>183</v>
-      </c>
-      <c r="B3" s="204"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="204"/>
+    <row r="3" spans="1:15" s="137" customFormat="1" ht="23.45" x14ac:dyDescent="0.45">
+      <c r="A3" s="205" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="205"/>
+      <c r="C3" s="205"/>
+      <c r="D3" s="205"/>
       <c r="E3" s="136"/>
       <c r="F3" s="136"/>
       <c r="G3" s="136"/>
@@ -3653,7 +3699,7 @@
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
     </row>
-    <row r="4" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="64" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
       <c r="B4" s="65"/>
       <c r="C4" s="65"/>
@@ -3679,65 +3725,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CA38"/>
+  <dimension ref="A1:CD38"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AU10" sqref="AU10"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AZ5" sqref="AZ5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="3" width="13.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="16" width="13.77734375" customWidth="1"/>
-    <col min="17" max="17" width="16.77734375" customWidth="1"/>
-    <col min="18" max="18" width="18.77734375" customWidth="1"/>
-    <col min="19" max="20" width="13.77734375" customWidth="1"/>
-    <col min="21" max="21" width="12.77734375" customWidth="1"/>
-    <col min="22" max="23" width="13.77734375" customWidth="1"/>
-    <col min="24" max="24" width="15.5546875" customWidth="1"/>
-    <col min="25" max="25" width="13.109375" customWidth="1"/>
-    <col min="26" max="26" width="13.88671875" customWidth="1"/>
-    <col min="27" max="27" width="14.44140625" customWidth="1"/>
+    <col min="12" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" customWidth="1"/>
+    <col min="19" max="20" width="13.7109375" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" customWidth="1"/>
+    <col min="22" max="23" width="13.7109375" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" customWidth="1"/>
+    <col min="25" max="25" width="13.140625" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" customWidth="1"/>
+    <col min="27" max="27" width="14.42578125" customWidth="1"/>
     <col min="28" max="28" width="20" customWidth="1"/>
-    <col min="29" max="29" width="13.88671875" customWidth="1"/>
-    <col min="30" max="30" width="13.109375" customWidth="1"/>
-    <col min="31" max="31" width="13.77734375" customWidth="1"/>
-    <col min="32" max="32" width="12.5546875" customWidth="1"/>
-    <col min="33" max="33" width="13.109375" customWidth="1"/>
+    <col min="29" max="29" width="13.85546875" customWidth="1"/>
+    <col min="30" max="30" width="13.140625" customWidth="1"/>
+    <col min="31" max="31" width="13.7109375" customWidth="1"/>
+    <col min="32" max="32" width="12.5703125" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" customWidth="1"/>
     <col min="34" max="34" width="12" customWidth="1"/>
-    <col min="35" max="37" width="16.6640625" customWidth="1"/>
-    <col min="38" max="49" width="13.77734375" customWidth="1"/>
-    <col min="50" max="50" width="22.44140625" customWidth="1"/>
+    <col min="35" max="37" width="16.7109375" customWidth="1"/>
+    <col min="38" max="52" width="13.7109375" customWidth="1"/>
+    <col min="53" max="53" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="205" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
-      <c r="F1" s="203"/>
-      <c r="G1" s="203"/>
-      <c r="H1" s="203"/>
-      <c r="I1" s="203"/>
-      <c r="J1" s="203"/>
-      <c r="K1" s="203"/>
-      <c r="L1" s="203"/>
-      <c r="M1" s="203"/>
-      <c r="N1" s="203"/>
-      <c r="O1" s="203"/>
-      <c r="P1" s="203"/>
+    <row r="1" spans="1:82" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="206" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="204"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
+      <c r="I1" s="204"/>
+      <c r="J1" s="204"/>
+      <c r="K1" s="204"/>
+      <c r="L1" s="204"/>
+      <c r="M1" s="204"/>
+      <c r="N1" s="204"/>
+      <c r="O1" s="204"/>
+      <c r="P1" s="204"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="20"/>
       <c r="S1" s="20"/>
@@ -3771,28 +3815,31 @@
       <c r="AU1" s="20"/>
       <c r="AV1" s="20"/>
       <c r="AW1" s="20"/>
-      <c r="BS1" s="26"/>
-      <c r="BT1" s="26"/>
-      <c r="BU1" s="26"/>
+      <c r="AX1" s="20"/>
+      <c r="AY1" s="20"/>
+      <c r="AZ1" s="20"/>
       <c r="BV1" s="26"/>
       <c r="BW1" s="26"/>
       <c r="BX1" s="26"/>
       <c r="BY1" s="26"/>
       <c r="BZ1" s="26"/>
       <c r="CA1" s="26"/>
+      <c r="CB1" s="26"/>
+      <c r="CC1" s="26"/>
+      <c r="CD1" s="26"/>
     </row>
-    <row r="2" spans="1:79" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53">
         <f>GeneralRemarks!A2</f>
         <v>41991</v>
       </c>
-      <c r="B2" s="207"/>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="207"/>
-      <c r="H2" s="207"/>
+      <c r="B2" s="208"/>
+      <c r="C2" s="208"/>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+      <c r="G2" s="208"/>
+      <c r="H2" s="208"/>
       <c r="I2" s="51"/>
       <c r="J2" s="51"/>
       <c r="K2" s="51"/>
@@ -3837,154 +3884,163 @@
       <c r="AU2" s="20"/>
       <c r="AV2" s="20"/>
       <c r="AW2" s="20"/>
-      <c r="AX2" s="71">
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20"/>
+      <c r="AZ2" s="20"/>
+      <c r="BA2" s="71">
         <f>A2</f>
         <v>41991</v>
       </c>
-      <c r="BS2" s="26"/>
-      <c r="BT2" s="26"/>
-      <c r="BU2" s="26"/>
       <c r="BV2" s="26"/>
       <c r="BW2" s="26"/>
       <c r="BX2" s="26"/>
       <c r="BY2" s="26"/>
       <c r="BZ2" s="26"/>
       <c r="CA2" s="26"/>
+      <c r="CB2" s="26"/>
+      <c r="CC2" s="26"/>
+      <c r="CD2" s="26"/>
     </row>
-    <row r="3" spans="1:79" s="1" customFormat="1" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:82" s="1" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="150" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>63</v>
+        <v>241</v>
       </c>
       <c r="C3" s="105" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="105" t="s">
         <v>62</v>
       </c>
       <c r="E3" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="105" t="s">
-        <v>82</v>
-      </c>
       <c r="G3" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="105" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="105" t="s">
-        <v>80</v>
-      </c>
       <c r="J3" s="105" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="105" t="s">
+        <v>172</v>
+      </c>
+      <c r="L3" s="105" t="s">
         <v>100</v>
       </c>
-      <c r="K3" s="105" t="s">
-        <v>173</v>
-      </c>
-      <c r="L3" s="105" t="s">
-        <v>101</v>
-      </c>
       <c r="M3" s="105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N3" s="105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O3" s="105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P3" s="105" t="s">
         <v>60</v>
       </c>
       <c r="Q3" s="151" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R3" s="105" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S3" s="105" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T3" s="105" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="U3" s="105" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="V3" s="105" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W3" s="105" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="X3" s="105" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Y3" s="105" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Z3" s="105" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AA3" s="105" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AB3" s="105" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AC3" s="105"/>
       <c r="AD3" s="105" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AE3" s="173" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AF3" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG3" s="149" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH3" s="105" t="s">
+        <v>226</v>
+      </c>
+      <c r="AI3" s="105" t="s">
         <v>236</v>
       </c>
-      <c r="AG3" s="149" t="s">
-        <v>178</v>
-      </c>
-      <c r="AH3" s="105" t="s">
-        <v>228</v>
-      </c>
-      <c r="AI3" s="105" t="s">
-        <v>238</v>
-      </c>
       <c r="AJ3" s="106" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AK3" s="106" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AL3" s="105"/>
       <c r="AM3" s="105"/>
       <c r="AN3" s="105"/>
       <c r="AO3" s="105"/>
-      <c r="AP3" s="105" t="s">
-        <v>218</v>
+      <c r="AP3" s="230" t="s">
+        <v>247</v>
       </c>
       <c r="AQ3" s="105"/>
       <c r="AR3" s="105"/>
       <c r="AS3" s="173" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AT3" s="105" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AU3" s="105"/>
       <c r="AV3" s="105"/>
       <c r="AW3" s="105"/>
-      <c r="AX3" s="150" t="s">
+      <c r="AX3" s="173" t="s">
+        <v>246</v>
+      </c>
+      <c r="AY3" s="173" t="s">
+        <v>248</v>
+      </c>
+      <c r="AZ3" s="173" t="s">
+        <v>254</v>
+      </c>
+      <c r="BA3" s="150" t="s">
         <v>57</v>
       </c>
-      <c r="AY3" s="2"/>
-      <c r="AZ3" s="2"/>
-      <c r="BA3" s="2"/>
       <c r="BB3" s="2"/>
       <c r="BC3" s="2"/>
       <c r="BD3" s="2"/>
@@ -4011,8 +4067,11 @@
       <c r="BY3" s="2"/>
       <c r="BZ3" s="2"/>
       <c r="CA3" s="2"/>
+      <c r="CB3" s="2"/>
+      <c r="CC3" s="2"/>
+      <c r="CD3" s="2"/>
     </row>
-    <row r="4" spans="1:79" s="1" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:82" s="1" customFormat="1" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="152" t="s">
         <v>41</v>
       </c>
@@ -4021,7 +4080,7 @@
         <v>DMI</v>
       </c>
       <c r="C4" s="107" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="108" t="s">
         <v>21</v>
@@ -4039,16 +4098,16 @@
         <v>23</v>
       </c>
       <c r="I4" s="108" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J4" s="107" t="s">
+        <v>148</v>
+      </c>
+      <c r="K4" s="107" t="s">
         <v>149</v>
       </c>
-      <c r="K4" s="107" t="s">
-        <v>150</v>
-      </c>
       <c r="L4" s="107" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M4" s="107" t="s">
         <v>42</v>
@@ -4156,7 +4215,7 @@
         <v>IDL</v>
       </c>
       <c r="AP4" s="108" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AQ4" s="108" t="str">
         <f t="shared" si="4"/>
@@ -4186,12 +4245,18 @@
         <f t="shared" si="4"/>
         <v>UCAN</v>
       </c>
-      <c r="AX4" s="152" t="s">
+      <c r="AX4" s="174" t="s">
+        <v>243</v>
+      </c>
+      <c r="AY4" s="174" t="s">
+        <v>249</v>
+      </c>
+      <c r="AZ4" s="174" t="s">
+        <v>257</v>
+      </c>
+      <c r="BA4" s="152" t="s">
         <v>41</v>
       </c>
-      <c r="AY4" s="2"/>
-      <c r="AZ4" s="2"/>
-      <c r="BA4" s="2"/>
       <c r="BB4" s="2"/>
       <c r="BC4" s="2"/>
       <c r="BD4" s="2"/>
@@ -4218,10 +4283,13 @@
       <c r="BY4" s="2"/>
       <c r="BZ4" s="2"/>
       <c r="CA4" s="2"/>
+      <c r="CB4" s="2"/>
+      <c r="CC4" s="2"/>
+      <c r="CD4" s="2"/>
     </row>
-    <row r="5" spans="1:79" s="128" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:82" s="128" customFormat="1" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="153" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="107"/>
       <c r="C5" s="107"/>
@@ -4232,13 +4300,13 @@
       <c r="H5" s="111"/>
       <c r="I5" s="111"/>
       <c r="J5" s="111" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K5" s="111" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L5" s="111" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M5" s="111"/>
       <c r="N5" s="111"/>
@@ -4277,12 +4345,12 @@
       <c r="AU5" s="123"/>
       <c r="AV5" s="123"/>
       <c r="AW5" s="123"/>
-      <c r="AX5" s="153" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY5" s="127"/>
-      <c r="AZ5" s="127"/>
-      <c r="BA5" s="127"/>
+      <c r="AX5" s="175"/>
+      <c r="AY5" s="175"/>
+      <c r="AZ5" s="175"/>
+      <c r="BA5" s="153" t="s">
+        <v>125</v>
+      </c>
       <c r="BB5" s="127"/>
       <c r="BC5" s="127"/>
       <c r="BD5" s="127"/>
@@ -4309,10 +4377,13 @@
       <c r="BY5" s="127"/>
       <c r="BZ5" s="127"/>
       <c r="CA5" s="127"/>
+      <c r="CB5" s="127"/>
+      <c r="CC5" s="127"/>
+      <c r="CD5" s="127"/>
     </row>
-    <row r="6" spans="1:79" s="1" customFormat="1" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:82" s="1" customFormat="1" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="152" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="110"/>
       <c r="C6" s="110"/>
@@ -4362,12 +4433,12 @@
       <c r="AU6" s="108"/>
       <c r="AV6" s="108"/>
       <c r="AW6" s="108"/>
-      <c r="AX6" s="152" t="s">
-        <v>64</v>
-      </c>
-      <c r="AY6" s="2"/>
-      <c r="AZ6" s="2"/>
-      <c r="BA6" s="2"/>
+      <c r="AX6" s="174"/>
+      <c r="AY6" s="174"/>
+      <c r="AZ6" s="174"/>
+      <c r="BA6" s="152" t="s">
+        <v>63</v>
+      </c>
       <c r="BB6" s="2"/>
       <c r="BC6" s="2"/>
       <c r="BD6" s="2"/>
@@ -4394,16 +4465,19 @@
       <c r="BY6" s="2"/>
       <c r="BZ6" s="2"/>
       <c r="CA6" s="2"/>
+      <c r="CB6" s="2"/>
+      <c r="CC6" s="2"/>
+      <c r="CD6" s="2"/>
     </row>
-    <row r="7" spans="1:79" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:82" s="1" customFormat="1" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="153" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7" s="159" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="159" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="159" t="s">
         <v>50</v>
@@ -4424,13 +4498,13 @@
         <v>50</v>
       </c>
       <c r="J7" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K7" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L7" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M7" s="160" t="s">
         <v>42</v>
@@ -4478,7 +4552,7 @@
         <v>38</v>
       </c>
       <c r="AB7" s="160" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AC7" s="160" t="s">
         <v>51</v>
@@ -4487,16 +4561,16 @@
         <v>48</v>
       </c>
       <c r="AE7" s="176" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AF7" s="160" t="s">
         <v>37</v>
       </c>
       <c r="AG7" s="160" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AH7" s="160" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AI7" s="160" t="s">
         <v>55</v>
@@ -4508,7 +4582,7 @@
         <v>53</v>
       </c>
       <c r="AL7" s="165" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AM7" s="165" t="s">
         <v>45</v>
@@ -4520,13 +4594,13 @@
         <v>46</v>
       </c>
       <c r="AP7" s="168" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AQ7" s="160" t="s">
+        <v>143</v>
+      </c>
+      <c r="AR7" s="160" t="s">
         <v>144</v>
-      </c>
-      <c r="AR7" s="160" t="s">
-        <v>145</v>
       </c>
       <c r="AS7" s="160" t="s">
         <v>56</v>
@@ -4538,17 +4612,23 @@
         <v>32</v>
       </c>
       <c r="AV7" s="160" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AW7" s="160" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX7" s="153" t="s">
-        <v>185</v>
-      </c>
-      <c r="AY7" s="2"/>
-      <c r="AZ7" s="2"/>
-      <c r="BA7" s="2"/>
+        <v>139</v>
+      </c>
+      <c r="AX7" s="176" t="s">
+        <v>243</v>
+      </c>
+      <c r="AY7" s="176" t="s">
+        <v>250</v>
+      </c>
+      <c r="AZ7" s="176" t="s">
+        <v>257</v>
+      </c>
+      <c r="BA7" s="153" t="s">
+        <v>184</v>
+      </c>
       <c r="BB7" s="2"/>
       <c r="BC7" s="2"/>
       <c r="BD7" s="2"/>
@@ -4575,10 +4655,13 @@
       <c r="BY7" s="2"/>
       <c r="BZ7" s="2"/>
       <c r="CA7" s="2"/>
+      <c r="CB7" s="2"/>
+      <c r="CC7" s="2"/>
+      <c r="CD7" s="2"/>
     </row>
-    <row r="8" spans="1:79" s="114" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:82" s="114" customFormat="1" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="153" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="161" t="s">
         <v>20</v>
@@ -4605,22 +4688,22 @@
         <v>58</v>
       </c>
       <c r="J8" s="162" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K8" s="162" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L8" s="162" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M8" s="162" t="s">
+        <v>114</v>
+      </c>
+      <c r="N8" s="162" t="s">
         <v>115</v>
       </c>
-      <c r="N8" s="162" t="s">
-        <v>116</v>
-      </c>
       <c r="O8" s="162" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P8" s="164" t="s">
         <v>25</v>
@@ -4635,40 +4718,40 @@
         <v>26</v>
       </c>
       <c r="T8" s="181" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U8" s="170" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="V8" s="170" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W8" s="170" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X8" s="170" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Y8" s="162" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z8" s="162" t="s">
         <v>93</v>
       </c>
-      <c r="Z8" s="162" t="s">
+      <c r="AA8" s="162" t="s">
         <v>94</v>
       </c>
-      <c r="AA8" s="162" t="s">
-        <v>95</v>
-      </c>
       <c r="AB8" s="162" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AC8" s="162" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD8" s="162" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AE8" s="177" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AF8" s="164" t="s">
         <v>27</v>
@@ -4683,53 +4766,59 @@
         <v>30</v>
       </c>
       <c r="AJ8" s="161" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AK8" s="161" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AL8" s="166" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM8" s="166" t="s">
+        <v>135</v>
+      </c>
+      <c r="AN8" s="169" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO8" s="169" t="s">
         <v>137</v>
       </c>
-      <c r="AM8" s="166" t="s">
+      <c r="AP8" s="169" t="s">
+        <v>138</v>
+      </c>
+      <c r="AQ8" s="164" t="s">
         <v>136</v>
       </c>
-      <c r="AN8" s="169" t="s">
-        <v>137</v>
-      </c>
-      <c r="AO8" s="169" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP8" s="169" t="s">
-        <v>139</v>
-      </c>
-      <c r="AQ8" s="164" t="s">
-        <v>137</v>
-      </c>
       <c r="AR8" s="162" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AS8" s="164" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AT8" s="164" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AU8" s="164" t="s">
         <v>24</v>
       </c>
       <c r="AV8" s="170" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AW8" s="164" t="s">
-        <v>147</v>
-      </c>
-      <c r="AX8" s="153" t="s">
-        <v>86</v>
-      </c>
-      <c r="AY8" s="113"/>
-      <c r="AZ8" s="113"/>
-      <c r="BA8" s="113"/>
+        <v>146</v>
+      </c>
+      <c r="AX8" s="229" t="s">
+        <v>244</v>
+      </c>
+      <c r="AY8" s="229" t="s">
+        <v>251</v>
+      </c>
+      <c r="AZ8" s="229" t="s">
+        <v>255</v>
+      </c>
+      <c r="BA8" s="153" t="s">
+        <v>85</v>
+      </c>
       <c r="BB8" s="113"/>
       <c r="BC8" s="113"/>
       <c r="BD8" s="113"/>
@@ -4756,116 +4845,121 @@
       <c r="BY8" s="113"/>
       <c r="BZ8" s="113"/>
       <c r="CA8" s="113"/>
+      <c r="CB8" s="113"/>
+      <c r="CC8" s="113"/>
+      <c r="CD8" s="113"/>
     </row>
-    <row r="9" spans="1:79" s="35" customFormat="1" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:82" s="35" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="152" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="109" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" s="109" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="109" t="s">
         <v>167</v>
       </c>
-      <c r="B9" s="109"/>
-      <c r="C9" s="109" t="s">
-        <v>201</v>
-      </c>
-      <c r="D9" s="109" t="s">
-        <v>168</v>
-      </c>
       <c r="E9" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F9" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G9" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H9" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I9" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J9" s="109" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K9" s="109" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L9" s="109" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M9" s="109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N9" s="109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O9" s="109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P9" s="109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q9" s="109"/>
       <c r="R9" s="109" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="S9" s="109" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T9" s="167" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U9" s="167" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="V9" s="167" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W9" s="167" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X9" s="167" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y9" s="109" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z9" s="109" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AA9" s="109" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AB9" s="109" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AC9" s="109"/>
       <c r="AD9" s="109" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE9" s="178" t="s">
+        <v>218</v>
+      </c>
+      <c r="AF9" s="109" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG9" s="109" t="s">
+        <v>176</v>
+      </c>
+      <c r="AH9" s="109" t="s">
+        <v>225</v>
+      </c>
+      <c r="AI9" s="109" t="s">
+        <v>228</v>
+      </c>
+      <c r="AJ9" s="109" t="s">
         <v>188</v>
       </c>
-      <c r="AE9" s="178" t="s">
-        <v>220</v>
-      </c>
-      <c r="AF9" s="109" t="s">
-        <v>235</v>
-      </c>
-      <c r="AG9" s="109" t="s">
-        <v>177</v>
-      </c>
-      <c r="AH9" s="109" t="s">
-        <v>227</v>
-      </c>
-      <c r="AI9" s="109" t="s">
-        <v>230</v>
-      </c>
-      <c r="AJ9" s="109" t="s">
-        <v>189</v>
-      </c>
       <c r="AK9" s="109" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AL9" s="167"/>
       <c r="AM9" s="167" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AN9" s="167"/>
       <c r="AO9" s="167"/>
@@ -4873,20 +4967,26 @@
       <c r="AQ9" s="109"/>
       <c r="AR9" s="109"/>
       <c r="AS9" s="178" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AT9" s="109" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AU9" s="109"/>
       <c r="AV9" s="109"/>
       <c r="AW9" s="109"/>
-      <c r="AX9" s="152" t="s">
-        <v>167</v>
-      </c>
-      <c r="AY9" s="70"/>
-      <c r="AZ9" s="70"/>
-      <c r="BA9" s="70"/>
+      <c r="AX9" s="178" t="s">
+        <v>245</v>
+      </c>
+      <c r="AY9" s="178" t="s">
+        <v>252</v>
+      </c>
+      <c r="AZ9" s="178" t="s">
+        <v>256</v>
+      </c>
+      <c r="BA9" s="152" t="s">
+        <v>166</v>
+      </c>
       <c r="BB9" s="70"/>
       <c r="BC9" s="70"/>
       <c r="BD9" s="70"/>
@@ -4913,17 +5013,20 @@
       <c r="BY9" s="70"/>
       <c r="BZ9" s="70"/>
       <c r="CA9" s="70"/>
+      <c r="CB9" s="70"/>
+      <c r="CC9" s="70"/>
+      <c r="CD9" s="70"/>
     </row>
-    <row r="10" spans="1:79" s="1" customFormat="1" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:82" s="1" customFormat="1" ht="101.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="152" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B10" s="163" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10" s="163"/>
       <c r="D10" s="163" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E10" s="163"/>
       <c r="F10" s="163"/>
@@ -4932,34 +5035,34 @@
       <c r="I10" s="163"/>
       <c r="J10" s="171"/>
       <c r="K10" s="171" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L10" s="171"/>
       <c r="M10" s="171"/>
       <c r="N10" s="171" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O10" s="171"/>
       <c r="P10" s="163" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q10" s="163"/>
       <c r="R10" s="109" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="S10" s="163"/>
       <c r="T10" s="163" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="U10" s="163"/>
       <c r="V10" s="163" t="s">
+        <v>210</v>
+      </c>
+      <c r="W10" s="163" t="s">
+        <v>209</v>
+      </c>
+      <c r="X10" s="163" t="s">
         <v>211</v>
-      </c>
-      <c r="W10" s="163" t="s">
-        <v>210</v>
-      </c>
-      <c r="X10" s="163" t="s">
-        <v>212</v>
       </c>
       <c r="Y10" s="109"/>
       <c r="Z10" s="109"/>
@@ -4974,14 +5077,14 @@
       <c r="AI10" s="109"/>
       <c r="AJ10" s="109"/>
       <c r="AK10" s="109" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL10" s="109"/>
       <c r="AM10" s="109"/>
       <c r="AN10" s="109"/>
       <c r="AO10" s="109"/>
       <c r="AP10" s="109" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AQ10" s="109"/>
       <c r="AR10" s="109"/>
@@ -4989,15 +5092,19 @@
       <c r="AT10" s="109"/>
       <c r="AU10" s="109"/>
       <c r="AV10" s="109" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AW10" s="109"/>
-      <c r="AX10" s="152" t="s">
-        <v>197</v>
-      </c>
-      <c r="AY10" s="2"/>
-      <c r="AZ10" s="2"/>
-      <c r="BA10" s="2"/>
+      <c r="AX10" s="178"/>
+      <c r="AY10" s="178" t="s">
+        <v>253</v>
+      </c>
+      <c r="AZ10" s="178" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA10" s="152" t="s">
+        <v>196</v>
+      </c>
       <c r="BB10" s="2"/>
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
@@ -5024,133 +5131,136 @@
       <c r="BY10" s="2"/>
       <c r="BZ10" s="2"/>
       <c r="CA10" s="2"/>
+      <c r="CB10" s="2"/>
+      <c r="CC10" s="2"/>
+      <c r="CD10" s="2"/>
     </row>
-    <row r="11" spans="1:79" s="128" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:82" s="128" customFormat="1" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="154" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C11" s="109"/>
       <c r="D11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q11" s="109"/>
       <c r="R11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="S11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="V11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="W11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="X11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Y11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Z11" s="109"/>
       <c r="AA11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AB11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AC11" s="109"/>
       <c r="AD11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AE11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AF11" s="109"/>
       <c r="AG11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AH11" s="109"/>
       <c r="AI11" s="109"/>
       <c r="AJ11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AL11" s="109"/>
       <c r="AM11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AN11" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO11" s="109"/>
       <c r="AP11" s="109"/>
       <c r="AQ11" s="109"/>
       <c r="AR11" s="109"/>
       <c r="AS11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AT11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AU11" s="109"/>
       <c r="AV11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AW11" s="109"/>
-      <c r="AX11" s="179" t="s">
-        <v>153</v>
-      </c>
-      <c r="AY11" s="127"/>
-      <c r="AZ11" s="127"/>
-      <c r="BA11" s="127"/>
+      <c r="AX11" s="228"/>
+      <c r="AY11" s="228"/>
+      <c r="AZ11" s="228"/>
+      <c r="BA11" s="179" t="s">
+        <v>152</v>
+      </c>
       <c r="BB11" s="127"/>
       <c r="BC11" s="127"/>
       <c r="BD11" s="127"/>
@@ -5177,18 +5287,21 @@
       <c r="BY11" s="127"/>
       <c r="BZ11" s="127"/>
       <c r="CA11" s="127"/>
+      <c r="CB11" s="127"/>
+      <c r="CC11" s="127"/>
+      <c r="CD11" s="127"/>
     </row>
-    <row r="12" spans="1:79" s="26" customFormat="1" ht="21.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="206" t="s">
-        <v>152</v>
-      </c>
-      <c r="B12" s="206"/>
-      <c r="C12" s="206"/>
-      <c r="D12" s="206"/>
-      <c r="E12" s="206"/>
-      <c r="F12" s="206"/>
-      <c r="G12" s="206"/>
-      <c r="H12" s="206"/>
+    <row r="12" spans="1:82" s="26" customFormat="1" ht="21.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="207" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="207"/>
+      <c r="C12" s="207"/>
+      <c r="D12" s="207"/>
+      <c r="E12" s="207"/>
+      <c r="F12" s="207"/>
+      <c r="G12" s="207"/>
+      <c r="H12" s="207"/>
       <c r="I12" s="120"/>
       <c r="J12" s="120"/>
       <c r="K12" s="120"/>
@@ -5230,16 +5343,19 @@
       <c r="AU12" s="120"/>
       <c r="AV12" s="120"/>
       <c r="AW12" s="120"/>
+      <c r="AX12" s="203"/>
+      <c r="AY12" s="203"/>
+      <c r="AZ12" s="203"/>
     </row>
-    <row r="13" spans="1:79" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="206" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="206"/>
-      <c r="C13" s="206"/>
-      <c r="D13" s="206"/>
-      <c r="E13" s="206"/>
-      <c r="F13" s="206"/>
+    <row r="13" spans="1:82" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="207" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="207"/>
+      <c r="C13" s="207"/>
+      <c r="D13" s="207"/>
+      <c r="E13" s="207"/>
+      <c r="F13" s="207"/>
       <c r="G13" s="131"/>
       <c r="H13" s="131"/>
       <c r="I13" s="131"/>
@@ -5282,19 +5398,22 @@
       <c r="AU13" s="131"/>
       <c r="AV13" s="131"/>
       <c r="AW13" s="131"/>
+      <c r="AX13" s="131"/>
+      <c r="AY13" s="131"/>
+      <c r="AZ13" s="131"/>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.3">
-      <c r="AX14" s="70"/>
+    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="BA14" s="70"/>
     </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
       <c r="N22" s="115"/>
     </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D24" s="64"/>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -5304,21 +5423,22 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A13:F13"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:AD7 AE7:AW10 B8:S8 U8:AD8 B9:AD11 AF11:AW11">
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="B7:AZ7 B8:S8 B9:AD11 AF11:AZ11 AE9:AZ10 U8:AW8">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE11">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",AE11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="AG3" r:id="rId1" display="mailto:John.Scinocca@ec.gc.ca"/>
+    <hyperlink ref="AP3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="47" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="47" fitToHeight="0" orientation="landscape" r:id="rId3"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="35" max="8" man="1"/>
   </colBreaks>
@@ -5333,69 +5453,68 @@
       <selection activeCell="AW3" sqref="AW3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="12" width="13.77734375" customWidth="1"/>
-    <col min="13" max="13" width="19.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" customWidth="1"/>
-    <col min="15" max="15" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
-    <col min="17" max="17" width="11.88671875" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" customWidth="1"/>
-    <col min="19" max="19" width="13.6640625" customWidth="1"/>
-    <col min="20" max="20" width="16.6640625" customWidth="1"/>
-    <col min="21" max="21" width="11.88671875" customWidth="1"/>
-    <col min="22" max="22" width="12.6640625" customWidth="1"/>
-    <col min="23" max="23" width="15.21875" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="15.44140625" customWidth="1"/>
-    <col min="26" max="26" width="12.6640625" customWidth="1"/>
-    <col min="27" max="27" width="11.21875" customWidth="1"/>
-    <col min="28" max="29" width="13.5546875" customWidth="1"/>
-    <col min="30" max="30" width="13.21875" customWidth="1"/>
-    <col min="31" max="31" width="11.88671875" customWidth="1"/>
-    <col min="32" max="32" width="10.88671875" customWidth="1"/>
-    <col min="33" max="33" width="11.6640625" customWidth="1"/>
-    <col min="34" max="35" width="19.77734375" customWidth="1"/>
-    <col min="36" max="36" width="9.44140625" customWidth="1"/>
-    <col min="37" max="37" width="14.77734375" customWidth="1"/>
-    <col min="38" max="39" width="12.77734375" customWidth="1"/>
-    <col min="40" max="40" width="11.6640625" customWidth="1"/>
-    <col min="41" max="41" width="9.88671875" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" customWidth="1"/>
+    <col min="28" max="29" width="13.5703125" customWidth="1"/>
+    <col min="30" max="30" width="13.28515625" customWidth="1"/>
+    <col min="31" max="31" width="11.85546875" customWidth="1"/>
+    <col min="32" max="32" width="10.85546875" customWidth="1"/>
+    <col min="33" max="33" width="11.7109375" customWidth="1"/>
+    <col min="34" max="35" width="19.7109375" customWidth="1"/>
+    <col min="36" max="36" width="9.42578125" customWidth="1"/>
+    <col min="37" max="37" width="14.7109375" customWidth="1"/>
+    <col min="38" max="39" width="12.7109375" customWidth="1"/>
+    <col min="40" max="40" width="11.7109375" customWidth="1"/>
+    <col min="41" max="41" width="9.85546875" customWidth="1"/>
     <col min="42" max="42" width="11" customWidth="1"/>
-    <col min="43" max="44" width="10.77734375" customWidth="1"/>
-    <col min="45" max="46" width="10.6640625" customWidth="1"/>
-    <col min="47" max="47" width="11.109375" customWidth="1"/>
-    <col min="48" max="48" width="10.5546875" customWidth="1"/>
-    <col min="49" max="49" width="10.77734375" customWidth="1"/>
-    <col min="50" max="50" width="9.88671875" customWidth="1"/>
-    <col min="51" max="51" width="14.33203125" customWidth="1"/>
-    <col min="52" max="52" width="13.6640625" customWidth="1"/>
-    <col min="53" max="53" width="19.21875" style="26" customWidth="1"/>
-    <col min="54" max="143" width="8.88671875" style="26"/>
+    <col min="43" max="46" width="10.7109375" customWidth="1"/>
+    <col min="47" max="47" width="11.140625" customWidth="1"/>
+    <col min="48" max="48" width="10.5703125" customWidth="1"/>
+    <col min="49" max="49" width="10.7109375" customWidth="1"/>
+    <col min="50" max="50" width="9.85546875" customWidth="1"/>
+    <col min="51" max="51" width="14.28515625" customWidth="1"/>
+    <col min="52" max="52" width="13.7109375" customWidth="1"/>
+    <col min="53" max="53" width="19.28515625" style="26" customWidth="1"/>
+    <col min="54" max="143" width="8.85546875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:144" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="203" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
-      <c r="F1" s="203"/>
-      <c r="G1" s="203"/>
-      <c r="H1" s="203"/>
-      <c r="I1" s="203"/>
-      <c r="J1" s="203"/>
-      <c r="K1" s="203"/>
-      <c r="L1" s="203"/>
-      <c r="M1" s="203"/>
-      <c r="N1" s="203"/>
-      <c r="O1" s="203"/>
-      <c r="P1" s="203"/>
-      <c r="Q1" s="203"/>
+    <row r="1" spans="1:144" ht="80.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="204" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="204"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
+      <c r="I1" s="204"/>
+      <c r="J1" s="204"/>
+      <c r="K1" s="204"/>
+      <c r="L1" s="204"/>
+      <c r="M1" s="204"/>
+      <c r="N1" s="204"/>
+      <c r="O1" s="204"/>
+      <c r="P1" s="204"/>
+      <c r="Q1" s="204"/>
       <c r="R1" s="21"/>
       <c r="S1" s="20"/>
       <c r="T1" s="20"/>
@@ -5500,7 +5619,7 @@
       <c r="B3" s="28" t="str">
         <f>AllEntries!B3</f>
         <v>O.B.Christensen
-obc@dmi.d</v>
+obc@dmi.dk</v>
       </c>
       <c r="C3" s="29" t="str">
         <f>AllEntries!C3</f>
@@ -5694,8 +5813,7 @@
       </c>
       <c r="AQ3" s="29" t="str">
         <f>AllEntries!AP3</f>
-        <v>robert.vautard
-@lsce.ipsl.fr</v>
+        <v>robert.vautard@lsce.ipsl.fr</v>
       </c>
       <c r="AR3" s="29">
         <f>AllEntries!AQ3</f>
@@ -5826,7 +5944,7 @@
       <c r="EM3" s="2"/>
       <c r="EN3" s="2"/>
     </row>
-    <row r="4" spans="1:144" s="1" customFormat="1" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:144" s="1" customFormat="1" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="73" t="str">
         <f>AllEntries!A4</f>
         <v>Data providing  center</v>
@@ -6031,7 +6149,7 @@
         <f>AllEntries!AW4</f>
         <v>UCAN</v>
       </c>
-      <c r="AZ4" s="210" t="s">
+      <c r="AZ4" s="211" t="s">
         <v>16</v>
       </c>
       <c r="BA4" s="73" t="s">
@@ -6129,7 +6247,7 @@
       <c r="EM4" s="2"/>
       <c r="EN4" s="2"/>
     </row>
-    <row r="5" spans="1:144" s="1" customFormat="1" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:144" s="1" customFormat="1" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="73" t="str">
         <f>AllEntries!A6</f>
         <v>URL, path etc. to data**</v>
@@ -6334,7 +6452,7 @@
         <f>AllEntries!AW6</f>
         <v>0</v>
       </c>
-      <c r="AZ5" s="211"/>
+      <c r="AZ5" s="212"/>
       <c r="BA5" s="73"/>
       <c r="BB5" s="2"/>
       <c r="BC5" s="2"/>
@@ -6428,7 +6546,7 @@
       <c r="EM5" s="2"/>
       <c r="EN5" s="2"/>
     </row>
-    <row r="6" spans="1:144" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:144" s="1" customFormat="1" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="74" t="str">
         <f>AllEntries!A8</f>
         <v xml:space="preserve">RCM name </v>
@@ -6633,7 +6751,7 @@
         <f>AllEntries!AW8</f>
         <v>WRF350I</v>
       </c>
-      <c r="AZ6" s="212"/>
+      <c r="AZ6" s="213"/>
       <c r="BA6" s="74" t="s">
         <v>19</v>
       </c>
@@ -6729,9 +6847,9 @@
       <c r="EM6" s="2"/>
       <c r="EN6" s="2"/>
     </row>
-    <row r="7" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="16">
         <f>(1*56+2*95+0)*AFR_44/1000</f>
@@ -6907,7 +7025,7 @@
       </c>
       <c r="EN7" s="26"/>
     </row>
-    <row r="8" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="75" t="s">
         <v>12</v>
       </c>
@@ -7085,7 +7203,7 @@
       </c>
       <c r="EN8" s="26"/>
     </row>
-    <row r="9" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="75" t="s">
         <v>13</v>
       </c>
@@ -7263,7 +7381,7 @@
       </c>
       <c r="EN9" s="26"/>
     </row>
-    <row r="10" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="75" t="s">
         <v>14</v>
       </c>
@@ -7441,7 +7559,7 @@
       </c>
       <c r="EN10" s="26"/>
     </row>
-    <row r="11" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="75" t="s">
         <v>43</v>
       </c>
@@ -7621,7 +7739,7 @@
       </c>
       <c r="EN11" s="26"/>
     </row>
-    <row r="12" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="75" t="s">
         <v>44</v>
       </c>
@@ -7797,14 +7915,14 @@
         <v>4459.0893749999987</v>
       </c>
       <c r="BA12" s="75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB12" s="104"/>
       <c r="EN12" s="26"/>
     </row>
-    <row r="13" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="18">
         <f>(1*56+1*95+21)*EUR_11/1000</f>
@@ -7848,7 +7966,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N13" s="18"/>
       <c r="O13" s="15"/>
@@ -7909,7 +8027,7 @@
         <v>0</v>
       </c>
       <c r="AH13" s="75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AI13" s="146"/>
       <c r="AJ13" s="15">
@@ -7978,13 +8096,13 @@
         <v>1714.1376</v>
       </c>
       <c r="BA13" s="75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="EN13" s="26"/>
     </row>
-    <row r="14" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="18">
         <f>(1*56+1*95+21)*EUR11tier1/1000</f>
@@ -8028,7 +8146,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N14" s="18"/>
       <c r="O14" s="15"/>
@@ -8089,7 +8207,7 @@
         <v>0</v>
       </c>
       <c r="AH14" s="75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AI14" s="146"/>
       <c r="AJ14" s="15">
@@ -8158,11 +8276,11 @@
         <v>47390.220000000008</v>
       </c>
       <c r="BA14" s="75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="EN14" s="26"/>
     </row>
-    <row r="15" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="75" t="s">
         <v>17</v>
       </c>
@@ -8340,9 +8458,9 @@
       </c>
       <c r="EN15" s="26"/>
     </row>
-    <row r="16" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="18">
         <f>(0*56+0*95+0)*MED44tier1/1000</f>
@@ -8386,7 +8504,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N16" s="18"/>
       <c r="O16" s="15"/>
@@ -8445,7 +8563,7 @@
         <v>0</v>
       </c>
       <c r="AH16" s="75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AI16" s="146"/>
       <c r="AJ16" s="15">
@@ -8514,11 +8632,11 @@
         <v>250.84784351438685</v>
       </c>
       <c r="BA16" s="75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="EN16" s="26"/>
     </row>
-    <row r="17" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="75" t="s">
         <v>18</v>
       </c>
@@ -8564,7 +8682,7 @@
         <v>16.981302477304197</v>
       </c>
       <c r="M17" s="75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N17" s="18"/>
       <c r="O17" s="15"/>
@@ -8623,7 +8741,7 @@
         <v>0</v>
       </c>
       <c r="AH17" s="75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AI17" s="146"/>
       <c r="AJ17" s="15">
@@ -8692,13 +8810,13 @@
         <v>33.962604954608395</v>
       </c>
       <c r="BA17" s="75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="EN17" s="26"/>
     </row>
-    <row r="18" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="18">
         <f t="shared" ref="B18:AY18" si="16">(0*56+0*95+0)*MED44tier1*4/1000</f>
@@ -8742,7 +8860,7 @@
         <v>489.72863394368363</v>
       </c>
       <c r="M18" s="75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N18" s="18"/>
       <c r="O18" s="15"/>
@@ -8801,7 +8919,7 @@
         <v>0</v>
       </c>
       <c r="AH18" s="75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AI18" s="146"/>
       <c r="AJ18" s="15">
@@ -8870,13 +8988,13 @@
         <v>979.45726788736727</v>
       </c>
       <c r="BA18" s="75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="EN18" s="26"/>
     </row>
-    <row r="19" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="18">
         <f t="shared" ref="B19:AY19" si="17">(0*56+0*95+0)*MED_44*16/1000</f>
@@ -8920,7 +9038,7 @@
         <v>5.1071586397907369</v>
       </c>
       <c r="M19" s="75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N19" s="18"/>
       <c r="O19" s="15"/>
@@ -8979,7 +9097,7 @@
         <v>0</v>
       </c>
       <c r="AH19" s="75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AI19" s="146"/>
       <c r="AJ19" s="15">
@@ -9048,13 +9166,13 @@
         <v>76.352021664871515</v>
       </c>
       <c r="BA19" s="75" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="EN19" s="26"/>
     </row>
-    <row r="20" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="18">
         <f t="shared" ref="B20:AY20" si="18">(0*56+0*95+0)*MED44tier1*16/1000</f>
@@ -9098,7 +9216,7 @@
         <v>147.28680720110785</v>
       </c>
       <c r="M20" s="75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N20" s="18"/>
       <c r="O20" s="15"/>
@@ -9157,7 +9275,7 @@
         <v>0</v>
       </c>
       <c r="AH20" s="75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AI20" s="146"/>
       <c r="AJ20" s="15">
@@ -9226,13 +9344,13 @@
         <v>2201.9377676565628</v>
       </c>
       <c r="BA20" s="75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="EN20" s="26"/>
     </row>
-    <row r="21" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="15"/>
@@ -9242,13 +9360,13 @@
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J21" s="50"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N21" s="18"/>
       <c r="O21" s="15"/>
@@ -9271,7 +9389,7 @@
       <c r="AF21" s="15"/>
       <c r="AG21" s="83"/>
       <c r="AH21" s="75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI21" s="146"/>
       <c r="AJ21" s="15"/>
@@ -9295,13 +9413,13 @@
         <v>0</v>
       </c>
       <c r="BA21" s="75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="EN21" s="26"/>
     </row>
-    <row r="22" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="85" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="86"/>
       <c r="C22" s="87"/>
@@ -9310,14 +9428,14 @@
       <c r="F22" s="87"/>
       <c r="G22" s="87"/>
       <c r="H22" s="88" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I22" s="87"/>
       <c r="J22" s="87"/>
       <c r="K22" s="87"/>
       <c r="L22" s="87"/>
       <c r="M22" s="85" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N22" s="18"/>
       <c r="O22" s="15"/>
@@ -9340,7 +9458,7 @@
       <c r="AF22" s="15"/>
       <c r="AG22" s="83"/>
       <c r="AH22" s="85" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AI22" s="147"/>
       <c r="AJ22" s="87"/>
@@ -9364,13 +9482,13 @@
         <v>0</v>
       </c>
       <c r="BA22" s="85" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="EN22" s="26"/>
     </row>
-    <row r="23" spans="1:144" s="103" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:144" s="103" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="15"/>
@@ -9384,7 +9502,7 @@
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N23" s="18"/>
       <c r="O23" s="15"/>
@@ -9410,7 +9528,7 @@
       <c r="AF23" s="15"/>
       <c r="AG23" s="83"/>
       <c r="AH23" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AI23" s="146"/>
       <c r="AJ23" s="15"/>
@@ -9434,7 +9552,7 @@
         <v>7.8432528081243271</v>
       </c>
       <c r="BA23" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BB23" s="26"/>
       <c r="BC23" s="26"/>
@@ -9528,9 +9646,9 @@
       <c r="EM23" s="26"/>
       <c r="EN23" s="26"/>
     </row>
-    <row r="24" spans="1:144" s="103" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:144" s="103" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="15"/>
@@ -9544,7 +9662,7 @@
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N24" s="18"/>
       <c r="O24" s="15"/>
@@ -9570,7 +9688,7 @@
       <c r="AF24" s="15"/>
       <c r="AG24" s="83"/>
       <c r="AH24" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AI24" s="146"/>
       <c r="AJ24" s="15"/>
@@ -9594,7 +9712,7 @@
         <v>252.19309701492537</v>
       </c>
       <c r="BA24" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BB24" s="26"/>
       <c r="BC24" s="26"/>
@@ -9688,9 +9806,9 @@
       <c r="EM24" s="26"/>
       <c r="EN24" s="26"/>
     </row>
-    <row r="25" spans="1:144" s="103" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:144" s="103" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="15">
@@ -9707,7 +9825,7 @@
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
       <c r="M25" s="75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N25" s="18">
         <f>(0*56+1*95+0)*ARC_44/1000</f>
@@ -9742,7 +9860,7 @@
       <c r="AF25" s="15"/>
       <c r="AG25" s="83"/>
       <c r="AH25" s="75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AI25" s="146"/>
       <c r="AJ25" s="15"/>
@@ -9766,7 +9884,7 @@
         <v>59.184267364209873</v>
       </c>
       <c r="BA25" s="75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BB25" s="26"/>
       <c r="BC25" s="26"/>
@@ -9860,9 +9978,9 @@
       <c r="EM25" s="26"/>
       <c r="EN25" s="26"/>
     </row>
-    <row r="26" spans="1:144" s="103" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:144" s="103" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="47"/>
       <c r="C26" s="48">
@@ -9879,7 +9997,7 @@
       <c r="K26" s="48"/>
       <c r="L26" s="48"/>
       <c r="M26" s="85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N26" s="47">
         <f>(0*56+1*95+0)*ARC44tier1/1000</f>
@@ -9914,7 +10032,7 @@
       <c r="AF26" s="48"/>
       <c r="AG26" s="112"/>
       <c r="AH26" s="85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AI26" s="147"/>
       <c r="AJ26" s="87"/>
@@ -9938,7 +10056,7 @@
         <v>1706.8319963071242</v>
       </c>
       <c r="BA26" s="85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BB26" s="26"/>
       <c r="BC26" s="26"/>
@@ -10032,7 +10150,7 @@
       <c r="EM26" s="26"/>
       <c r="EN26" s="26"/>
     </row>
-    <row r="27" spans="1:144" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:144" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="84" t="s">
         <v>9</v>
       </c>
@@ -10228,26 +10346,26 @@
       </c>
       <c r="EN27" s="26"/>
     </row>
-    <row r="28" spans="1:144" s="26" customFormat="1" ht="37.200000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="213" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="213"/>
-      <c r="C28" s="213"/>
-      <c r="D28" s="213"/>
-      <c r="E28" s="213"/>
-      <c r="F28" s="213"/>
-      <c r="G28" s="213"/>
-      <c r="H28" s="213"/>
-      <c r="I28" s="213"/>
-      <c r="J28" s="213"/>
-      <c r="K28" s="213"/>
-      <c r="L28" s="213"/>
-      <c r="M28" s="213"/>
-      <c r="N28" s="213"/>
-      <c r="O28" s="213"/>
-      <c r="P28" s="213"/>
-      <c r="Q28" s="213"/>
+    <row r="28" spans="1:144" s="26" customFormat="1" ht="37.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="214" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="214"/>
+      <c r="C28" s="214"/>
+      <c r="D28" s="214"/>
+      <c r="E28" s="214"/>
+      <c r="F28" s="214"/>
+      <c r="G28" s="214"/>
+      <c r="H28" s="214"/>
+      <c r="I28" s="214"/>
+      <c r="J28" s="214"/>
+      <c r="K28" s="214"/>
+      <c r="L28" s="214"/>
+      <c r="M28" s="214"/>
+      <c r="N28" s="214"/>
+      <c r="O28" s="214"/>
+      <c r="P28" s="214"/>
+      <c r="Q28" s="214"/>
       <c r="R28" s="40"/>
       <c r="S28" s="40"/>
       <c r="T28" s="40"/>
@@ -10282,70 +10400,70 @@
       <c r="AW28" s="30"/>
       <c r="AX28" s="30"/>
     </row>
-    <row r="29" spans="1:144" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="214" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="214"/>
-      <c r="C29" s="214"/>
-      <c r="D29" s="214"/>
-      <c r="E29" s="214"/>
-      <c r="F29" s="214"/>
-      <c r="G29" s="214"/>
-      <c r="H29" s="214"/>
-      <c r="I29" s="214"/>
-      <c r="J29" s="214"/>
-      <c r="K29" s="214"/>
-      <c r="L29" s="214"/>
-      <c r="M29" s="214"/>
-      <c r="N29" s="214"/>
-      <c r="O29" s="214"/>
-      <c r="P29" s="214"/>
-      <c r="Q29" s="214"/>
-      <c r="R29" s="214"/>
-      <c r="S29" s="214"/>
-      <c r="T29" s="214"/>
-      <c r="U29" s="214"/>
-      <c r="V29" s="214"/>
-      <c r="W29" s="214"/>
-      <c r="X29" s="214"/>
-      <c r="Y29" s="214"/>
-      <c r="Z29" s="214"/>
-      <c r="AA29" s="214"/>
-      <c r="AB29" s="214"/>
-      <c r="AC29" s="214"/>
-      <c r="AD29" s="214"/>
-      <c r="AE29" s="214"/>
-      <c r="AF29" s="214"/>
-      <c r="AG29" s="214"/>
-      <c r="AH29" s="214"/>
-      <c r="AI29" s="214"/>
-      <c r="AJ29" s="214"/>
-      <c r="AK29" s="214"/>
-      <c r="AL29" s="214"/>
-      <c r="AM29" s="214"/>
-      <c r="AN29" s="214"/>
-      <c r="AO29" s="214"/>
-      <c r="AP29" s="214"/>
-      <c r="AQ29" s="214"/>
-      <c r="AR29" s="214"/>
-      <c r="AS29" s="214"/>
-      <c r="AT29" s="214"/>
-      <c r="AU29" s="214"/>
-      <c r="AV29" s="214"/>
-      <c r="AW29" s="214"/>
-      <c r="AX29" s="214"/>
+    <row r="29" spans="1:144" s="26" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A29" s="215" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="215"/>
+      <c r="C29" s="215"/>
+      <c r="D29" s="215"/>
+      <c r="E29" s="215"/>
+      <c r="F29" s="215"/>
+      <c r="G29" s="215"/>
+      <c r="H29" s="215"/>
+      <c r="I29" s="215"/>
+      <c r="J29" s="215"/>
+      <c r="K29" s="215"/>
+      <c r="L29" s="215"/>
+      <c r="M29" s="215"/>
+      <c r="N29" s="215"/>
+      <c r="O29" s="215"/>
+      <c r="P29" s="215"/>
+      <c r="Q29" s="215"/>
+      <c r="R29" s="215"/>
+      <c r="S29" s="215"/>
+      <c r="T29" s="215"/>
+      <c r="U29" s="215"/>
+      <c r="V29" s="215"/>
+      <c r="W29" s="215"/>
+      <c r="X29" s="215"/>
+      <c r="Y29" s="215"/>
+      <c r="Z29" s="215"/>
+      <c r="AA29" s="215"/>
+      <c r="AB29" s="215"/>
+      <c r="AC29" s="215"/>
+      <c r="AD29" s="215"/>
+      <c r="AE29" s="215"/>
+      <c r="AF29" s="215"/>
+      <c r="AG29" s="215"/>
+      <c r="AH29" s="215"/>
+      <c r="AI29" s="215"/>
+      <c r="AJ29" s="215"/>
+      <c r="AK29" s="215"/>
+      <c r="AL29" s="215"/>
+      <c r="AM29" s="215"/>
+      <c r="AN29" s="215"/>
+      <c r="AO29" s="215"/>
+      <c r="AP29" s="215"/>
+      <c r="AQ29" s="215"/>
+      <c r="AR29" s="215"/>
+      <c r="AS29" s="215"/>
+      <c r="AT29" s="215"/>
+      <c r="AU29" s="215"/>
+      <c r="AV29" s="215"/>
+      <c r="AW29" s="215"/>
+      <c r="AX29" s="215"/>
     </row>
     <row r="30" spans="1:144" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="215" t="s">
+      <c r="A30" s="216" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="215"/>
-      <c r="C30" s="215"/>
-      <c r="D30" s="215"/>
-      <c r="E30" s="215"/>
-      <c r="F30" s="214"/>
-      <c r="G30" s="214"/>
+      <c r="B30" s="216"/>
+      <c r="C30" s="216"/>
+      <c r="D30" s="216"/>
+      <c r="E30" s="216"/>
+      <c r="F30" s="215"/>
+      <c r="G30" s="215"/>
       <c r="H30" s="19"/>
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
@@ -10377,7 +10495,7 @@
       <c r="AV30" s="19"/>
       <c r="AW30" s="19"/>
     </row>
-    <row r="31" spans="1:144" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:144" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>0</v>
       </c>
@@ -10387,13 +10505,13 @@
       <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="216" t="s">
+      <c r="D31" s="217" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="217"/>
+      <c r="E31" s="218"/>
       <c r="F31" s="14"/>
     </row>
-    <row r="32" spans="1:144" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>5</v>
       </c>
@@ -10405,14 +10523,14 @@
         <f>C33*98*63/194/201</f>
         <v>460.27127250346206</v>
       </c>
-      <c r="D32" s="218">
+      <c r="D32" s="219">
         <f t="shared" ref="D32:D37" si="33">(B32+C32)/1</f>
         <v>476.23114325280812</v>
       </c>
-      <c r="E32" s="219"/>
+      <c r="E32" s="220"/>
       <c r="F32" s="14"/>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>3</v>
       </c>
@@ -10423,14 +10541,14 @@
       <c r="C33" s="10">
         <v>2907</v>
       </c>
-      <c r="D33" s="220">
+      <c r="D33" s="221">
         <f t="shared" si="33"/>
         <v>3007.8</v>
       </c>
-      <c r="E33" s="221"/>
+      <c r="E33" s="222"/>
       <c r="F33" s="14"/>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>15</v>
       </c>
@@ -10442,14 +10560,14 @@
         <f>4*AFR44tier1</f>
         <v>11628</v>
       </c>
-      <c r="D34" s="220">
+      <c r="D34" s="221">
         <f t="shared" si="33"/>
         <v>12031.2</v>
       </c>
-      <c r="E34" s="221"/>
+      <c r="E34" s="222"/>
       <c r="F34" s="14"/>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="93" t="s">
         <v>4</v>
       </c>
@@ -10460,16 +10578,16 @@
       <c r="C35" s="95">
         <v>13005</v>
       </c>
-      <c r="D35" s="220">
+      <c r="D35" s="221">
         <f t="shared" si="33"/>
         <v>13475.4</v>
       </c>
-      <c r="E35" s="221"/>
+      <c r="E35" s="222"/>
       <c r="F35" s="14"/>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="101" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" s="9">
         <f>B33*125*87/194/201</f>
@@ -10479,16 +10597,16 @@
         <f>C33*125*97/194/201</f>
         <v>903.91791044776119</v>
       </c>
-      <c r="D36" s="220">
+      <c r="D36" s="221">
         <f t="shared" si="33"/>
         <v>932.02992768118168</v>
       </c>
-      <c r="E36" s="221"/>
+      <c r="E36" s="222"/>
       <c r="F36" s="26"/>
     </row>
-    <row r="37" spans="1:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:49" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="96" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" s="6">
         <f>B33*116*133/194/201</f>
@@ -10498,34 +10616,34 @@
         <f>C33*116*133/194/201</f>
         <v>1150.1563317433452</v>
       </c>
-      <c r="D37" s="222">
+      <c r="D37" s="223">
         <f t="shared" si="33"/>
         <v>1190.0379135251578</v>
       </c>
-      <c r="E37" s="223"/>
+      <c r="E37" s="224"/>
       <c r="F37" s="26"/>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A38" s="208" t="s">
+    <row r="38" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A38" s="209" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="208"/>
-      <c r="C38" s="208"/>
-      <c r="D38" s="208"/>
-      <c r="E38" s="208"/>
-      <c r="F38" s="209"/>
-      <c r="G38" s="209"/>
+      <c r="B38" s="209"/>
+      <c r="C38" s="209"/>
+      <c r="D38" s="209"/>
+      <c r="E38" s="209"/>
+      <c r="F38" s="210"/>
+      <c r="G38" s="210"/>
     </row>
-    <row r="39" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A39" s="209" t="s">
+    <row r="39" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A39" s="210" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="209"/>
-      <c r="C39" s="209"/>
-      <c r="D39" s="209"/>
-      <c r="E39" s="209"/>
-      <c r="F39" s="209"/>
-      <c r="G39" s="209"/>
+      <c r="B39" s="210"/>
+      <c r="C39" s="210"/>
+      <c r="D39" s="210"/>
+      <c r="E39" s="210"/>
+      <c r="F39" s="210"/>
+      <c r="G39" s="210"/>
       <c r="H39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
@@ -10590,103 +10708,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="AP1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="BA3" sqref="BA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" customWidth="1"/>
-    <col min="11" max="11" width="21.88671875" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" customWidth="1"/>
-    <col min="13" max="13" width="23.109375" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" style="62" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" style="62" customWidth="1"/>
-    <col min="18" max="18" width="20.109375" customWidth="1"/>
-    <col min="19" max="19" width="17.77734375" customWidth="1"/>
-    <col min="20" max="20" width="16.6640625" customWidth="1"/>
-    <col min="21" max="21" width="18.33203125" customWidth="1"/>
-    <col min="22" max="22" width="21.109375" customWidth="1"/>
-    <col min="23" max="23" width="15.6640625" customWidth="1"/>
-    <col min="24" max="24" width="26.5546875" customWidth="1"/>
-    <col min="25" max="25" width="19.21875" customWidth="1"/>
-    <col min="26" max="26" width="21.33203125" customWidth="1"/>
-    <col min="27" max="27" width="18.88671875" customWidth="1"/>
-    <col min="28" max="28" width="17.77734375" customWidth="1"/>
-    <col min="29" max="29" width="22.109375" customWidth="1"/>
-    <col min="30" max="30" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" style="62" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" style="62" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" customWidth="1"/>
+    <col min="22" max="22" width="21.140625" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" customWidth="1"/>
+    <col min="24" max="24" width="26.5703125" customWidth="1"/>
+    <col min="25" max="25" width="19.28515625" customWidth="1"/>
+    <col min="26" max="26" width="21.28515625" customWidth="1"/>
+    <col min="27" max="27" width="18.85546875" customWidth="1"/>
+    <col min="28" max="28" width="17.7109375" customWidth="1"/>
+    <col min="29" max="29" width="22.140625" customWidth="1"/>
+    <col min="30" max="30" width="18.42578125" customWidth="1"/>
     <col min="31" max="31" width="21" customWidth="1"/>
-    <col min="32" max="32" width="16.44140625" customWidth="1"/>
-    <col min="33" max="33" width="19.77734375" customWidth="1"/>
+    <col min="32" max="32" width="16.42578125" customWidth="1"/>
+    <col min="33" max="33" width="19.7109375" customWidth="1"/>
     <col min="34" max="35" width="19" customWidth="1"/>
-    <col min="36" max="36" width="19.44140625" customWidth="1"/>
-    <col min="37" max="37" width="17.77734375" customWidth="1"/>
-    <col min="38" max="38" width="22.44140625" customWidth="1"/>
+    <col min="36" max="36" width="19.42578125" customWidth="1"/>
+    <col min="37" max="37" width="17.7109375" customWidth="1"/>
+    <col min="38" max="38" width="22.42578125" customWidth="1"/>
     <col min="39" max="39" width="23" customWidth="1"/>
-    <col min="40" max="40" width="22.5546875" customWidth="1"/>
-    <col min="41" max="41" width="20.88671875" customWidth="1"/>
-    <col min="42" max="42" width="22.21875" customWidth="1"/>
-    <col min="43" max="43" width="17.44140625" customWidth="1"/>
-    <col min="44" max="44" width="19.5546875" customWidth="1"/>
+    <col min="40" max="40" width="22.5703125" customWidth="1"/>
+    <col min="41" max="41" width="20.85546875" customWidth="1"/>
+    <col min="42" max="42" width="22.28515625" customWidth="1"/>
+    <col min="43" max="43" width="17.42578125" customWidth="1"/>
+    <col min="44" max="44" width="19.5703125" customWidth="1"/>
     <col min="45" max="45" width="17" customWidth="1"/>
-    <col min="46" max="46" width="17.77734375" customWidth="1"/>
-    <col min="47" max="47" width="17.33203125" customWidth="1"/>
-    <col min="48" max="48" width="19.109375" customWidth="1"/>
-    <col min="49" max="50" width="19.44140625" customWidth="1"/>
-    <col min="51" max="51" width="17.6640625" customWidth="1"/>
-    <col min="52" max="52" width="19.5546875" customWidth="1"/>
-    <col min="53" max="53" width="21.44140625" customWidth="1"/>
-    <col min="54" max="54" width="16.6640625" customWidth="1"/>
-    <col min="76" max="81" width="8.88671875" style="26"/>
+    <col min="46" max="46" width="17.7109375" customWidth="1"/>
+    <col min="47" max="47" width="17.28515625" customWidth="1"/>
+    <col min="48" max="48" width="19.140625" customWidth="1"/>
+    <col min="49" max="50" width="19.42578125" customWidth="1"/>
+    <col min="51" max="51" width="17.7109375" customWidth="1"/>
+    <col min="52" max="52" width="19.5703125" customWidth="1"/>
+    <col min="53" max="53" width="21.42578125" customWidth="1"/>
+    <col min="54" max="54" width="16.7109375" customWidth="1"/>
+    <col min="76" max="81" width="8.85546875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="225" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
-      <c r="G1" s="225"/>
-      <c r="H1" s="225"/>
-      <c r="I1" s="225"/>
-      <c r="J1" s="225" t="str">
+    <row r="1" spans="1:81" ht="80.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="226" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
+      <c r="J1" s="226" t="str">
         <f>A1</f>
         <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
       </c>
-      <c r="K1" s="225"/>
-      <c r="L1" s="225"/>
-      <c r="M1" s="225"/>
-      <c r="N1" s="225"/>
-      <c r="O1" s="225"/>
-      <c r="P1" s="225"/>
-      <c r="Q1" s="225"/>
-      <c r="R1" s="225"/>
-      <c r="S1" s="226" t="str">
+      <c r="K1" s="226"/>
+      <c r="L1" s="226"/>
+      <c r="M1" s="226"/>
+      <c r="N1" s="226"/>
+      <c r="O1" s="226"/>
+      <c r="P1" s="226"/>
+      <c r="Q1" s="226"/>
+      <c r="R1" s="226"/>
+      <c r="S1" s="227" t="str">
         <f>A1</f>
         <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
       </c>
-      <c r="T1" s="226"/>
-      <c r="U1" s="226"/>
-      <c r="V1" s="226"/>
-      <c r="W1" s="226"/>
-      <c r="X1" s="226"/>
-      <c r="Y1" s="226"/>
-      <c r="Z1" s="226"/>
-      <c r="AA1" s="226"/>
+      <c r="T1" s="227"/>
+      <c r="U1" s="227"/>
+      <c r="V1" s="227"/>
+      <c r="W1" s="227"/>
+      <c r="X1" s="227"/>
+      <c r="Y1" s="227"/>
+      <c r="Z1" s="227"/>
+      <c r="AA1" s="227"/>
       <c r="AB1" s="190" t="str">
         <f>A1</f>
         <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
@@ -10699,18 +10817,18 @@
       <c r="AH1" s="190"/>
       <c r="AI1" s="190"/>
       <c r="AJ1" s="191"/>
-      <c r="AK1" s="226" t="str">
+      <c r="AK1" s="227" t="str">
         <f>A1</f>
         <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
       </c>
-      <c r="AL1" s="226"/>
-      <c r="AM1" s="226"/>
-      <c r="AN1" s="226"/>
-      <c r="AO1" s="226"/>
-      <c r="AP1" s="226"/>
-      <c r="AQ1" s="226"/>
-      <c r="AR1" s="226"/>
-      <c r="AS1" s="226"/>
+      <c r="AL1" s="227"/>
+      <c r="AM1" s="227"/>
+      <c r="AN1" s="227"/>
+      <c r="AO1" s="227"/>
+      <c r="AP1" s="227"/>
+      <c r="AQ1" s="227"/>
+      <c r="AR1" s="227"/>
+      <c r="AS1" s="227"/>
       <c r="AT1" s="190"/>
       <c r="AU1" s="192"/>
       <c r="AV1" s="192"/>
@@ -10796,9 +10914,9 @@
       <c r="AZ2" s="20"/>
       <c r="BB2" s="20"/>
     </row>
-    <row r="3" spans="1:81" s="1" customFormat="1" ht="32.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:81" s="1" customFormat="1" ht="32.450000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="118" t="str">
         <f>AllEntries!AR7</f>
@@ -10833,7 +10951,7 @@
         <v>CLMcom</v>
       </c>
       <c r="J3" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K3" s="118" t="str">
         <f>AllEntries!F7</f>
@@ -10868,7 +10986,7 @@
         <v>CRP-GL</v>
       </c>
       <c r="S3" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T3" s="118" t="str">
         <f>AllEntries!AH7</f>
@@ -10903,7 +11021,7 @@
         <v>ICTP</v>
       </c>
       <c r="AB3" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC3" s="118" t="str">
         <f>AllEntries!AO7</f>
@@ -10938,7 +11056,7 @@
         <v>MIUB</v>
       </c>
       <c r="AK3" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AL3" s="118" t="str">
         <f>AllEntries!AJ7</f>
@@ -10973,7 +11091,7 @@
         <v>SMHI</v>
       </c>
       <c r="AT3" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AU3" s="118" t="str">
         <f>AllEntries!P7</f>
@@ -11007,7 +11125,7 @@
         <f>AllEntries!Y7</f>
         <v>UQAM</v>
       </c>
-      <c r="BC3" s="224"/>
+      <c r="BC3" s="225"/>
       <c r="BD3" s="2"/>
       <c r="BE3" s="2"/>
       <c r="BF3" s="2"/>
@@ -11035,9 +11153,9 @@
       <c r="CB3" s="2"/>
       <c r="CC3" s="2"/>
     </row>
-    <row r="4" spans="1:81" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:81" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="138" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AR9),"",AllEntries!AR9)</f>
@@ -11072,7 +11190,7 @@
         <v>Climate Limited-area Modelling Community (CLM-Community)</v>
       </c>
       <c r="J4" s="138" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!F9),"",AllEntries!F9)</f>
@@ -11107,7 +11225,7 @@
         <v/>
       </c>
       <c r="S4" s="138" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AH9),"",AllEntries!AH9)</f>
@@ -11123,7 +11241,7 @@
       </c>
       <c r="W4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!B9),"",AllEntries!B9)</f>
-        <v/>
+        <v>Danish Meteorological Institute</v>
       </c>
       <c r="X4" s="195" t="str">
         <f>IF(ISBLANK(AllEntries!AB9),"",AllEntries!AB9)</f>
@@ -11142,7 +11260,7 @@
         <v xml:space="preserve"> Abdus Salam International Centre for Theoretical Physics</v>
       </c>
       <c r="AB4" s="138" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AC4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AO9),"",AllEntries!AO9)</f>
@@ -11177,7 +11295,7 @@
         <v/>
       </c>
       <c r="AK4" s="138" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AL4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!AJ9),"",AllEntries!AJ9)</f>
@@ -11212,7 +11330,7 @@
         <v>Swedish Meteorological and Hydrological Institute, Rossby Centre</v>
       </c>
       <c r="AT4" s="138" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AU4" s="188" t="str">
         <f>IF(ISBLANK(AllEntries!P9),"",AllEntries!P9)</f>
@@ -11246,7 +11364,7 @@
         <f>IF(ISBLANK(AllEntries!Y9),"",AllEntries!Y9)</f>
         <v>Universite du Quebec a Montreal</v>
       </c>
-      <c r="BC4" s="224"/>
+      <c r="BC4" s="225"/>
       <c r="BD4" s="2"/>
       <c r="BE4" s="2"/>
       <c r="BF4" s="2"/>
@@ -11274,9 +11392,9 @@
       <c r="CB4" s="2"/>
       <c r="CC4" s="2"/>
     </row>
-    <row r="5" spans="1:81" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:81" s="1" customFormat="1" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="142" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="119" t="str">
         <f>AllEntries!AR8</f>
@@ -11311,7 +11429,7 @@
         <v>CCLM4-8-17</v>
       </c>
       <c r="J5" s="142" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K5" s="119" t="str">
         <f>AllEntries!F8</f>
@@ -11346,7 +11464,7 @@
         <v>WRF331A</v>
       </c>
       <c r="S5" s="142" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T5" s="119" t="str">
         <f>AllEntries!AH8</f>
@@ -11381,7 +11499,7 @@
         <v>RegCM4-3</v>
       </c>
       <c r="AB5" s="142" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AC5" s="119" t="str">
         <f>AllEntries!AO8</f>
@@ -11416,7 +11534,7 @@
         <v>WRF331A</v>
       </c>
       <c r="AK5" s="142" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AL5" s="119" t="str">
         <f>AllEntries!AJ8</f>
@@ -11451,7 +11569,7 @@
         <v>RCAO-SN</v>
       </c>
       <c r="AT5" s="142" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AU5" s="119" t="str">
         <f>AllEntries!P8</f>
@@ -11485,7 +11603,7 @@
         <f>AllEntries!Y8</f>
         <v>CRCM5</v>
       </c>
-      <c r="BC5" s="224"/>
+      <c r="BC5" s="225"/>
       <c r="BD5" s="2"/>
       <c r="BE5" s="2"/>
       <c r="BF5" s="2"/>
@@ -11513,9 +11631,9 @@
       <c r="CB5" s="2"/>
       <c r="CC5" s="2"/>
     </row>
-    <row r="6" spans="1:81" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:81" s="1" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="119" t="str">
         <f>IF(ISBLANK(B9),"",CONCATENATE(B3,"-",B5))</f>
@@ -11550,7 +11668,7 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="J6" s="74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K6" s="119" t="str">
         <f t="shared" ref="K6" si="3">IF(ISBLANK(K9),"",CONCATENATE(K3,"-",K5))</f>
@@ -11585,7 +11703,7 @@
         <v>CRP-GL-WRF331A</v>
       </c>
       <c r="S6" s="74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T6" s="119" t="str">
         <f>IF(ISBLANK(T9),"",CONCATENATE(T3,"-",T5))</f>
@@ -11620,7 +11738,7 @@
         <v>ICTP-RegCM4-3</v>
       </c>
       <c r="AB6" s="74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC6" s="119" t="str">
         <f>IF(ISBLANK(AC9),"",CONCATENATE(AC3,"-",AC5))</f>
@@ -11655,7 +11773,7 @@
         <v>MIUB-WRF331A</v>
       </c>
       <c r="AK6" s="74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AL6" s="119" t="str">
         <f>IF(ISBLANK(AL9),"",CONCATENATE(AL3,"-",AL5))</f>
@@ -11690,7 +11808,7 @@
         <v>SMHI-RCAO-SN</v>
       </c>
       <c r="AT6" s="74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AU6" s="119" t="str">
         <f t="shared" ref="AU6" si="21">IF(ISBLANK(AU9),"",CONCATENATE(AU3,"-",AU5))</f>
@@ -11752,9 +11870,9 @@
       <c r="CB6" s="2"/>
       <c r="CC6" s="2"/>
     </row>
-    <row r="7" spans="1:81" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:81" s="1" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="140" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AR11),"unknown",AllEntries!AR11)</f>
@@ -11789,7 +11907,7 @@
         <v>non-commercial only</v>
       </c>
       <c r="J7" s="140" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!F11),"unknown",AllEntries!F11)</f>
@@ -11824,7 +11942,7 @@
         <v>unrestricted</v>
       </c>
       <c r="S7" s="140" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="T7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AH11),"unknown",AllEntries!AH11)</f>
@@ -11859,7 +11977,7 @@
         <v>unrestricted</v>
       </c>
       <c r="AB7" s="140" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AC7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AO11),"unknown",AllEntries!AO11)</f>
@@ -11894,7 +12012,7 @@
         <v>unknown</v>
       </c>
       <c r="AK7" s="140" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AL7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!AJ11),"unknown",AllEntries!AJ11)</f>
@@ -11929,7 +12047,7 @@
         <v>unrestricted</v>
       </c>
       <c r="AT7" s="140" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AU7" s="189" t="str">
         <f>IF(ISBLANK(AllEntries!P11),"",AllEntries!P11)</f>
@@ -11993,164 +12111,164 @@
     </row>
     <row r="8" spans="1:81" s="36" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="141" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="H8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="I8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="J8" s="141" t="s">
         <v>186</v>
       </c>
-      <c r="C8" s="133" t="s">
+      <c r="K8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="L8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="M8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="N8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="O8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="P8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="R8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="S8" s="141" t="s">
         <v>186</v>
       </c>
-      <c r="D8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="E8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="F8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="G8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="H8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="I8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="J8" s="141" t="s">
-        <v>187</v>
-      </c>
-      <c r="K8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="L8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="M8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="N8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="O8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="P8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="R8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="S8" s="141" t="s">
-        <v>187</v>
-      </c>
       <c r="T8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="W8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="X8" s="133"/>
       <c r="Y8" s="133" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="Z8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AA8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB8" s="141" t="s">
         <v>186</v>
       </c>
-      <c r="AA8" s="133" t="s">
+      <c r="AC8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AD8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AE8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AF8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AG8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AH8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AI8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AJ8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AK8" s="141" t="s">
         <v>186</v>
       </c>
-      <c r="AB8" s="141" t="s">
-        <v>187</v>
-      </c>
-      <c r="AC8" s="133" t="s">
+      <c r="AL8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AM8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AN8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AO8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AP8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AQ8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AR8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AS8" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="AT8" s="141" t="s">
         <v>186</v>
       </c>
-      <c r="AD8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AE8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AF8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AG8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AH8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AI8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AJ8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AK8" s="141" t="s">
-        <v>187</v>
-      </c>
-      <c r="AL8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AM8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AN8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AO8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AP8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AQ8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AR8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AS8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="AT8" s="141" t="s">
-        <v>187</v>
-      </c>
       <c r="AU8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AV8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AW8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AX8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AY8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AZ8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="BA8" s="133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="BB8" s="132" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="BC8" s="134"/>
       <c r="BD8" s="135"/>
@@ -12182,155 +12300,155 @@
     </row>
     <row r="9" spans="1:81" s="36" customFormat="1" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="184" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="185" t="s">
-        <v>159</v>
-      </c>
-      <c r="D9" s="185" t="s">
-        <v>160</v>
-      </c>
       <c r="E9" s="185" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F9" s="185"/>
       <c r="G9" s="185" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H9" s="185" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I9" s="185" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J9" s="184" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K9" s="185" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L9" s="185" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M9" s="185" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N9" s="185" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O9" s="185" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P9" s="185" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q9" s="185" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R9" s="185" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S9" s="184" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T9" s="186" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="U9" s="185" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V9" s="185" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="W9" s="185" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X9" s="185"/>
       <c r="Y9" s="185"/>
       <c r="Z9" s="185" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA9" s="185" t="s">
         <v>156</v>
       </c>
-      <c r="AA9" s="185" t="s">
-        <v>157</v>
-      </c>
       <c r="AB9" s="184" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AC9" s="185" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AD9" s="185" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AE9" s="185" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AF9" s="185"/>
       <c r="AG9" s="185" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH9" s="185" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI9" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="AH9" s="185" t="s">
-        <v>118</v>
-      </c>
-      <c r="AI9" s="185" t="s">
-        <v>119</v>
-      </c>
       <c r="AJ9" s="185" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AK9" s="184" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AL9" s="185" t="s">
+        <v>157</v>
+      </c>
+      <c r="AM9" s="185" t="s">
+        <v>157</v>
+      </c>
+      <c r="AN9" s="185" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO9" s="185" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP9" s="185" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ9" s="185" t="s">
+        <v>222</v>
+      </c>
+      <c r="AR9" s="185" t="s">
+        <v>154</v>
+      </c>
+      <c r="AS9" s="185" t="s">
+        <v>154</v>
+      </c>
+      <c r="AT9" s="184" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU9" s="185" t="s">
+        <v>154</v>
+      </c>
+      <c r="AV9" s="185" t="s">
+        <v>154</v>
+      </c>
+      <c r="AW9" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="AM9" s="185" t="s">
+      <c r="AX9" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="AN9" s="185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO9" s="185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP9" s="185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ9" s="185" t="s">
-        <v>224</v>
-      </c>
-      <c r="AR9" s="185" t="s">
-        <v>155</v>
-      </c>
-      <c r="AS9" s="185" t="s">
-        <v>155</v>
-      </c>
-      <c r="AT9" s="184" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU9" s="185" t="s">
-        <v>155</v>
-      </c>
-      <c r="AV9" s="185" t="s">
-        <v>155</v>
-      </c>
-      <c r="AW9" s="185" t="s">
-        <v>159</v>
-      </c>
-      <c r="AX9" s="185" t="s">
-        <v>159</v>
-      </c>
       <c r="AY9" s="185" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AZ9" s="185" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="BA9" s="185" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BB9" s="187"/>
       <c r="BC9" s="134"/>
@@ -12361,7 +12479,7 @@
       <c r="CB9" s="135"/>
       <c r="CC9" s="135"/>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:81" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="63"/>
       <c r="J11" s="63"/>
       <c r="S11" s="63"/>
@@ -12369,7 +12487,7 @@
       <c r="AK11" s="63"/>
       <c r="AT11" s="63"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D18" s="60"/>
     </row>
   </sheetData>
@@ -12402,33 +12520,33 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="65.21875" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="26"/>
     </row>
-    <row r="3" spans="2:6" ht="25.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="25.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="155" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="156" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="156" t="s">
+      <c r="D3" s="156" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="156" t="s">
+      <c r="E3" s="157" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="158" t="s">
         <v>195</v>
-      </c>
-      <c r="E3" s="157" t="s">
-        <v>199</v>
-      </c>
-      <c r="F3" s="158" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30.6" x14ac:dyDescent="0.3">
@@ -12440,26 +12558,26 @@
       </c>
       <c r="D4" s="109"/>
       <c r="E4" s="163" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F4" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="159" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" s="161" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E5" s="163"/>
       <c r="F5" s="109"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B6" s="159" t="s">
         <v>49</v>
       </c>
@@ -12467,16 +12585,16 @@
         <v>58</v>
       </c>
       <c r="D6" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" s="163" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F6" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" s="159" t="s">
         <v>50</v>
       </c>
@@ -12484,14 +12602,14 @@
         <v>58</v>
       </c>
       <c r="D7" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E7" s="163"/>
       <c r="F7" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="159" t="s">
         <v>50</v>
       </c>
@@ -12499,14 +12617,14 @@
         <v>58</v>
       </c>
       <c r="D8" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E8" s="163"/>
       <c r="F8" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" s="160" t="s">
         <v>50</v>
       </c>
@@ -12514,14 +12632,14 @@
         <v>58</v>
       </c>
       <c r="D9" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E9" s="163"/>
       <c r="F9" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B10" s="160" t="s">
         <v>50</v>
       </c>
@@ -12529,14 +12647,14 @@
         <v>58</v>
       </c>
       <c r="D10" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E10" s="163"/>
       <c r="F10" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" s="160" t="s">
         <v>50</v>
       </c>
@@ -12544,108 +12662,108 @@
         <v>58</v>
       </c>
       <c r="D11" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E11" s="163"/>
       <c r="F11" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" s="162" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" s="109" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" s="162" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" s="109" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E13" s="171" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F13" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" s="162" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D14" s="109" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E14" s="171"/>
       <c r="F14" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="160" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="162" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E15" s="171"/>
       <c r="F15" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="160" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="162" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" s="109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E16" s="171" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F16" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="160" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="162" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D17" s="109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E17" s="171"/>
       <c r="F17" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="61.15" x14ac:dyDescent="0.3">
       <c r="B18" s="160" t="s">
         <v>42</v>
       </c>
@@ -12653,16 +12771,16 @@
         <v>25</v>
       </c>
       <c r="D18" s="109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E18" s="163" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F18" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="160" t="s">
         <v>40</v>
       </c>
@@ -12673,7 +12791,7 @@
       <c r="E19" s="163"/>
       <c r="F19" s="109"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="160" t="s">
         <v>47</v>
       </c>
@@ -12681,16 +12799,16 @@
         <v>26</v>
       </c>
       <c r="D20" s="109" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E20" s="109" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F20" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B21" s="160" t="s">
         <v>39</v>
       </c>
@@ -12698,164 +12816,164 @@
         <v>26</v>
       </c>
       <c r="D21" s="109" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E21" s="163"/>
       <c r="F21" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" s="168" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="170" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" s="167" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E22" s="163"/>
       <c r="F22" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="168" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="170" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D23" s="167" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E23" s="163" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F23" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="168" t="s">
         <v>52</v>
       </c>
       <c r="C24" s="170" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D24" s="167" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E24" s="163" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F24" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="168" t="s">
         <v>52</v>
       </c>
       <c r="C25" s="170" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" s="167" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E25" s="163" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F25" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B26" s="160" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="162" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" s="109" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E26" s="109"/>
       <c r="F26" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="160" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="162" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D27" s="109" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E27" s="109"/>
       <c r="F27" s="109"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="160" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="162" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D28" s="109" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E28" s="109"/>
       <c r="F28" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="160" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C29" s="162" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D29" s="109" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E29" s="109"/>
       <c r="F29" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B30" s="160" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="162" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" s="109"/>
       <c r="E30" s="109"/>
       <c r="F30" s="109"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B31" s="160" t="s">
         <v>48</v>
       </c>
       <c r="C31" s="162" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D31" s="109" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E31" s="109"/>
       <c r="F31" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B32" s="160" t="s">
         <v>37</v>
       </c>
@@ -12866,22 +12984,22 @@
       <c r="E32" s="109"/>
       <c r="F32" s="109"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B33" s="160" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C33" s="162" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="109" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E33" s="109"/>
       <c r="F33" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B34" s="160" t="s">
         <v>54</v>
       </c>
@@ -12892,7 +13010,7 @@
       <c r="E34" s="109"/>
       <c r="F34" s="109"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B35" s="160" t="s">
         <v>55</v>
       </c>
@@ -12903,19 +13021,19 @@
       <c r="E35" s="109"/>
       <c r="F35" s="109"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B36" s="160" t="s">
         <v>53</v>
       </c>
       <c r="C36" s="161" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" s="109" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E36" s="109"/>
       <c r="F36" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="30.6" x14ac:dyDescent="0.3">
@@ -12923,126 +13041,126 @@
         <v>53</v>
       </c>
       <c r="C37" s="161" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D37" s="109" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E37" s="109" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F37" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B38" s="165" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C38" s="166" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D38" s="167"/>
       <c r="E38" s="109"/>
       <c r="F38" s="109"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B39" s="165" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="166" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D39" s="167" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E39" s="109"/>
       <c r="F39" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B40" s="168" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="169" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D40" s="167"/>
       <c r="E40" s="109"/>
       <c r="F40" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B41" s="168" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="169" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D41" s="167"/>
       <c r="E41" s="109"/>
       <c r="F41" s="109"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B42" s="168" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C42" s="169" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D42" s="167"/>
       <c r="E42" s="109" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F42" s="109"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B43" s="160" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C43" s="164" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D43" s="109"/>
       <c r="E43" s="109"/>
       <c r="F43" s="109"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B44" s="160" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="162" t="s">
         <v>145</v>
-      </c>
-      <c r="C44" s="162" t="s">
-        <v>146</v>
       </c>
       <c r="D44" s="109"/>
       <c r="E44" s="109"/>
       <c r="F44" s="109"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B45" s="160" t="s">
         <v>56</v>
       </c>
       <c r="C45" s="164" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D45" s="109"/>
       <c r="E45" s="109"/>
       <c r="F45" s="109"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B46" s="160" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="164" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D46" s="109"/>
       <c r="E46" s="109"/>
       <c r="F46" s="109"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B47" s="160" t="s">
         <v>32</v>
       </c>
@@ -13053,27 +13171,27 @@
       <c r="E47" s="109"/>
       <c r="F47" s="109"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B48" s="160" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="170" t="s">
         <v>140</v>
-      </c>
-      <c r="C48" s="170" t="s">
-        <v>141</v>
       </c>
       <c r="D48" s="109"/>
       <c r="E48" s="109" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F48" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B49" s="160" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C49" s="164" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D49" s="109"/>
       <c r="E49" s="109"/>
@@ -13089,77 +13207,77 @@
     <sortCondition ref="C4:C49"/>
   </sortState>
   <conditionalFormatting sqref="B5:F5 B21:F22 B7:F12 B26:F27 B38:F41 B19:F19 B17:F17 B14:F15 B49:F49 B43:F47 B30:F36">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:F20">
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:F6">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:F24">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37:F37">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:F23">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:F25">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:F18">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:F16">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:F13">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:F48">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:F42">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:F29">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:F28">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B28)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Extended details in Bjerkness Centre information
</commit_message>
<xml_diff>
--- a/CORDEX_ESGF_coordination_issues.xlsx
+++ b/CORDEX_ESGF_coordination_issues.xlsx
@@ -51,11 +51,11 @@
     <definedName name="MED44tier1" localSheetId="2">DatVol!$C$32</definedName>
     <definedName name="MED44tier1" localSheetId="0">GeneralRemarks!#REF!</definedName>
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
-    <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$BA$9</definedName>
+    <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$BC$9</definedName>
     <definedName name="Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$BA$5</definedName>
     <definedName name="Print_Area" localSheetId="2">DatVol!$A$1:$AZ$39</definedName>
     <definedName name="Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$BA$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$BC$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">ControlledVocabulary!$A$1:$BB$9</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">DatVol!$A$1:$BA$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">GeneralRemarks!$A$1:$O$4</definedName>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="264">
   <si>
     <t>Domain</t>
   </si>
@@ -1335,6 +1335,24 @@
   </si>
   <si>
     <t>ULg</t>
+  </si>
+  <si>
+    <t>Bjerknes Centre for Climate Research and Uni Research</t>
+  </si>
+  <si>
+    <t>Martin King, cordex@uni.no</t>
+  </si>
+  <si>
+    <t>EUR-11, EUR-44</t>
+  </si>
+  <si>
+    <t>AFR-44, EAS-44</t>
+  </si>
+  <si>
+    <t>WRF361</t>
+  </si>
+  <si>
+    <t>Martin King cordex@uni.no</t>
   </si>
 </sst>
 </file>
@@ -2581,7 +2599,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="231">
+  <cellXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3070,6 +3088,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3142,14 +3172,8 @@
     <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3159,7 +3183,47 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -3646,20 +3710,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="208" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="204"/>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
-      <c r="E1" s="204"/>
-      <c r="F1" s="204"/>
-      <c r="G1" s="204"/>
-      <c r="H1" s="204"/>
-      <c r="I1" s="204"/>
-      <c r="J1" s="204"/>
-      <c r="K1" s="204"/>
-      <c r="L1" s="204"/>
+      <c r="B1" s="208"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
+      <c r="G1" s="208"/>
+      <c r="H1" s="208"/>
+      <c r="I1" s="208"/>
+      <c r="J1" s="208"/>
+      <c r="K1" s="208"/>
+      <c r="L1" s="208"/>
       <c r="M1" s="21"/>
       <c r="N1" s="20"/>
       <c r="O1" s="20"/>
@@ -3684,12 +3748,12 @@
       <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" s="137" customFormat="1" ht="23.45" x14ac:dyDescent="0.45">
-      <c r="A3" s="205" t="s">
+      <c r="A3" s="209" t="s">
         <v>182</v>
       </c>
-      <c r="B3" s="205"/>
-      <c r="C3" s="205"/>
-      <c r="D3" s="205"/>
+      <c r="B3" s="209"/>
+      <c r="C3" s="209"/>
+      <c r="D3" s="209"/>
       <c r="E3" s="136"/>
       <c r="F3" s="136"/>
       <c r="G3" s="136"/>
@@ -3725,10 +3789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CD38"/>
+  <dimension ref="A1:CF38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AZ5" sqref="AZ5"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AO20" sqref="AO20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3759,29 +3823,29 @@
     <col min="33" max="33" width="13.140625" customWidth="1"/>
     <col min="34" max="34" width="12" customWidth="1"/>
     <col min="35" max="37" width="16.7109375" customWidth="1"/>
-    <col min="38" max="52" width="13.7109375" customWidth="1"/>
-    <col min="53" max="53" width="22.42578125" customWidth="1"/>
+    <col min="38" max="54" width="13.7109375" customWidth="1"/>
+    <col min="55" max="55" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="206" t="s">
+    <row r="1" spans="1:84" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="210" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="204"/>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
-      <c r="E1" s="204"/>
-      <c r="F1" s="204"/>
-      <c r="G1" s="204"/>
-      <c r="H1" s="204"/>
-      <c r="I1" s="204"/>
-      <c r="J1" s="204"/>
-      <c r="K1" s="204"/>
-      <c r="L1" s="204"/>
-      <c r="M1" s="204"/>
-      <c r="N1" s="204"/>
-      <c r="O1" s="204"/>
-      <c r="P1" s="204"/>
+      <c r="B1" s="208"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
+      <c r="G1" s="208"/>
+      <c r="H1" s="208"/>
+      <c r="I1" s="208"/>
+      <c r="J1" s="208"/>
+      <c r="K1" s="208"/>
+      <c r="L1" s="208"/>
+      <c r="M1" s="208"/>
+      <c r="N1" s="208"/>
+      <c r="O1" s="208"/>
+      <c r="P1" s="208"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="20"/>
       <c r="S1" s="20"/>
@@ -3818,8 +3882,8 @@
       <c r="AX1" s="20"/>
       <c r="AY1" s="20"/>
       <c r="AZ1" s="20"/>
-      <c r="BV1" s="26"/>
-      <c r="BW1" s="26"/>
+      <c r="BA1" s="20"/>
+      <c r="BB1" s="20"/>
       <c r="BX1" s="26"/>
       <c r="BY1" s="26"/>
       <c r="BZ1" s="26"/>
@@ -3827,19 +3891,21 @@
       <c r="CB1" s="26"/>
       <c r="CC1" s="26"/>
       <c r="CD1" s="26"/>
+      <c r="CE1" s="26"/>
+      <c r="CF1" s="26"/>
     </row>
-    <row r="2" spans="1:82" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:84" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53">
         <f>GeneralRemarks!A2</f>
         <v>41991</v>
       </c>
-      <c r="B2" s="208"/>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
-      <c r="H2" s="208"/>
+      <c r="B2" s="212"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="212"/>
+      <c r="F2" s="212"/>
+      <c r="G2" s="212"/>
+      <c r="H2" s="212"/>
       <c r="I2" s="51"/>
       <c r="J2" s="51"/>
       <c r="K2" s="51"/>
@@ -3887,12 +3953,12 @@
       <c r="AX2" s="20"/>
       <c r="AY2" s="20"/>
       <c r="AZ2" s="20"/>
-      <c r="BA2" s="71">
+      <c r="BA2" s="20"/>
+      <c r="BB2" s="20"/>
+      <c r="BC2" s="71">
         <f>A2</f>
         <v>41991</v>
       </c>
-      <c r="BV2" s="26"/>
-      <c r="BW2" s="26"/>
       <c r="BX2" s="26"/>
       <c r="BY2" s="26"/>
       <c r="BZ2" s="26"/>
@@ -3900,8 +3966,10 @@
       <c r="CB2" s="26"/>
       <c r="CC2" s="26"/>
       <c r="CD2" s="26"/>
+      <c r="CE2" s="26"/>
+      <c r="CF2" s="26"/>
     </row>
-    <row r="3" spans="1:82" s="1" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:84" s="1" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="150" t="s">
         <v>57</v>
       </c>
@@ -4012,37 +4080,43 @@
         <v>97</v>
       </c>
       <c r="AL3" s="105"/>
-      <c r="AM3" s="105"/>
-      <c r="AN3" s="105"/>
-      <c r="AO3" s="105"/>
-      <c r="AP3" s="230" t="s">
+      <c r="AM3" s="232" t="s">
+        <v>263</v>
+      </c>
+      <c r="AN3" s="232" t="s">
+        <v>259</v>
+      </c>
+      <c r="AO3" s="232" t="s">
+        <v>259</v>
+      </c>
+      <c r="AP3" s="105"/>
+      <c r="AQ3" s="105"/>
+      <c r="AR3" s="207" t="s">
         <v>247</v>
       </c>
-      <c r="AQ3" s="105"/>
-      <c r="AR3" s="105"/>
-      <c r="AS3" s="173" t="s">
+      <c r="AS3" s="105"/>
+      <c r="AT3" s="105"/>
+      <c r="AU3" s="173" t="s">
         <v>216</v>
       </c>
-      <c r="AT3" s="105" t="s">
+      <c r="AV3" s="105" t="s">
         <v>237</v>
       </c>
-      <c r="AU3" s="105"/>
-      <c r="AV3" s="105"/>
       <c r="AW3" s="105"/>
-      <c r="AX3" s="173" t="s">
+      <c r="AX3" s="105"/>
+      <c r="AY3" s="105"/>
+      <c r="AZ3" s="173" t="s">
         <v>246</v>
       </c>
-      <c r="AY3" s="173" t="s">
+      <c r="BA3" s="173" t="s">
         <v>248</v>
       </c>
-      <c r="AZ3" s="173" t="s">
+      <c r="BB3" s="173" t="s">
         <v>254</v>
       </c>
-      <c r="BA3" s="150" t="s">
+      <c r="BC3" s="150" t="s">
         <v>57</v>
       </c>
-      <c r="BB3" s="2"/>
-      <c r="BC3" s="2"/>
       <c r="BD3" s="2"/>
       <c r="BE3" s="2"/>
       <c r="BF3" s="2"/>
@@ -4070,8 +4144,10 @@
       <c r="CB3" s="2"/>
       <c r="CC3" s="2"/>
       <c r="CD3" s="2"/>
+      <c r="CE3" s="2"/>
+      <c r="CF3" s="2"/>
     </row>
-    <row r="4" spans="1:82" s="1" customFormat="1" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:84" s="1" customFormat="1" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="152" t="s">
         <v>41</v>
       </c>
@@ -4203,62 +4279,68 @@
         <v>MIUB</v>
       </c>
       <c r="AM4" s="108" t="str">
-        <f t="shared" ref="AM4:AW4" si="4">AM7</f>
+        <f t="shared" ref="AM4" si="4">AM7</f>
         <v>BCCR</v>
       </c>
       <c r="AN4" s="108" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AN4" si="5">AN7</f>
+        <v>BCCR</v>
+      </c>
+      <c r="AO4" s="108" t="str">
+        <f t="shared" ref="AO4:AY4" si="6">AO7</f>
+        <v>BCCR</v>
+      </c>
+      <c r="AP4" s="108" t="str">
+        <f t="shared" si="6"/>
         <v>CRP-GL</v>
       </c>
-      <c r="AO4" s="108" t="str">
-        <f t="shared" si="4"/>
+      <c r="AQ4" s="108" t="str">
+        <f t="shared" si="6"/>
         <v>IDL</v>
       </c>
-      <c r="AP4" s="108" t="s">
+      <c r="AR4" s="108" t="s">
         <v>164</v>
       </c>
-      <c r="AQ4" s="108" t="str">
-        <f t="shared" si="4"/>
+      <c r="AS4" s="108" t="str">
+        <f t="shared" si="6"/>
         <v>AUTH-Met</v>
       </c>
-      <c r="AR4" s="108" t="str">
-        <f t="shared" si="4"/>
+      <c r="AT4" s="108" t="str">
+        <f t="shared" si="6"/>
         <v>AUTH-LHTEE</v>
       </c>
-      <c r="AS4" s="108" t="str">
-        <f t="shared" si="4"/>
+      <c r="AU4" s="108" t="str">
+        <f t="shared" si="6"/>
         <v>NUIM</v>
       </c>
-      <c r="AT4" s="108" t="str">
-        <f t="shared" si="4"/>
+      <c r="AV4" s="108" t="str">
+        <f t="shared" si="6"/>
         <v>UHOH</v>
       </c>
-      <c r="AU4" s="108" t="str">
-        <f t="shared" si="4"/>
+      <c r="AW4" s="108" t="str">
+        <f t="shared" si="6"/>
         <v>UM</v>
       </c>
-      <c r="AV4" s="108" t="str">
-        <f t="shared" si="4"/>
+      <c r="AX4" s="108" t="str">
+        <f t="shared" si="6"/>
         <v>UCAN</v>
       </c>
-      <c r="AW4" s="108" t="str">
-        <f t="shared" si="4"/>
+      <c r="AY4" s="108" t="str">
+        <f t="shared" si="6"/>
         <v>UCAN</v>
       </c>
-      <c r="AX4" s="174" t="s">
+      <c r="AZ4" s="174" t="s">
         <v>243</v>
       </c>
-      <c r="AY4" s="174" t="s">
+      <c r="BA4" s="174" t="s">
         <v>249</v>
       </c>
-      <c r="AZ4" s="174" t="s">
+      <c r="BB4" s="174" t="s">
         <v>257</v>
       </c>
-      <c r="BA4" s="152" t="s">
+      <c r="BC4" s="152" t="s">
         <v>41</v>
       </c>
-      <c r="BB4" s="2"/>
-      <c r="BC4" s="2"/>
       <c r="BD4" s="2"/>
       <c r="BE4" s="2"/>
       <c r="BF4" s="2"/>
@@ -4286,8 +4368,10 @@
       <c r="CB4" s="2"/>
       <c r="CC4" s="2"/>
       <c r="CD4" s="2"/>
+      <c r="CE4" s="2"/>
+      <c r="CF4" s="2"/>
     </row>
-    <row r="5" spans="1:82" s="128" customFormat="1" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:84" s="128" customFormat="1" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="153" t="s">
         <v>125</v>
       </c>
@@ -4335,24 +4419,24 @@
       <c r="AK5" s="124"/>
       <c r="AL5" s="125"/>
       <c r="AM5" s="125"/>
-      <c r="AN5" s="126"/>
-      <c r="AO5" s="126"/>
+      <c r="AN5" s="125"/>
+      <c r="AO5" s="125"/>
       <c r="AP5" s="126"/>
-      <c r="AQ5" s="123"/>
-      <c r="AR5" s="123"/>
+      <c r="AQ5" s="126"/>
+      <c r="AR5" s="126"/>
       <c r="AS5" s="123"/>
       <c r="AT5" s="123"/>
       <c r="AU5" s="123"/>
       <c r="AV5" s="123"/>
       <c r="AW5" s="123"/>
-      <c r="AX5" s="175"/>
-      <c r="AY5" s="175"/>
+      <c r="AX5" s="123"/>
+      <c r="AY5" s="123"/>
       <c r="AZ5" s="175"/>
-      <c r="BA5" s="153" t="s">
+      <c r="BA5" s="175"/>
+      <c r="BB5" s="175"/>
+      <c r="BC5" s="153" t="s">
         <v>125</v>
       </c>
-      <c r="BB5" s="127"/>
-      <c r="BC5" s="127"/>
       <c r="BD5" s="127"/>
       <c r="BE5" s="127"/>
       <c r="BF5" s="127"/>
@@ -4380,8 +4464,10 @@
       <c r="CB5" s="127"/>
       <c r="CC5" s="127"/>
       <c r="CD5" s="127"/>
+      <c r="CE5" s="127"/>
+      <c r="CF5" s="127"/>
     </row>
-    <row r="6" spans="1:82" s="1" customFormat="1" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:84" s="1" customFormat="1" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="152" t="s">
         <v>63</v>
       </c>
@@ -4433,14 +4519,14 @@
       <c r="AU6" s="108"/>
       <c r="AV6" s="108"/>
       <c r="AW6" s="108"/>
-      <c r="AX6" s="174"/>
-      <c r="AY6" s="174"/>
+      <c r="AX6" s="108"/>
+      <c r="AY6" s="108"/>
       <c r="AZ6" s="174"/>
-      <c r="BA6" s="152" t="s">
+      <c r="BA6" s="174"/>
+      <c r="BB6" s="174"/>
+      <c r="BC6" s="152" t="s">
         <v>63</v>
       </c>
-      <c r="BB6" s="2"/>
-      <c r="BC6" s="2"/>
       <c r="BD6" s="2"/>
       <c r="BE6" s="2"/>
       <c r="BF6" s="2"/>
@@ -4468,8 +4554,10 @@
       <c r="CB6" s="2"/>
       <c r="CC6" s="2"/>
       <c r="CD6" s="2"/>
+      <c r="CE6" s="2"/>
+      <c r="CF6" s="2"/>
     </row>
-    <row r="7" spans="1:82" s="1" customFormat="1" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:84" s="1" customFormat="1" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="153" t="s">
         <v>184</v>
       </c>
@@ -4587,50 +4675,54 @@
       <c r="AM7" s="165" t="s">
         <v>45</v>
       </c>
-      <c r="AN7" s="168" t="s">
+      <c r="AN7" s="165" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO7" s="165" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP7" s="168" t="s">
         <v>36</v>
       </c>
-      <c r="AO7" s="168" t="s">
+      <c r="AQ7" s="168" t="s">
         <v>46</v>
       </c>
-      <c r="AP7" s="168" t="s">
+      <c r="AR7" s="168" t="s">
         <v>163</v>
       </c>
-      <c r="AQ7" s="160" t="s">
+      <c r="AS7" s="160" t="s">
         <v>143</v>
       </c>
-      <c r="AR7" s="160" t="s">
+      <c r="AT7" s="160" t="s">
         <v>144</v>
       </c>
-      <c r="AS7" s="160" t="s">
+      <c r="AU7" s="160" t="s">
         <v>56</v>
       </c>
-      <c r="AT7" s="160" t="s">
+      <c r="AV7" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="AU7" s="160" t="s">
+      <c r="AW7" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="AV7" s="160" t="s">
+      <c r="AX7" s="160" t="s">
         <v>139</v>
       </c>
-      <c r="AW7" s="160" t="s">
+      <c r="AY7" s="160" t="s">
         <v>139</v>
       </c>
-      <c r="AX7" s="176" t="s">
+      <c r="AZ7" s="176" t="s">
         <v>243</v>
       </c>
-      <c r="AY7" s="176" t="s">
+      <c r="BA7" s="176" t="s">
         <v>250</v>
       </c>
-      <c r="AZ7" s="176" t="s">
+      <c r="BB7" s="176" t="s">
         <v>257</v>
       </c>
-      <c r="BA7" s="153" t="s">
+      <c r="BC7" s="153" t="s">
         <v>184</v>
       </c>
-      <c r="BB7" s="2"/>
-      <c r="BC7" s="2"/>
       <c r="BD7" s="2"/>
       <c r="BE7" s="2"/>
       <c r="BF7" s="2"/>
@@ -4658,8 +4750,10 @@
       <c r="CB7" s="2"/>
       <c r="CC7" s="2"/>
       <c r="CD7" s="2"/>
+      <c r="CE7" s="2"/>
+      <c r="CF7" s="2"/>
     </row>
-    <row r="8" spans="1:82" s="114" customFormat="1" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:84" s="114" customFormat="1" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="153" t="s">
         <v>85</v>
       </c>
@@ -4777,50 +4871,54 @@
       <c r="AM8" s="166" t="s">
         <v>135</v>
       </c>
-      <c r="AN8" s="169" t="s">
+      <c r="AN8" s="166" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO8" s="166" t="s">
+        <v>262</v>
+      </c>
+      <c r="AP8" s="169" t="s">
         <v>136</v>
       </c>
-      <c r="AO8" s="169" t="s">
+      <c r="AQ8" s="169" t="s">
         <v>137</v>
       </c>
-      <c r="AP8" s="169" t="s">
+      <c r="AR8" s="169" t="s">
         <v>138</v>
       </c>
-      <c r="AQ8" s="164" t="s">
+      <c r="AS8" s="164" t="s">
         <v>136</v>
       </c>
-      <c r="AR8" s="162" t="s">
+      <c r="AT8" s="162" t="s">
         <v>145</v>
       </c>
-      <c r="AS8" s="164" t="s">
+      <c r="AU8" s="164" t="s">
         <v>174</v>
       </c>
-      <c r="AT8" s="164" t="s">
+      <c r="AV8" s="164" t="s">
         <v>238</v>
       </c>
-      <c r="AU8" s="164" t="s">
+      <c r="AW8" s="164" t="s">
         <v>24</v>
       </c>
-      <c r="AV8" s="170" t="s">
+      <c r="AX8" s="170" t="s">
         <v>140</v>
       </c>
-      <c r="AW8" s="164" t="s">
+      <c r="AY8" s="164" t="s">
         <v>146</v>
       </c>
-      <c r="AX8" s="229" t="s">
+      <c r="AZ8" s="206" t="s">
         <v>244</v>
       </c>
-      <c r="AY8" s="229" t="s">
+      <c r="BA8" s="206" t="s">
         <v>251</v>
       </c>
-      <c r="AZ8" s="229" t="s">
+      <c r="BB8" s="206" t="s">
         <v>255</v>
       </c>
-      <c r="BA8" s="153" t="s">
+      <c r="BC8" s="153" t="s">
         <v>85</v>
       </c>
-      <c r="BB8" s="113"/>
-      <c r="BC8" s="113"/>
       <c r="BD8" s="113"/>
       <c r="BE8" s="113"/>
       <c r="BF8" s="113"/>
@@ -4848,8 +4946,10 @@
       <c r="CB8" s="113"/>
       <c r="CC8" s="113"/>
       <c r="CD8" s="113"/>
+      <c r="CE8" s="113"/>
+      <c r="CF8" s="113"/>
     </row>
-    <row r="9" spans="1:82" s="35" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:84" s="35" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="152" t="s">
         <v>166</v>
       </c>
@@ -4959,36 +5059,40 @@
       </c>
       <c r="AL9" s="167"/>
       <c r="AM9" s="167" t="s">
-        <v>190</v>
-      </c>
-      <c r="AN9" s="167"/>
-      <c r="AO9" s="167"/>
+        <v>258</v>
+      </c>
+      <c r="AN9" s="167" t="s">
+        <v>258</v>
+      </c>
+      <c r="AO9" s="167" t="s">
+        <v>258</v>
+      </c>
       <c r="AP9" s="167"/>
-      <c r="AQ9" s="109"/>
-      <c r="AR9" s="109"/>
-      <c r="AS9" s="178" t="s">
+      <c r="AQ9" s="167"/>
+      <c r="AR9" s="167"/>
+      <c r="AS9" s="109"/>
+      <c r="AT9" s="109"/>
+      <c r="AU9" s="178" t="s">
         <v>215</v>
       </c>
-      <c r="AT9" s="109" t="s">
+      <c r="AV9" s="109" t="s">
         <v>239</v>
       </c>
-      <c r="AU9" s="109"/>
-      <c r="AV9" s="109"/>
       <c r="AW9" s="109"/>
-      <c r="AX9" s="178" t="s">
+      <c r="AX9" s="109"/>
+      <c r="AY9" s="109"/>
+      <c r="AZ9" s="178" t="s">
         <v>245</v>
       </c>
-      <c r="AY9" s="178" t="s">
+      <c r="BA9" s="178" t="s">
         <v>252</v>
       </c>
-      <c r="AZ9" s="178" t="s">
+      <c r="BB9" s="178" t="s">
         <v>256</v>
       </c>
-      <c r="BA9" s="152" t="s">
+      <c r="BC9" s="152" t="s">
         <v>166</v>
       </c>
-      <c r="BB9" s="70"/>
-      <c r="BC9" s="70"/>
       <c r="BD9" s="70"/>
       <c r="BE9" s="70"/>
       <c r="BF9" s="70"/>
@@ -5016,8 +5120,10 @@
       <c r="CB9" s="70"/>
       <c r="CC9" s="70"/>
       <c r="CD9" s="70"/>
+      <c r="CE9" s="70"/>
+      <c r="CF9" s="70"/>
     </row>
-    <row r="10" spans="1:82" s="1" customFormat="1" ht="101.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:84" s="1" customFormat="1" ht="101.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="152" t="s">
         <v>196</v>
       </c>
@@ -5080,33 +5186,39 @@
         <v>208</v>
       </c>
       <c r="AL10" s="109"/>
-      <c r="AM10" s="109"/>
-      <c r="AN10" s="109"/>
-      <c r="AO10" s="109"/>
-      <c r="AP10" s="109" t="s">
+      <c r="AM10" s="109" t="s">
+        <v>260</v>
+      </c>
+      <c r="AN10" s="109" t="s">
+        <v>261</v>
+      </c>
+      <c r="AO10" s="109" t="s">
+        <v>104</v>
+      </c>
+      <c r="AP10" s="109"/>
+      <c r="AQ10" s="109"/>
+      <c r="AR10" s="109" t="s">
         <v>197</v>
       </c>
-      <c r="AQ10" s="109"/>
-      <c r="AR10" s="109"/>
       <c r="AS10" s="109"/>
       <c r="AT10" s="109"/>
       <c r="AU10" s="109"/>
-      <c r="AV10" s="109" t="s">
+      <c r="AV10" s="109"/>
+      <c r="AW10" s="109"/>
+      <c r="AX10" s="109" t="s">
         <v>199</v>
       </c>
-      <c r="AW10" s="109"/>
-      <c r="AX10" s="178"/>
-      <c r="AY10" s="178" t="s">
+      <c r="AY10" s="109"/>
+      <c r="AZ10" s="178"/>
+      <c r="BA10" s="178" t="s">
         <v>253</v>
       </c>
-      <c r="AZ10" s="178" t="s">
+      <c r="BB10" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="BA10" s="152" t="s">
+      <c r="BC10" s="152" t="s">
         <v>196</v>
       </c>
-      <c r="BB10" s="2"/>
-      <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
       <c r="BE10" s="2"/>
       <c r="BF10" s="2"/>
@@ -5134,8 +5246,10 @@
       <c r="CB10" s="2"/>
       <c r="CC10" s="2"/>
       <c r="CD10" s="2"/>
+      <c r="CE10" s="2"/>
+      <c r="CF10" s="2"/>
     </row>
-    <row r="11" spans="1:82" s="128" customFormat="1" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:84" s="128" customFormat="1" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="154" t="s">
         <v>152</v>
       </c>
@@ -5240,29 +5354,33 @@
       <c r="AN11" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="AO11" s="109"/>
-      <c r="AP11" s="109"/>
+      <c r="AO11" s="109" t="s">
+        <v>175</v>
+      </c>
+      <c r="AP11" s="109" t="s">
+        <v>175</v>
+      </c>
       <c r="AQ11" s="109"/>
       <c r="AR11" s="109"/>
-      <c r="AS11" s="109" t="s">
+      <c r="AS11" s="109"/>
+      <c r="AT11" s="109"/>
+      <c r="AU11" s="109" t="s">
         <v>180</v>
       </c>
-      <c r="AT11" s="109" t="s">
-        <v>180</v>
-      </c>
-      <c r="AU11" s="109"/>
       <c r="AV11" s="109" t="s">
         <v>180</v>
       </c>
       <c r="AW11" s="109"/>
-      <c r="AX11" s="228"/>
-      <c r="AY11" s="228"/>
-      <c r="AZ11" s="228"/>
-      <c r="BA11" s="179" t="s">
+      <c r="AX11" s="109" t="s">
+        <v>180</v>
+      </c>
+      <c r="AY11" s="109"/>
+      <c r="AZ11" s="205"/>
+      <c r="BA11" s="205"/>
+      <c r="BB11" s="205"/>
+      <c r="BC11" s="179" t="s">
         <v>152</v>
       </c>
-      <c r="BB11" s="127"/>
-      <c r="BC11" s="127"/>
       <c r="BD11" s="127"/>
       <c r="BE11" s="127"/>
       <c r="BF11" s="127"/>
@@ -5290,18 +5408,20 @@
       <c r="CB11" s="127"/>
       <c r="CC11" s="127"/>
       <c r="CD11" s="127"/>
+      <c r="CE11" s="127"/>
+      <c r="CF11" s="127"/>
     </row>
-    <row r="12" spans="1:82" s="26" customFormat="1" ht="21.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="207" t="s">
+    <row r="12" spans="1:84" s="26" customFormat="1" ht="21.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="211" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="207"/>
-      <c r="C12" s="207"/>
-      <c r="D12" s="207"/>
-      <c r="E12" s="207"/>
-      <c r="F12" s="207"/>
-      <c r="G12" s="207"/>
-      <c r="H12" s="207"/>
+      <c r="B12" s="211"/>
+      <c r="C12" s="211"/>
+      <c r="D12" s="211"/>
+      <c r="E12" s="211"/>
+      <c r="F12" s="211"/>
+      <c r="G12" s="211"/>
+      <c r="H12" s="211"/>
       <c r="I12" s="120"/>
       <c r="J12" s="120"/>
       <c r="K12" s="120"/>
@@ -5332,8 +5452,8 @@
       <c r="AJ12" s="120"/>
       <c r="AK12" s="120"/>
       <c r="AL12" s="120"/>
-      <c r="AM12" s="120"/>
-      <c r="AN12" s="120"/>
+      <c r="AM12" s="204"/>
+      <c r="AN12" s="204"/>
       <c r="AO12" s="120"/>
       <c r="AP12" s="120"/>
       <c r="AQ12" s="120"/>
@@ -5343,19 +5463,21 @@
       <c r="AU12" s="120"/>
       <c r="AV12" s="120"/>
       <c r="AW12" s="120"/>
-      <c r="AX12" s="203"/>
-      <c r="AY12" s="203"/>
+      <c r="AX12" s="120"/>
+      <c r="AY12" s="120"/>
       <c r="AZ12" s="203"/>
+      <c r="BA12" s="203"/>
+      <c r="BB12" s="203"/>
     </row>
-    <row r="13" spans="1:82" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="207" t="s">
+    <row r="13" spans="1:84" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="211" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="207"/>
-      <c r="C13" s="207"/>
-      <c r="D13" s="207"/>
-      <c r="E13" s="207"/>
-      <c r="F13" s="207"/>
+      <c r="B13" s="211"/>
+      <c r="C13" s="211"/>
+      <c r="D13" s="211"/>
+      <c r="E13" s="211"/>
+      <c r="F13" s="211"/>
       <c r="G13" s="131"/>
       <c r="H13" s="131"/>
       <c r="I13" s="131"/>
@@ -5401,9 +5523,11 @@
       <c r="AX13" s="131"/>
       <c r="AY13" s="131"/>
       <c r="AZ13" s="131"/>
+      <c r="BA13" s="131"/>
+      <c r="BB13" s="131"/>
     </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="BA14" s="70"/>
+    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="BC14" s="70"/>
     </row>
     <row r="22" spans="4:14" x14ac:dyDescent="0.25">
       <c r="N22" s="115"/>
@@ -5423,19 +5547,29 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A13:F13"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:AZ7 B8:S8 B9:AD11 AF11:AZ11 AE9:AZ10 U8:AW8">
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="B7:AL7 B8:S8 B9:AD11 AF11:AL11 AE9:AL10 U8:AL8 AO8:AY8 AO9:BB11 AO7:BB7">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE11">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",AE11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN7:AN11">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",AN7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM7:AM11">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",AM7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="AG3" r:id="rId1" display="mailto:John.Scinocca@ec.gc.ca"/>
-    <hyperlink ref="AP3" r:id="rId2"/>
+    <hyperlink ref="AR3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="47" fitToHeight="0" orientation="landscape" r:id="rId3"/>
@@ -5496,25 +5630,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:144" ht="80.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="208" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="204"/>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
-      <c r="E1" s="204"/>
-      <c r="F1" s="204"/>
-      <c r="G1" s="204"/>
-      <c r="H1" s="204"/>
-      <c r="I1" s="204"/>
-      <c r="J1" s="204"/>
-      <c r="K1" s="204"/>
-      <c r="L1" s="204"/>
-      <c r="M1" s="204"/>
-      <c r="N1" s="204"/>
-      <c r="O1" s="204"/>
-      <c r="P1" s="204"/>
-      <c r="Q1" s="204"/>
+      <c r="B1" s="208"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
+      <c r="G1" s="208"/>
+      <c r="H1" s="208"/>
+      <c r="I1" s="208"/>
+      <c r="J1" s="208"/>
+      <c r="K1" s="208"/>
+      <c r="L1" s="208"/>
+      <c r="M1" s="208"/>
+      <c r="N1" s="208"/>
+      <c r="O1" s="208"/>
+      <c r="P1" s="208"/>
+      <c r="Q1" s="208"/>
       <c r="R1" s="21"/>
       <c r="S1" s="20"/>
       <c r="T1" s="20"/>
@@ -5799,41 +5933,41 @@
         <f>AllEntries!AL3</f>
         <v>0</v>
       </c>
-      <c r="AN3" s="29">
-        <f>AllEntries!AM3</f>
-        <v>0</v>
+      <c r="AN3" s="29" t="str">
+        <f>AllEntries!AO3</f>
+        <v>Martin King, cordex@uni.no</v>
       </c>
       <c r="AO3" s="29">
-        <f>AllEntries!AN3</f>
+        <f>AllEntries!AP3</f>
         <v>0</v>
       </c>
       <c r="AP3" s="29">
-        <f>AllEntries!AO3</f>
+        <f>AllEntries!AQ3</f>
         <v>0</v>
       </c>
       <c r="AQ3" s="29" t="str">
-        <f>AllEntries!AP3</f>
+        <f>AllEntries!AR3</f>
         <v>robert.vautard@lsce.ipsl.fr</v>
       </c>
       <c r="AR3" s="29">
-        <f>AllEntries!AQ3</f>
+        <f>AllEntries!AS3</f>
         <v>0</v>
       </c>
       <c r="AS3" s="29">
-        <f>AllEntries!AR3</f>
+        <f>AllEntries!AT3</f>
         <v>0</v>
       </c>
       <c r="AT3" s="29" t="str">
-        <f>AllEntries!AS3</f>
+        <f>AllEntries!AU3</f>
         <v>Rowan Fealy : rowan.fealy
 @nuim.ie</v>
       </c>
       <c r="AU3" s="29" t="str">
-        <f>AllEntries!AT3</f>
+        <f>AllEntries!AV3</f>
         <v>Kirsten.Warrach-Sagi@uni-hohenheim.de</v>
       </c>
       <c r="AV3" s="29">
-        <f>AllEntries!AU3</f>
+        <f>AllEntries!AW3</f>
         <v>0</v>
       </c>
       <c r="AW3" s="29" t="e">
@@ -5841,11 +5975,11 @@
         <v>#REF!</v>
       </c>
       <c r="AX3" s="41">
-        <f>AllEntries!AV3</f>
+        <f>AllEntries!AX3</f>
         <v>0</v>
       </c>
       <c r="AY3" s="27">
-        <f>AllEntries!AW3</f>
+        <f>AllEntries!AY3</f>
         <v>0</v>
       </c>
       <c r="AZ3" s="78"/>
@@ -6102,39 +6236,39 @@
         <v>MIUB</v>
       </c>
       <c r="AN4" s="35" t="str">
-        <f>AllEntries!AM4</f>
+        <f>AllEntries!AO4</f>
         <v>BCCR</v>
       </c>
       <c r="AO4" s="35" t="str">
-        <f>AllEntries!AN4</f>
+        <f>AllEntries!AP4</f>
         <v>CRP-GL</v>
       </c>
       <c r="AP4" s="35" t="str">
-        <f>AllEntries!AO4</f>
+        <f>AllEntries!AQ4</f>
         <v>IDL</v>
       </c>
       <c r="AQ4" s="35" t="str">
-        <f>AllEntries!AP4</f>
+        <f>AllEntries!AR4</f>
         <v>IPSL/INERIS</v>
       </c>
       <c r="AR4" s="35" t="str">
-        <f>AllEntries!AQ4</f>
+        <f>AllEntries!AS4</f>
         <v>AUTH-Met</v>
       </c>
       <c r="AS4" s="35" t="str">
-        <f>AllEntries!AR4</f>
+        <f>AllEntries!AT4</f>
         <v>AUTH-LHTEE</v>
       </c>
       <c r="AT4" s="35" t="str">
-        <f>AllEntries!AS4</f>
+        <f>AllEntries!AU4</f>
         <v>NUIM</v>
       </c>
       <c r="AU4" s="35" t="str">
-        <f>AllEntries!AT4</f>
+        <f>AllEntries!AV4</f>
         <v>UHOH</v>
       </c>
       <c r="AV4" s="35" t="str">
-        <f>AllEntries!AU4</f>
+        <f>AllEntries!AW4</f>
         <v>UM</v>
       </c>
       <c r="AW4" s="35" t="e">
@@ -6142,14 +6276,14 @@
         <v>#REF!</v>
       </c>
       <c r="AX4" s="42" t="str">
-        <f>AllEntries!AV4</f>
+        <f>AllEntries!AX4</f>
         <v>UCAN</v>
       </c>
       <c r="AY4" s="33" t="str">
-        <f>AllEntries!AW4</f>
+        <f>AllEntries!AY4</f>
         <v>UCAN</v>
       </c>
-      <c r="AZ4" s="211" t="s">
+      <c r="AZ4" s="215" t="s">
         <v>16</v>
       </c>
       <c r="BA4" s="73" t="s">
@@ -6405,39 +6539,39 @@
         <v>0</v>
       </c>
       <c r="AN5" s="35">
-        <f>AllEntries!AM6</f>
+        <f>AllEntries!AO6</f>
         <v>0</v>
       </c>
       <c r="AO5" s="35">
-        <f>AllEntries!AN6</f>
+        <f>AllEntries!AP6</f>
         <v>0</v>
       </c>
       <c r="AP5" s="35">
-        <f>AllEntries!AO6</f>
+        <f>AllEntries!AQ6</f>
         <v>0</v>
       </c>
       <c r="AQ5" s="35">
-        <f>AllEntries!AP6</f>
+        <f>AllEntries!AR6</f>
         <v>0</v>
       </c>
       <c r="AR5" s="35">
-        <f>AllEntries!AQ6</f>
+        <f>AllEntries!AS6</f>
         <v>0</v>
       </c>
       <c r="AS5" s="35">
-        <f>AllEntries!AR6</f>
+        <f>AllEntries!AT6</f>
         <v>0</v>
       </c>
       <c r="AT5" s="35">
-        <f>AllEntries!AS6</f>
+        <f>AllEntries!AU6</f>
         <v>0</v>
       </c>
       <c r="AU5" s="35">
-        <f>AllEntries!AT6</f>
+        <f>AllEntries!AV6</f>
         <v>0</v>
       </c>
       <c r="AV5" s="35">
-        <f>AllEntries!AU6</f>
+        <f>AllEntries!AW6</f>
         <v>0</v>
       </c>
       <c r="AW5" s="35" t="e">
@@ -6445,14 +6579,14 @@
         <v>#REF!</v>
       </c>
       <c r="AX5" s="42">
-        <f>AllEntries!AV6</f>
+        <f>AllEntries!AX6</f>
         <v>0</v>
       </c>
       <c r="AY5" s="33">
-        <f>AllEntries!AW6</f>
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="212"/>
+        <f>AllEntries!AY6</f>
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="216"/>
       <c r="BA5" s="73"/>
       <c r="BB5" s="2"/>
       <c r="BC5" s="2"/>
@@ -6704,39 +6838,39 @@
         <v>WRF331A</v>
       </c>
       <c r="AN6" s="38" t="str">
-        <f>AllEntries!AM8</f>
-        <v>WRF331C</v>
+        <f>AllEntries!AO8</f>
+        <v>WRF361</v>
       </c>
       <c r="AO6" s="39" t="str">
-        <f>AllEntries!AN8</f>
+        <f>AllEntries!AP8</f>
         <v>WRF331A</v>
       </c>
       <c r="AP6" s="39" t="str">
-        <f>AllEntries!AO8</f>
+        <f>AllEntries!AQ8</f>
         <v>WRF331D</v>
       </c>
       <c r="AQ6" s="39" t="str">
-        <f>AllEntries!AP8</f>
+        <f>AllEntries!AR8</f>
         <v>WRF331F</v>
       </c>
       <c r="AR6" s="25" t="str">
-        <f>AllEntries!AQ8</f>
+        <f>AllEntries!AS8</f>
         <v>WRF331A</v>
       </c>
       <c r="AS6" s="24" t="str">
-        <f>AllEntries!AR8</f>
+        <f>AllEntries!AT8</f>
         <v>WRF321B</v>
       </c>
       <c r="AT6" s="25" t="str">
-        <f>AllEntries!AS8</f>
+        <f>AllEntries!AU8</f>
         <v>WRF341E</v>
       </c>
       <c r="AU6" s="25" t="str">
-        <f>AllEntries!AT8</f>
+        <f>AllEntries!AV8</f>
         <v>WRF361H</v>
       </c>
       <c r="AV6" s="25" t="str">
-        <f>AllEntries!AU8</f>
+        <f>AllEntries!AW8</f>
         <v>WRF331</v>
       </c>
       <c r="AW6" s="37" t="e">
@@ -6744,14 +6878,14 @@
         <v>#REF!</v>
       </c>
       <c r="AX6" s="43" t="str">
-        <f>AllEntries!AV8</f>
+        <f>AllEntries!AX8</f>
         <v>WRF331G</v>
       </c>
       <c r="AY6" s="81" t="str">
-        <f>AllEntries!AW8</f>
+        <f>AllEntries!AY8</f>
         <v>WRF350I</v>
       </c>
-      <c r="AZ6" s="213"/>
+      <c r="AZ6" s="217"/>
       <c r="BA6" s="74" t="s">
         <v>19</v>
       </c>
@@ -10346,26 +10480,26 @@
       </c>
       <c r="EN27" s="26"/>
     </row>
-    <row r="28" spans="1:144" s="26" customFormat="1" ht="37.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="214" t="s">
+    <row r="28" spans="1:144" s="26" customFormat="1" ht="37.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="218" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="214"/>
-      <c r="C28" s="214"/>
-      <c r="D28" s="214"/>
-      <c r="E28" s="214"/>
-      <c r="F28" s="214"/>
-      <c r="G28" s="214"/>
-      <c r="H28" s="214"/>
-      <c r="I28" s="214"/>
-      <c r="J28" s="214"/>
-      <c r="K28" s="214"/>
-      <c r="L28" s="214"/>
-      <c r="M28" s="214"/>
-      <c r="N28" s="214"/>
-      <c r="O28" s="214"/>
-      <c r="P28" s="214"/>
-      <c r="Q28" s="214"/>
+      <c r="B28" s="218"/>
+      <c r="C28" s="218"/>
+      <c r="D28" s="218"/>
+      <c r="E28" s="218"/>
+      <c r="F28" s="218"/>
+      <c r="G28" s="218"/>
+      <c r="H28" s="218"/>
+      <c r="I28" s="218"/>
+      <c r="J28" s="218"/>
+      <c r="K28" s="218"/>
+      <c r="L28" s="218"/>
+      <c r="M28" s="218"/>
+      <c r="N28" s="218"/>
+      <c r="O28" s="218"/>
+      <c r="P28" s="218"/>
+      <c r="Q28" s="218"/>
       <c r="R28" s="40"/>
       <c r="S28" s="40"/>
       <c r="T28" s="40"/>
@@ -10400,70 +10534,70 @@
       <c r="AW28" s="30"/>
       <c r="AX28" s="30"/>
     </row>
-    <row r="29" spans="1:144" s="26" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A29" s="215" t="s">
+    <row r="29" spans="1:144" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="219" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="215"/>
-      <c r="C29" s="215"/>
-      <c r="D29" s="215"/>
-      <c r="E29" s="215"/>
-      <c r="F29" s="215"/>
-      <c r="G29" s="215"/>
-      <c r="H29" s="215"/>
-      <c r="I29" s="215"/>
-      <c r="J29" s="215"/>
-      <c r="K29" s="215"/>
-      <c r="L29" s="215"/>
-      <c r="M29" s="215"/>
-      <c r="N29" s="215"/>
-      <c r="O29" s="215"/>
-      <c r="P29" s="215"/>
-      <c r="Q29" s="215"/>
-      <c r="R29" s="215"/>
-      <c r="S29" s="215"/>
-      <c r="T29" s="215"/>
-      <c r="U29" s="215"/>
-      <c r="V29" s="215"/>
-      <c r="W29" s="215"/>
-      <c r="X29" s="215"/>
-      <c r="Y29" s="215"/>
-      <c r="Z29" s="215"/>
-      <c r="AA29" s="215"/>
-      <c r="AB29" s="215"/>
-      <c r="AC29" s="215"/>
-      <c r="AD29" s="215"/>
-      <c r="AE29" s="215"/>
-      <c r="AF29" s="215"/>
-      <c r="AG29" s="215"/>
-      <c r="AH29" s="215"/>
-      <c r="AI29" s="215"/>
-      <c r="AJ29" s="215"/>
-      <c r="AK29" s="215"/>
-      <c r="AL29" s="215"/>
-      <c r="AM29" s="215"/>
-      <c r="AN29" s="215"/>
-      <c r="AO29" s="215"/>
-      <c r="AP29" s="215"/>
-      <c r="AQ29" s="215"/>
-      <c r="AR29" s="215"/>
-      <c r="AS29" s="215"/>
-      <c r="AT29" s="215"/>
-      <c r="AU29" s="215"/>
-      <c r="AV29" s="215"/>
-      <c r="AW29" s="215"/>
-      <c r="AX29" s="215"/>
+      <c r="B29" s="219"/>
+      <c r="C29" s="219"/>
+      <c r="D29" s="219"/>
+      <c r="E29" s="219"/>
+      <c r="F29" s="219"/>
+      <c r="G29" s="219"/>
+      <c r="H29" s="219"/>
+      <c r="I29" s="219"/>
+      <c r="J29" s="219"/>
+      <c r="K29" s="219"/>
+      <c r="L29" s="219"/>
+      <c r="M29" s="219"/>
+      <c r="N29" s="219"/>
+      <c r="O29" s="219"/>
+      <c r="P29" s="219"/>
+      <c r="Q29" s="219"/>
+      <c r="R29" s="219"/>
+      <c r="S29" s="219"/>
+      <c r="T29" s="219"/>
+      <c r="U29" s="219"/>
+      <c r="V29" s="219"/>
+      <c r="W29" s="219"/>
+      <c r="X29" s="219"/>
+      <c r="Y29" s="219"/>
+      <c r="Z29" s="219"/>
+      <c r="AA29" s="219"/>
+      <c r="AB29" s="219"/>
+      <c r="AC29" s="219"/>
+      <c r="AD29" s="219"/>
+      <c r="AE29" s="219"/>
+      <c r="AF29" s="219"/>
+      <c r="AG29" s="219"/>
+      <c r="AH29" s="219"/>
+      <c r="AI29" s="219"/>
+      <c r="AJ29" s="219"/>
+      <c r="AK29" s="219"/>
+      <c r="AL29" s="219"/>
+      <c r="AM29" s="219"/>
+      <c r="AN29" s="219"/>
+      <c r="AO29" s="219"/>
+      <c r="AP29" s="219"/>
+      <c r="AQ29" s="219"/>
+      <c r="AR29" s="219"/>
+      <c r="AS29" s="219"/>
+      <c r="AT29" s="219"/>
+      <c r="AU29" s="219"/>
+      <c r="AV29" s="219"/>
+      <c r="AW29" s="219"/>
+      <c r="AX29" s="219"/>
     </row>
-    <row r="30" spans="1:144" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="216" t="s">
+    <row r="30" spans="1:144" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="220" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="216"/>
-      <c r="C30" s="216"/>
-      <c r="D30" s="216"/>
-      <c r="E30" s="216"/>
-      <c r="F30" s="215"/>
-      <c r="G30" s="215"/>
+      <c r="B30" s="220"/>
+      <c r="C30" s="220"/>
+      <c r="D30" s="220"/>
+      <c r="E30" s="220"/>
+      <c r="F30" s="219"/>
+      <c r="G30" s="219"/>
       <c r="H30" s="19"/>
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
@@ -10495,7 +10629,7 @@
       <c r="AV30" s="19"/>
       <c r="AW30" s="19"/>
     </row>
-    <row r="31" spans="1:144" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:144" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>0</v>
       </c>
@@ -10505,13 +10639,13 @@
       <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="217" t="s">
+      <c r="D31" s="221" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="218"/>
+      <c r="E31" s="222"/>
       <c r="F31" s="14"/>
     </row>
-    <row r="32" spans="1:144" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:144" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>5</v>
       </c>
@@ -10523,14 +10657,14 @@
         <f>C33*98*63/194/201</f>
         <v>460.27127250346206</v>
       </c>
-      <c r="D32" s="219">
+      <c r="D32" s="223">
         <f t="shared" ref="D32:D37" si="33">(B32+C32)/1</f>
         <v>476.23114325280812</v>
       </c>
-      <c r="E32" s="220"/>
+      <c r="E32" s="224"/>
       <c r="F32" s="14"/>
     </row>
-    <row r="33" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>3</v>
       </c>
@@ -10541,14 +10675,14 @@
       <c r="C33" s="10">
         <v>2907</v>
       </c>
-      <c r="D33" s="221">
+      <c r="D33" s="225">
         <f t="shared" si="33"/>
         <v>3007.8</v>
       </c>
-      <c r="E33" s="222"/>
+      <c r="E33" s="226"/>
       <c r="F33" s="14"/>
     </row>
-    <row r="34" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>15</v>
       </c>
@@ -10560,14 +10694,14 @@
         <f>4*AFR44tier1</f>
         <v>11628</v>
       </c>
-      <c r="D34" s="221">
+      <c r="D34" s="225">
         <f t="shared" si="33"/>
         <v>12031.2</v>
       </c>
-      <c r="E34" s="222"/>
+      <c r="E34" s="226"/>
       <c r="F34" s="14"/>
     </row>
-    <row r="35" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A35" s="93" t="s">
         <v>4</v>
       </c>
@@ -10578,14 +10712,14 @@
       <c r="C35" s="95">
         <v>13005</v>
       </c>
-      <c r="D35" s="221">
+      <c r="D35" s="225">
         <f t="shared" si="33"/>
         <v>13475.4</v>
       </c>
-      <c r="E35" s="222"/>
+      <c r="E35" s="226"/>
       <c r="F35" s="14"/>
     </row>
-    <row r="36" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A36" s="101" t="s">
         <v>109</v>
       </c>
@@ -10597,14 +10731,14 @@
         <f>C33*125*97/194/201</f>
         <v>903.91791044776119</v>
       </c>
-      <c r="D36" s="221">
+      <c r="D36" s="225">
         <f t="shared" si="33"/>
         <v>932.02992768118168</v>
       </c>
-      <c r="E36" s="222"/>
+      <c r="E36" s="226"/>
       <c r="F36" s="26"/>
     </row>
-    <row r="37" spans="1:49" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="96" t="s">
         <v>104</v>
       </c>
@@ -10616,34 +10750,34 @@
         <f>C33*116*133/194/201</f>
         <v>1150.1563317433452</v>
       </c>
-      <c r="D37" s="223">
+      <c r="D37" s="227">
         <f t="shared" si="33"/>
         <v>1190.0379135251578</v>
       </c>
-      <c r="E37" s="224"/>
+      <c r="E37" s="228"/>
       <c r="F37" s="26"/>
     </row>
-    <row r="38" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A38" s="209" t="s">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A38" s="213" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="209"/>
-      <c r="C38" s="209"/>
-      <c r="D38" s="209"/>
-      <c r="E38" s="209"/>
-      <c r="F38" s="210"/>
-      <c r="G38" s="210"/>
+      <c r="B38" s="213"/>
+      <c r="C38" s="213"/>
+      <c r="D38" s="213"/>
+      <c r="E38" s="213"/>
+      <c r="F38" s="214"/>
+      <c r="G38" s="214"/>
     </row>
-    <row r="39" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A39" s="210" t="s">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A39" s="214" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="210"/>
-      <c r="C39" s="210"/>
-      <c r="D39" s="210"/>
-      <c r="E39" s="210"/>
-      <c r="F39" s="210"/>
-      <c r="G39" s="210"/>
+      <c r="B39" s="214"/>
+      <c r="C39" s="214"/>
+      <c r="D39" s="214"/>
+      <c r="E39" s="214"/>
+      <c r="F39" s="214"/>
+      <c r="G39" s="214"/>
       <c r="H39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
@@ -10770,41 +10904,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" ht="80.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="230" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
-      <c r="I1" s="226"/>
-      <c r="J1" s="226" t="str">
+      <c r="B1" s="230"/>
+      <c r="C1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="230"/>
+      <c r="F1" s="230"/>
+      <c r="G1" s="230"/>
+      <c r="H1" s="230"/>
+      <c r="I1" s="230"/>
+      <c r="J1" s="230" t="str">
         <f>A1</f>
         <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
       </c>
-      <c r="K1" s="226"/>
-      <c r="L1" s="226"/>
-      <c r="M1" s="226"/>
-      <c r="N1" s="226"/>
-      <c r="O1" s="226"/>
-      <c r="P1" s="226"/>
-      <c r="Q1" s="226"/>
-      <c r="R1" s="226"/>
-      <c r="S1" s="227" t="str">
+      <c r="K1" s="230"/>
+      <c r="L1" s="230"/>
+      <c r="M1" s="230"/>
+      <c r="N1" s="230"/>
+      <c r="O1" s="230"/>
+      <c r="P1" s="230"/>
+      <c r="Q1" s="230"/>
+      <c r="R1" s="230"/>
+      <c r="S1" s="231" t="str">
         <f>A1</f>
         <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
       </c>
-      <c r="T1" s="227"/>
-      <c r="U1" s="227"/>
-      <c r="V1" s="227"/>
-      <c r="W1" s="227"/>
-      <c r="X1" s="227"/>
-      <c r="Y1" s="227"/>
-      <c r="Z1" s="227"/>
-      <c r="AA1" s="227"/>
+      <c r="T1" s="231"/>
+      <c r="U1" s="231"/>
+      <c r="V1" s="231"/>
+      <c r="W1" s="231"/>
+      <c r="X1" s="231"/>
+      <c r="Y1" s="231"/>
+      <c r="Z1" s="231"/>
+      <c r="AA1" s="231"/>
       <c r="AB1" s="190" t="str">
         <f>A1</f>
         <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
@@ -10817,18 +10951,18 @@
       <c r="AH1" s="190"/>
       <c r="AI1" s="190"/>
       <c r="AJ1" s="191"/>
-      <c r="AK1" s="227" t="str">
+      <c r="AK1" s="231" t="str">
         <f>A1</f>
         <v>Controlled Vocabulary of RCM names and institute names involved in Euro-CORDEX, Africa-CORDEX, or Mediterranean-CORDEX</v>
       </c>
-      <c r="AL1" s="227"/>
-      <c r="AM1" s="227"/>
-      <c r="AN1" s="227"/>
-      <c r="AO1" s="227"/>
-      <c r="AP1" s="227"/>
-      <c r="AQ1" s="227"/>
-      <c r="AR1" s="227"/>
-      <c r="AS1" s="227"/>
+      <c r="AL1" s="231"/>
+      <c r="AM1" s="231"/>
+      <c r="AN1" s="231"/>
+      <c r="AO1" s="231"/>
+      <c r="AP1" s="231"/>
+      <c r="AQ1" s="231"/>
+      <c r="AR1" s="231"/>
+      <c r="AS1" s="231"/>
       <c r="AT1" s="190"/>
       <c r="AU1" s="192"/>
       <c r="AV1" s="192"/>
@@ -10919,11 +11053,11 @@
         <v>87</v>
       </c>
       <c r="B3" s="118" t="str">
-        <f>AllEntries!AR7</f>
+        <f>AllEntries!AT7</f>
         <v>AUTH-LHTEE</v>
       </c>
       <c r="C3" s="118" t="str">
-        <f>AllEntries!AQ7</f>
+        <f>AllEntries!AS7</f>
         <v>AUTH-Met</v>
       </c>
       <c r="D3" s="118" t="str">
@@ -10931,7 +11065,7 @@
         <v>AWI</v>
       </c>
       <c r="E3" s="118" t="str">
-        <f>AllEntries!AM7</f>
+        <f>AllEntries!AO7</f>
         <v>BCCR</v>
       </c>
       <c r="F3" s="197" t="str">
@@ -10982,7 +11116,7 @@
         <v>CNRM</v>
       </c>
       <c r="R3" s="118" t="str">
-        <f>AllEntries!AN7</f>
+        <f>AllEntries!AP7</f>
         <v>CRP-GL</v>
       </c>
       <c r="S3" s="77" t="s">
@@ -11024,7 +11158,7 @@
         <v>87</v>
       </c>
       <c r="AC3" s="118" t="str">
-        <f>AllEntries!AO7</f>
+        <f>AllEntries!AQ7</f>
         <v>IDL</v>
       </c>
       <c r="AD3" s="118" t="str">
@@ -11032,7 +11166,7 @@
         <v>IITM</v>
       </c>
       <c r="AE3" s="118" t="str">
-        <f>AllEntries!AP7</f>
+        <f>AllEntries!AR7</f>
         <v>IPSL-INERIS</v>
       </c>
       <c r="AF3" s="197" t="str">
@@ -11079,7 +11213,7 @@
         <v>MPI-CSC</v>
       </c>
       <c r="AQ3" s="118" t="str">
-        <f>AllEntries!AS7</f>
+        <f>AllEntries!AU7</f>
         <v>NUIM</v>
       </c>
       <c r="AR3" s="118" t="str">
@@ -11102,11 +11236,11 @@
         <v>SMHI</v>
       </c>
       <c r="AW3" s="118" t="str">
-        <f>AllEntries!AV7</f>
+        <f>AllEntries!AX7</f>
         <v>UCAN</v>
       </c>
       <c r="AX3" s="118" t="str">
-        <f>AllEntries!AW7</f>
+        <f>AllEntries!AY7</f>
         <v>UCAN</v>
       </c>
       <c r="AY3" s="118" t="str">
@@ -11114,18 +11248,18 @@
         <v>UCLM</v>
       </c>
       <c r="AZ3" s="118" t="str">
-        <f>AllEntries!AT7</f>
+        <f>AllEntries!AV7</f>
         <v>UHOH</v>
       </c>
       <c r="BA3" s="118" t="str">
-        <f>AllEntries!AU7</f>
+        <f>AllEntries!AW7</f>
         <v>UM</v>
       </c>
       <c r="BB3" s="200" t="str">
         <f>AllEntries!Y7</f>
         <v>UQAM</v>
       </c>
-      <c r="BC3" s="225"/>
+      <c r="BC3" s="229"/>
       <c r="BD3" s="2"/>
       <c r="BE3" s="2"/>
       <c r="BF3" s="2"/>
@@ -11158,11 +11292,11 @@
         <v>181</v>
       </c>
       <c r="B4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AR9),"",AllEntries!AR9)</f>
+        <f>IF(ISBLANK(AllEntries!AT9),"",AllEntries!AT9)</f>
         <v/>
       </c>
       <c r="C4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AQ9),"",AllEntries!AQ9)</f>
+        <f>IF(ISBLANK(AllEntries!AS9),"",AllEntries!AS9)</f>
         <v/>
       </c>
       <c r="D4" s="188" t="str">
@@ -11170,8 +11304,8 @@
         <v>Alfred Wegener Institute, Helmholtz Centre for Polar and Marine Research</v>
       </c>
       <c r="E4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AM9),"",AllEntries!AM9)</f>
-        <v>Bjerknes Centre for Climate Research</v>
+        <f>IF(ISBLANK(AllEntries!AO9),"",AllEntries!AO9)</f>
+        <v>Bjerknes Centre for Climate Research and Uni Research</v>
       </c>
       <c r="F4" s="195" t="str">
         <f>IF(ISBLANK(AllEntries!AG9),"",AllEntries!AG9)</f>
@@ -11221,7 +11355,7 @@
         <v>Centre National de Recherches Meteorologiques</v>
       </c>
       <c r="R4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AN9),"",AllEntries!AN9)</f>
+        <f>IF(ISBLANK(AllEntries!AP9),"",AllEntries!AP9)</f>
         <v/>
       </c>
       <c r="S4" s="138" t="s">
@@ -11263,7 +11397,7 @@
         <v>181</v>
       </c>
       <c r="AC4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AO9),"",AllEntries!AO9)</f>
+        <f>IF(ISBLANK(AllEntries!AQ9),"",AllEntries!AQ9)</f>
         <v/>
       </c>
       <c r="AD4" s="188" t="str">
@@ -11271,7 +11405,7 @@
         <v>Indian Institute of Tropical Meteorology</v>
       </c>
       <c r="AE4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AP9),"",AllEntries!AP9)</f>
+        <f>IF(ISBLANK(AllEntries!AR9),"",AllEntries!AR9)</f>
         <v/>
       </c>
       <c r="AF4" s="195" t="str">
@@ -11318,7 +11452,7 @@
         <v>Helmholtz-Zentrum Geesthacht, Climate Service Center, Max Planck Institute for Meteorology</v>
       </c>
       <c r="AQ4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AS9),"",AllEntries!AS9)</f>
+        <f>IF(ISBLANK(AllEntries!AU9),"",AllEntries!AU9)</f>
         <v>National University of Ireland Maynooth</v>
       </c>
       <c r="AR4" s="188" t="str">
@@ -11341,11 +11475,11 @@
         <v>Swedish Meteorological and Hydrological Institute, Rossby Centre</v>
       </c>
       <c r="AW4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AV9),"",AllEntries!AV9)</f>
+        <f>IF(ISBLANK(AllEntries!AX9),"",AllEntries!AX9)</f>
         <v/>
       </c>
       <c r="AX4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AW9),"",AllEntries!AW9)</f>
+        <f>IF(ISBLANK(AllEntries!AY9),"",AllEntries!AY9)</f>
         <v/>
       </c>
       <c r="AY4" s="188" t="str">
@@ -11353,18 +11487,18 @@
         <v>University of Castilla-La Mancha, Toledo, Spain</v>
       </c>
       <c r="AZ4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AT9),"",AllEntries!AT9)</f>
+        <f>IF(ISBLANK(AllEntries!AV9),"",AllEntries!AV9)</f>
         <v xml:space="preserve">University of Hohenheim </v>
       </c>
       <c r="BA4" s="188" t="str">
-        <f>IF(ISBLANK(AllEntries!AU9),"",AllEntries!AU9)</f>
+        <f>IF(ISBLANK(AllEntries!AW9),"",AllEntries!AW9)</f>
         <v/>
       </c>
       <c r="BB4" s="201" t="str">
         <f>IF(ISBLANK(AllEntries!Y9),"",AllEntries!Y9)</f>
         <v>Universite du Quebec a Montreal</v>
       </c>
-      <c r="BC4" s="225"/>
+      <c r="BC4" s="229"/>
       <c r="BD4" s="2"/>
       <c r="BE4" s="2"/>
       <c r="BF4" s="2"/>
@@ -11397,11 +11531,11 @@
         <v>85</v>
       </c>
       <c r="B5" s="119" t="str">
-        <f>AllEntries!AR8</f>
+        <f>AllEntries!AT8</f>
         <v>WRF321B</v>
       </c>
       <c r="C5" s="119" t="str">
-        <f>AllEntries!AQ8</f>
+        <f>AllEntries!AS8</f>
         <v>WRF331A</v>
       </c>
       <c r="D5" s="119" t="str">
@@ -11409,8 +11543,8 @@
         <v>HIRHAM5</v>
       </c>
       <c r="E5" s="119" t="str">
-        <f>AllEntries!AM8</f>
-        <v>WRF331C</v>
+        <f>AllEntries!AO8</f>
+        <v>WRF361</v>
       </c>
       <c r="F5" s="198" t="str">
         <f>AllEntries!AG8</f>
@@ -11460,7 +11594,7 @@
         <v>ARPEGE52</v>
       </c>
       <c r="R5" s="119" t="str">
-        <f>AllEntries!AN8</f>
+        <f>AllEntries!AP8</f>
         <v>WRF331A</v>
       </c>
       <c r="S5" s="142" t="s">
@@ -11502,7 +11636,7 @@
         <v>85</v>
       </c>
       <c r="AC5" s="119" t="str">
-        <f>AllEntries!AO8</f>
+        <f>AllEntries!AQ8</f>
         <v>WRF331D</v>
       </c>
       <c r="AD5" s="119" t="str">
@@ -11510,7 +11644,7 @@
         <v>RegCM4-1</v>
       </c>
       <c r="AE5" s="119" t="str">
-        <f>AllEntries!AP8</f>
+        <f>AllEntries!AR8</f>
         <v>WRF331F</v>
       </c>
       <c r="AF5" s="198" t="str">
@@ -11557,7 +11691,7 @@
         <v>REMO2009</v>
       </c>
       <c r="AQ5" s="119" t="str">
-        <f>AllEntries!AS8</f>
+        <f>AllEntries!AU8</f>
         <v>WRF341E</v>
       </c>
       <c r="AR5" s="119" t="str">
@@ -11580,11 +11714,11 @@
         <v>RCA4-SN</v>
       </c>
       <c r="AW5" s="119" t="str">
-        <f>AllEntries!AV8</f>
+        <f>AllEntries!AX8</f>
         <v>WRF331G</v>
       </c>
       <c r="AX5" s="119" t="str">
-        <f>AllEntries!AW8</f>
+        <f>AllEntries!AY8</f>
         <v>WRF350I</v>
       </c>
       <c r="AY5" s="119" t="str">
@@ -11592,18 +11726,18 @@
         <v>PROMES</v>
       </c>
       <c r="AZ5" s="119" t="str">
-        <f>AllEntries!AT8</f>
+        <f>AllEntries!AV8</f>
         <v>WRF361H</v>
       </c>
       <c r="BA5" s="119" t="str">
-        <f>AllEntries!AU8</f>
+        <f>AllEntries!AW8</f>
         <v>WRF331</v>
       </c>
       <c r="BB5" s="202" t="str">
         <f>AllEntries!Y8</f>
         <v>CRCM5</v>
       </c>
-      <c r="BC5" s="225"/>
+      <c r="BC5" s="229"/>
       <c r="BD5" s="2"/>
       <c r="BE5" s="2"/>
       <c r="BF5" s="2"/>
@@ -11649,7 +11783,7 @@
       </c>
       <c r="E6" s="119" t="str">
         <f>IF(ISBLANK(E9),"",CONCATENATE(E3,"-",E5))</f>
-        <v>BCCR-WRF331C</v>
+        <v>BCCR-WRF361</v>
       </c>
       <c r="F6" s="198" t="str">
         <f>CONCATENATE(F3,"-",F5)</f>
@@ -11875,11 +12009,11 @@
         <v>150</v>
       </c>
       <c r="B7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AR11),"unknown",AllEntries!AR11)</f>
+        <f>IF(ISBLANK(AllEntries!AT11),"unknown",AllEntries!AT11)</f>
         <v>unknown</v>
       </c>
       <c r="C7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AQ11),"unknown",AllEntries!AQ11)</f>
+        <f>IF(ISBLANK(AllEntries!AS11),"unknown",AllEntries!AS11)</f>
         <v>unknown</v>
       </c>
       <c r="D7" s="189" t="str">
@@ -11887,7 +12021,7 @@
         <v>unknown</v>
       </c>
       <c r="E7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AM11),"unknown",AllEntries!AM11)</f>
+        <f>IF(ISBLANK(AllEntries!AO11),"unknown",AllEntries!AO11)</f>
         <v>unrestricted</v>
       </c>
       <c r="F7" s="189" t="str">
@@ -11938,7 +12072,7 @@
         <v>unrestricted</v>
       </c>
       <c r="R7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AN11),"unknown",AllEntries!AN11)</f>
+        <f>IF(ISBLANK(AllEntries!AP11),"unknown",AllEntries!AP11)</f>
         <v>unrestricted</v>
       </c>
       <c r="S7" s="140" t="s">
@@ -11980,7 +12114,7 @@
         <v>150</v>
       </c>
       <c r="AC7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AO11),"unknown",AllEntries!AO11)</f>
+        <f>IF(ISBLANK(AllEntries!AQ11),"unknown",AllEntries!AQ11)</f>
         <v>unknown</v>
       </c>
       <c r="AD7" s="189" t="str">
@@ -11988,7 +12122,7 @@
         <v>non-commercial only</v>
       </c>
       <c r="AE7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AP11),"unknown",AllEntries!AP11)</f>
+        <f>IF(ISBLANK(AllEntries!AR11),"unknown",AllEntries!AR11)</f>
         <v>unknown</v>
       </c>
       <c r="AF7" s="189" t="str">
@@ -12035,7 +12169,7 @@
         <v>unrestricted</v>
       </c>
       <c r="AQ7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AS11),"unknown",AllEntries!AS11)</f>
+        <f>IF(ISBLANK(AllEntries!AU11),"unknown",AllEntries!AU11)</f>
         <v>non-commercial only</v>
       </c>
       <c r="AR7" s="189" t="str">
@@ -12058,11 +12192,11 @@
         <v>unrestricted</v>
       </c>
       <c r="AW7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AV11),"unknown",AllEntries!AV11)</f>
+        <f>IF(ISBLANK(AllEntries!AX11),"unknown",AllEntries!AX11)</f>
         <v>non-commercial only</v>
       </c>
       <c r="AX7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AW11),"unknown",AllEntries!AW11)</f>
+        <f>IF(ISBLANK(AllEntries!AY11),"unknown",AllEntries!AY11)</f>
         <v>unknown</v>
       </c>
       <c r="AY7" s="189" t="str">
@@ -12070,11 +12204,11 @@
         <v>unknown</v>
       </c>
       <c r="AZ7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AT11),"unknown",AllEntries!AT11)</f>
+        <f>IF(ISBLANK(AllEntries!AV11),"unknown",AllEntries!AV11)</f>
         <v>non-commercial only</v>
       </c>
       <c r="BA7" s="189" t="str">
-        <f>IF(ISBLANK(AllEntries!AU11),"unknown",AllEntries!AU11)</f>
+        <f>IF(ISBLANK(AllEntries!AW11),"unknown",AllEntries!AW11)</f>
         <v>unknown</v>
       </c>
       <c r="BB7" s="129" t="str">
@@ -12487,7 +12621,7 @@
       <c r="AK11" s="63"/>
       <c r="AT11" s="63"/>
     </row>
-    <row r="18" spans="4:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="60"/>
     </row>
   </sheetData>
@@ -13053,7 +13187,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="165" t="s">
         <v>142</v>
       </c>
@@ -13064,7 +13198,7 @@
       <c r="E38" s="109"/>
       <c r="F38" s="109"/>
     </row>
-    <row r="39" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="165" t="s">
         <v>45</v>
       </c>
@@ -13079,7 +13213,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="168" t="s">
         <v>36</v>
       </c>
@@ -13092,7 +13226,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="168" t="s">
         <v>46</v>
       </c>
@@ -13103,7 +13237,7 @@
       <c r="E41" s="109"/>
       <c r="F41" s="109"/>
     </row>
-    <row r="42" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="168" t="s">
         <v>163</v>
       </c>
@@ -13116,7 +13250,7 @@
       </c>
       <c r="F42" s="109"/>
     </row>
-    <row r="43" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="160" t="s">
         <v>143</v>
       </c>
@@ -13127,7 +13261,7 @@
       <c r="E43" s="109"/>
       <c r="F43" s="109"/>
     </row>
-    <row r="44" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="160" t="s">
         <v>144</v>
       </c>
@@ -13138,7 +13272,7 @@
       <c r="E44" s="109"/>
       <c r="F44" s="109"/>
     </row>
-    <row r="45" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="160" t="s">
         <v>56</v>
       </c>
@@ -13149,7 +13283,7 @@
       <c r="E45" s="109"/>
       <c r="F45" s="109"/>
     </row>
-    <row r="46" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="160" t="s">
         <v>33</v>
       </c>
@@ -13160,7 +13294,7 @@
       <c r="E46" s="109"/>
       <c r="F46" s="109"/>
     </row>
-    <row r="47" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="160" t="s">
         <v>32</v>
       </c>
@@ -13171,7 +13305,7 @@
       <c r="E47" s="109"/>
       <c r="F47" s="109"/>
     </row>
-    <row r="48" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="160" t="s">
         <v>139</v>
       </c>
@@ -13186,7 +13320,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="160" t="s">
         <v>139</v>
       </c>
@@ -13207,77 +13341,77 @@
     <sortCondition ref="C4:C49"/>
   </sortState>
   <conditionalFormatting sqref="B5:F5 B21:F22 B7:F12 B26:F27 B38:F41 B19:F19 B17:F17 B14:F15 B49:F49 B43:F47 B30:F36">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:F20">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:F6">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:F24">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37:F37">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:F23">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:F25">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:F18">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:F16">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:F13">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:F48">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:F42">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:F29">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:F28">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B28)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>